<commit_message>
try count of the metabolite hits
</commit_message>
<xml_diff>
--- a/test/experiments_filter.xlsx
+++ b/test/experiments_filter.xlsx
@@ -91,6 +91,42 @@
     <t>MTBLC17270; MTBLC81298; MTBLC10432; MTBLC16865; MTBLC143727; MTBLC81244; MTBLC67818; MTBLC111; MTBLC4464; MTBLC70101; MTBLC84828; MTBLC86241; MTBLC141535; MTBLC183976; MTBLC16984; MTBLC44369; MTBLC74340; MTBLC55430; MTBLC86436; MTBLC34112; MTBLC64496; MTBLC165594; MTBLC75568; MTBLC50599; MTBLC75062; MTBLC64489; MTBLC50450; MTBLC36466; MTBLC140477; MTBLC86248; MTBLC75216; MTBLC86092; MTBLC74963; MTBLC190958; MTBLC190960; MTBLC75466; MTBLC28468; MTBLC69081; MTBLC86167; MTBLC84829; MTBLC29069; MTBLC78226; MTBLC60657; MTBLC140861; MTBLC183969; MTBLC190967; MTBLC74669; MTBLC52333; MTBLC45240; MTBLC16164; MTBLC53003; MTBLC190971; MTBLC183971; MTBLC15559; MTBLC92059; MTBLC190974; MTBLC183986; MTBLC166500; MTBLC991; MTBLC27822; MTBLC18112; MTBLC15866; MTBLC190994; MTBLC20450; MTBLC18316; MTBLC82020; MTBLC183992; MTBLC182618; MTBLC178448; MTBLC41250; MTBLC190998; MTBLC191000; MTBLC955; MTBLC15698; MTBLC17622; MTBLC34076; MTBLC29585; MTBLC191014; MTBLC27794; MTBLC36206; MTBLC1582; MTBLC180391; MTBLC27596; MTBLC38635; MTBLC28345; MTBLC45213; MTBLC82321; MTBLC82343; MTBLC27637; MTBLC28335; MTBLC183883; MTBLC42334; MTBLC82569; MTBLC17645; MTBLC59026; MTBLC171939; MTBLC1864; MTBLC63800; MTBLC180385; MTBLC142593; MTBLC15815; MTBLC5141; MTBLC178626; MTBLC1895; MTBLC181128; MTBLC1904; MTBLC1911; MTBLC82509; MTBLC166563; MTBLC17405; MTBLC18311; MTBLC191035; MTBLC27983; MTBLC10070; MTBLC17957; MTBLC15887; MTBLC80636; MTBLC83455; MTBLC27551; MTBLC2110; MTBLC2003; MTBLC28952; MTBLC29022; MTBLC182534; MTBLC153787; MTBLC175789; MTBLC191050; MTBLC80703; MTBLC84199; MTBLC169008; MTBLC166605; MTBLC17899; MTBLC122149; MTBLC46195; MTBLC57589; MTBLC73024; MTBLC15355; MTBLC51739; MTBLC16708; MTBLC16335; MTBLC28931; MTBLC17431; MTBLC73393; MTBLC132793; MTBLC6173; MTBLC82170; MTBLC51211; MTBLC2622; MTBLC37023; MTBLC40050; MTBLC2704; MTBLC184022; MTBLC17296; MTBLC81728; MTBLC31225; MTBLC85253; MTBLC2813; MTBLC157792; MTBLC29016; MTBLC184023; MTBLC223316; MTBLC2873; MTBLC137245; MTBLC15930; MTBLC33421; MTBLC3001; MTBLC51348; MTBLC28179; MTBLC116735; MTBLC17987; MTBLC70476; MTBLC16958; MTBLC16469; MTBLC17750; MTBLC85533; MTBLC3087; MTBLC3127; MTBLC34578; MTBLC83106; MTBLC78661; MTBLC3223; MTBLC81806; MTBLC17395; MTBLC27732; MTBLC16841; MTBLC3387; MTBLC3391; MTBLC3410; MTBLC3441; MTBLC27860; MTBLC3474; MTBLC16755; MTBLC17698; MTBLC3606; MTBLC3655; MTBLC15354; MTBLC17333; MTBLC27509; MTBLC80805; MTBLC70721; MTBLC27965; MTBLC28322; MTBLC80741; MTBLC28794; MTBLC16919; MTBLC16737; MTBLC31439; MTBLC28671; MTBLC82112; MTBLC81955; MTBLC27641; MTBLC15773; MTBLC4021; MTBLC17141; MTBLC16040; MTBLC37550; MTBLC17784; MTBLC18268; MTBLC17061; MTBLC62324; MTBLC65327; MTBLC34664; MTBLC177036; MTBLC191092; MTBLC4388; MTBLC4428; MTBLC4435; MTBLC27373; MTBLC4470; MTBLC16583; MTBLC4512; MTBLC34694; MTBLC195269; MTBLC28123; MTBLC4527; MTBLC7071; MTBLC134841; MTBLC28917; MTBLC17874; MTBLC7087; MTBLC16057; MTBLC39183; MTBLC82093; MTBLC82143; MTBLC81842; MTBLC15356; MTBLC26271; MTBLC27897; MTBLC165591; MTBLC165583; MTBLC181802; MTBLC36798; MTBLC16813; MTBLC4744; MTBLC4747; MTBLC31530; MTBLC4786; MTBLC15407; MTBLC4811; MTBLC4828; MTBLC28412; MTBLC142245; MTBLC490095; MTBLC17474; MTBLC81827; MTBLC113535; MTBLC166543; MTBLC28600; MTBLC38680; MTBLC82159; MTBLC81917; MTBLC17818; MTBLC63115; MTBLC5094; MTBLC39291; MTBLC81920; MTBLC33083; MTBLC28266; MTBLC5132; MTBLC81923; MTBLC48427; MTBLC15728; MTBLC73705; MTBLC79628; MTBLC5294; MTBLC42768; MTBLC5298; MTBLC17858; MTBLC73514; MTBLC36313; MTBLC27471; MTBLC5553; MTBLC28172; MTBLC27943; MTBLC28121; MTBLC5633; MTBLC137124; MTBLC49793; MTBLC189167; MTBLC5712; MTBLC80834; MTBLC74059; MTBLC27570; MTBLC5747; MTBLC28631; MTBLC17594; MTBLC5827; MTBLC17368; MTBLC5856; MTBLC2894; MTBLC82022; MTBLC16031; MTBLC17566; MTBLC33070; MTBLC28909; MTBLC5962; MTBLC27539; MTBLC16135; MTBLC84838; MTBLC184058; MTBLC34800; MTBLC82189; MTBLC6257; MTBLC6133; MTBLC39243; MTBLC18344; MTBLC15334; MTBLC184062; MTBLC29110; MTBLC609827; MTBLC16347; MTBLC15400; MTBLC16349; MTBLC17587; MTBLC27747; MTBLC60107; MTBLC73580; MTBLC17490; MTBLC30913; MTBLC53210; MTBLC16927; MTBLC17394; MTBLC17716; MTBLC131762; MTBLC63791; MTBLC6426; MTBLC6456; MTBLC6507; MTBLC116278; MTBLC64566; MTBLC181926; MTBLC17781; MTBLC160118; MTBLC29623; MTBLC66682; MTBLC6717; MTBLC60607; MTBLC16796; MTBLC78277; MTBLC6754; MTBLC82141; MTBLC81823; MTBLC6791; MTBLC6820; MTBLC6821; MTBLC181042; MTBLC31837; MTBLC107736; MTBLC34846; MTBLC6935; MTBLC135005; MTBLC75283; MTBLC50729; MTBLC131342; MTBLC86396; MTBLC34856; MTBLC75281; MTBLC191137; MTBLC85262; MTBLC84634; MTBLC83358; MTBLC27744; MTBLC42298; MTBLC63154; MTBLC53480; MTBLC60152; MTBLC191060; MTBLC86910; MTBLC46979; MTBLC132722; MTBLC188227; MTBLC190815; MTBLC181934; MTBLC59732; MTBLC17519; MTBLC67045; MTBLC35807; MTBLC63866; MTBLC184082; MTBLC72959; MTBLC67033; MTBLC78759; MTBLC176482; MTBLC34860; MTBLC64349; MTBLC63971; MTBLC17929; MTBLC15940; MTBLC18723; MTBLC7602; MTBLC125411; MTBLC7633; MTBLC27410; MTBLC16160; MTBLC66892; MTBLC44794; MTBLC73039; MTBLC15805; MTBLC28285; MTBLC7751; MTBLC69832; MTBLC81937; MTBLC74475; MTBLC71465; MTBLC78646; MTBLC7916; MTBLC7939; MTBLC9970; MTBLC83569; MTBLC39631; MTBLC45081; MTBLC179164; MTBLC8024; MTBLC8029; MTBLC36421; MTBLC17884; MTBLC38786; MTBLC18132; MTBLC36605; MTBLC46961; MTBLC34922; MTBLC8205; MTBLC8206; MTBLC30531; MTBLC78549; MTBLC18049; MTBLC82267; MTBLC50305; MTBLC8357; MTBLC73646; MTBLC141395; MTBLC74797; MTBLC134898; MTBLC34934; MTBLC26276; MTBLC34935; MTBLC70778; MTBLC32061; MTBLC8499; MTBLC81941; MTBLC64535; MTBLC39311; MTBLC81866; MTBLC81828; MTBLC16227; MTBLC17310; MTBLC16410; MTBLC16709; MTBLC8674; MTBLC45141; MTBLC33135; MTBLC32816; MTBLC17521; MTBLC8772; MTBLC8822; MTBLC8825; MTBLC156194; MTBLC8863; MTBLC8891; MTBLC16563; MTBLC15694; MTBLC17509; MTBLC94493; MTBLC15578; MTBLC66435; MTBLC156168; MTBLC82228; MTBLC9079; MTBLC9111; MTBLC27496; MTBLC83476; MTBLC34976; MTBLC28374; MTBLC16393; MTBLC35280; MTBLC34900; MTBLC9300; MTBLC4312; MTBLC82218; MTBLC53727; MTBLC102265; MTBLC9367; MTBLC82043; MTBLC9430; MTBLC63625; MTBLC9463; MTBLC35000; MTBLC165595; MTBLC44920; MTBLC39175; MTBLC83453; MTBLC27712; MTBLC63631; MTBLC48669; MTBLC35697; MTBLC16522; MTBLC38905; MTBLC9683; MTBLC9682; MTBLC9700; MTBLC28621; MTBLC9715; MTBLC18123; MTBLC15724; MTBLC28329; MTBLC9754; MTBLC157895; MTBLC17568; MTBLC29703; MTBLC145239; MTBLC9936; MTBLC9951; MTBLC16954; MTBLC10056; MTBLC18107; MTBLC10106; MTBLC63892; MTBLC27362; MTBLC10110; MTBLC10125; MTBLC64486; MTBLC85020; MTBLC84527; MTBLC28854; MTBLC15913; MTBLC35619; MTBLC183836; MTBLC89397; MTBLC180751; MTBLC10136; MTBLC79099; MTBLC79207; MTBLC79203; MTBLC116509; MTBLC73215; MTBLC28877; MTBLC16354; MTBLC183861; MTBLC183862; MTBLC34080; MTBLC190945; MTBLC79113; MTBLC74850; MTBLC133600; MTBLC60427; MTBLC85963; MTBLC27418; MTBLC190949; MTBLC28667; MTBLC72639; MTBLC190953; MTBLC55328; MTBLC91517; MTBLC182093; MTBLC190959; MTBLC180516; MTBLC78268; MTBLC183870; MTBLC30793; MTBLC19644; MTBLC81049; MTBLC44229; MTBLC79096; MTBLC15753; MTBLC34230; MTBLC42017; MTBLC28755; MTBLC17713; MTBLC69426; MTBLC183882; MTBLC17947; MTBLC180531; MTBLC20067; MTBLC35932; MTBLC17794; MTBLC68531; MTBLC61312; MTBLC17597; MTBLC30817; MTBLC39076; MTBLC16318; MTBLC39349; MTBLC17549; MTBLC183892; MTBLC183893; MTBLC28849; MTBLC34162; MTBLC78741; MTBLC191007; MTBLC17224; MTBLC15830; MTBLC80470; MTBLC81133; MTBLC191013; MTBLC177497; MTBLC28820; MTBLC183896; MTBLC50099; MTBLC27957; MTBLC40410; MTBLC17709; MTBLC30832; MTBLC15676; MTBLC17925; MTBLC2624; MTBLC22653; MTBLC48131; MTBLC36622; MTBLC30746; MTBLC30813; MTBLC41321; MTBLC3703; MTBLC16231; MTBLC28125; MTBLC32805; MTBLC16508; MTBLC30769; MTBLC3962; MTBLC27891; MTBLC17562; MTBLC28797; MTBLC18333; MTBLC17364; MTBLC16893; MTBLC16176; MTBLC16313; MTBLC27605; MTBLC17924; MTBLC4331; MTBLC17172; MTBLC134081; MTBLC490877; MTBLC17755; MTBLC68664; MTBLC18237; MTBLC28300; MTBLC17822; MTBLC4676; MTBLC30805; MTBLC45599; MTBLC18243; MTBLC4778; MTBLC191040; MTBLC4735; MTBLC4909; MTBLC172329; MTBLC81853; MTBLC82017; MTBLC36575; MTBLC42471; MTBLC5202; MTBLC107639; MTBLC5276; MTBLC76051; MTBLC75430; MTBLC36274; MTBLC63484; MTBLC16235; MTBLC32365; MTBLC191048; MTBLC18089; MTBLC5792; MTBLC17596; MTBLC17808; MTBLC5973; MTBLC30887; MTBLC34799; MTBLC24898; MTBLC17965; MTBLC191052; MTBLC43572; MTBLC81220; MTBLC422; MTBLC16977; MTBLC18183; MTBLC15908; MTBLC16857; MTBLC6343; MTBLC182549; MTBLC25094; MTBLC6643; MTBLC6650; MTBLC30794; MTBLC135976; MTBLC6784; MTBLC45129; MTBLC191133; MTBLC6956; MTBLC17268; MTBLC28875; MTBLC170015; MTBLC16259; MTBLC21563; MTBLC191062; MTBLC73685; MTBLC17768; MTBLC183936; MTBLC183705; MTBLC44356; MTBLC66614; MTBLC191074; MTBLC29019; MTBLC138644; MTBLC28842; MTBLC16196; MTBLC16536; MTBLC16742; MTBLC1015; MTBLC69833; MTBLC18058; MTBLC7822; MTBLC44909; MTBLC27849; MTBLC15756; MTBLC74661; MTBLC66849; MTBLC64517; MTBLC64516; MTBLC64433; MTBLC64504; MTBLC64525; MTBLC64519; MTBLC64521; MTBLC134451; MTBLC141588; MTBLC71731; MTBLC134239; MTBLC42504; MTBLC141297; MTBLC136229; MTBLC156031; MTBLC73635; MTBLC50392; MTBLC184087; MTBLC191120; MTBLC44897; MTBLC28915; MTBLC37712; MTBLC16285; MTBLC136235; MTBLC136239; MTBLC50212; MTBLC183950; MTBLC8427; MTBLC17026; MTBLC30768; MTBLC17802; MTBLC44992; MTBLC35584; MTBLC93953; MTBLC81849; MTBLC16365; MTBLC16675; MTBLC48562; MTBLC27810; MTBLC28592; MTBLC183953; MTBLC9008; MTBLC15611; MTBLC28813; MTBLC190218; MTBLC190228; MTBLC138578; MTBLC52330; MTBLC16265; MTBLC17992; MTBLC187382; MTBLC15891; MTBLC81816; MTBLC15702; MTBLC9481; MTBLC144238; MTBLC91429; MTBLC33540; MTBLC182146; MTBLC169666; MTBLC32806; MTBLC27036; MTBLC114185; MTBLC16264; MTBLC64850; MTBLC27226; MTBLC16704; MTBLC30816; MTBLC15318</t>
   </si>
   <si>
+    <t>MTBLS650</t>
+  </si>
+  <si>
+    <t>Global untargeted serum metabolomic analyses nominate metabolic pathways responsive to loss of expression of the orphan metallo beta-lactamase, MBLAC1</t>
+  </si>
+  <si>
+    <t>The &lt;i&gt;C. elegans&lt;/i&gt; gene swip-10 encodes an orphan metallo beta-lactamase that genetic studies indicate is vital for limiting neuronal excitability and viability. Sequence analysis indicates that the mammalian gene Mblac1 is the likely ortholog of swip-10, with greatest sequence identity localized to the encoded protein's single metallo beta-lactamase domain. The substrate for the SWIP-10 protein remains unknown and to date no functional roles have been ascribed to MBLAC1, though we have shown that the protein binds the neuroprotective beta-lactam antibiotic, ceftriaxone. To gain insight into the functional role of MBLAC1 in vivo, we used CRISPR/Cas9 methods to disrupt N-terminal coding sequences of the mouse Mblac1 gene, resulting in a complete loss of protein expression in viable, homozygous knockout (KO) animals. Using serum from both WT and KO mice, we performed global, untargeted metabolomic analyses, resolving small molecules via hydrophilic interaction chromatography (HILIC) based ultra-performance liquid chromatography, coupled to mass spectrometry (UPLC-MS/MS). Unsupervised principal component analysis reliably segregated the metabolomes of MBLAC1 KO and WT mice, with 92 features subsequently nominated as significantly different by ANOVA, and for which we made tentative and putative metabolite assignments. Bioinformatic analyses of these molecules nominate validated pathways subserving bile acid biosynthesis and linoleate metabolism, networks known to be responsive to metabolic and oxidative stress. Our findings lead to hypotheses that can guide future targeted studies seeking to identify the substrate for MBLAC1 and how substrate hydrolysis supports the neuroprotective actions of ceftriaxone.&lt;br&gt;</t>
+  </si>
+  <si>
+    <t>Ultra-Performance Liquid Chromatography-Mass Spectrometry; tandem mass spectrometry; untargeted metabolites; Beta-Lactamase; ceftriaxone; SWIP-10 protein, C elegans</t>
+  </si>
+  <si>
+    <t>Global untargeted serum metabolomic analyses nominate metabolic pathways responsive to loss of expression of the orphan metallo beta-lactamase, MBLAC1. 10.1039/c7mo00022g. PMID:29868674</t>
+  </si>
+  <si>
+    <t>Our initial untargeted study made use of serum collected from 3, age-(1216 weeks) and sex-(female) matched WT and KO mice. WT mice were commercially obtained C57BL/6J mice (Jackson Labs, Bar Harbor Maine, USA). Our subsequent pathway validation study reported is derived from serum collected from 4 sex-(female) matched WT and KO littermates (aged 1216 weeks) bred from Mblac1 heterozygous parents. Following rapid decapitation of mice, 0.50.75 ml of trunk blood (blood immediately collected from the body at the site of decapitation) was collected, allowed to coagulate on ice for 30 min and centrifuged (15 min at 5000 rpm).</t>
+  </si>
+  <si>
+    <t>Serum (50 l) was collected into fresh tubes followed by addition of ice cold 80% methanol (5x by volume), then stored at -80 C overnight. On the next day, samples were centrifuged at 10 000 rpm for 15 min to eliminate methanol precipitated proteins. This methanol precipitation step was repeated and the metabolite containing supernatant was dried via speed-vacuum and stored at -80 C until analysis.</t>
+  </si>
+  <si>
+    <t>For mass spectrometry analysis, dried extracts were reconstituted in 100 l of acetonitrile/water (80:20, v/v) and centrifuged for 5 min at 15 000 rpm to remove insoluble material. Quality control (QC) samples were prepared by pooling equal volumes from each experimental sample.&lt;br&gt;&lt;br&gt;MS analyses were performed on a Q-Exactive HF hybrid mass spectrometer (Thermo Fisher Scientific, Bremen, Germany) equipped with a Vanquish UHPLC binary system and autosampler (Thermo Fisher Scientific, Germany). Extracts (5 l injection volume) were separated on a SeQuant ZIC-HILIC 3.5 m, 2.1 mm x 100 mm column (Millipore Corporation, Darmstadt, Germany) held at 40 C. Liquid chromatography was performed at a 200 l/min using solvent A (5 mM ammonium formate in 90% water, 10% acetonitrile) and solvent B (5 mM ammonium formate in 90% acetonitrile, 10% water) with the following gradient: 90% B for 2 min, 9040% B over 16 min, 40% B held 2 min, and 4090% B over 10 min, 90% B held 10 min (gradient length 40 min).</t>
+  </si>
+  <si>
+    <t>Full MS analyses were acquired on a Thermo Fisher Scientific Q-Exactive HF hybrid mass spectrometer over a mass range of m/z 701050 under an ESI positive profile mode and separately under an ESI negative profile mode. Full mass scan was used at a resolution of 120 000 with a scan rate at ~3.5 Hz. The automatic gain control (AGC) target was set at 1 x 10^6 ions, and maximum ion injection time (IT) was at 100 ms. Source ionization parameters were optimized with the spray voltage at 3.0 kV, and other parameters were as follows: transfer temperature at 280 C; S-Lens level at 40; heater temperature at 325 C; Sheath gas at 40, Aux gas at 10, and sweep gas flow at 1. Data dependent(DD) MS/MS spectra were acquired using a data dependent scanning mode in which 1 full MS scan (m/z 701050) was followed by 2 MS/MS scans. MS/MS scans are acquired in profile mode using an isolation width of 1.3 m/z, stepped collision energy (NCE 20, 40, 60), and a dynamic exclusion of 6 s. MS/MS spectra were collected at a resolution of 15 000 with an AGC target set at 2 x 10^5 ions, and IT of 100 ms. To assess instrument performance and reproducibility throughout our experimental run sequence, we monitored the retention times and peak areas for a subset of identified endogenous molecules (n = 10) observed in the 3 DD QC pool runs bracketing the experimental FMS QC and experimental run sequence (visualized using Skyline (www.skyline.ms)[1]).&lt;br&gt;&lt;br&gt;Full MS (FMS) data was acquired for the QC pool, in both HILIC-POS (3 FMS QC runs) and HILIC-NEG (1 FMS QC runs) methods, to use as a retention time alignment reference within Progenesis QI for subsequent normalization and data quantitation. MS/MS (data dependent (DD)) acquisitions for pooled QCs were run to assess instrument performance over time and used for feature annotation.&lt;br&gt;&lt;br&gt;Ref:&lt;br&gt;[1] MacLean B, Tomazela DM, Shulman N, Chambers M, Finney GL, Frewen B, Kern R, Tabb DL, Liebler DC, MacCoss MJ. Skyline: an open source document editor for creating and analyzing targeted proteomics experiments. Bioinformatics. 2010 Apr 1;26(7):966-8. doi:10.1093/bioinformatics/btq054. PMID:20147306</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;UPLC-MS/MS raw data were imported, processed, normalized, and reviewed using Progenesis QI v.2.1 (Non-linear Dynamics, Newcastle, UK).&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;Tentative and putative annotations were determined within Progenesis using accurate mass measurements (&amp;lt;5 ppm error), isotope distribution similarity, and manual assessment of fragmentation spectrum matching (when applicable) from the Human Metabolome Database (HMDB)[1], Metlin[2], MassBank[3], and the National Institute of Standards and Technology (NIST) database[4]. Additional putative annotations were assigned using Compound Discoverer 2.0 (Thermo Scientific, Waltham,MA, USA).&amp;nbsp; Increased confidence in the annotation of many features was achieved by manually assessing spectral match and RT consistencies between experimental data and chemical standards within a curated in-house library. Chemical standards (purchased from Sigma Aldrich (St. Louis, MO) unless otherwise specified) were prepared at a concentration of 10 ng/l in acetonitrile/water (80/20, v/v).&lt;/div&gt;&lt;div&gt;&lt;br&gt;&lt;/div&gt;&lt;div&gt;Ref:&lt;/div&gt;&lt;div&gt;[1] Wishart DS, Jewison T, Guo AC, Wilson M, Knox C, Liu Yet al. HMDB 3.0--The Human Metabolome Database in 2013. Nucleic Acids Res. 2013 Jan;41(Database issue):D801-7. doi: 10.1093/nar/gks1065. PMID:23161693&lt;/div&gt;&lt;div&gt;[2] Smith CA, O'Maille G, Want EJ, Qin C, Trauger SA, Brandon TR, Custodio DE, Abagyan R, Siuzdak G. METLIN: a metabolite mass spectral database. Ther Drug Monit. 2005 Dec;27(6):747-51. PMID:16404815&lt;/div&gt;&lt;div&gt;[3] Horai H, Arita M, Kanaya S, Nihei Y, Ikeda T, Suwa K, Ojima Y et al. MassBank: a public repository for sharing mass spectral data for life sciences. J Mass Spectrom. 2010 Jul;45(7):703-14. doi:10.1002/jms.1777. PMID:20623627&lt;/div&gt;&lt;div&gt;[4] F. S. A. Jablonski, C. J. Powell and A. Y. Lee, NIST Electron Elastic-Scattering Cross-Section Database  Version 4.0, National Institute of Standards and Technology, Gaithersburg, MD, 2016. doi:10.6028/NIST.NSRDS.64&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>MTBLC18049; MTBLC17568; MTBLC16343; MTBLC16010; MTBLC16092; MTBLC24898; MTBLC72772; MTBLC22653; MTBLC18257; MTBLC22660; MTBLC31697; MTBLC74112; MTBLC88954; MTBLC18123; MTBLC27248; MTBLC143235; MTBLC16811; MTBLC27570; MTBLC30985; MTBLC143246; MTBLC53003; MTBLC6804; MTBLC17604; MTBLC2274; MTBLC70959; MTBLC18211; MTBLC132244; MTBLC17533; MTBLC27480; MTBLC16543; MTBLC143240; MTBLC16828; MTBLC28683; MTBLC143241; MTBLC143247; MTBLC53480; MTBLC143239; MTBLC70976; MTBLC7027; MTBLC70749; MTBLC143249; MTBLC143248; MTBLC17361; MTBLC88543; MTBLC68830; MTBLC89234; MTBLC73067; MTBLC73134; MTBLC28865; MTBLC9410; MTBLC136143; MTBLC136120; MTBLC64566; MTBLC143227; MTBLC131989; MTBLC77890; MTBLC134600; MTBLC143230; MTBLC143226; MTBLC26836; MTBLC17847; MTBLC27398; MTBLC30845; MTBLC139272; MTBLC17597; MTBLC1157; MTBLC16458; MTBLC40992; MTBLC24898; MTBLC72772; MTBLC17364; MTBLC17053; MTBLC68566; MTBLC32811; MTBLC62318; MTBLC16742; MTBLC4312; MTBLC32980; MTBLC143250; MTBLC17775; MTBLC32354; MTBLC32805; MTBLC22652; MTBLC16552; MTBLC42017; MTBLC143244; MTBLC27480; MTBLC24266; MTBLC89901; MTBLC16296; MTBLC24813; MTBLC43355; MTBLC39567; MTBLC16450; MTBLC143237; MTBLC89621; MTBLC17802; MTBLC70976; MTBLC28716; MTBLC2869; MTBLC55328; MTBLC143251; MTBLC143236; MTBLC17351; MTBLC87986; MTBLC72815; MTBLC72665; MTBLC143242; MTBLC139134; MTBLC28834; MTBLC143243; MTBLC73134; MTBLC143245; MTBLC16525; MTBLC52022; MTBLC143228; MTBLC143238</t>
+  </si>
+  <si>
     <t>MTBLS4187</t>
   </si>
   <si>
@@ -127,40 +163,76 @@
     <t>MTBLC28842; MTBLC15756; MTBLC17351; MTBLC16196; MTBLC28125; MTBLC15843; MTBLC18102; MTBLC84834; MTBLC88543; MTBLC68830; MTBLC57589; MTBLC7676; MTBLC16737; MTBLC89717; MTBLC73054; MTBLC89746; MTBLC28867; MTBLC89716; MTBLC85095; MTBLC20392; MTBLC15699; MTBLC16347; MTBLC17895; MTBLC17203; MTBLC17750; MTBLC15971; MTBLC18211; MTBLC73061; MTBLC16828; MTBLC16977; MTBLC17196; MTBLC16015; MTBLC17115; MTBLC16643; MTBLC15603; MTBLC17490; MTBLC75145; MTBLC18050; MTBLC68440; MTBLC17295; MTBLC15428; MTBLC17053; MTBLC16467; MTBLC73074; MTBLC18019; MTBLC18257; MTBLC16919; MTBLC28733; MTBLC86255; MTBLC64561; MTBLC64563; MTBLC90008; MTBLC176694; MTBLC74535; MTBLC91146; MTBLC86184; MTBLC86086; MTBLC170661; MTBLC89545; MTBLC86094; MTBLC73873; MTBLC86259; MTBLC74343; MTBLC72737; MTBLC137889; MTBLC83055; MTBLC89731; MTBLC86099; MTBLC88990; MTBLC134073; MTBLC84822; MTBLC65107; MTBLC88910; MTBLC72959; MTBLC86176; MTBLC83359; MTBLC90483; MTBLC74533; MTBLC86170; MTBLC190464; MTBLC67042; MTBLC170598; MTBLC86109; MTBLC75026; MTBLC64483; MTBLC73851; MTBLC83058; MTBLC74348; MTBLC88685; MTBLC133617; MTBLC170346; MTBLC75038; MTBLC89903; MTBLC85037; MTBLC167278; MTBLC170619; MTBLC73865; MTBLC89892; MTBLC83718; MTBLC190465; MTBLC149661; MTBLC74450; MTBLC190466; MTBLC89973; MTBLC67045; MTBLC170412; MTBLC78266; MTBLC72999; MTBLC170213; MTBLC28374; MTBLC190467; MTBLC190160; MTBLC75304; MTBLC60657; MTBLC88897; MTBLC64486; MTBLC140773; MTBLC189930</t>
   </si>
   <si>
-    <t>MTBLS650</t>
-  </si>
-  <si>
-    <t>Global untargeted serum metabolomic analyses nominate metabolic pathways responsive to loss of expression of the orphan metallo beta-lactamase, MBLAC1</t>
-  </si>
-  <si>
-    <t>The &lt;i&gt;C. elegans&lt;/i&gt; gene swip-10 encodes an orphan metallo beta-lactamase that genetic studies indicate is vital for limiting neuronal excitability and viability. Sequence analysis indicates that the mammalian gene Mblac1 is the likely ortholog of swip-10, with greatest sequence identity localized to the encoded protein's single metallo beta-lactamase domain. The substrate for the SWIP-10 protein remains unknown and to date no functional roles have been ascribed to MBLAC1, though we have shown that the protein binds the neuroprotective beta-lactam antibiotic, ceftriaxone. To gain insight into the functional role of MBLAC1 in vivo, we used CRISPR/Cas9 methods to disrupt N-terminal coding sequences of the mouse Mblac1 gene, resulting in a complete loss of protein expression in viable, homozygous knockout (KO) animals. Using serum from both WT and KO mice, we performed global, untargeted metabolomic analyses, resolving small molecules via hydrophilic interaction chromatography (HILIC) based ultra-performance liquid chromatography, coupled to mass spectrometry (UPLC-MS/MS). Unsupervised principal component analysis reliably segregated the metabolomes of MBLAC1 KO and WT mice, with 92 features subsequently nominated as significantly different by ANOVA, and for which we made tentative and putative metabolite assignments. Bioinformatic analyses of these molecules nominate validated pathways subserving bile acid biosynthesis and linoleate metabolism, networks known to be responsive to metabolic and oxidative stress. Our findings lead to hypotheses that can guide future targeted studies seeking to identify the substrate for MBLAC1 and how substrate hydrolysis supports the neuroprotective actions of ceftriaxone.&lt;br&gt;</t>
-  </si>
-  <si>
-    <t>Ultra-Performance Liquid Chromatography-Mass Spectrometry; tandem mass spectrometry; untargeted metabolites; Beta-Lactamase; ceftriaxone; SWIP-10 protein, C elegans</t>
-  </si>
-  <si>
-    <t>Global untargeted serum metabolomic analyses nominate metabolic pathways responsive to loss of expression of the orphan metallo beta-lactamase, MBLAC1. 10.1039/c7mo00022g. PMID:29868674</t>
-  </si>
-  <si>
-    <t>Our initial untargeted study made use of serum collected from 3, age-(1216 weeks) and sex-(female) matched WT and KO mice. WT mice were commercially obtained C57BL/6J mice (Jackson Labs, Bar Harbor Maine, USA). Our subsequent pathway validation study reported is derived from serum collected from 4 sex-(female) matched WT and KO littermates (aged 1216 weeks) bred from Mblac1 heterozygous parents. Following rapid decapitation of mice, 0.50.75 ml of trunk blood (blood immediately collected from the body at the site of decapitation) was collected, allowed to coagulate on ice for 30 min and centrifuged (15 min at 5000 rpm).</t>
-  </si>
-  <si>
-    <t>Serum (50 l) was collected into fresh tubes followed by addition of ice cold 80% methanol (5x by volume), then stored at -80 C overnight. On the next day, samples were centrifuged at 10 000 rpm for 15 min to eliminate methanol precipitated proteins. This methanol precipitation step was repeated and the metabolite containing supernatant was dried via speed-vacuum and stored at -80 C until analysis.</t>
-  </si>
-  <si>
-    <t>For mass spectrometry analysis, dried extracts were reconstituted in 100 l of acetonitrile/water (80:20, v/v) and centrifuged for 5 min at 15 000 rpm to remove insoluble material. Quality control (QC) samples were prepared by pooling equal volumes from each experimental sample.&lt;br&gt;&lt;br&gt;MS analyses were performed on a Q-Exactive HF hybrid mass spectrometer (Thermo Fisher Scientific, Bremen, Germany) equipped with a Vanquish UHPLC binary system and autosampler (Thermo Fisher Scientific, Germany). Extracts (5 l injection volume) were separated on a SeQuant ZIC-HILIC 3.5 m, 2.1 mm x 100 mm column (Millipore Corporation, Darmstadt, Germany) held at 40 C. Liquid chromatography was performed at a 200 l/min using solvent A (5 mM ammonium formate in 90% water, 10% acetonitrile) and solvent B (5 mM ammonium formate in 90% acetonitrile, 10% water) with the following gradient: 90% B for 2 min, 9040% B over 16 min, 40% B held 2 min, and 4090% B over 10 min, 90% B held 10 min (gradient length 40 min).</t>
-  </si>
-  <si>
-    <t>Full MS analyses were acquired on a Thermo Fisher Scientific Q-Exactive HF hybrid mass spectrometer over a mass range of m/z 701050 under an ESI positive profile mode and separately under an ESI negative profile mode. Full mass scan was used at a resolution of 120 000 with a scan rate at ~3.5 Hz. The automatic gain control (AGC) target was set at 1 x 10^6 ions, and maximum ion injection time (IT) was at 100 ms. Source ionization parameters were optimized with the spray voltage at 3.0 kV, and other parameters were as follows: transfer temperature at 280 C; S-Lens level at 40; heater temperature at 325 C; Sheath gas at 40, Aux gas at 10, and sweep gas flow at 1. Data dependent(DD) MS/MS spectra were acquired using a data dependent scanning mode in which 1 full MS scan (m/z 701050) was followed by 2 MS/MS scans. MS/MS scans are acquired in profile mode using an isolation width of 1.3 m/z, stepped collision energy (NCE 20, 40, 60), and a dynamic exclusion of 6 s. MS/MS spectra were collected at a resolution of 15 000 with an AGC target set at 2 x 10^5 ions, and IT of 100 ms. To assess instrument performance and reproducibility throughout our experimental run sequence, we monitored the retention times and peak areas for a subset of identified endogenous molecules (n = 10) observed in the 3 DD QC pool runs bracketing the experimental FMS QC and experimental run sequence (visualized using Skyline (www.skyline.ms)[1]).&lt;br&gt;&lt;br&gt;Full MS (FMS) data was acquired for the QC pool, in both HILIC-POS (3 FMS QC runs) and HILIC-NEG (1 FMS QC runs) methods, to use as a retention time alignment reference within Progenesis QI for subsequent normalization and data quantitation. MS/MS (data dependent (DD)) acquisitions for pooled QCs were run to assess instrument performance over time and used for feature annotation.&lt;br&gt;&lt;br&gt;Ref:&lt;br&gt;[1] MacLean B, Tomazela DM, Shulman N, Chambers M, Finney GL, Frewen B, Kern R, Tabb DL, Liebler DC, MacCoss MJ. Skyline: an open source document editor for creating and analyzing targeted proteomics experiments. Bioinformatics. 2010 Apr 1;26(7):966-8. doi:10.1093/bioinformatics/btq054. PMID:20147306</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;UPLC-MS/MS raw data were imported, processed, normalized, and reviewed using Progenesis QI v.2.1 (Non-linear Dynamics, Newcastle, UK).&lt;/div&gt;</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;Tentative and putative annotations were determined within Progenesis using accurate mass measurements (&amp;lt;5 ppm error), isotope distribution similarity, and manual assessment of fragmentation spectrum matching (when applicable) from the Human Metabolome Database (HMDB)[1], Metlin[2], MassBank[3], and the National Institute of Standards and Technology (NIST) database[4]. Additional putative annotations were assigned using Compound Discoverer 2.0 (Thermo Scientific, Waltham,MA, USA).&amp;nbsp; Increased confidence in the annotation of many features was achieved by manually assessing spectral match and RT consistencies between experimental data and chemical standards within a curated in-house library. Chemical standards (purchased from Sigma Aldrich (St. Louis, MO) unless otherwise specified) were prepared at a concentration of 10 ng/l in acetonitrile/water (80/20, v/v).&lt;/div&gt;&lt;div&gt;&lt;br&gt;&lt;/div&gt;&lt;div&gt;Ref:&lt;/div&gt;&lt;div&gt;[1] Wishart DS, Jewison T, Guo AC, Wilson M, Knox C, Liu Yet al. HMDB 3.0--The Human Metabolome Database in 2013. Nucleic Acids Res. 2013 Jan;41(Database issue):D801-7. doi: 10.1093/nar/gks1065. PMID:23161693&lt;/div&gt;&lt;div&gt;[2] Smith CA, O'Maille G, Want EJ, Qin C, Trauger SA, Brandon TR, Custodio DE, Abagyan R, Siuzdak G. METLIN: a metabolite mass spectral database. Ther Drug Monit. 2005 Dec;27(6):747-51. PMID:16404815&lt;/div&gt;&lt;div&gt;[3] Horai H, Arita M, Kanaya S, Nihei Y, Ikeda T, Suwa K, Ojima Y et al. MassBank: a public repository for sharing mass spectral data for life sciences. J Mass Spectrom. 2010 Jul;45(7):703-14. doi:10.1002/jms.1777. PMID:20623627&lt;/div&gt;&lt;div&gt;[4] F. S. A. Jablonski, C. J. Powell and A. Y. Lee, NIST Electron Elastic-Scattering Cross-Section Database  Version 4.0, National Institute of Standards and Technology, Gaithersburg, MD, 2016. doi:10.6028/NIST.NSRDS.64&lt;/div&gt;</t>
-  </si>
-  <si>
-    <t>MTBLC18049; MTBLC17568; MTBLC16343; MTBLC16010; MTBLC16092; MTBLC24898; MTBLC72772; MTBLC22653; MTBLC18257; MTBLC22660; MTBLC31697; MTBLC74112; MTBLC88954; MTBLC18123; MTBLC27248; MTBLC143235; MTBLC16811; MTBLC27570; MTBLC30985; MTBLC143246; MTBLC53003; MTBLC6804; MTBLC17604; MTBLC2274; MTBLC70959; MTBLC18211; MTBLC132244; MTBLC17533; MTBLC27480; MTBLC16543; MTBLC143240; MTBLC16828; MTBLC28683; MTBLC143241; MTBLC143247; MTBLC53480; MTBLC143239; MTBLC70976; MTBLC7027; MTBLC70749; MTBLC143249; MTBLC143248; MTBLC17361; MTBLC88543; MTBLC68830; MTBLC89234; MTBLC73067; MTBLC73134; MTBLC28865; MTBLC9410; MTBLC136143; MTBLC136120; MTBLC64566; MTBLC143227; MTBLC131989; MTBLC77890; MTBLC134600; MTBLC143230; MTBLC143226; MTBLC26836; MTBLC17847; MTBLC27398; MTBLC30845; MTBLC139272; MTBLC17597; MTBLC1157; MTBLC16458; MTBLC40992; MTBLC24898; MTBLC72772; MTBLC17364; MTBLC17053; MTBLC68566; MTBLC32811; MTBLC62318; MTBLC16742; MTBLC4312; MTBLC32980; MTBLC143250; MTBLC17775; MTBLC32354; MTBLC32805; MTBLC22652; MTBLC16552; MTBLC42017; MTBLC143244; MTBLC27480; MTBLC24266; MTBLC89901; MTBLC16296; MTBLC24813; MTBLC43355; MTBLC39567; MTBLC16450; MTBLC143237; MTBLC89621; MTBLC17802; MTBLC70976; MTBLC28716; MTBLC2869; MTBLC55328; MTBLC143251; MTBLC143236; MTBLC17351; MTBLC87986; MTBLC72815; MTBLC72665; MTBLC143242; MTBLC139134; MTBLC28834; MTBLC143243; MTBLC73134; MTBLC143245; MTBLC16525; MTBLC52022; MTBLC143228; MTBLC143238</t>
+    <t>MTBLS1066</t>
+  </si>
+  <si>
+    <t>Untargeted Metabolomics Reveals Molecular Effects of Ketogenic Diet on Healthy and Tumor Xenograft Mouse Models</t>
+  </si>
+  <si>
+    <t>The application of ketogenic diet (KD) (high fat/low carbohydrate/adequate protein) as an auxiliary cancer therapy is a field of growing attention. KD provides sufficient energy supply for healthy cells, while possibly impairing energy production in highly glycolytic tumor cells. Moreover, KD regulates insulin and tumor related growth factors (like insulin growth factor-1, IGF-1). In order to provide molecular evidence for the proposed additional inhibition of tumor growth when combining chemotherapy with KD, we applied untargeted quantitative metabolome analysis on a spontaneous breast cancer xenograft mouse model, using MDA-MB-468 cells. Healthy mice and mice bearing breast cancer xenografts and receiving cyclophosphamide chemotherapy were compared after treatment with control diet and KD. Metabolomic profiling was performed on plasma samples, applying high-performance liquid chromatography coupled to tandem mass spectrometry. Statistical analysis revealed metabolic fingerprints comprising numerous significantly regulated features in the group of mice bearing breast cancer. This fingerprint disappeared after treatment with KD, resulting in recovery to the metabolic status observed in healthy mice receiving control diet. Moreover, amino acid metabolism as well as fatty acid transport were found to be affected by both the tumor and the applied KD. Our results provide clear evidence of a significant molecular effect of adjuvant KD in the context of tumor growth inhibition and suggest additional mechanisms of tumor suppression beyond the proposed constrain in energy supply of tumor cells.</t>
+  </si>
+  <si>
+    <t>Ketogenic Diet; breast cancer; Xenograft; untargeted metabolites; ultra-performance liquid chromatography-mass spectrometry</t>
+  </si>
+  <si>
+    <t>Untargeted Metabolomics Reveals Molecular Effects of Ketogenic Diet on Healthy and Tumor Xenograft Mouse Models. 10.3390/ijms20163873. PMID:31398922</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;MDA-MB-468 cell line (ATCC, HTB-132) was used for the generation of breast cancer xenografts. Cells were cultivated in high glucose DMEM medium (Sigma-Aldrich, St. Louis, MO, USA) supplemented with heat-inactivated fetal bovine serum (Gibco, Vienna, Austria) and penicillin/streptomycin amphotericin B solution (Lonza, Cologne, Germany).&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;All in vivo experiments were performed on female CD-1 nu/nu mice (Charles River, Sulzfeld, Germany), the animals were group-housed and had unlimited access to food and water. Xenografts were established as previously described[1][2]. Briefly, a suspension of 1.5 x 10^7 MDA-MB-468 cells in serum-free medium and matrigel (BD Biosciences, Austria) were injected into the right flank of 5- to 6-week-old mice.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;As soon as tumor size reached 300350 mm^3 (i.e., 25 weeks after injection of tumor cells), mice were randomized into different dietary intervention groups (CTRL, LCT-MCT8; n = 56)[1]. As mice are able to keep blood glucose levels and show lower ketosis on 2:1 to 4:1 diets, compared to humans, we decided to use an 8:1 diet in our mouse model, to reach at least a ketosis over 2 mmol/l. Dietary interventions were combined with oral metronomic chemotherapy with CPA (30 mg/kg). The healthy, 7 weeks old, mice were fed with the experimental diets (CTRL, LCT-MCT8; see Table S2 in the paper associated with this study)[1][2]. All animals were monitored twice a week for body weight using a digital scale. Blood glucose and ketone body (beta-hydroxybutyrate) levels were monitored once a week using a specific enzyme-based kit (Precision Xceed, Abbott Laboratories, Vienna, Austria). Tumor volume was measured twice a week in the xenografts bearing mice, by using a caliper and calculating the volume according to the formula 4/3 Pi  d1/2  d2/2  d3/2 (ddimension).&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Breast cancer bearing mice were euthanized after 80 days of treatment, whereas healthy mice after 40 days. Therefore, mice were injected with 10 mul/g of anesthetic mix (ketamine 20.5 mg/mL, xylazine 5.4 mg/mL, acepromazine 270 mug/ml in saline solution), and after checking for absence of reflexes from the paw, heart puncture was performed. Mice were then immediately euthanized via head-neck dislocation. Blood was transferred into tubes (BD Microtainer PSTTM LH tubes; BD Biosciences, Vienna, Austria) and plasma was collected as described in the manufactures protocol, and snap frozen in liquid nitrogen[1][2].&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Ref:&lt;/p&gt;&lt;p&gt;[1] Aminzadeh-Gohari S., Feichtinger R.G., Vidali S., Locker F., Rutherford T., ODonnel M., Stger-Kleiber A., Mayr J.A., Sperl W., Kofler B. A ketogenic diet supplemented with medium-chain triglycerides enhances the anti-tumor and anti-angiogenic efficacy of chemotherapy on neuroblastoma xenografts in a cd1-nu mouse model. Oncotarget. 2017;8:6472864744. doi:10.18632/oncotarget.20041. PMID:29029389&lt;/p&gt;&lt;p&gt;[2] Vidali S., Aminzadeh-Gohari S., Feichtinger R.G., Vatrinet R., Koller A., Locker F., Rutherford T., ODonnell M., Stger-Kleiber A., Lambert B., et al. The ketogenic diet is not feasible as a therapy in a cd-1 nu/nu mouse model of renal cell carcinoma with features of stauffers syndrome. Oncotarget. 2017;8:5720157215. doi:10.18632/oncotarget.19306. PMID:28915665&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Metabolites were extracted by adding 810 l of ice-cold methanol (VWR, Rednor, Pennsylvania, USA), containing 10 mol/l ethylparaben (Fluka, Buchs, Switzerland), 2 mol/l 3-nitro-L-tyrosine (Sigma-Aldrich, St. Louis, MO, USA), and 4 mol/l d4-succinate (Sigma-Aldrich) to 90 l of plasma. The internal standards ethylparaben, 3-nitro-L-tyrosine and d4-succinate were used for quality control for the assessment of the system stability. Proteins were pelleted in a centrifuge (HERMLE, Wehingen, Germany) at 18,620 rpm for 10 min at 4 C. The supernatant was evaporated to dryness in a vacuum concentrator (Eppendorf, Hamburg, Germany) at room temperature, followed by resuspension in 90 l 50% methanol.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;An ultra-high-performance liquid chromatography (UHPLC) system consisting of an Accela 1250 pump, a Column Oven 300 (all from Thermo Fisher Scientific, Bremen, Germany), and an LC PAL DLW Option Autosampler with a 100 l syringe (from CTC Analytics AG, Zwingen, Switzerland) was coupled to a hybrid quadrupole-Orbitrap mass spectrometer (Model Q Exactive Plus; Thermo Fisher Scientific). A quality control sample (pool) was generated by merging an aliquot (10 l) of all samples included in the study. Prior to injection into the UHPLC-MS system, samples and pools were diluted 1:5 with Millipore water for reversed phase mode and 1:3 with acetonitrile (VWR, Rednor, PA, USA) for HILIC mode separation.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Each sequence started with 3 blank runs, followed by 3 pool injections and finished with 1 pool and 1 blank run. In between, a blank run and a pool run were conducted after every third sample. Each sample was measured in 4 different selectivity and ionization mode combinations, which were RPpositive ionization, RPnegative ionization, HILICpositive ionization, and HILICnegative ionization, resulting in 4 data sets per study. For each combination an exclusion list of the 100 most abundant ions obtained from prior blank runs was generated, to avoid MS fragmentation of chemical or electronic noise signals.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;For RP-UHPLC separations, a 100 x 2.1 mm i.d. Hypersil Gold aQ column (Thermo Fisher Scientific) packed with 1.9 m octadecyl silica particles was applied. For column protection, a 4.0 x 3.0 mm i.d. C18 Security Guard pre-column (Phenomenex, Torrance, CA, USA) was installed. In reversed phase mode, mobile phase A and B were Millipore water and acetonitrile, both containing 0.10% formic acid (Sigma-Aldrich). The HPLC method started with holding 100% A for 1.5 min, followed by a linear gradient to 100% B in 6.5 min. After washing for 2.0 min at 100% B, the column was re-equilibrated to starting conditions for 3.0 min, resulting in a total run time of 13.0 min.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;HILIC-UHPLC separations were performed using a 150 x 2.0 mm i.d. Nucleodur HILIC column (Macherey-Nagel, Dren, Germany), packed with 1.8 m zwitterionic functionalized particles. Additionally, a 4.0 x 2.0 mm i.d. Nucleodur HILIC 1.8 m pre-column, also from Macherey-Nagel was applied to protect the column. In the HILIC mode, mobile phase A contained 50 mM ammonium formate in 50% acetonitrile, while mobile phase B was 10 mM ammonium formate (Sigma-Aldrich) in 90% acetonitrile. After holding 100% B for 3.0 min a linear gradient to 100% A in 17.0 min was applied. The column was washed for 2.0 min at 100% A and re-equilibrated to starting conditions for 8.0 min, resulting in a total run time of 30.0 min. In both modes a flow rate of 0.30 l/min and an injection volume of 2.70 l were applied. The column temperature was held constant at 30 C.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Mass spectrometry data was collected on a Thermo Q Exactive Plus hybrid quadrupole-Orbitrap mass spectrometer (Thermo Fisher Scientific) equipped with a heated electrospray ion source operating in the positive or negative ion mode. Apart from the run time of 13.0 min in RP mode and 30.0 min in HILIC mode, MS settings of the data-dependent Top 5 method were identical for both selectivity modes. Scan range and resolution of MS1 scans were set to 80850 m/z and 70,000, respectively, using an AGC target of 1 x 10^6 and a maximum injection time of 50 ms. The 5 most abundant ions of the MS1 scan were isolated with an isolation window of 0.8 m/z, fragmented via HCD applying stepped normalized collision energies of 20, 40, 60 and acquired in centroid mode. The maximum injection time was set to 64 ms with an AGC target of 5 x 10^4 at a resolution of 17,500. In addition to an exclusion of charges greater than 2, dynamic exclusion of 5.0 s was used, in order to avoid multiple fragmentations of the same ions. Using these settings, all samples were measured in the positive and negative ionization mode in separated sequences for each selectivity and ionization mode. Tune parameters were a capillary temperature of 320 C, a probe heater temperature of 350 C and an S-lens level of 50 for both ionization modes. Differing settings were a sprayer voltage of 4.0 and 3.5 kV, sheath gas flow rate of 35 and 45, as well as an auxiliary gas flow rate of 5 and 10 in positive and negative ionization mode, respectively.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Acquired raw files were converted to .mzML files using the MSConvert tool of the ProteoWizard software (version 3.0.8688). The resulting files were further processed using a bioinformatic workflow in the Konstanz Information Miner (KNIME) [1], version 3.3.4 with integrated OpenMS 2.1.0 software [2] (see Tables S3S7 in the paper associated with this study for detailed settings). The applied KNIME workflow can be accessed here https://www.myexperiment.org/workflows/5109.html. After peak picking, feature detection and feature alignment, data was filtered, normalized and statistically evaluated using Linear Models for Microarray Data (LIMMA) [3] followed by Benjamini-Hochberg correction [4] for multiple testing.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;The MTX study design and data treatment involved stringent filtering of 'noise' signals or such originating from the chemical background, which enabled the reduction of chemical and electronic artefacts. Along that line, the HPLC-MS signals were aligned retention time wise, followed by exclusion of features that did not exceed a threshold of 5-fold the median intensity of the corresponding signal in the blank from further data processing. In the next step, data was normalized via a robust regression to account for variations occurring during sample preparation and measurement. Features showing instable signals in the quality control runs and those not being present in a sufficient number of replicates or treatment conditions were removed. Filtering was based on peak area threshold in blank runs, as well as on relative standard deviation in quality control samples and occurrence in biological replicates. &lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Ref:&lt;/p&gt;&lt;p&gt;[1] Berthold, M.R.; Cebron, N.; Dill, F.; Gabriel, T.R.; Ktter, T.; Meinl, T.; Ohl, P.; Thiel, K.; Wiswedel, B. Knime-the konstanz information miner: Version 2.0 and beyond. AcM SIGKDD explorations Newsletter 2009, 11, 26-31.&lt;/p&gt;&lt;p&gt;[2] Rst, H.L.; Sachsenberg, T.; Aiche, S.; Bielow, C.; Weisser, H.; Aicheler, F.; Andreotti, S.; Ehrlich, H.-C.; Gutenbrunner, P.; Kenar, E., et al. Openms: A flexible open-source software platform for mass spectrometry data analysis. Nat. Methods 2016, 13, 741. doi:10.1038/nmeth.3959. PMID:27575624&lt;/p&gt;&lt;p&gt;[3] Smyth, G.K. Linear models and empirical bayes methods for assessing differential expression in microarray experiments. Stat. Appl. Genet. Mol. Biol. 2004, 3, 1-25. doi:10.2202/1544-6115.1027. PMID:16646809&lt;/p&gt;&lt;p&gt;[4] Hochberg, Y.; Benjamini, Y. More powerful procedures for multiple significance testing. Stat. Med. 1990, 9, 811-818. doi:10.1002/sim.4780090710. PMID:2218183&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Identification was done in a multiple step approach: (1) Monoisotopic mass search in the HMDB[1]; (2) molecular structure database search using SIRIUS in combination with CSI:FingerID[2]-[5]; (3) manual fragment spectra search using METLIN for all signals that resulted in a hit after step 1, but not after step 2[6]; (4) verification of database hits via comparison of retention time and fragment spectra of reference standards. For detailed settings of the applied software used for identification see Tables S8 and S9 in the paper associated with this study. Principal component analyses were generated using SIMCA (version 13.0.3.0; Umetrics, Umea, Sweden).&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;All reference standards, besides N(5)-acetylornithine, 5,6-dihydrouridine, and N-acetyltaurine were purchased from Sigma Aldrich and measured on the same instrument using the same methods as for plasma and tumor tissue samples. N(5)-acetylornithine and 5,6-dihydrouridine were customly synthesized by MedChemTronica (Sollentuna, Sweden) and AKos GmbH (Lrrach, Germany) respectively, while N-acetytaurine was synthesized inhouse. Retention time and MS2 spectra concordance between samples and standards was assessed manually by visual comparison.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Ref:&lt;/p&gt;&lt;p&gt;[1] Wishart, D.S.; Jewison, T.; Guo, A.C.; Wilson, M.; Knox, C.; Liu, Y.; Djoumbou, Y.; Mandal, R.; Aziat, F.; Dong, E. Hmdb 3.0 - the human metabolome database in 2013. Nucleic Acids Res. 2012, 41, D801-D807. doi:10.1093/nar/gks1065. PMID:23161693&lt;/p&gt;&lt;p&gt;[2] Rst, H.L.; Sachsenberg, T.; Aiche, S.; Bielow, C.; Weisser, H.; Aicheler, F.; Andreotti, S.; Ehrlich, H.-C.; Gutenbrunner, P.; Kenar, E., et al. Openms: A flexible open-source software platform for mass spectrometry data analysis. Nat. Methods 2016, 13, 741. doi:10.1038/nmeth.3959. PMID:27575624&lt;/p&gt;&lt;p&gt;[3] Bcker, S.; Letzel, M.C.; Liptk, Z.; Pervukhin, A. Sirius: Decomposing isotope patterns for metabolite identification. Bioinformatics 2008, 25, 218-224. doi:10.1093/bioinformatics/btn603. PMID:19015140&lt;/p&gt;&lt;p&gt;[4] Bcker, S.; Dhrkop, K. Fragmentation trees reloaded. Journal of cheminformatics 2016, 8, 5. doi:10.1186/s13321-016-0116-8. PMID:26839597&lt;/p&gt;&lt;p&gt;[5] Dhrkop, K.; Shen, H.; Meusel, M.; Rousu, J.; Bcker, S. Searching molecular structure databases with tandem mass spectra using csi: Fingerid. Proc. Natl. Acad. Sci. U.S.A.2015, 112, 12580-12585. doi:10.1073/pnas.1509788112. PMID:26392543&lt;/p&gt;&lt;p&gt;[6] Smith, C.A.; O'Maille, G.; Want, E.J.; Qin, C.; Trauger, S.A.; Brandon, T.R.; Custodio, D.E.; Abagyan, R.; Siuzdak, G. Metlin: A metabolite mass spectral database. Ther. Drug Monitoring 2005, 27, 747-751. doi:10.1097/01.ftd.0000179845.53213.39. PMID:16404815&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>MTBLC18211; MTBLC28300; MTBLC73685; MTBLC27226; MTBLC18300; MTBLC37024; MTBLC145052; MTBLC30846; MTBLC15344; MTBLC17533; MTBLC18186; MTBLC18211; MTBLC17724; MTBLC7916; MTBLC26271; MTBLC17822; MTBLC73074; MTBLC37024; MTBLC16449; MTBLC68568; MTBLC18186; MTBLC84415; MTBLC30832; MTBLC28300; MTBLC133179; MTBLC17385; MTBLC17822; MTBLC9300; MTBLC27226; MTBLC23774; MTBLC86910; MTBLC22653; MTBLC18211; MTBLC16811; MTBLC73685; MTBLC26986; MTBLC84415; MTBLC18211; MTBLC7916; MTBLC17822; MTBLC73074; MTBLC73026; MTBLC73061; MTBLC16811; MTBLC73685; MTBLC26271; MTBLC16675; MTBLC18186</t>
+  </si>
+  <si>
+    <t>MTBLS7006</t>
+  </si>
+  <si>
+    <t>The Toxoplasma micropore mediates endocytosis for selective nutrient salvage from host cell compartments</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Apicomplexan parasite growth and replication relies on nutrient acquisition from host cells, in which intracellular multiplication occurs, yet the mechanisms that underlie the nutrient salvage remain elusive. Numerous ultrastructural studies have documented a plasma membrane invagination with a dense neck, termed the micropore, on the surface of intracellular parasites. However, the function of this structure remains unknown. Here we validate the micropore as an essential organelle for endocytosis of nutrients from the host cell cytosol and Golgi in the model apicomplexan &lt;em&gt;Toxoplasma gondii&lt;/em&gt;. Detailed analyses demonstrated that Kelch13 is localized at the dense neck of the organelle and functions as a protein hub at the micropore for endocytic uptake. Intriguingly, maximal activity of the micropore requires the ceramide de novo synthesis pathway in the parasite. Thus, this study provides insights into the machinery underlying acquisition of host cell-derived nutrients by apicomplexan parasites that are otherwise sequestered from host cell compartments.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Toxoplasma; untargeted metabolites; gas chromatography-mass spectrometry; ultra-performance liquid chromatography-mass spectrometry; tandem mass spectrometry; auxin-inducible degron</t>
+  </si>
+  <si>
+    <t>The Toxoplasma micropore mediates endocytosis for selective nutrient salvage from host cell compartments. 10.1038/s41467-023-36571-4. PMID:36813769</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Parasite and host cell culture&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;The previously described lines RHdeltaku80deltahxgprt&lt;strong&gt;[1]&lt;/strong&gt; and RHdeltaku80deltahxgprt/TIR1&lt;strong&gt;[2]&lt;/strong&gt;, referred to as RHku80and TIR1, were used to generate the transgenic lines (T. gondii tachyzoites) reported here. The parental lines and derived lines (&lt;strong&gt;Data S1&lt;/strong&gt;&amp;nbsp;in the paper associated with this study) were grown in human foreskin fibroblasts HFF-1 (ATCC SCRC-1041) in D5 media composed of Dulbeccos modified Eagle medium (DMEM) (12800-082, Thermo Fisher Scientific), supplemented with 5% heat-inactivated fetal bovine serum (10099-141, Gibco), 2mM glutamine (G0200, Solarbio Biotech) and 100 units penicillin-streptomycin (P1410, Solarbio Biotech) at 37 C with 5% CO2. HFF-1 cells were cultured in the same media and conditions, and were all maintained as mycoplasma negative&lt;strong&gt;[3]&lt;/strong&gt;. The TIR1 parental line, and their derived AID lines were cultured in HFF monolayers with 500mM auxin (I2886, Sigma-Aldrich) (+IAA) or 0.1% ethanol alone (IAA) for phenotypic assays, as previously described&lt;strong&gt;[2][4]&lt;/strong&gt;. Parasites were allowed to naturally egress or were mechanically lysed by passing through 22g needles, and harvested by filtration through 3.0 m polycarbonate membranes, from which extracellular parasites were used for experimental assays.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Plasmid design and construction&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;All plasmids (&lt;strong&gt;Data S2&lt;/strong&gt;) were generated by a Basic Seamless Cloning and Assembly kit (CU201-02, TransGen Biotech) using existing plasmids as templates. Briefly, the pCas9-sgRNA plasmids were generated using a previously described plasmid (Addgene 54467) as the template, and 3 fragments were amplified using 3 pairs of primers named as Cas9-F1/R1, Cas9-sgRNA xx/Cas9-R2 and Cas9-F2/R3 (&lt;strong&gt;Data S3&lt;/strong&gt;). The Cas9-sgRNA xx primer contains the sgRNA sequences (20 mer) which target a specific locus either upstream of the start codon (pCas9-sgRNA 5) or downstream of the stop codon (pCas9-sgRNA 3). The sgRNA design was selected from the prediction webpage&lt;strong&gt;[5]&lt;/strong&gt;. The generic plasmids used for the amplicons targeting at the C-terminus of a gene were generated previously&lt;strong&gt;[4]&lt;/strong&gt;, such as pLinker-AID-3xHA-DHFR (addgene 86669), pLinker-AID-Ty-HXGPRT (addgene 86667) and pLinker-AID-3xHA-HXGPRT (addgene 86553), or generated in this study by cloning the fragment of AID-Ty or TurboID-Ty (amplified from addgene 1116904) into the backbone of pLinker-AID-3xHA-DHFR, producing pLinker-AID-Ty-DHFR and pLinker-TurboID-Ty-DHFR. The generic plasmids used for the amplicons targeting at the N-terminus of a gene were generated using the backbone of a plasmid named pN-Ty-DHFR or pN-Ty-HXGPRT&lt;strong&gt;[6]&lt;/strong&gt;, by replacement of the Ty region with Ty-TurboID, Ty-AID, HA-AID, C-myc-AID, 6HA or 6Ty. Primers used for the plasmid generation were listed for each plasmid in &lt;strong&gt;Data S3&lt;/strong&gt; and plasmids generated in this study were listed in &lt;strong&gt;Data S2&lt;/strong&gt;. The DNA regions, including epitopes, AID and TurboID in the newly prepared plasmids were checked by DNA sequencing. The plasmid for complementation of the Ty-AID- Kelch13 line was generated by cloning the Kelch13 fragment into pN-Ty-HXGPRT to replace the Ty region and was generated using primers listed in &lt;strong&gt;Data S3&lt;/strong&gt;.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Generation of T. gondii lines&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;CRISPR-Cas9 tagging technology was used for generation of all lines (&lt;strong&gt;Data S1&lt;/strong&gt;) that contain endogenous fusions at the C-terminus of proteins, and at the N-terminus of proteins in the parental lines of the RHku80KO or TIR1 line&lt;strong&gt;[4]&lt;/strong&gt;. In brief, the CRISPR/Cas9 sgRNA 3 plasmids (&lt;strong&gt;Data S2&lt;/strong&gt;) and CRISPR/Cas9 sgRNA 5 plasmids (&lt;strong&gt;Data S2&lt;/strong&gt;) can efficiently produce Cas9 and sgRNA to create DNA double strand breaks (DSB) in parasites, and facilitates the integration of a tagging amplicon. The amplicon for the C-terminal tagging was generated from a generic plasmid (with the name pLinker-) containing a tag (6HA, AID-3xHA, AID-3Ty, 6Ty or TurboID-3Ty, etc) as described above, using a pair of primers L and T (&lt;strong&gt;Data S3&lt;/strong&gt;). The amplicon for the N-terminal tagging was generated from a generic tagging plasmid (with the name pN-) containing a tag (Ty-TurboID, Ty-AID, HA-AID, myc-AID) using a pair of primers M and NL. The amplicon was then combined with the corresponding CRISPR/Cas9 sgRNA 3 or 5 plasmid (&lt;strong&gt;Data S2&lt;/strong&gt;) and transfected into recipient lines. The drug selection was followed on the second day based on the resistance marker used in the amplicons. The resistance markers with LoxP sites were excised by transfection with pmini-Cre&lt;strong&gt;[7]&lt;/strong&gt;. The cpl gene in the TIR1-AID lines was deleted using a similar CRISPR-Cas9 strategy&lt;strong&gt;[3]&lt;/strong&gt;. The complementation lines were generated by direct transfection with the plasmids containing the wild type gene (&lt;strong&gt;Data S2&lt;/strong&gt;). Transfection and drug selection were performed with 25mug/mL mycophenolic acid (M5255, Sigma-Aldrich) and 25mug/mL 6-xanthine (X4002, Sigma-Aldrich), 200mug/mL 6-thioxanthine (S96242, Shanghai Yuanye Biotech), or 3muM pyrimethamine (46706, Sigma-Aldrich)&lt;strong&gt;[4][6]&lt;/strong&gt;. The lines were confirmed by IFA and diagnostic PCR, as illustrated in &lt;strong&gt;Figure S3a/S3b&lt;/strong&gt;, and the PCR was designed for testing the integration site and the endogenous region with primers listed in &lt;strong&gt;Data S3&lt;/strong&gt;.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Refs:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;[1]&lt;/strong&gt; Huynh MH, Carruthers VB. Tagging of endogenous genes in a Toxoplasma gondii strain lacking Ku80. Eukaryot Cell. 2009 Apr;8(4):530-9. doi:10.1128/EC.00358-08. Epub 2009 Feb 13. PMID:19218426.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;[2]&lt;/strong&gt; Brown KM, Long S, Sibley LD. Plasma Membrane Association by N-Acylation Governs PKG Function in Toxoplasma gondii. mBio. 2017 May 2;8(3):e00375-17. doi:10.1128/mBio.00375-17. PMID:28465425.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;[3]&lt;/strong&gt; Long S, Wang Q, Sibley LD. Analysis of Noncanonical Calcium-Dependent Protein Kinases in Toxoplasma gondii by Targeted Gene Deletion Using CRISPR/Cas9. Infect Immun. 2016 Apr 22;84(5):1262-1273. doi:10.1128/IAI.01173-15. PMID:26755159.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;[4]&lt;/strong&gt; Long S, Brown KM, Drewry LL, Anthony B, Phan IQH, Sibley LD. Calmodulin-like proteins localized to the conoid regulate motility and cell invasion by Toxoplasma gondii. PLoS Pathog. 2017 May 5;13(5):e1006379. doi:10.1371/journal.ppat.1006379. PMID:28475612.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;[5]&lt;/strong&gt; Brown KM, Long S, Sibley LD. Conditional Knockdown of Proteins Using Auxin-inducible Degron (AID) Fusions in Toxoplasma gondii. Bio Protoc. 2018 Feb 20;8(4):e2728. doi:10.21769/BioProtoc.2728. PMID:29644255.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;[6]&lt;/strong&gt; Long S, Anthony B, Drewry LL, Sibley LD. A conserved ankyrin repeat-containing protein regulates conoid stability, motility and cell invasion in Toxoplasma gondii. Nat Commun. 2017 Dec 21;8(1):2236. doi:10.1038/s41467-017-02341-2. PMID:29269729.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;[7]&lt;/strong&gt; Heaslip AT, Dzierszinski F, Stein B, Hu K. TgMORN1 is a key organizer for the basal complex of Toxoplasma gondii. PLoS Pathog. 2010 Feb 5;6(2):e1000754. doi:10.1371/journal.ppat.1000754. PMID:20140195.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Untargeted metabolomics by GCMS&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Parasites were grown in the presence of 500M auxin (IAA) for 36h, subsequently washed with cold PBS twice, scraped and mechanically forced to egress (for harvesting on ice) by filtration through 3.0 mum polycarbonate membranes. The parasite harvesting was performed either at room temperature (&lt;strong&gt;experiment 1&lt;/strong&gt;) or on ice (&lt;strong&gt;experiment 2&lt;/strong&gt;). Parasites were centrifuged at 500 xg at 4C (&amp;gt;2 x10^8 parasites), and the pellets were immediately quenched by addition of -40C methanol and sterile ddH2O (400L methanol+100L&amp;nbsp;ddH2O). The parasite resuspension (250muL) was added with 250muL 80% methanol, and sonicated on ice 1min with 5 cycles. The mixture was vortexed and centrifuged to collect the supernatants. The supernatant (120L) was mixed with 5L 50g/mL L-corleucine, and dried under a nitrogen stream. The residue was reconstituted in 20L of 20mg/mL methoxyamine hydrochloride in pyridine (containing 5g/mL n-alkanes standards), and the resulting mixture was then incubated at 37C for 90min. The mixture was further mixed with 20L BSTFA (with 1% TMCS), and incubated at 70C for 60min prior to GC-MS metabolomics analysis. The quality control (QC) sample was pooled from all samples, processed as the sample preparation.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Untargeted metabolomics by LCMS&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;The above parasite resuspension (250muL) (80% methanol) was mixed with 250muL 80% methanol, and sonicated on ice with 1min on and 1min off for 4 cycles, followed by incubation on ice for 30min. After centrifugation at 15,000 x g, 4C and 15min, the supernatant (200muL) was dried under a nitrogen stream, and reconstituted in 40muL of 10% methanol (including 100ng/mL hexadecanoyl-L-carnitine-d3, decanoyl-L-carnitine-d3 and 1000ng/mL valine-13C5-15N, leucine-13C6, decanoic-d19 acid, octadecanoic-d35 acid, tetradecanoic-d27 acid, phenylalanine-d5, 3-chloro-D-phenylalanine and octanoic-d15 acid) prior to performing UHPLC-HRMS/MS analysis. The quality control (QC) sample was pulling all the prepared samples together.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Untargeted metabolomics by GCMS&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;The GC-MS analysis was performed on Agilent7890A/5975C GC-MS system (Agilent Technologies Inc., CA, USA). An OPTIMA 5 MS Accent fused-silica capillary column was utilized to separate the derivatives. Helium was used as a carrier gas at a constant flow rate of 1mL/min through the column. The injection volume was 1L and the solvent delay time was 5min. The initial oven temperature was held at 60C for 1min, ramped to 240C at a rate of 12C/min, to 320C at 40C/min, and finally held at 320C for 4min.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Untargeted metabolomics by LCMS&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;The LC-MS analysis was performed on a Thermo Fisher Ultimate 3000 UHPLC system with a Waters ACQUITY UPLC BEH C18 column (2.1mm x 100mm, 1.7mum), using standard positive and negative modes. For the positive mode: the mobile phases consisted of (A) water and (B) methanol, both with 0.1% formic acid. A linear gradient elution was performed with the following program: 0min, 2% B; 12min, 95% B; 15min, 100% B and held to 18.1min; 18.1min, 2% B and held to 20min. For the negative mode: the mobile phases contained (A) water and (B) methanol:water (95:5, v/v), both with 6.5mM ammonium bicarbonate. A linear gradient elution was performed with the following program: 0min, 2% B; 9min, 70% B; 14min, 100% B and held to 18min; 18.1min, 2% B and held to 20min. The flow rate was 0.25mL/min, and the injection volume was 2muL for the positive mode and 3muL for the negative mode.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Untargeted metabolomics by GCMS&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;The GC-MS analysis was performed on Agilent7890A/5975C GC-MS system (Agilent Technologies Inc., CA, USA). The temperatures of injector, transfer line and electron impact ion source were set to 250, 260 and 230C, respectively. The electron ionization (EI) energy was 70eV, and data was collected in a full scan mode (50-600 m/z).&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Untargeted metabolomics by LCMS&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;The MS acquisition was performed on a Thermo Fisher Q Exactive Hybrid Quadrupole-Orbitrap Mass Spectrometry (QE) in Heated Electrospray Ionization Positive (HESI+) and Negative (HESI-) mode. The main parameters of the ion source were set as follows: the spray voltage was 3500 V and both capillary temperature and auxiliary temperature degrees were 350 C. The sheath gas flow rate was 40 (arbitrary units) in the positive ion mode and the auxiliary gas flow rate was 10 (arbitrary units). The S-Lens RF was set to 50 in arbitrary units. The full scan was performed at a range of70-1000 m/z, with the resolution set at 35,000 (200) and the AGC target at 3 x10^6. The fragment ion of the top 10 precursors in each scan was acquired by &lt;strong&gt;data-dependent acquisition&lt;/strong&gt; (&lt;strong&gt;DDA&lt;/strong&gt;) with HCD energy at 20, 30 and 40eV, mass resolution of 17,500 FWHM and AGC Target of 5 x10^5.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Untargeted metabolomics by GCMS&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;The peak picking, alignment, deconvolution and further processing of resulting raw data were carried out according to the previously published protocols&lt;strong&gt;[1]&lt;/strong&gt;. The final data was exported as a peak table file, including observations, variables (rt_mz) and peak areas. The data was normalized against the total peak value of total peaks, and differential metabolites were identified by statistical analysis performed in &lt;strong&gt;R&lt;/strong&gt; platform. In the analysis, parametric and nonparametric tests were carried out using one-way ANOVA with Dunnetts multiple comparison, to identify differential metabolites, with p&amp;lt;0.05 and a fold change &amp;gt;1.2, for further analysis. Enrichment of Metabolic Pathways were analyzed using the differential metabolite database commercially generated above. &lt;strong&gt;MetaboAnalyst&lt;/strong&gt; 5.0 server was used to enrich the metabolite sets with KEGG, in which the p value below 0.05 was considered to be significant. The statistical analysis was performed in the software based on hypergeometric test.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Untargeted metabolomics by LCMS&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;The raw data was transformed to &lt;strong&gt;mzXML&lt;/strong&gt; format by &lt;strong&gt;ProteoWizard&lt;/strong&gt; and then processed by &lt;strong&gt;XCMS&lt;/strong&gt; and &lt;strong&gt;CAMERA&lt;/strong&gt; packages in the &lt;strong&gt;R&lt;/strong&gt; software platform. In &lt;strong&gt;XCMS&lt;/strong&gt; package, the peak picking (method=centWave, ppm=5, peakwidth=c(5,20), snthresh=10), alignment (bw=6 and 3 for the first and second grouping, respectively) and retention time correction (method=obiwarp) were conducted. In &lt;strong&gt;CAMERA&lt;/strong&gt; package, the annotations of isotope peak, adducts and fragments were performed with default parameters. The final data was exported as a peak table file, including sample names, variables (rt_mz) and peak areas. The peak areas data was normalized to internal standards before the statistical analysis. The in-house database was referenced to identify the compound by using m/z (MS1), mass spectra (MS2) and retention times (RT). Normalization for relative parasite amounts was based on the total integrated peak area values of metabolites within an experimental batch. Similar analysis was performed for the identification of differential metabolites and enrichment of pathways as described for the GC-MS analysis.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Ref:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;[1]&lt;/strong&gt; Gao X, Pujos-Guillot E, Sbdio JL. Development of a quantitative metabolomic approach to study clinical human fecal water metabolome based on trimethylsilylation derivatization and GC/MS analysis. Anal Chem. 2010 Aug 1;82(15):6447-56. doi:10.1021/ac1006552. PMID:20669995.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;The following parameters were applied in compound identification: (1) accurate mass to charge ratio (m/z) of parent ion, denoted as MS1; (2) mass spectra of fragment ions, denoted as MS2; and (3) chromatographic retention times (RT). The above parameters were matched against the in-house database (containing MS1, MS2 and chromatographic retention times), as well as public or commercial databases such as &lt;strong&gt;mzCloud&lt;/strong&gt;, &lt;strong&gt;MoNA&lt;/strong&gt; and &lt;strong&gt;HMDB&lt;/strong&gt; database. The tolerances of MS1 and MS2 to theoretical mass to charge ratio were limited to 0.005 Da and 0.05 Da, respectively, and the threshold of MS2 matching similarity was set to 70%. RT tolerance is set to 0.5 min for in-house database, and infinity for public or commercial library. All compounds identified by software were reviewed by experienced expert.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>MTBLC17268; MTBLC24266; MTBLC17596; MTBLC17964; MTBLC16958; MTBLC88003; MTBLC18237; MTBLC15741; MTBLC18012; MTBLC6650; MTBLC30769; MTBLC18257; MTBLC16865; MTBLC30915; MTBLC25094; MTBLC15978; MTBLC37024; MTBLC28875; MTBLC28716; MTBLC18183; MTBLC4170; MTBLC7916; MTBLC15882; MTBLC16027; MTBLC15784; MTBLC5457; MTBLC16196; MTBLC15428; MTBLC32154; MTBLC17270; MTBLC17929; MTBLC340824; MTBLC16540; MTBLC42504; MTBLC15721; MTBLC16113; MTBLC17797; MTBLC32816; MTBLC17050; MTBLC17154; MTBLC27897; MTBLC17151; MTBLC27997; MTBLC29864; MTBLC67042; MTBLC30831; MTBLC15891; MTBLC17724; MTBLC72959; MTBLC7676; MTBLC17533; MTBLC17311; MTBLC16797; MTBLC28867; MTBLC17200; MTBLC88454; MTBLC133032; MTBLC30915; MTBLC72689; MTBLC66847; MTBLC18053; MTBLC134594; MTBLC16919; MTBLC136176; MTBLC21547; MTBLC85693; MTBLC141588; MTBLC17515; MTBLC153069; MTBLC84838; MTBLC65301; MTBLC90464; MTBLC73688; MTBLC15746; MTBLC6650; MTBLC78646; MTBLC18148; MTBLC17929; MTBLC15978; MTBLC17015; MTBLC37024; MTBLC40265; MTBLC18019; MTBLC82912; MTBLC7125; MTBLC84385; MTBLC36313; MTBLC17191; MTBLC27389; MTBLC84394; MTBLC17659; MTBLC16015; MTBLC141435; MTBLC15354; MTBLC15799; MTBLC32425; MTBLC59265; MTBLC16467; MTBLC16695; MTBLC180019; MTBLC17750; MTBLC28875; MTBLC144044; MTBLC37024; MTBLC30915; MTBLC73990; MTBLC17050; MTBLC17549; MTBLC16027; MTBLC17475; MTBLC28822; MTBLC16958; MTBLC16737; MTBLC88003; MTBLC18012; MTBLC16865; MTBLC4170; MTBLC33508; MTBLC15978; MTBLC15428; MTBLC16668; MTBLC42111; MTBLC25094; MTBLC340824; MTBLC17154; MTBLC18257; MTBLC16995; MTBLC7916; MTBLC17964; MTBLC18183; MTBLC33017; MTBLC17797; MTBLC37455; MTBLC27897; MTBLC16695; MTBLC64489; MTBLC84385; MTBLC67042; MTBLC72959; MTBLC72957; MTBLC64487; MTBLC84386; MTBLC75465; MTBLC74831; MTBLC15799; MTBLC64486; MTBLC91309; MTBLC131739; MTBLC74966; MTBLC91305; MTBLC136083; MTBLC131982; MTBLC131985; MTBLC136140; MTBLC72998; MTBLC75342; MTBLC73134; MTBLC145273; MTBLC62837; MTBLC16196; MTBLC59265; MTBLC15756; MTBLC28875; MTBLC16015; MTBLC18012; MTBLC15741; MTBLC6650; MTBLC30769; MTBLC30915; MTBLC141435; MTBLC24266; MTBLC16856; MTBLC169683; MTBLC16027; MTBLC18066; MTBLC27389; MTBLC75004; MTBLC21547; MTBLC17562; MTBLC45979; MTBLC50048; MTBLC16737; MTBLC30911; MTBLC73713; MTBLC15652; MTBLC28053; MTBLC44897; MTBLC17138; MTBLC57589; MTBLC44747; MTBLC17533; MTBLC73688; MTBLC18019; MTBLC16467; MTBLC16414; MTBLC17203; MTBLC18148; MTBLC7916; MTBLC16797; MTBLC31515; MTBLC32425; MTBLC28846; MTBLC44215; MTBLC7125; MTBLC62833; MTBLC17013; MTBLC4170; MTBLC17154; MTBLC142245; MTBLC180019; MTBLC15843; MTBLC16235; MTBLC45996; MTBLC73731; MTBLC15721; MTBLC73067; MTBLC86147; MTBLC42504; MTBLC17351; MTBLC82969; MTBLC75115; MTBLC48153; MTBLC17677; MTBLC82846; MTBLC84328; MTBLC32816; MTBLC71466; MTBLC61204; MTBLC36005; MTBLC40279; MTBLC17239; MTBLC192695</t>
   </si>
   <si>
     <t>MTBLS1219</t>
@@ -271,78 +343,6 @@
     <t>MTBLC15354; MTBLC17115; MTBLC16737; MTBLC17203; MTBLC17750; MTBLC16857; MTBLC15891; MTBLC15603; MTBLC17196; MTBLC15729; MTBLC16708; MTBLC17368; MTBLC16244; MTBLC18050; MTBLC16643; MTBLC17712; MTBLC15971; MTBLC17295; MTBLC27596; MTBLC16467; MTBLC16349; MTBLC21549; MTBLC73024; MTBLC16828; MTBLC16946; MTBLC16704; MTBLC18385; MTBLC17596; MTBLC73685; MTBLC16977; MTBLC28123; MTBLC15901; MTBLC27468; MTBLC17342; MTBLC6151; MTBLC30633; MTBLC17768; MTBLC16682; MTBLC16919; MTBLC27248; MTBLC28621; MTBLC16288; MTBLC17775; MTBLC7274; MTBLC21547; MTBLC17895; MTBLC17311; MTBLC73089; MTBLC17659; MTBLC15786; MTBLC17780; MTBLC506227; MTBLC27574; MTBLC17802; MTBLC73881; MTBLC50398; MTBLC15870; MTBLC16697; MTBLC9360; MTBLC16656; MTBLC75314; MTBLC28230; MTBLC27410; MTBLC75145; MTBLC11060; MTBLC1604; MTBLC9425; MTBLC16437; MTBLC82387; MTBLC73527; MTBLC17929; MTBLC42025; MTBLC28867; MTBLC73580; MTBLC7676; MTBLC9173; MTBLC74404; MTBLC23774; MTBLC16441; MTBLC88762; MTBLC73506; MTBLC5828; MTBLC6542; MTBLC73040; MTBLC82984; MTBLC137124; MTBLC73688; MTBLC71169; MTBLC3222; MTBLC5834; MTBLC64517; MTBLC16530; MTBLC16424; MTBLC49000; MTBLC15614; MTBLC17364; MTBLC30745; MTBLC1879; MTBLC15728; MTBLC18019; MTBLC15966; MTBLC17151; MTBLC17924; MTBLC31885; MTBLC17374; MTBLC27373; MTBLC15927; MTBLC28716; MTBLC72850; MTBLC32425; MTBLC44247; MTBLC15977; MTBLC35964; MTBLC19591; MTBLC9592; MTBLC17418; MTBLC132837; MTBLC35962; MTBLC34787; MTBLC36790; MTBLC16310; MTBLC28998; MTBLC20092; MTBLC15384; MTBLC45807; MTBLC84268; MTBLC74435; MTBLC23812; MTBLC73752; MTBLC4969; MTBLC32585; MTBLC5757; MTBLC31038; MTBLC38249; MTBLC132843; MTBLC34769; MTBLC17219; MTBLC78700; MTBLC73740; MTBLC64305; MTBLC5968; MTBLC29064; MTBLC35045; MTBLC17130; MTBLC157; MTBLC31529; MTBLC74099; MTBLC28242; MTBLC33301; MTBLC18435; MTBLC19144; MTBLC74439; MTBLC2202; MTBLC17901; MTBLC2884; MTBLC15929; MTBLC74430; MTBLC84852; MTBLC28702; MTBLC469; MTBLC31112; MTBLC39564; MTBLC73982; MTBLC37270; MTBLC73718; MTBLC86050; MTBLC74475; MTBLC29736; MTBLC80538; MTBLC74437; MTBLC73707; MTBLC16020; MTBLC116314; MTBLC34900; MTBLC80537; MTBLC34293; MTBLC18102; MTBLC28695; MTBLC34496; MTBLC34811; MTBLC30820; MTBLC5897; MTBLC5643; MTBLC17618; MTBLC3918; MTBLC137055; MTBLC139482; MTBLC73736; MTBLC139483; MTBLC73060; MTBLC4393; MTBLC80672; MTBLC131695; MTBLC138496; MTBLC73109; MTBLC4930; MTBLC73923; MTBLC28670; MTBLC74123; MTBLC74129; MTBLC15392; MTBLC15396; MTBLC28598; MTBLC18292; MTBLC141; MTBLC15577; MTBLC15619; MTBLC28998; MTBLC84945; MTBLC15648; MTBLC15654; MTBLC18226; MTBLC27681; MTBLC17532; MTBLC34018; MTBLC34019; MTBLC80672; MTBLC11060; MTBLC15667; MTBLC138194; MTBLC508; MTBLC16968; MTBLC73850; MTBLC138421; MTBLC79207; MTBLC18961; MTBLC73873; MTBLC55458; MTBLC73882; MTBLC74963; MTBLC79097; MTBLC73797; MTBLC72998; MTBLC73134; MTBLC64496; MTBLC28733; MTBLC16020; MTBLC73959; MTBLC16797; MTBLC90479; MTBLC75036; MTBLC28610; MTBLC28468; MTBLC86344; MTBLC133617; MTBLC131924; MTBLC39785; MTBLC73793; MTBLC86162; MTBLC86094; MTBLC75062; MTBLC64489; MTBLC86285; MTBLC32425; MTBLC17252; MTBLC18295; MTBLC29466; MTBLC32976; MTBLC49015; MTBLC23812; MTBLC35964; MTBLC87594; MTBLC28695; MTBLC84212; MTBLC84095; MTBLC73979; MTBLC16444; MTBLC18112; MTBLC60872; MTBLC38546; MTBLC88762; MTBLC60954; MTBLC31082; MTBLC1142; MTBLC73026; MTBLC86366; MTBLC17059; MTBLC73990; MTBLC71012; MTBLC30831; MTBLC30882; MTBLC30820; MTBLC80587; MTBLC1284; MTBLC77761; MTBLC1274; MTBLC36592; MTBLC79494; MTBLC18314; MTBLC27767; MTBLC16104; MTBLC566519; MTBLC76341; MTBLC16939; MTBLC31108; MTBLC27444; MTBLC1461; MTBLC41254; MTBLC17947; MTBLC31112; MTBLC79577; MTBLC15821; MTBLC15786; MTBLC15793; MTBLC28580; MTBLC27440; MTBLC16530; MTBLC16584; MTBLC70857; MTBLC1604; MTBLC17397; MTBLC16286; MTBLC28242; MTBLC28883; MTBLC17442; MTBLC28483; MTBLC17645; MTBLC16865; MTBLC18062; MTBLC15728; MTBLC34407; MTBLC16711; MTBLC30830; MTBLC18115; MTBLC28595; MTBLC1879; MTBLC48430; MTBLC17064; MTBLC15777; MTBLC17405; MTBLC18020; MTBLC16244; MTBLC17509; MTBLC27468; MTBLC15901; MTBLC2015; MTBLC23774; MTBLC2024; MTBLC80473; MTBLC17549; MTBLC15887; MTBLC17780; MTBLC27823; MTBLC20607; MTBLC27551; MTBLC78440; MTBLC18130; MTBLC16924; MTBLC39153; MTBLC16010; MTBLC16545; MTBLC34464; MTBLC138496; MTBLC29501; MTBLC58183; MTBLC18287; MTBLC2202; MTBLC137055; MTBLC16123; MTBLC28921; MTBLC48991; MTBLC15830; MTBLC74064; MTBLC137237; MTBLC16299; MTBLC9261; MTBLC88543; MTBLC116314; MTBLC84573; MTBLC84795; MTBLC84829; MTBLC136371; MTBLC60428; MTBLC84812; MTBLC2374; MTBLC32636; MTBLC15348; MTBLC15349; MTBLC2412; MTBLC40410; MTBLC16708; MTBLC16335; MTBLC73341; MTBLC15676; MTBLC17027; MTBLC2608; MTBLC17884; MTBLC10329; MTBLC16363; MTBLC2617; MTBLC2730; MTBLC2740; MTBLC2814; MTBLC2818; MTBLC137245; MTBLC16239; MTBLC77065; MTBLC15870; MTBLC16990; MTBLC15956; MTBLC74092; MTBLC17618; MTBLC3222; MTBLC27732; MTBLC74096; MTBLC74099; MTBLC171741; MTBLC36274; MTBLC15354; MTBLC32805; MTBLC16919; MTBLC16737; MTBLC29563; MTBLC15977; MTBLC17766; MTBLC58563; MTBLC137150; MTBLC17364; MTBLC4110; MTBLC15966; MTBLC16867; MTBLC16313; MTBLC38833; MTBLC41865; MTBLC20386; MTBLC35079; MTBLC15426; MTBLC16691; MTBLC74110; MTBLC16583; MTBLC28123; MTBLC50710; MTBLC18395; MTBLC16370; MTBLC36005; MTBLC34726; MTBLC4676; MTBLC4685; MTBLC16852; MTBLC4746; MTBLC41948; MTBLC4892; MTBLC4914; MTBLC4930; MTBLC4943; MTBLC4969; MTBLC5054; MTBLC80654; MTBLC28613; MTBLC34769; MTBLC29585; MTBLC61521; MTBLC73707; MTBLC16834; MTBLC84716; MTBLC73849; MTBLC73040; MTBLC15428; MTBLC17687; MTBLC70744; MTBLC74135; MTBLC16344; MTBLC32365; MTBLC74303; MTBLC42025; MTBLC70749; MTBLC18089; MTBLC27747; MTBLC28050; MTBLC5757; MTBLC28297; MTBLC72995; MTBLC88772; MTBLC5828; MTBLC5832; MTBLC5834; MTBLC17368; MTBLC74062; MTBLC74075; MTBLC74327; MTBLC17406; MTBLC16974; MTBLC5897; MTBLC35581; MTBLC18086; MTBLC16411; MTBLC70811; MTBLC27406; MTBLC24813; MTBLC17840; MTBLC17596; MTBLC6031; MTBLC80617; MTBLC16092; MTBLC70984; MTBLC18344; MTBLC18042; MTBLC52136; MTBLC33094; MTBLC16977; MTBLC16467; MTBLC17196; MTBLC17053; MTBLC68600; MTBLC16349; MTBLC89930; MTBLC16283; MTBLC68434; MTBLC16015; MTBLC18050; MTBLC27676; MTBLC15971; MTBLC17443; MTBLC17191; MTBLC74076; MTBLC16946; MTBLC15603; MTBLC18019; MTBLC16643; MTBLC18102; MTBLC15729; MTBLC17295; MTBLC30633; MTBLC17203; MTBLC61696; MTBLC17897; MTBLC17115; MTBLC16857; MTBLC16828; MTBLC17895; MTBLC17215; MTBLC29023; MTBLC6320; MTBLC16414; MTBLC6409; MTBLC74323; MTBLC73579; MTBLC16441; MTBLC72715; MTBLC82984; MTBLC17351; MTBLC6483; MTBLC16026; MTBLC6542; MTBLC74330; MTBLC73851; MTBLC72737; MTBLC64561; MTBLC88685; MTBLC74344; MTBLC74348; MTBLC131743; MTBLC133145; MTBLC76233; MTBLC72741; MTBLC72746; MTBLC72749; MTBLC83058; MTBLC72747; MTBLC16072; MTBLC6790; MTBLC6804; MTBLC16628; MTBLC38307; MTBLC28282; MTBLC27596; MTBLC73733; MTBLC73725; MTBLC29639; MTBLC49255; MTBLC72959; MTBLC78646; MTBLC21494; MTBLC40521; MTBLC73688; MTBLC16682; MTBLC79971; MTBLC506227; MTBLC40992; MTBLC21547; MTBLC49002; MTBLC21549; MTBLC16437; MTBLC17786; MTBLC16259; MTBLC88824; MTBLC73685; MTBLC17768; MTBLC17072; MTBLC16532; MTBLC29643; MTBLC15859; MTBLC15737; MTBLC71028; MTBLC138529; MTBLC21489; MTBLC17691; MTBLC7274; MTBLC61129; MTBLC80959; MTBLC7307; MTBLC7308; MTBLC16440; MTBLC15733; MTBLC16394; MTBLC16463; MTBLC29009; MTBLC16354; MTBLC74439; MTBLC15927; MTBLC74438; MTBLC28101; MTBLC17927; MTBLC27410; MTBLC27838; MTBLC15805; MTBLC31885; MTBLC19289; MTBLC27574; MTBLC7386; MTBLC70989; MTBLC17394; MTBLC17311; MTBLC17752; MTBLC16570; MTBLC17604; MTBLC7453; MTBLC28670; MTBLC28229; MTBLC17154; MTBLC18723; MTBLC7563; MTBLC16268; MTBLC90022; MTBLC17981; MTBLC73024; MTBLC7676; MTBLC28717; MTBLC17490; MTBLC28867; MTBLC16160; MTBLC7715; MTBLC34900; MTBLC7728; MTBLC27542; MTBLC72689; MTBLC84058; MTBLC16536; MTBLC16742; MTBLC7804; MTBLC79424; MTBLC74475; MTBLC7906; MTBLC7916; MTBLC27373; MTBLC89520; MTBLC89518; MTBLC89517; MTBLC89514; MTBLC89583; MTBLC89590; MTBLC88935; MTBLC89013; MTBLC89648; MTBLC89542; MTBLC89534; MTBLC89181; MTBLC88894; MTBLC50713; MTBLC73631; MTBLC73635; MTBLC72723; MTBLC73636; MTBLC8055; MTBLC16424; MTBLC25979; MTBLC8087; MTBLC51402; MTBLC8200; MTBLC86084; MTBLC18049; MTBLC8281; MTBLC17381; MTBLC47914; MTBLC8501; MTBLC72738; MTBLC17802; MTBLC8612; MTBLC17148; MTBLC17310; MTBLC16709; MTBLC36751; MTBLC33135; MTBLC17362; MTBLC16179; MTBLC8870; MTBLC16807; MTBLC17163; MTBLC17728; MTBLC27461; MTBLC9173; MTBLC136272; MTBLC138571; MTBLC64486; MTBLC84488; MTBLC83358; MTBLC86086; MTBLC83359; MTBLC74533; MTBLC136284; MTBLC37550; MTBLC34984; MTBLC71169; MTBLC9367; MTBLC15891; MTBLC26863; MTBLC9425; MTBLC15372; MTBLC58128; MTBLC28177; MTBLC58047; MTBLC9592; MTBLC71179; MTBLC89717; MTBLC133206; MTBLC16558; MTBLC28621; MTBLC50711; MTBLC9750; MTBLC15884; MTBLC74870; MTBLC15760; MTBLC17775; MTBLC17967; MTBLC16704; MTBLC27248; MTBLC73698; MTBLC73703; MTBLC73704; MTBLC28258; MTBLC17712; MTBLC18107; MTBLC17151; MTBLC15333; MTBLC15741; MTBLC16857; MTBLC15891; MTBLC16010; MTBLC17196; MTBLC17368; MTBLC18050; MTBLC16015; MTBLC17712; MTBLC15971; MTBLC17295; MTBLC27596; MTBLC16467; MTBLC15824; MTBLC17895; MTBLC30769; MTBLC16828; MTBLC16283; MTBLC29069; MTBLC41948; MTBLC45696; MTBLC30831; MTBLC30841; MTBLC30830; MTBLC37373; MTBLC1148; MTBLC17115; MTBLC17568; MTBLC16530; MTBLC1157; MTBLC16974; MTBLC27468; MTBLC17415; MTBLC48430; MTBLC16682; MTBLC17053; MTBLC16562; MTBLC15908; MTBLC28508; MTBLC30763; MTBLC27248; MTBLC15966; MTBLC17981; MTBLC16292; MTBLC65327; MTBLC18101; MTBLC7265; MTBLC16742; MTBLC15676; MTBLC15753; MTBLC30923; MTBLC15583; MTBLC48093; MTBLC33510; MTBLC16104; MTBLC17775; MTBLC32805; MTBLC18268; MTBLC22652; MTBLC18089; MTBLC17385; MTBLC17405; MTBLC18072; MTBLC15830; MTBLC17752; MTBLC35704; MTBLC21549; MTBLC17663; MTBLC35453; MTBLC30887; MTBLC17305; MTBLC27480; MTBLC31132; MTBLC17764; MTBLC16704; MTBLC141; MTBLC28613; MTBLC17884; MTBLC17596; MTBLC58377; MTBLC15843; MTBLC16755; MTBLC74330; MTBLC36274; MTBLC17687; MTBLC26066; MTBLC74021; MTBLC40410; MTBLC37051; MTBLC40992; MTBLC55534; MTBLC138491; MTBLC15567; MTBLC18119; MTBLC64390; MTBLC27905; MTBLC61696; MTBLC17394; MTBLC43945; MTBLC29612; MTBLC34018; MTBLC17130; MTBLC80587; MTBLC73685; MTBLC508; MTBLC9008; MTBLC80473; MTBLC74062; MTBLC79971; MTBLC43355; MTBLC53678; MTBLC40521; MTBLC73635; MTBLC34662; MTBLC41254; MTBLC74438; MTBLC90022; MTBLC8098; MTBLC20607; MTBLC8087; MTBLC8984; MTBLC73707; MTBLC25722; MTBLC72723; MTBLC15655; MTBLC32636; MTBLC27581; MTBLC36005; MTBLC4606; MTBLC57905; MTBLC37550; MTBLC88735; MTBLC71169; MTBLC131743; MTBLC73134; MTBLC74938; MTBLC41321; MTBLC76233; MTBLC133145; MTBLC9347; MTBLC72747; MTBLC83053; MTBLC79097; MTBLC137220; MTBLC16256; MTBLC17724; MTBLC17594; MTBLC18355; MTBLC16344; MTBLC27904; MTBLC27913; MTBLC28580; MTBLC16919; MTBLC17667; MTBLC16444; MTBLC17655; MTBLC15737; MTBLC17364; MTBLC28816; MTBLC50519; MTBLC38307; MTBLC30882; MTBLC17645; MTBLC49049; MTBLC27681; MTBLC1670; MTBLC17647; MTBLC17100; MTBLC15667; MTBLC17151; MTBLC8478; MTBLC17406; MTBLC17275; MTBLC2024; MTBLC16440; MTBLC17937; MTBLC15591; MTBLC17897; MTBLC16871; MTBLC27440; MTBLC44747; MTBLC18042; MTBLC28297; MTBLC27956; MTBLC7274; MTBLC21547; MTBLC16278; MTBLC15859; MTBLC30850; MTBLC16217; MTBLC17032; MTBLC4139; MTBLC17516; MTBLC18344; MTBLC17947; MTBLC71028; MTBLC16026; MTBLC21099; MTBLC16142; MTBLC4178; MTBLC16852; MTBLC31885; MTBLC24813; MTBLC17442; MTBLC1098; MTBLC16259; MTBLC28595; MTBLC16802; MTBLC28542; MTBLC61521; MTBLC49002; MTBLC16160; MTBLC17780; MTBLC17381; MTBLC17802; MTBLC27973; MTBLC88405; MTBLC18107; MTBLC39457; MTBLC50547; MTBLC27450; MTBLC10048; MTBLC1463; MTBLC16545; MTBLC64276; MTBLC9592; MTBLC4480; MTBLC17760; MTBLC1113; MTBLC6859; MTBLC2600; MTBLC45564; MTBLC16536; MTBLC43451; MTBLC17064; MTBLC23812; MTBLC16558; MTBLC16817; MTBLC4969; MTBLC74031; MTBLC34699; MTBLC84212; MTBLC86366; MTBLC30531; MTBLC10423; MTBLC10366; MTBLC32810; MTBLC1604; MTBLC48991; MTBLC62207; MTBLC137439; MTBLC88769; MTBLC1403; MTBLC31119; MTBLC89192; MTBLC17786; MTBLC32806; MTBLC34715; MTBLC9300; MTBLC17072; MTBLC16713; MTBLC132188; MTBLC74064; MTBLC32111; MTBLC16409; MTBLC52859; MTBLC50606; MTBLC137237; MTBLC1274; MTBLC29466; MTBLC17443; MTBLC74129; MTBLC29063; MTBLC74099; MTBLC16879; MTBLC41865; MTBLC34697; MTBLC73979; MTBLC73845; MTBLC17132; MTBLC71684; MTBLC4316; MTBLC74407; MTBLC73713; MTBLC16834; MTBLC89182; MTBLC89312; MTBLC34556; MTBLC171741; MTBLC2884; MTBLC29089; MTBLC5298; MTBLC34019; MTBLC545687; MTBLC137245; MTBLC4676; MTBLC73698; MTBLC31112; MTBLC77198; MTBLC5457; MTBLC23774; MTBLC68848; MTBLC68600; MTBLC73510; MTBLC17691; MTBLC28670; MTBLC68434; MTBLC136817; MTBLC15847; MTBLC62825; MTBLC89276; MTBLC79993; MTBLC74092; MTBLC6798; MTBLC73631; MTBLC87986; MTBLC70989; MTBLC84058; MTBLC28695; MTBLC21615; MTBLC8612; MTBLC16741; MTBLC44395; MTBLC28448; MTBLC70811; MTBLC73688; MTBLC6063; MTBLC136803; MTBLC19289; MTBLC73961; MTBLC3183; MTBLC77065; MTBLC7906; MTBLC74323; MTBLC15608; MTBLC16220; MTBLC80091; MTBLC9522; MTBLC134458; MTBLC89405; MTBLC2260; MTBLC5170; MTBLC133003; MTBLC9370; MTBLC9075; MTBLC37419; MTBLC18471; MTBLC91030; MTBLC73490; MTBLC138421; MTBLC7891; MTBLC88771; MTBLC131924; MTBLC88733; MTBLC72749; MTBLC88728; MTBLC4914; MTBLC85038; MTBLC133617; MTBLC90479; MTBLC79207; MTBLC86344; MTBLC10607; MTBLC35053; MTBLC17151; MTBLC17712; MTBLC27248; MTBLC16704; MTBLC17775; MTBLC73718; MTBLC545687; MTBLC32806; MTBLC15891; MTBLC50519; MTBLC71169; MTBLC28173; MTBLC16802; MTBLC16945; MTBLC8883; MTBLC17802; MTBLC89836; MTBLC26066; MTBLC27905; MTBLC74438; MTBLC74439; MTBLC16440; MTBLC7274; MTBLC74430; MTBLC73685; MTBLC17786; MTBLC16437; MTBLC21549; MTBLC21547; MTBLC40992; MTBLC16682; MTBLC73688; MTBLC139484; MTBLC139485; MTBLC6951; MTBLC75757; MTBLC87254; MTBLC16600; MTBLC16857; MTBLC17115; MTBLC17295; MTBLC15971; MTBLC18050; MTBLC27913; MTBLC27956; MTBLC17196; MTBLC16467; MTBLC16977; MTBLC18164; MTBLC17596; MTBLC17368; MTBLC30841; MTBLC137439; MTBLC30531; MTBLC5457; MTBLC16834; MTBLC73707; MTBLC4921; MTBLC4793; MTBLC73728; MTBLC4676; MTBLC47794; MTBLC18395; MTBLC16583; MTBLC28816; MTBLC4311; MTBLC65327; MTBLC15966; MTBLC4139; MTBLC16023; MTBLC27904; MTBLC55534; MTBLC16919; MTBLC32805; MTBLC74099; MTBLC15858; MTBLC80024; MTBLC2805; MTBLC17027; MTBLC15676; MTBLC40410; MTBLC2368; MTBLC34229; MTBLC15830; MTBLC16545; MTBLC16010; MTBLC45564; MTBLC139486; MTBLC2024; MTBLC48430; MTBLC15621; MTBLC30830; MTBLC17710; MTBLC74031; MTBLC17960; MTBLC68503; MTBLC16530; MTBLC28580; MTBLC29479; MTBLC17978; MTBLC15591; MTBLC17947; MTBLC15754; MTBLC34314; MTBLC18168; MTBLC30820; MTBLC37051; MTBLC34293; MTBLC1157; MTBLC36458; MTBLC84852; MTBLC84853; MTBLC73753; MTBLC18355; MTBLC17243; MTBLC17764; MTBLC16444; MTBLC80969; MTBLC28695; MTBLC17415; MTBLC79511; MTBLC15908; MTBLC55328; MTBLC15655; MTBLC17314; MTBLC39567; MTBLC17130; MTBLC17409; MTBLC692; MTBLC34116; MTBLC448; MTBLC15566; MTBLC80537; MTBLC34506; MTBLC84855</t>
   </si>
   <si>
-    <t>MTBLS1066</t>
-  </si>
-  <si>
-    <t>Untargeted Metabolomics Reveals Molecular Effects of Ketogenic Diet on Healthy and Tumor Xenograft Mouse Models</t>
-  </si>
-  <si>
-    <t>The application of ketogenic diet (KD) (high fat/low carbohydrate/adequate protein) as an auxiliary cancer therapy is a field of growing attention. KD provides sufficient energy supply for healthy cells, while possibly impairing energy production in highly glycolytic tumor cells. Moreover, KD regulates insulin and tumor related growth factors (like insulin growth factor-1, IGF-1). In order to provide molecular evidence for the proposed additional inhibition of tumor growth when combining chemotherapy with KD, we applied untargeted quantitative metabolome analysis on a spontaneous breast cancer xenograft mouse model, using MDA-MB-468 cells. Healthy mice and mice bearing breast cancer xenografts and receiving cyclophosphamide chemotherapy were compared after treatment with control diet and KD. Metabolomic profiling was performed on plasma samples, applying high-performance liquid chromatography coupled to tandem mass spectrometry. Statistical analysis revealed metabolic fingerprints comprising numerous significantly regulated features in the group of mice bearing breast cancer. This fingerprint disappeared after treatment with KD, resulting in recovery to the metabolic status observed in healthy mice receiving control diet. Moreover, amino acid metabolism as well as fatty acid transport were found to be affected by both the tumor and the applied KD. Our results provide clear evidence of a significant molecular effect of adjuvant KD in the context of tumor growth inhibition and suggest additional mechanisms of tumor suppression beyond the proposed constrain in energy supply of tumor cells.</t>
-  </si>
-  <si>
-    <t>Ketogenic Diet; breast cancer; Xenograft; untargeted metabolites; ultra-performance liquid chromatography-mass spectrometry</t>
-  </si>
-  <si>
-    <t>Untargeted Metabolomics Reveals Molecular Effects of Ketogenic Diet on Healthy and Tumor Xenograft Mouse Models. 10.3390/ijms20163873. PMID:31398922</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;MDA-MB-468 cell line (ATCC, HTB-132) was used for the generation of breast cancer xenografts. Cells were cultivated in high glucose DMEM medium (Sigma-Aldrich, St. Louis, MO, USA) supplemented with heat-inactivated fetal bovine serum (Gibco, Vienna, Austria) and penicillin/streptomycin amphotericin B solution (Lonza, Cologne, Germany).&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;All in vivo experiments were performed on female CD-1 nu/nu mice (Charles River, Sulzfeld, Germany), the animals were group-housed and had unlimited access to food and water. Xenografts were established as previously described[1][2]. Briefly, a suspension of 1.5 x 10^7 MDA-MB-468 cells in serum-free medium and matrigel (BD Biosciences, Austria) were injected into the right flank of 5- to 6-week-old mice.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;As soon as tumor size reached 300350 mm^3 (i.e., 25 weeks after injection of tumor cells), mice were randomized into different dietary intervention groups (CTRL, LCT-MCT8; n = 56)[1]. As mice are able to keep blood glucose levels and show lower ketosis on 2:1 to 4:1 diets, compared to humans, we decided to use an 8:1 diet in our mouse model, to reach at least a ketosis over 2 mmol/l. Dietary interventions were combined with oral metronomic chemotherapy with CPA (30 mg/kg). The healthy, 7 weeks old, mice were fed with the experimental diets (CTRL, LCT-MCT8; see Table S2 in the paper associated with this study)[1][2]. All animals were monitored twice a week for body weight using a digital scale. Blood glucose and ketone body (beta-hydroxybutyrate) levels were monitored once a week using a specific enzyme-based kit (Precision Xceed, Abbott Laboratories, Vienna, Austria). Tumor volume was measured twice a week in the xenografts bearing mice, by using a caliper and calculating the volume according to the formula 4/3 Pi  d1/2  d2/2  d3/2 (ddimension).&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Breast cancer bearing mice were euthanized after 80 days of treatment, whereas healthy mice after 40 days. Therefore, mice were injected with 10 mul/g of anesthetic mix (ketamine 20.5 mg/mL, xylazine 5.4 mg/mL, acepromazine 270 mug/ml in saline solution), and after checking for absence of reflexes from the paw, heart puncture was performed. Mice were then immediately euthanized via head-neck dislocation. Blood was transferred into tubes (BD Microtainer PSTTM LH tubes; BD Biosciences, Vienna, Austria) and plasma was collected as described in the manufactures protocol, and snap frozen in liquid nitrogen[1][2].&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Ref:&lt;/p&gt;&lt;p&gt;[1] Aminzadeh-Gohari S., Feichtinger R.G., Vidali S., Locker F., Rutherford T., ODonnel M., Stger-Kleiber A., Mayr J.A., Sperl W., Kofler B. A ketogenic diet supplemented with medium-chain triglycerides enhances the anti-tumor and anti-angiogenic efficacy of chemotherapy on neuroblastoma xenografts in a cd1-nu mouse model. Oncotarget. 2017;8:6472864744. doi:10.18632/oncotarget.20041. PMID:29029389&lt;/p&gt;&lt;p&gt;[2] Vidali S., Aminzadeh-Gohari S., Feichtinger R.G., Vatrinet R., Koller A., Locker F., Rutherford T., ODonnell M., Stger-Kleiber A., Lambert B., et al. The ketogenic diet is not feasible as a therapy in a cd-1 nu/nu mouse model of renal cell carcinoma with features of stauffers syndrome. Oncotarget. 2017;8:5720157215. doi:10.18632/oncotarget.19306. PMID:28915665&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Metabolites were extracted by adding 810 l of ice-cold methanol (VWR, Rednor, Pennsylvania, USA), containing 10 mol/l ethylparaben (Fluka, Buchs, Switzerland), 2 mol/l 3-nitro-L-tyrosine (Sigma-Aldrich, St. Louis, MO, USA), and 4 mol/l d4-succinate (Sigma-Aldrich) to 90 l of plasma. The internal standards ethylparaben, 3-nitro-L-tyrosine and d4-succinate were used for quality control for the assessment of the system stability. Proteins were pelleted in a centrifuge (HERMLE, Wehingen, Germany) at 18,620 rpm for 10 min at 4 C. The supernatant was evaporated to dryness in a vacuum concentrator (Eppendorf, Hamburg, Germany) at room temperature, followed by resuspension in 90 l 50% methanol.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;An ultra-high-performance liquid chromatography (UHPLC) system consisting of an Accela 1250 pump, a Column Oven 300 (all from Thermo Fisher Scientific, Bremen, Germany), and an LC PAL DLW Option Autosampler with a 100 l syringe (from CTC Analytics AG, Zwingen, Switzerland) was coupled to a hybrid quadrupole-Orbitrap mass spectrometer (Model Q Exactive Plus; Thermo Fisher Scientific). A quality control sample (pool) was generated by merging an aliquot (10 l) of all samples included in the study. Prior to injection into the UHPLC-MS system, samples and pools were diluted 1:5 with Millipore water for reversed phase mode and 1:3 with acetonitrile (VWR, Rednor, PA, USA) for HILIC mode separation.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Each sequence started with 3 blank runs, followed by 3 pool injections and finished with 1 pool and 1 blank run. In between, a blank run and a pool run were conducted after every third sample. Each sample was measured in 4 different selectivity and ionization mode combinations, which were RPpositive ionization, RPnegative ionization, HILICpositive ionization, and HILICnegative ionization, resulting in 4 data sets per study. For each combination an exclusion list of the 100 most abundant ions obtained from prior blank runs was generated, to avoid MS fragmentation of chemical or electronic noise signals.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;For RP-UHPLC separations, a 100 x 2.1 mm i.d. Hypersil Gold aQ column (Thermo Fisher Scientific) packed with 1.9 m octadecyl silica particles was applied. For column protection, a 4.0 x 3.0 mm i.d. C18 Security Guard pre-column (Phenomenex, Torrance, CA, USA) was installed. In reversed phase mode, mobile phase A and B were Millipore water and acetonitrile, both containing 0.10% formic acid (Sigma-Aldrich). The HPLC method started with holding 100% A for 1.5 min, followed by a linear gradient to 100% B in 6.5 min. After washing for 2.0 min at 100% B, the column was re-equilibrated to starting conditions for 3.0 min, resulting in a total run time of 13.0 min.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;HILIC-UHPLC separations were performed using a 150 x 2.0 mm i.d. Nucleodur HILIC column (Macherey-Nagel, Dren, Germany), packed with 1.8 m zwitterionic functionalized particles. Additionally, a 4.0 x 2.0 mm i.d. Nucleodur HILIC 1.8 m pre-column, also from Macherey-Nagel was applied to protect the column. In the HILIC mode, mobile phase A contained 50 mM ammonium formate in 50% acetonitrile, while mobile phase B was 10 mM ammonium formate (Sigma-Aldrich) in 90% acetonitrile. After holding 100% B for 3.0 min a linear gradient to 100% A in 17.0 min was applied. The column was washed for 2.0 min at 100% A and re-equilibrated to starting conditions for 8.0 min, resulting in a total run time of 30.0 min. In both modes a flow rate of 0.30 l/min and an injection volume of 2.70 l were applied. The column temperature was held constant at 30 C.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Mass spectrometry data was collected on a Thermo Q Exactive Plus hybrid quadrupole-Orbitrap mass spectrometer (Thermo Fisher Scientific) equipped with a heated electrospray ion source operating in the positive or negative ion mode. Apart from the run time of 13.0 min in RP mode and 30.0 min in HILIC mode, MS settings of the data-dependent Top 5 method were identical for both selectivity modes. Scan range and resolution of MS1 scans were set to 80850 m/z and 70,000, respectively, using an AGC target of 1 x 10^6 and a maximum injection time of 50 ms. The 5 most abundant ions of the MS1 scan were isolated with an isolation window of 0.8 m/z, fragmented via HCD applying stepped normalized collision energies of 20, 40, 60 and acquired in centroid mode. The maximum injection time was set to 64 ms with an AGC target of 5 x 10^4 at a resolution of 17,500. In addition to an exclusion of charges greater than 2, dynamic exclusion of 5.0 s was used, in order to avoid multiple fragmentations of the same ions. Using these settings, all samples were measured in the positive and negative ionization mode in separated sequences for each selectivity and ionization mode. Tune parameters were a capillary temperature of 320 C, a probe heater temperature of 350 C and an S-lens level of 50 for both ionization modes. Differing settings were a sprayer voltage of 4.0 and 3.5 kV, sheath gas flow rate of 35 and 45, as well as an auxiliary gas flow rate of 5 and 10 in positive and negative ionization mode, respectively.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Acquired raw files were converted to .mzML files using the MSConvert tool of the ProteoWizard software (version 3.0.8688). The resulting files were further processed using a bioinformatic workflow in the Konstanz Information Miner (KNIME) [1], version 3.3.4 with integrated OpenMS 2.1.0 software [2] (see Tables S3S7 in the paper associated with this study for detailed settings). The applied KNIME workflow can be accessed here https://www.myexperiment.org/workflows/5109.html. After peak picking, feature detection and feature alignment, data was filtered, normalized and statistically evaluated using Linear Models for Microarray Data (LIMMA) [3] followed by Benjamini-Hochberg correction [4] for multiple testing.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;The MTX study design and data treatment involved stringent filtering of 'noise' signals or such originating from the chemical background, which enabled the reduction of chemical and electronic artefacts. Along that line, the HPLC-MS signals were aligned retention time wise, followed by exclusion of features that did not exceed a threshold of 5-fold the median intensity of the corresponding signal in the blank from further data processing. In the next step, data was normalized via a robust regression to account for variations occurring during sample preparation and measurement. Features showing instable signals in the quality control runs and those not being present in a sufficient number of replicates or treatment conditions were removed. Filtering was based on peak area threshold in blank runs, as well as on relative standard deviation in quality control samples and occurrence in biological replicates. &lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Ref:&lt;/p&gt;&lt;p&gt;[1] Berthold, M.R.; Cebron, N.; Dill, F.; Gabriel, T.R.; Ktter, T.; Meinl, T.; Ohl, P.; Thiel, K.; Wiswedel, B. Knime-the konstanz information miner: Version 2.0 and beyond. AcM SIGKDD explorations Newsletter 2009, 11, 26-31.&lt;/p&gt;&lt;p&gt;[2] Rst, H.L.; Sachsenberg, T.; Aiche, S.; Bielow, C.; Weisser, H.; Aicheler, F.; Andreotti, S.; Ehrlich, H.-C.; Gutenbrunner, P.; Kenar, E., et al. Openms: A flexible open-source software platform for mass spectrometry data analysis. Nat. Methods 2016, 13, 741. doi:10.1038/nmeth.3959. PMID:27575624&lt;/p&gt;&lt;p&gt;[3] Smyth, G.K. Linear models and empirical bayes methods for assessing differential expression in microarray experiments. Stat. Appl. Genet. Mol. Biol. 2004, 3, 1-25. doi:10.2202/1544-6115.1027. PMID:16646809&lt;/p&gt;&lt;p&gt;[4] Hochberg, Y.; Benjamini, Y. More powerful procedures for multiple significance testing. Stat. Med. 1990, 9, 811-818. doi:10.1002/sim.4780090710. PMID:2218183&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Identification was done in a multiple step approach: (1) Monoisotopic mass search in the HMDB[1]; (2) molecular structure database search using SIRIUS in combination with CSI:FingerID[2]-[5]; (3) manual fragment spectra search using METLIN for all signals that resulted in a hit after step 1, but not after step 2[6]; (4) verification of database hits via comparison of retention time and fragment spectra of reference standards. For detailed settings of the applied software used for identification see Tables S8 and S9 in the paper associated with this study. Principal component analyses were generated using SIMCA (version 13.0.3.0; Umetrics, Umea, Sweden).&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;All reference standards, besides N(5)-acetylornithine, 5,6-dihydrouridine, and N-acetyltaurine were purchased from Sigma Aldrich and measured on the same instrument using the same methods as for plasma and tumor tissue samples. N(5)-acetylornithine and 5,6-dihydrouridine were customly synthesized by MedChemTronica (Sollentuna, Sweden) and AKos GmbH (Lrrach, Germany) respectively, while N-acetytaurine was synthesized inhouse. Retention time and MS2 spectra concordance between samples and standards was assessed manually by visual comparison.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Ref:&lt;/p&gt;&lt;p&gt;[1] Wishart, D.S.; Jewison, T.; Guo, A.C.; Wilson, M.; Knox, C.; Liu, Y.; Djoumbou, Y.; Mandal, R.; Aziat, F.; Dong, E. Hmdb 3.0 - the human metabolome database in 2013. Nucleic Acids Res. 2012, 41, D801-D807. doi:10.1093/nar/gks1065. PMID:23161693&lt;/p&gt;&lt;p&gt;[2] Rst, H.L.; Sachsenberg, T.; Aiche, S.; Bielow, C.; Weisser, H.; Aicheler, F.; Andreotti, S.; Ehrlich, H.-C.; Gutenbrunner, P.; Kenar, E., et al. Openms: A flexible open-source software platform for mass spectrometry data analysis. Nat. Methods 2016, 13, 741. doi:10.1038/nmeth.3959. PMID:27575624&lt;/p&gt;&lt;p&gt;[3] Bcker, S.; Letzel, M.C.; Liptk, Z.; Pervukhin, A. Sirius: Decomposing isotope patterns for metabolite identification. Bioinformatics 2008, 25, 218-224. doi:10.1093/bioinformatics/btn603. PMID:19015140&lt;/p&gt;&lt;p&gt;[4] Bcker, S.; Dhrkop, K. Fragmentation trees reloaded. Journal of cheminformatics 2016, 8, 5. doi:10.1186/s13321-016-0116-8. PMID:26839597&lt;/p&gt;&lt;p&gt;[5] Dhrkop, K.; Shen, H.; Meusel, M.; Rousu, J.; Bcker, S. Searching molecular structure databases with tandem mass spectra using csi: Fingerid. Proc. Natl. Acad. Sci. U.S.A.2015, 112, 12580-12585. doi:10.1073/pnas.1509788112. PMID:26392543&lt;/p&gt;&lt;p&gt;[6] Smith, C.A.; O'Maille, G.; Want, E.J.; Qin, C.; Trauger, S.A.; Brandon, T.R.; Custodio, D.E.; Abagyan, R.; Siuzdak, G. Metlin: A metabolite mass spectral database. Ther. Drug Monitoring 2005, 27, 747-751. doi:10.1097/01.ftd.0000179845.53213.39. PMID:16404815&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>MTBLC18211; MTBLC28300; MTBLC73685; MTBLC27226; MTBLC18300; MTBLC37024; MTBLC145052; MTBLC30846; MTBLC15344; MTBLC17533; MTBLC18186; MTBLC18211; MTBLC17724; MTBLC7916; MTBLC26271; MTBLC17822; MTBLC73074; MTBLC37024; MTBLC16449; MTBLC68568; MTBLC18186; MTBLC84415; MTBLC30832; MTBLC28300; MTBLC133179; MTBLC17385; MTBLC17822; MTBLC9300; MTBLC27226; MTBLC23774; MTBLC86910; MTBLC22653; MTBLC18211; MTBLC16811; MTBLC73685; MTBLC26986; MTBLC84415; MTBLC18211; MTBLC7916; MTBLC17822; MTBLC73074; MTBLC73026; MTBLC73061; MTBLC16811; MTBLC73685; MTBLC26271; MTBLC16675; MTBLC18186</t>
-  </si>
-  <si>
-    <t>MTBLS7006</t>
-  </si>
-  <si>
-    <t>The Toxoplasma micropore mediates endocytosis for selective nutrient salvage from host cell compartments</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Apicomplexan parasite growth and replication relies on nutrient acquisition from host cells, in which intracellular multiplication occurs, yet the mechanisms that underlie the nutrient salvage remain elusive. Numerous ultrastructural studies have documented a plasma membrane invagination with a dense neck, termed the micropore, on the surface of intracellular parasites. However, the function of this structure remains unknown. Here we validate the micropore as an essential organelle for endocytosis of nutrients from the host cell cytosol and Golgi in the model apicomplexan &lt;em&gt;Toxoplasma gondii&lt;/em&gt;. Detailed analyses demonstrated that Kelch13 is localized at the dense neck of the organelle and functions as a protein hub at the micropore for endocytic uptake. Intriguingly, maximal activity of the micropore requires the ceramide de novo synthesis pathway in the parasite. Thus, this study provides insights into the machinery underlying acquisition of host cell-derived nutrients by apicomplexan parasites that are otherwise sequestered from host cell compartments.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Toxoplasma; untargeted metabolites; gas chromatography-mass spectrometry; ultra-performance liquid chromatography-mass spectrometry; tandem mass spectrometry; auxin-inducible degron</t>
-  </si>
-  <si>
-    <t>The Toxoplasma micropore mediates endocytosis for selective nutrient salvage from host cell compartments. 10.1038/s41467-023-36571-4. PMID:36813769</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Parasite and host cell culture&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;The previously described lines RHdeltaku80deltahxgprt&lt;strong&gt;[1]&lt;/strong&gt; and RHdeltaku80deltahxgprt/TIR1&lt;strong&gt;[2]&lt;/strong&gt;, referred to as RHku80and TIR1, were used to generate the transgenic lines (T. gondii tachyzoites) reported here. The parental lines and derived lines (&lt;strong&gt;Data S1&lt;/strong&gt;&amp;nbsp;in the paper associated with this study) were grown in human foreskin fibroblasts HFF-1 (ATCC SCRC-1041) in D5 media composed of Dulbeccos modified Eagle medium (DMEM) (12800-082, Thermo Fisher Scientific), supplemented with 5% heat-inactivated fetal bovine serum (10099-141, Gibco), 2mM glutamine (G0200, Solarbio Biotech) and 100 units penicillin-streptomycin (P1410, Solarbio Biotech) at 37 C with 5% CO2. HFF-1 cells were cultured in the same media and conditions, and were all maintained as mycoplasma negative&lt;strong&gt;[3]&lt;/strong&gt;. The TIR1 parental line, and their derived AID lines were cultured in HFF monolayers with 500mM auxin (I2886, Sigma-Aldrich) (+IAA) or 0.1% ethanol alone (IAA) for phenotypic assays, as previously described&lt;strong&gt;[2][4]&lt;/strong&gt;. Parasites were allowed to naturally egress or were mechanically lysed by passing through 22g needles, and harvested by filtration through 3.0 m polycarbonate membranes, from which extracellular parasites were used for experimental assays.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Plasmid design and construction&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;All plasmids (&lt;strong&gt;Data S2&lt;/strong&gt;) were generated by a Basic Seamless Cloning and Assembly kit (CU201-02, TransGen Biotech) using existing plasmids as templates. Briefly, the pCas9-sgRNA plasmids were generated using a previously described plasmid (Addgene 54467) as the template, and 3 fragments were amplified using 3 pairs of primers named as Cas9-F1/R1, Cas9-sgRNA xx/Cas9-R2 and Cas9-F2/R3 (&lt;strong&gt;Data S3&lt;/strong&gt;). The Cas9-sgRNA xx primer contains the sgRNA sequences (20 mer) which target a specific locus either upstream of the start codon (pCas9-sgRNA 5) or downstream of the stop codon (pCas9-sgRNA 3). The sgRNA design was selected from the prediction webpage&lt;strong&gt;[5]&lt;/strong&gt;. The generic plasmids used for the amplicons targeting at the C-terminus of a gene were generated previously&lt;strong&gt;[4]&lt;/strong&gt;, such as pLinker-AID-3xHA-DHFR (addgene 86669), pLinker-AID-Ty-HXGPRT (addgene 86667) and pLinker-AID-3xHA-HXGPRT (addgene 86553), or generated in this study by cloning the fragment of AID-Ty or TurboID-Ty (amplified from addgene 1116904) into the backbone of pLinker-AID-3xHA-DHFR, producing pLinker-AID-Ty-DHFR and pLinker-TurboID-Ty-DHFR. The generic plasmids used for the amplicons targeting at the N-terminus of a gene were generated using the backbone of a plasmid named pN-Ty-DHFR or pN-Ty-HXGPRT&lt;strong&gt;[6]&lt;/strong&gt;, by replacement of the Ty region with Ty-TurboID, Ty-AID, HA-AID, C-myc-AID, 6HA or 6Ty. Primers used for the plasmid generation were listed for each plasmid in &lt;strong&gt;Data S3&lt;/strong&gt; and plasmids generated in this study were listed in &lt;strong&gt;Data S2&lt;/strong&gt;. The DNA regions, including epitopes, AID and TurboID in the newly prepared plasmids were checked by DNA sequencing. The plasmid for complementation of the Ty-AID- Kelch13 line was generated by cloning the Kelch13 fragment into pN-Ty-HXGPRT to replace the Ty region and was generated using primers listed in &lt;strong&gt;Data S3&lt;/strong&gt;.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Generation of T. gondii lines&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;CRISPR-Cas9 tagging technology was used for generation of all lines (&lt;strong&gt;Data S1&lt;/strong&gt;) that contain endogenous fusions at the C-terminus of proteins, and at the N-terminus of proteins in the parental lines of the RHku80KO or TIR1 line&lt;strong&gt;[4]&lt;/strong&gt;. In brief, the CRISPR/Cas9 sgRNA 3 plasmids (&lt;strong&gt;Data S2&lt;/strong&gt;) and CRISPR/Cas9 sgRNA 5 plasmids (&lt;strong&gt;Data S2&lt;/strong&gt;) can efficiently produce Cas9 and sgRNA to create DNA double strand breaks (DSB) in parasites, and facilitates the integration of a tagging amplicon. The amplicon for the C-terminal tagging was generated from a generic plasmid (with the name pLinker-) containing a tag (6HA, AID-3xHA, AID-3Ty, 6Ty or TurboID-3Ty, etc) as described above, using a pair of primers L and T (&lt;strong&gt;Data S3&lt;/strong&gt;). The amplicon for the N-terminal tagging was generated from a generic tagging plasmid (with the name pN-) containing a tag (Ty-TurboID, Ty-AID, HA-AID, myc-AID) using a pair of primers M and NL. The amplicon was then combined with the corresponding CRISPR/Cas9 sgRNA 3 or 5 plasmid (&lt;strong&gt;Data S2&lt;/strong&gt;) and transfected into recipient lines. The drug selection was followed on the second day based on the resistance marker used in the amplicons. The resistance markers with LoxP sites were excised by transfection with pmini-Cre&lt;strong&gt;[7]&lt;/strong&gt;. The cpl gene in the TIR1-AID lines was deleted using a similar CRISPR-Cas9 strategy&lt;strong&gt;[3]&lt;/strong&gt;. The complementation lines were generated by direct transfection with the plasmids containing the wild type gene (&lt;strong&gt;Data S2&lt;/strong&gt;). Transfection and drug selection were performed with 25mug/mL mycophenolic acid (M5255, Sigma-Aldrich) and 25mug/mL 6-xanthine (X4002, Sigma-Aldrich), 200mug/mL 6-thioxanthine (S96242, Shanghai Yuanye Biotech), or 3muM pyrimethamine (46706, Sigma-Aldrich)&lt;strong&gt;[4][6]&lt;/strong&gt;. The lines were confirmed by IFA and diagnostic PCR, as illustrated in &lt;strong&gt;Figure S3a/S3b&lt;/strong&gt;, and the PCR was designed for testing the integration site and the endogenous region with primers listed in &lt;strong&gt;Data S3&lt;/strong&gt;.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Refs:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;[1]&lt;/strong&gt; Huynh MH, Carruthers VB. Tagging of endogenous genes in a Toxoplasma gondii strain lacking Ku80. Eukaryot Cell. 2009 Apr;8(4):530-9. doi:10.1128/EC.00358-08. Epub 2009 Feb 13. PMID:19218426.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;[2]&lt;/strong&gt; Brown KM, Long S, Sibley LD. Plasma Membrane Association by N-Acylation Governs PKG Function in Toxoplasma gondii. mBio. 2017 May 2;8(3):e00375-17. doi:10.1128/mBio.00375-17. PMID:28465425.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;[3]&lt;/strong&gt; Long S, Wang Q, Sibley LD. Analysis of Noncanonical Calcium-Dependent Protein Kinases in Toxoplasma gondii by Targeted Gene Deletion Using CRISPR/Cas9. Infect Immun. 2016 Apr 22;84(5):1262-1273. doi:10.1128/IAI.01173-15. PMID:26755159.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;[4]&lt;/strong&gt; Long S, Brown KM, Drewry LL, Anthony B, Phan IQH, Sibley LD. Calmodulin-like proteins localized to the conoid regulate motility and cell invasion by Toxoplasma gondii. PLoS Pathog. 2017 May 5;13(5):e1006379. doi:10.1371/journal.ppat.1006379. PMID:28475612.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;[5]&lt;/strong&gt; Brown KM, Long S, Sibley LD. Conditional Knockdown of Proteins Using Auxin-inducible Degron (AID) Fusions in Toxoplasma gondii. Bio Protoc. 2018 Feb 20;8(4):e2728. doi:10.21769/BioProtoc.2728. PMID:29644255.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;[6]&lt;/strong&gt; Long S, Anthony B, Drewry LL, Sibley LD. A conserved ankyrin repeat-containing protein regulates conoid stability, motility and cell invasion in Toxoplasma gondii. Nat Commun. 2017 Dec 21;8(1):2236. doi:10.1038/s41467-017-02341-2. PMID:29269729.&lt;/p&gt;&lt;p&gt;&lt;strong&gt;[7]&lt;/strong&gt; Heaslip AT, Dzierszinski F, Stein B, Hu K. TgMORN1 is a key organizer for the basal complex of Toxoplasma gondii. PLoS Pathog. 2010 Feb 5;6(2):e1000754. doi:10.1371/journal.ppat.1000754. PMID:20140195.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Untargeted metabolomics by GCMS&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;Parasites were grown in the presence of 500M auxin (IAA) for 36h, subsequently washed with cold PBS twice, scraped and mechanically forced to egress (for harvesting on ice) by filtration through 3.0 mum polycarbonate membranes. The parasite harvesting was performed either at room temperature (&lt;strong&gt;experiment 1&lt;/strong&gt;) or on ice (&lt;strong&gt;experiment 2&lt;/strong&gt;). Parasites were centrifuged at 500 xg at 4C (&amp;gt;2 x10^8 parasites), and the pellets were immediately quenched by addition of -40C methanol and sterile ddH2O (400L methanol+100L&amp;nbsp;ddH2O). The parasite resuspension (250muL) was added with 250muL 80% methanol, and sonicated on ice 1min with 5 cycles. The mixture was vortexed and centrifuged to collect the supernatants. The supernatant (120L) was mixed with 5L 50g/mL L-corleucine, and dried under a nitrogen stream. The residue was reconstituted in 20L of 20mg/mL methoxyamine hydrochloride in pyridine (containing 5g/mL n-alkanes standards), and the resulting mixture was then incubated at 37C for 90min. The mixture was further mixed with 20L BSTFA (with 1% TMCS), and incubated at 70C for 60min prior to GC-MS metabolomics analysis. The quality control (QC) sample was pooled from all samples, processed as the sample preparation.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Untargeted metabolomics by LCMS&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;The above parasite resuspension (250muL) (80% methanol) was mixed with 250muL 80% methanol, and sonicated on ice with 1min on and 1min off for 4 cycles, followed by incubation on ice for 30min. After centrifugation at 15,000 x g, 4C and 15min, the supernatant (200muL) was dried under a nitrogen stream, and reconstituted in 40muL of 10% methanol (including 100ng/mL hexadecanoyl-L-carnitine-d3, decanoyl-L-carnitine-d3 and 1000ng/mL valine-13C5-15N, leucine-13C6, decanoic-d19 acid, octadecanoic-d35 acid, tetradecanoic-d27 acid, phenylalanine-d5, 3-chloro-D-phenylalanine and octanoic-d15 acid) prior to performing UHPLC-HRMS/MS analysis. The quality control (QC) sample was pulling all the prepared samples together.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Untargeted metabolomics by GCMS&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;The GC-MS analysis was performed on Agilent7890A/5975C GC-MS system (Agilent Technologies Inc., CA, USA). An OPTIMA 5 MS Accent fused-silica capillary column was utilized to separate the derivatives. Helium was used as a carrier gas at a constant flow rate of 1mL/min through the column. The injection volume was 1L and the solvent delay time was 5min. The initial oven temperature was held at 60C for 1min, ramped to 240C at a rate of 12C/min, to 320C at 40C/min, and finally held at 320C for 4min.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Untargeted metabolomics by LCMS&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;The LC-MS analysis was performed on a Thermo Fisher Ultimate 3000 UHPLC system with a Waters ACQUITY UPLC BEH C18 column (2.1mm x 100mm, 1.7mum), using standard positive and negative modes. For the positive mode: the mobile phases consisted of (A) water and (B) methanol, both with 0.1% formic acid. A linear gradient elution was performed with the following program: 0min, 2% B; 12min, 95% B; 15min, 100% B and held to 18.1min; 18.1min, 2% B and held to 20min. For the negative mode: the mobile phases contained (A) water and (B) methanol:water (95:5, v/v), both with 6.5mM ammonium bicarbonate. A linear gradient elution was performed with the following program: 0min, 2% B; 9min, 70% B; 14min, 100% B and held to 18min; 18.1min, 2% B and held to 20min. The flow rate was 0.25mL/min, and the injection volume was 2muL for the positive mode and 3muL for the negative mode.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Untargeted metabolomics by GCMS&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;The GC-MS analysis was performed on Agilent7890A/5975C GC-MS system (Agilent Technologies Inc., CA, USA). The temperatures of injector, transfer line and electron impact ion source were set to 250, 260 and 230C, respectively. The electron ionization (EI) energy was 70eV, and data was collected in a full scan mode (50-600 m/z).&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Untargeted metabolomics by LCMS&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;The MS acquisition was performed on a Thermo Fisher Q Exactive Hybrid Quadrupole-Orbitrap Mass Spectrometry (QE) in Heated Electrospray Ionization Positive (HESI+) and Negative (HESI-) mode. The main parameters of the ion source were set as follows: the spray voltage was 3500 V and both capillary temperature and auxiliary temperature degrees were 350 C. The sheath gas flow rate was 40 (arbitrary units) in the positive ion mode and the auxiliary gas flow rate was 10 (arbitrary units). The S-Lens RF was set to 50 in arbitrary units. The full scan was performed at a range of70-1000 m/z, with the resolution set at 35,000 (200) and the AGC target at 3 x10^6. The fragment ion of the top 10 precursors in each scan was acquired by &lt;strong&gt;data-dependent acquisition&lt;/strong&gt; (&lt;strong&gt;DDA&lt;/strong&gt;) with HCD energy at 20, 30 and 40eV, mass resolution of 17,500 FWHM and AGC Target of 5 x10^5.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Untargeted metabolomics by GCMS&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;The peak picking, alignment, deconvolution and further processing of resulting raw data were carried out according to the previously published protocols&lt;strong&gt;[1]&lt;/strong&gt;. The final data was exported as a peak table file, including observations, variables (rt_mz) and peak areas. The data was normalized against the total peak value of total peaks, and differential metabolites were identified by statistical analysis performed in &lt;strong&gt;R&lt;/strong&gt; platform. In the analysis, parametric and nonparametric tests were carried out using one-way ANOVA with Dunnetts multiple comparison, to identify differential metabolites, with p&amp;lt;0.05 and a fold change &amp;gt;1.2, for further analysis. Enrichment of Metabolic Pathways were analyzed using the differential metabolite database commercially generated above. &lt;strong&gt;MetaboAnalyst&lt;/strong&gt; 5.0 server was used to enrich the metabolite sets with KEGG, in which the p value below 0.05 was considered to be significant. The statistical analysis was performed in the software based on hypergeometric test.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Untargeted metabolomics by LCMS&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;The raw data was transformed to &lt;strong&gt;mzXML&lt;/strong&gt; format by &lt;strong&gt;ProteoWizard&lt;/strong&gt; and then processed by &lt;strong&gt;XCMS&lt;/strong&gt; and &lt;strong&gt;CAMERA&lt;/strong&gt; packages in the &lt;strong&gt;R&lt;/strong&gt; software platform. In &lt;strong&gt;XCMS&lt;/strong&gt; package, the peak picking (method=centWave, ppm=5, peakwidth=c(5,20), snthresh=10), alignment (bw=6 and 3 for the first and second grouping, respectively) and retention time correction (method=obiwarp) were conducted. In &lt;strong&gt;CAMERA&lt;/strong&gt; package, the annotations of isotope peak, adducts and fragments were performed with default parameters. The final data was exported as a peak table file, including sample names, variables (rt_mz) and peak areas. The peak areas data was normalized to internal standards before the statistical analysis. The in-house database was referenced to identify the compound by using m/z (MS1), mass spectra (MS2) and retention times (RT). Normalization for relative parasite amounts was based on the total integrated peak area values of metabolites within an experimental batch. Similar analysis was performed for the identification of differential metabolites and enrichment of pathways as described for the GC-MS analysis.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Ref:&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;[1]&lt;/strong&gt; Gao X, Pujos-Guillot E, Sbdio JL. Development of a quantitative metabolomic approach to study clinical human fecal water metabolome based on trimethylsilylation derivatization and GC/MS analysis. Anal Chem. 2010 Aug 1;82(15):6447-56. doi:10.1021/ac1006552. PMID:20669995.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;The following parameters were applied in compound identification: (1) accurate mass to charge ratio (m/z) of parent ion, denoted as MS1; (2) mass spectra of fragment ions, denoted as MS2; and (3) chromatographic retention times (RT). The above parameters were matched against the in-house database (containing MS1, MS2 and chromatographic retention times), as well as public or commercial databases such as &lt;strong&gt;mzCloud&lt;/strong&gt;, &lt;strong&gt;MoNA&lt;/strong&gt; and &lt;strong&gt;HMDB&lt;/strong&gt; database. The tolerances of MS1 and MS2 to theoretical mass to charge ratio were limited to 0.005 Da and 0.05 Da, respectively, and the threshold of MS2 matching similarity was set to 70%. RT tolerance is set to 0.5 min for in-house database, and infinity for public or commercial library. All compounds identified by software were reviewed by experienced expert.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>MTBLC17268; MTBLC24266; MTBLC17596; MTBLC17964; MTBLC16958; MTBLC88003; MTBLC18237; MTBLC15741; MTBLC18012; MTBLC6650; MTBLC30769; MTBLC18257; MTBLC16865; MTBLC30915; MTBLC25094; MTBLC15978; MTBLC37024; MTBLC28875; MTBLC28716; MTBLC18183; MTBLC4170; MTBLC7916; MTBLC15882; MTBLC16027; MTBLC15784; MTBLC5457; MTBLC16196; MTBLC15428; MTBLC32154; MTBLC17270; MTBLC17929; MTBLC340824; MTBLC16540; MTBLC42504; MTBLC15721; MTBLC16113; MTBLC17797; MTBLC32816; MTBLC17050; MTBLC17154; MTBLC27897; MTBLC17151; MTBLC27997; MTBLC29864; MTBLC67042; MTBLC30831; MTBLC15891; MTBLC17724; MTBLC72959; MTBLC7676; MTBLC17533; MTBLC17311; MTBLC16797; MTBLC28867; MTBLC17200; MTBLC88454; MTBLC133032; MTBLC30915; MTBLC72689; MTBLC66847; MTBLC18053; MTBLC134594; MTBLC16919; MTBLC136176; MTBLC21547; MTBLC85693; MTBLC141588; MTBLC17515; MTBLC153069; MTBLC84838; MTBLC65301; MTBLC90464; MTBLC73688; MTBLC15746; MTBLC6650; MTBLC78646; MTBLC18148; MTBLC17929; MTBLC15978; MTBLC17015; MTBLC37024; MTBLC40265; MTBLC18019; MTBLC82912; MTBLC7125; MTBLC84385; MTBLC36313; MTBLC17191; MTBLC27389; MTBLC84394; MTBLC17659; MTBLC16015; MTBLC141435; MTBLC15354; MTBLC15799; MTBLC32425; MTBLC59265; MTBLC16467; MTBLC16695; MTBLC180019; MTBLC17750; MTBLC28875; MTBLC144044; MTBLC37024; MTBLC30915; MTBLC73990; MTBLC17050; MTBLC17549; MTBLC16027; MTBLC17475; MTBLC28822; MTBLC16958; MTBLC16737; MTBLC88003; MTBLC18012; MTBLC16865; MTBLC4170; MTBLC33508; MTBLC15978; MTBLC15428; MTBLC16668; MTBLC42111; MTBLC25094; MTBLC340824; MTBLC17154; MTBLC18257; MTBLC16995; MTBLC7916; MTBLC17964; MTBLC18183; MTBLC33017; MTBLC17797; MTBLC37455; MTBLC27897; MTBLC16695; MTBLC64489; MTBLC84385; MTBLC67042; MTBLC72959; MTBLC72957; MTBLC64487; MTBLC84386; MTBLC75465; MTBLC74831; MTBLC15799; MTBLC64486; MTBLC91309; MTBLC131739; MTBLC74966; MTBLC91305; MTBLC136083; MTBLC131982; MTBLC131985; MTBLC136140; MTBLC72998; MTBLC75342; MTBLC73134; MTBLC145273; MTBLC62837; MTBLC16196; MTBLC59265; MTBLC15756; MTBLC28875; MTBLC16015; MTBLC18012; MTBLC15741; MTBLC6650; MTBLC30769; MTBLC30915; MTBLC141435; MTBLC24266; MTBLC16856; MTBLC169683; MTBLC16027; MTBLC18066; MTBLC27389; MTBLC75004; MTBLC21547; MTBLC17562; MTBLC45979; MTBLC50048; MTBLC16737; MTBLC30911; MTBLC73713; MTBLC15652; MTBLC28053; MTBLC44897; MTBLC17138; MTBLC57589; MTBLC44747; MTBLC17533; MTBLC73688; MTBLC18019; MTBLC16467; MTBLC16414; MTBLC17203; MTBLC18148; MTBLC7916; MTBLC16797; MTBLC31515; MTBLC32425; MTBLC28846; MTBLC44215; MTBLC7125; MTBLC62833; MTBLC17013; MTBLC4170; MTBLC17154; MTBLC142245; MTBLC180019; MTBLC15843; MTBLC16235; MTBLC45996; MTBLC73731; MTBLC15721; MTBLC73067; MTBLC86147; MTBLC42504; MTBLC17351; MTBLC82969; MTBLC75115; MTBLC48153; MTBLC17677; MTBLC82846; MTBLC84328; MTBLC32816; MTBLC71466; MTBLC61204; MTBLC36005; MTBLC40279; MTBLC17239; MTBLC192695</t>
-  </si>
-  <si>
     <t>MTBLS1903</t>
   </si>
   <si>
@@ -451,6 +451,42 @@
     <t>MTBLC72665; MTBLC15551; MTBLC72663; MTBLC16359; MTBLC15843; MTBLC53487; MTBLC16525; MTBLC65136; MTBLC36005; MTBLC27997; MTBLC30781; MTBLC64563; MTBLC22652; MTBLC194379; MTBLC17626; MTBLC64566; MTBLC30797; MTBLC72384; MTBLC43355; MTBLC64560; MTBLC16960; MTBLC15824; MTBLC183705; MTBLC86542; MTBLC17858; MTBLC16755; MTBLC136218; MTBLC64549; MTBLC183253; MTBLC64561; MTBLC183255; MTBLC37011; MTBLC17351; MTBLC34130; MTBLC194376; MTBLC183825; MTBLC64568; MTBLC156126; MTBLC15741; MTBLC75097; MTBLC30769; MTBLC14314; MTBLC24266; MTBLC190189; MTBLC180275; MTBLC30829; MTBLC228737; MTBLC16002; MTBLC72795; MTBLC14336; MTBLC228787; MTBLC15908; MTBLC55328; MTBLC16446; MTBLC16899; MTBLC136485; MTBLC36751; MTBLC229814; MTBLC166934; MTBLC72606; MTBLC183244; MTBLC64390; MTBLC5390; MTBLC30813; MTBLC17118; MTBLC60647; MTBLC16300; MTBLC4676; MTBLC136170; MTBLC183661; MTBLC18268; MTBLC177850; MTBLC228770; MTBLC87818; MTBLC72737; MTBLC141511; MTBLC9008; MTBLC17859; MTBLC21547; MTBLC138794; MTBLC165324; MTBLC74349; MTBLC134594; MTBLC28044; MTBLC17202; MTBLC17069; MTBLC28875; MTBLC73018; MTBLC59270; MTBLC20067; MTBLC62084; MTBLC166932; MTBLC70979; MTBLC17242; MTBLC17553; MTBLC16831; MTBLC141435; MTBLC193578; MTBLC36259; MTBLC27570; MTBLC17385; MTBLC91286; MTBLC9300; MTBLC91218; MTBLC49584; MTBLC72802; MTBLC17361; MTBLC166933; MTBLC18012; MTBLC32796; MTBLC183659; MTBLC136113; MTBLC34133; MTBLC30832; MTBLC15721; MTBLC16043; MTBLC91312; MTBLC167715; MTBLC16264; MTBLC16761; MTBLC73853; MTBLC64481; MTBLC183648; MTBLC15628; MTBLC183252; MTBLC165343; MTBLC16027; MTBLC6499; MTBLC138556; MTBLC167775; MTBLC4873; MTBLC190567; MTBLC16345; MTBLC68502; MTBLC16914; MTBLC190534; MTBLC15554; MTBLC741548; MTBLC132745; MTBLC183932; MTBLC17369; MTBLC17409; MTBLC27386; MTBLC190671; MTBLC72639; MTBLC72392; MTBLC16217; MTBLC19702; MTBLC28670; MTBLC183646; MTBLC30746; MTBLC75095; MTBLC21557; MTBLC68555; MTBLC132958; MTBLC30838; MTBLC228759; MTBLC18211; MTBLC71018; MTBLC183349; MTBLC88459; MTBLC183258; MTBLC64559; MTBLC19289; MTBLC172574; MTBLC228699; MTBLC72782; MTBLC183650; MTBLC17549; MTBLC73580; MTBLC190527; MTBLC134589; MTBLC84526; MTBLC183760; MTBLC15919; MTBLC165283; MTBLC16325; MTBLC27849; MTBLC228676; MTBLC33216; MTBLC136230; MTBLC15846; MTBLC32805; MTBLC27747; MTBLC228556; MTBLC138084; MTBLC137228; MTBLC190545; MTBLC17189; MTBLC28635; MTBLC44897; MTBLC41321; MTBLC89417; MTBLC190548; MTBLC17200; MTBLC6130; MTBLC16938; MTBLC104011; MTBLC17138; MTBLC137590; MTBLC4178; MTBLC190526; MTBLC183665; MTBLC27407; MTBLC17474; MTBLC190741; MTBLC145255; MTBLC12962; MTBLC73770; MTBLC17947; MTBLC89991; MTBLC190192; MTBLC28997; MTBLC183327; MTBLC15753; MTBLC183332; MTBLC67057; MTBLC74484; MTBLC81559; MTBLC132983; MTBLC72999; MTBLC183254; MTBLC190590; MTBLC25998; MTBLC85039; MTBLC73989; MTBLC24344; MTBLC132403; MTBLC18346; MTBLC28031; MTBLC17816; MTBLC170073; MTBLC184291; MTBLC88458; MTBLC132744; MTBLC85000; MTBLC67056; MTBLC33830; MTBLC18332; MTBLC18009; MTBLC30853; MTBLC89512; MTBLC72657; MTBLC15751; MTBLC42265; MTBLC190637; MTBLC228752; MTBLC89644; MTBLC16973; MTBLC15682; MTBLC228745; MTBLC50397; MTBLC55481; MTBLC53678; MTBLC67900; MTBLC190554; MTBLC67059; MTBLC228700; MTBLC15652; MTBLC10072; MTBLC27562; MTBLC183358; MTBLC17808; MTBLC189055; MTBLC15811; MTBLC27814; MTBLC63986; MTBLC90468; MTBLC228717; MTBLC165340; MTBLC84094; MTBLC39567; MTBLC73259; MTBLC34146; MTBLC1015; MTBLC131988; MTBLC32980; MTBLC6784; MTBLC189600; MTBLC190528; MTBLC67058; MTBLC67119; MTBLC16450; MTBLC72382; MTBLC16691; MTBLC16742; MTBLC74750; MTBLC183259; MTBLC37998; MTBLC16298; MTBLC6052; MTBLC32818; MTBLC44747; MTBLC59016; MTBLC28158; MTBLC16440; MTBLC184236; MTBLC27485; MTBLC15414; MTBLC28846; MTBLC183703; MTBLC41865; MTBLC34939; MTBLC15545; MTBLC190566; MTBLC167802; MTBLC48861; MTBLC165310; MTBLC183317; MTBLC192640; MTBLC18403; MTBLC228819; MTBLC34306; MTBLC190598; MTBLC44510; MTBLC17306; MTBLC34494; MTBLC35374; MTBLC73726; MTBLC189467; MTBLC72398; MTBLC73688; MTBLC37510; MTBLC17969; MTBLC29019; MTBLC28587; MTBLC183362; MTBLC15548; MTBLC26536; MTBLC76451; MTBLC68441; MTBLC31959; MTBLC545959; MTBLC145243; MTBLC17239; MTBLC64575; MTBLC15756; MTBLC72387; MTBLC139132; MTBLC28667; MTBLC16196; MTBLC72385; MTBLC195266; MTBLC28728; MTBLC16750; MTBLC88108; MTBLC84441; MTBLC16704; MTBLC64483; MTBLC82846; MTBLC52449; MTBLC228791; MTBLC70984; MTBLC183236; MTBLC91296; MTBLC138532; MTBLC72381; MTBLC17443; MTBLC15373; MTBLC131993; MTBLC64565; MTBLC40410; MTBLC17012; MTBLC52075; MTBLC64567; MTBLC64569; MTBLC73828; MTBLC53210; MTBLC72736; MTBLC12777; MTBLC90433; MTBLC136141; MTBLC172431; MTBLC142219; MTBLC72605; MTBLC16424; MTBLC73723; MTBLC17482; MTBLC174217; MTBLC26711; MTBLC89310; MTBLC18240; MTBLC183350; MTBLC76308; MTBLC72734; MTBLC67168; MTBLC48928; MTBLC192587; MTBLC16827; MTBLC132244; MTBLC72998; MTBLC72735; MTBLC27436; MTBLC64576; MTBLC44811; MTBLC70976; MTBLC78668; MTBLC42539; MTBLC166929; MTBLC18323; MTBLC16753; MTBLC18107; MTBLC73912; MTBLC169985; MTBLC72394; MTBLC230582; MTBLC73788; MTBLC15698; MTBLC16908; MTBLC28716; MTBLC64153; MTBLC183496; MTBLC17748; MTBLC17515; MTBLC89633; MTBLC28842; MTBLC73024; MTBLC72390; MTBLC35045; MTBLC2877; MTBLC18377; MTBLC2495; MTBLC28077; MTBLC24848; MTBLC16581; MTBLC194178; MTBLC15765; MTBLC16870; MTBLC545687; MTBLC68433; MTBLC15694; MTBLC183722; MTBLC30851; MTBLC28689; MTBLC16856; MTBLC70989; MTBLC28834; MTBLC89825; MTBLC72386; MTBLC72844; MTBLC48153; MTBLC16734; MTBLC228541; MTBLC90452; MTBLC228805; MTBLC30805; MTBLC61058; MTBLC176838; MTBLC228795; MTBLC132559; MTBLC39246; MTBLC17621; MTBLC170124; MTBLC6257; MTBLC17263; MTBLC17650; MTBLC73830; MTBLC169528; MTBLC190537; MTBLC228562; MTBLC36575; MTBLC73994; MTBLC73713; MTBLC84212; MTBLC16556; MTBLC113543; MTBLC25013; MTBLC30763; MTBLC40799; MTBLC34135; MTBLC27647; MTBLC9299; MTBLC31345; MTBLC143045; MTBLC17786; MTBLC7466; MTBLC16988; MTBLC33198; MTBLC16551; MTBLC116314; MTBLC74475; MTBLC75342; MTBLC34900; MTBLC16919; MTBLC15354; MTBLC17295; MTBLC73067; MTBLC17154; MTBLC18347; MTBLC132244; MTBLC26271; MTBLC17126; MTBLC17750; MTBLC16811; MTBLC69081; MTBLC57589; MTBLC68616; MTBLC28884; MTBLC27266; MTBLC41117; MTBLC16235; MTBLC78646; MTBLC17568; MTBLC1606; MTBLC25094; MTBLC17964; MTBLC28867; MTBLC49033; MTBLC71466; MTBLC46968; MTBLC37024; MTBLC25682; MTBLC16349; MTBLC17597; MTBLC16040; MTBLC178624; MTBLC18295; MTBLC143245; MTBLC73261; MTBLC16411; MTBLC28671; MTBLC15765; MTBLC68830; MTBLC193587; MTBLC35581; MTBLC167782; MTBLC68499; MTBLC73580; MTBLC16092; MTBLC70958; MTBLC15971; MTBLC16436; MTBLC72843; MTBLC90727; MTBLC16610; MTBLC17311; MTBLC16393; MTBLC184023; MTBLC26986; MTBLC15846; MTBLC17515; MTBLC69438; MTBLC15940; MTBLC183418; MTBLC29009; MTBLC49285; MTBLC170016; MTBLC24813; MTBLC27911; MTBLC44237; MTBLC16171; MTBLC17752; MTBLC71464; MTBLC7027; MTBLC2274; MTBLC167742; MTBLC63866; MTBLC41308; MTBLC27468; MTBLC167400; MTBLC20794; MTBLC28918; MTBLC21803; MTBLC4828; MTBLC68451; MTBLC28579; MTBLC183426; MTBLC16962; MTBLC34800; MTBLC28940; MTBLC50202; MTBLC16680; MTBLC132837; MTBLC18344; MTBLC60175; MTBLC27632; MTBLC35720; MTBLC17821; MTBLC15746; MTBLC6857; MTBLC41899; MTBLC228605; MTBLC183339; MTBLC17747; MTBLC17368; MTBLC18089; MTBLC27480; MTBLC177535; MTBLC16015; MTBLC27897; MTBLC61204; MTBLC17061; MTBLC17895; MTBLC18183; MTBLC17596; MTBLC28865; MTBLC17687; MTBLC7916; MTBLC16709; MTBLC16027; MTBLC17509; MTBLC17053; MTBLC17562; MTBLC17712; MTBLC16708; MTBLC17884; MTBLC16946; MTBLC74099; MTBLC73830; MTBLC17015; MTBLC15727; MTBLC16927; MTBLC72782; MTBLC31445; MTBLC143163; MTBLC16990; MTBLC17405; MTBLC9211; MTBLC50145; MTBLC183493; MTBLC176697; MTBLC190600; MTBLC183451; MTBLC190618; MTBLC69187; MTBLC18176; MTBLC156288; MTBLC183699; MTBLC228511; MTBLC176723; MTBLC176699; MTBLC28801; MTBLC64564; MTBLC136071; MTBLC27747; MTBLC144783; MTBLC176730; MTBLC85299; MTBLC190647; MTBLC70101; MTBLC28158; MTBLC68503; MTBLC177499; MTBLC84940; MTBLC29016; MTBLC71415; MTBLC171809; MTBLC190661; MTBLC183755; MTBLC86952; MTBLC30260; MTBLC190604; MTBLC3088; MTBLC65408; MTBLC36773; MTBLC183462; MTBLC177606; MTBLC182459; MTBLC134584; MTBLC53486; MTBLC165632; MTBLC228554; MTBLC190560; MTBLC190627; MTBLC29019; MTBLC15891; MTBLC183484; MTBLC180593; MTBLC194256; MTBLC48981; MTBLC18132; MTBLC181232; MTBLC183438; MTBLC70749; MTBLC18292; MTBLC91272; MTBLC64349; MTBLC18095; MTBLC172338; MTBLC194258; MTBLC190666; MTBLC190634; MTBLC167825; MTBLC42255; MTBLC89242; MTBLC68567; MTBLC70960; MTBLC183406; MTBLC73707; MTBLC190585; MTBLC228653; MTBLC66951; MTBLC34162; MTBLC52392; MTBLC183424; MTBLC27596; MTBLC28794; MTBLC9107; MTBLC183379; MTBLC27452; MTBLC183751; MTBLC61646; MTBLC4903; MTBLC192607; MTBLC90355; MTBLC157713; MTBLC17553; MTBLC190555; MTBLC183726; MTBLC174991; MTBLC67058; MTBLC506227; MTBLC38108; MTBLC17115; MTBLC61694; MTBLC190660; MTBLC16437; MTBLC190638; MTBLC183718; MTBLC64294; MTBLC183003; MTBLC183453; MTBLC9410; MTBLC183455; MTBLC47397; MTBLC143747; MTBLC16576; MTBLC183815; MTBLC192574; MTBLC74767; MTBLC17033; MTBLC18123; MTBLC4743; MTBLC74514; MTBLC190535; MTBLC16634; MTBLC27595; MTBLC37084; MTBLC17287; MTBLC140927; MTBLC21626; MTBLC72853; MTBLC94459; MTBLC183428; MTBLC50519; MTBLC190643; MTBLC183671; MTBLC192615; MTBLC170045; MTBLC7125; MTBLC177034; MTBLC170055; MTBLC86549; MTBLC14336; MTBLC183390; MTBLC176703; MTBLC192580; MTBLC167729; MTBLC190659; MTBLC2003; MTBLC190648; MTBLC168877; MTBLC89605; MTBLC9592; MTBLC16374; MTBLC201644; MTBLC190641; MTBLC136088; MTBLC27510; MTBLC134592; MTBLC73530; MTBLC89649; MTBLC183677; MTBLC190652; MTBLC194266; MTBLC134583; MTBLC16973; MTBLC183667; MTBLC181585; MTBLC194257; MTBLC182859; MTBLC192673; MTBLC62434; MTBLC15584; MTBLC228641; MTBLC134761; MTBLC183687; MTBLC228618; MTBLC132121; MTBLC15729; MTBLC228598; MTBLC28952; MTBLC183758; MTBLC3291; MTBLC176815; MTBLC183348; MTBLC183666; MTBLC190630; MTBLC228524; MTBLC228697; MTBLC583580; MTBLC73805; MTBLC228827; MTBLC190603; MTBLC175067; MTBLC15760; MTBLC182253; MTBLC74791; MTBLC75539; MTBLC15676; MTBLC183366; MTBLC190670; MTBLC192627; MTBLC190579; MTBLC183696; MTBLC17645; MTBLC78576; MTBLC4874; MTBLC26756; MTBLC89469; MTBLC183780; MTBLC28821; MTBLC188539; MTBLC183468; MTBLC183757; MTBLC70700; MTBLC320061; MTBLC228418; MTBLC74112; MTBLC183779; MTBLC228552; MTBLC16831; MTBLC16998; MTBLC89187; MTBLC228383; MTBLC190611; MTBLC183404; MTBLC24898; MTBLC94054; MTBLC37574; MTBLC178528; MTBLC183706; MTBLC55484; MTBLC183756; MTBLC27624; MTBLC16354; MTBLC4047; MTBLC194705; MTBLC177788; MTBLC177643; MTBLC6483; MTBLC144413; MTBLC189466; MTBLC17252; MTBLC18280; MTBLC228816; MTBLC64032; MTBLC28747; MTBLC17160; MTBLC183449; MTBLC6052; MTBLC228479; MTBLC74860; MTBLC183734; MTBLC183429; MTBLC192635; MTBLC183375; MTBLC15964; MTBLC190612; MTBLC192649; MTBLC182136; MTBLC87625; MTBLC9172; MTBLC192628; MTBLC165312; MTBLC90230; MTBLC68234; MTBLC183788; MTBLC3359; MTBLC190077; MTBLC136995; MTBLC28327; MTBLC125255; MTBLC16737; MTBLC228692; MTBLC64850; MTBLC228833; MTBLC183414; MTBLC85239; MTBLC5280; MTBLC183416; MTBLC186084; MTBLC67054; MTBLC182811; MTBLC16347; MTBLC64213; MTBLC183723; MTBLC194296; MTBLC174632; MTBLC194254; MTBLC16380; MTBLC181895; MTBLC183679; MTBLC228542; MTBLC190639; MTBLC91867; MTBLC192567; MTBLC183471; MTBLC32425; MTBLC194271; MTBLC170053; MTBLC46195; MTBLC134637; MTBLC177757; MTBLC190633; MTBLC139247; MTBLC16010; MTBLC228508; MTBLC1189; MTBLC10575; MTBLC165341; MTBLC17659; MTBLC192630; MTBLC190582; MTBLC27953; MTBLC183474; MTBLC190621; MTBLC16562; MTBLC178755; MTBLC228285; MTBLC228602; MTBLC228547; MTBLC59750; MTBLC170038; MTBLC183435; MTBLC17460; MTBLC192578; MTBLC3724; MTBLC228727; MTBLC8067; MTBLC132364; MTBLC84883; MTBLC48093; MTBLC111321; MTBLC228654; MTBLC93822; MTBLC17362; MTBLC228830; MTBLC183329; MTBLC174357; MTBLC183793; MTBLC183503; MTBLC80567; MTBLC35018; MTBLC184078; MTBLC4629; MTBLC1148; MTBLC181492; MTBLC67056; MTBLC46372; MTBLC17898; MTBLC192563; MTBLC67989; MTBLC183446; MTBLC182892; MTBLC88439; MTBLC45910; MTBLC228559; MTBLC42534; MTBLC17561; MTBLC63791; MTBLC31111; MTBLC137830; MTBLC190538; MTBLC64153; MTBLC17780; MTBLC135014; MTBLC228725; MTBLC66682; MTBLC190578; MTBLC143265; MTBLC183353; MTBLC64818; MTBLC190601; MTBLC228439; MTBLC9215; MTBLC195104; MTBLC197140; MTBLC8229; MTBLC74879; MTBLC228390; MTBLC183775; MTBLC157747; MTBLC17342; MTBLC168044; MTBLC9629; MTBLC89557; MTBLC181543; MTBLC15714; MTBLC173611; MTBLC86088; MTBLC93879; MTBLC94686; MTBLC183689; MTBLC168762; MTBLC24536; MTBLC190550; MTBLC64983; MTBLC228822; MTBLC6695; MTBLC133246; MTBLC181031; MTBLC16695; MTBLC167561; MTBLC37277; MTBLC228810; MTBLC81771; MTBLC192626; MTBLC4471; MTBLC190592; MTBLC228606; MTBLC89741; MTBLC228831; MTBLC38572; MTBLC741548; MTBLC2065; MTBLC181115; MTBLC167853; MTBLC183345; MTBLC191070; MTBLC2295; MTBLC183681; MTBLC16828; MTBLC47417; MTBLC182331; MTBLC28195; MTBLC183846; MTBLC228643; MTBLC18385; MTBLC15956; MTBLC90936; MTBLC228600; MTBLC4640; MTBLC18088; MTBLC16796; MTBLC16330; MTBLC6775; MTBLC183740; MTBLC192605; MTBLC108595; MTBLC32365; MTBLC19475; MTBLC32692; MTBLC52446; MTBLC18311; MTBLC16857; MTBLC28689; MTBLC136805; MTBLC4591; MTBLC2766; MTBLC1582; MTBLC192666; MTBLC46932; MTBLC66729; MTBLC16174; MTBLC15413; MTBLC34350; MTBLC228437; MTBLC135338; MTBLC183452; MTBLC18332; MTBLC8107; MTBLC73510; MTBLC16418; MTBLC94680; MTBLC37455; MTBLC48526; MTBLC183445; MTBLC167367; MTBLC192671; MTBLC183727; MTBLC183717; MTBLC228424; MTBLC34450; MTBLC16344; MTBLC192675; MTBLC9171; MTBLC39867; MTBLC17713; MTBLC228428; MTBLC228593; MTBLC190655; MTBLC16164; MTBLC139579; MTBLC6754; MTBLC48400; MTBLC172483; MTBLC10432; MTBLC75095; MTBLC27961; MTBLC5262; MTBLC16467; MTBLC189117; MTBLC192644; MTBLC16530; MTBLC16443; MTBLC190588; MTBLC165293; MTBLC183463; MTBLC183747; MTBLC228564; MTBLC45725; MTBLC183684; MTBLC10073; MTBLC228532; MTBLC183322; MTBLC64277; MTBLC17312; MTBLC8809; MTBLC174296; MTBLC183731; MTBLC75648; MTBLC228384; MTBLC1387; MTBLC16020; MTBLC194288; MTBLC68447; MTBLC131425; MTBLC60989; MTBLC228639; MTBLC156175; MTBLC228586; MTBLC8269; MTBLC89640; MTBLC165524; MTBLC132583; MTBLC183355; MTBLC17196; MTBLC192585; MTBLC27794; MTBLC16865; MTBLC228503; MTBLC67818; MTBLC31742; MTBLC16532; MTBLC190624; MTBLC183504; MTBLC18241; MTBLC17310; MTBLC183505; MTBLC192590; MTBLC48541; MTBLC53170; MTBLC28997; MTBLC84836; MTBLC183730; MTBLC70481; MTBLC23965; MTBLC190650; MTBLC228494; MTBLC90459; MTBLC6643; MTBLC183460; MTBLC165591; MTBLC183743; MTBLC228687; MTBLC228507; MTBLC27838; MTBLC15768; MTBLC138785; MTBLC89656; MTBLC7625; MTBLC48991; MTBLC167785; MTBLC7865; MTBLC134593; MTBLC183401; MTBLC192633; MTBLC103855; MTBLC228433; MTBLC183767; MTBLC183408; MTBLC228665; MTBLC17256; MTBLC140861; MTBLC190654; MTBLC183431; MTBLC18723; MTBLC183719; MTBLC30860; MTBLC80447; MTBLC65121; MTBLC34464; MTBLC86655; MTBLC190668; MTBLC192735; MTBLC183482; MTBLC228608; MTBLC192601; MTBLC228668; MTBLC45979; MTBLC2740; MTBLC228578; MTBLC72723; MTBLC16226; MTBLC1784; MTBLC136085; MTBLC136089; MTBLC77006; MTBLC15882; MTBLC74763; MTBLC167860; MTBLC168507; MTBLC190664; MTBLC27551; MTBLC17858; MTBLC48430; MTBLC16566; MTBLC170023; MTBLC228584; MTBLC16600; MTBLC75913; MTBLC137125; MTBLC75757; MTBLC70744; MTBLC16543; MTBLC15550; MTBLC64568; MTBLC68433; MTBLC48131; MTBLC9300; MTBLC22198; MTBLC17775; MTBLC45996; MTBLC165794; MTBLC16410; MTBLC16373; MTBLC72391; MTBLC16813; MTBLC73527; MTBLC29073; MTBLC89929; MTBLC67055; MTBLC17134; MTBLC27823; MTBLC31459; MTBLC16908; MTBLC35465; MTBLC17345; MTBLC17490; MTBLC82969; MTBLC16283; MTBLC30845; MTBLC82965; MTBLC7563; MTBLC9481; MTBLC88456; MTBLC22653; MTBLC39236; MTBLC58527; MTBLC28054; MTBLC19289; MTBLC134510; MTBLC74903; MTBLC104011; MTBLC16032; MTBLC28822; MTBLC27974; MTBLC82679; MTBLC40070; MTBLC16856; MTBLC85235; MTBLC73517; MTBLC85252; MTBLC78697; MTBLC183683; MTBLC21363; MTBLC37025; MTBLC138533; MTBLC15344; MTBLC138537; MTBLC167719; MTBLC74838; MTBLC16494; MTBLC89315; MTBLC195592; MTBLC17215; MTBLC36632; MTBLC17026; MTBLC40131; MTBLC36006; MTBLC192679; MTBLC47977; MTBLC81689; MTBLC1457; MTBLC165842; MTBLC16313; MTBLC28955; MTBLC16335; MTBLC180410; MTBLC79735; MTBLC73017; MTBLC135870; MTBLC68329; MTBLC17594; MTBLC72625; MTBLC141472; MTBLC17622; MTBLC192676; MTBLC190595; MTBLC64565; MTBLC15544; MTBLC63795; MTBLC73026; MTBLC228794; MTBLC228696; MTBLC137054; MTBLC44454; MTBLC164107; MTBLC16761; MTBLC64549; MTBLC28171; MTBLC15560; MTBLC21563; MTBLC8638; MTBLC28792; MTBLC17609; MTBLC17381; MTBLC88522; MTBLC137725; MTBLC28140; MTBLC27931; MTBLC181441; MTBLC17172; MTBLC28099; MTBLC28324; MTBLC228529</t>
   </si>
   <si>
+    <t>MTBLS49</t>
+  </si>
+  <si>
+    <t>Metabolomics guides rational development of a simplified cell culture medium for drug screening against Trypanosoma brucei</t>
+  </si>
+  <si>
+    <t>In vitro culture methods underpin many experimental approaches to biology and drug discovery. The modification of established cell culture methods to be more biologically relevant, or to optimise growth, is traditionally a laborious task. Emerging metabolomics technology enables rapid evaluation of intra- and extra-cellular metabolites, and can be applied to the rational development of cell culture medium. In this study, untargeted semi-quantitative, and targeted quantitative, metabolomic analyses of fresh and spent media revealed the major nutritional requirements for growth of bloodstream-form Trypanosoma brucei. The standard culture medium (HMI11) contained unnecessarily high concentrations of 32 nutrients that were subsequently removed to more closely resemble concentrations normally found in blood. Our new minimal medium (CMM) supports in vitro growth equivalent to HMI11, and causes no significant perturbation of metabolite levels for 94% of the detected metabolome (&lt; 3-fold change; a = 0.05). Importantly, improved sensitivity was observed for drug activity studies in whole cell phenotypic screens, and in metabolomics mode of action assays. 400-fold decreases in IC50 were observed for pentamidine and methotrexate, suggesting inhibition of activity by nutrients present in HMI11. CMM is suitable for routine cell culture and offers important advantages for metabolomics studies and drug activity screening.</t>
+  </si>
+  <si>
+    <t>drug screening/evaluation; culture medium; liquid chromatography-mass spectrometry; untargeted metabolites</t>
+  </si>
+  <si>
+    <t>Metabolomics guides rational development of a simplified cell culture medium for drug screening against Trypanosoma brucei. 10.1128/aac.00044-13. PMID:23571546</t>
+  </si>
+  <si>
+    <t>Bloodstream-form Trypanosoma brucei brucei (s427) were cultured in vitro in either HMI11 (Gibco), CMM or modified media with 10% FCS Gold (PAA). Cell culture grade (or high purity) D-glucose, L-cysteine, L-glutamine and all other medium components were purchased from Sigma Aldrich. 5 ml cultures were maintained in 25 ml vented flasks (Corning) at 37 C with 5% CO2. Cultures were grown to a maximum density of 4 x 106 cells/ml and sub-cultured by 1 in 100 or 1 in 1000 dilution, every 2 or 3 days, respectively. Cell counts were obtained by haemocytometer (Neubauer).</t>
+  </si>
+  <si>
+    <t>Metabolite extraction was performed according to previously described methods [1][2]. 25 ml of cell culture was quenched by rapid cooling to 4 C in a dry ice/ethanol bath. Cell pellets were obtained by centrifugation at 1250 x g for 10 minutes, and 5 l spent media was removed and extracted by addition of 100 l chloroform/methanol/water (1:3:1). The remaining cell pellet was washed with 1 ml PBS, and the washed pellet (5  107 cells) was extracted with 100 l chloroform/methanol/water (1:3:1) by mixing for 1 h at 4 C, before centrifugation to remove precipitate. The resulting metabolite solution was stored at -80 C until analysis by liquid chromatography-mass spectrometry (LC-MS). Comparative data from HMI11 and CMM cell pellets and spent media are from 5 independent biological replicates.&lt;/p&gt;Ref:&lt;/br&gt;[1] Saunders EC, Ng WW, Chambers JM, Ng M, Naderer T, Kramer JO, Likic VA, McConville MJ. 2011. Isotopomer profiling of Leishmania mexicana promastigotes reveals important roles for succinate fermentation and aspartate uptake in tricarboxylic acid cycle (TCA) anaplerosis, glutamate synthesis, and growth. J. Biol. Chem. 286:2770627717. doi:10.1074/jbc.M110.213553. PMID:21636575&lt;/br&gt;[2] t'Kindt R, Jankevics A, Scheltema RA, Zheng L, Watson DG, Dujardin JC, Breitling R, Coombs GH, Decuypere S. 2010. Towards an unbiased metabolic profiling of protozoan parasites: optimisation of a Leishmania sampling protocol for HILIC-Orbitrap analysis. Anal. Bioanal. Chem. 398:20592069. doi:10.1007/s00216-010-4139-0. PMID:20824428&lt;/br&gt;</t>
+  </si>
+  <si>
+    <t>The LC separation was performed using hydrophilic interaction chromatography with a ZIC-HILIC 150 mm x 4.6 mm, 5 m column (Merck Sequant), operated by a Dionex UltiMate liquid chromatography system (Dionex, Camberley, Surrey), and coupled to a FAMOS autosampler. The LC mobile phase was a linear gradient from 80% B to 20% B over 30 min, followed by an 8 min wash with 5% B, and 8 min re-equilibration with 80% B, where solvent B is 0.08% formic acid in acetonitrile and solvent A is 0.1% formic acid in water. The flow rate was 300 l/min, column temperature 20 C, injection volume 10 l, and samples were maintained at 4 C.</t>
+  </si>
+  <si>
+    <t>The mass spectrometry was performed using an Orbitrap Exactive (Thermo Fisher Scientific, Hemel Hempstead, U.K.) with a HESI 2 probe. The spectrometer was operated in polarity switching mode, with the following settings: resolution 50,000, AGC 1 x 106, m/z range 701400, sheath gas 40, auxiliary gas 20, sweep gas 1, probe temperature 275 C, and capillary temperature 250 C. For positive mode ionization: source voltage +4 kV, capillary voltage +50 V, tube voltage +70 V, skimmer voltage +20 V. For negative mode ionization: source voltage -3.5 kV, capillary voltage -50 V, tube voltage -70 V, skimmer voltage -20 V. Mass calibration was performed for each polarity immediately before each analysis batch, within 48 h for all samples. The calibration mass range was extended to cover small metabolites by inclusion of low-mass contaminants with the standard Thermo calmix masses (below m/z 1400), acetonitrile dimer for positive ion electrospray ionization (PIESI) mode (m/z 83.0604) and C3H5O3 for negative ion electrospray ionization (NIESI) mode (m/z 89.0244). To enhance calibration stability, lock-mass correction was also applied to each analytical run using these ubiquitous low-mass contaminants.</t>
+  </si>
+  <si>
+    <t>Peak-picking by XCMS - http://metlin.scripps.edu/xcms/ (Centwave), peak matching and annotation by mzMatch, and noise filtering and metabolite identification by IDEOM (http://mzmatch.sourceforge.net/ideom.php), using the default parameters.</t>
+  </si>
+  <si>
+    <t>Metabolite identification is based on accurate mass and predicted retention time, which is accepted as a level 3 standard of identification by the Metabolomics Standards Initiative (MSI), but should be considered as a putative identification. Retention time was verified by authentic standards for the major HMI11 components and other metabolites where possible.</t>
+  </si>
+  <si>
+    <t>MTBLC16235; MTBLC17754; MTBLC17748; MTBLC17712; MTBLC16977; MTBLC17154; MTBLC41531|MTBLC45658; MTBLC16870; MTBLC17509; MTBLC16335; MTBLC17361; MTBLC27596; MTBLC15354; MTBLC17053; MTBLC16467; MTBLC17196; MTBLC17368; MTBLC18385; MTBLC16015; MTBLC15971; MTBLC16704; MTBLC17015; MTBLC17895; MTBLC17115; MTBLC15603; MTBLC17203; MTBLC15729; MTBLC16414; MTBLC17515; MTBLC48950; MTBLC16643; MTBLC18050; MTBLC16349; MTBLC18019; MTBLC16857; MTBLC47977; MTBLC17295; MTBLC17568; MTBLC15940; MTBLC17561; MTBLC17596; MTBLC16750; MTBLC16610; MTBLC16283; MTBLC16319; MTBLC17405; MTBLC18062; MTBLC6151; MTBLC73949; MTBLC17821; MTBLC28474; MTBLC16530; MTBLC16410; MTBLC1606|MTBLC70966|MTBLC74763|MTBLC73087|MTBLC74765|MTBLC74766; MTBLC16671; MTBLC17016; MTBLC16570; MTBLC27248; MTBLC7274; MTBLC27470; MTBLC17232; MTBLC15946; MTBLC28712; MTBLC17884; MTBLC17311; MTBLC27574; MTBLC15428; MTBLC15891; MTBLC37023; MTBLC2198; MTBLC7916; MTBLC30913; MTBLC17374; MTBLC27676; MTBLC18123; MTBLC16946; MTBLC9533; MTBLC16828; MTBLC15887; MTBLC15727; MTBLC48005; MTBLC28123; MTBLC17562; MTBLC16919; MTBLC16668; MTBLC20000; MTBLC16463; MTBLC17752; MTBLC17381; MTBLC17780; MTBLC27713; MTBLC41218; MTBLC51824; MTBLC15420; MTBLC61521; MTBLC43997; MTBLC73960; MTBLC7858; MTBLC73291; MTBLC73292; MTBLC73881; MTBLC73293; MTBLC74085; MTBLC73368; MTBLC17920; MTBLC29136; MTBLC73436; MTBLC17417; MTBLC15870; MTBLC73647; MTBLC17342; MTBLC5277; MTBLC74048; MTBLC73605; MTBLC27578; MTBLC73758; MTBLC73386; MTBLC16437; MTBLC15968; MTBLC73514; MTBLC15997; MTBLC32571; MTBLC74111; MTBLC74321; MTBLC73450; MTBLC28182; MTBLC73600; MTBLC73654; MTBLC73589; MTBLC73700; MTBLC7728; MTBLC6329; MTBLC5649; MTBLC2600; MTBLC73445; MTBLC6988; MTBLC55357; MTBLC73959; MTBLC73581; MTBLC73313; MTBLC45530; MTBLC73527; MTBLC50395; MTBLC28867; MTBLC73422; MTBLC11060; MTBLC73653; MTBLC73331; MTBLC73604; MTBLC27747; MTBLC17929; MTBLC73426; MTBLC73598; MTBLC74135; MTBLC73447; MTBLC73521; MTBLC74521; MTBLC73574; MTBLC73350; MTBLC73671; MTBLC73518; MTBLC73703; MTBLC74079; MTBLC756; MTBLC34237; MTBLC73525; MTBLC5583; MTBLC73704; MTBLC73606; MTBLC73513; MTBLC73414; MTBLC3222; MTBLC15336; MTBLC34792; MTBLC73505; MTBLC29563; MTBLC74516; MTBLC73903; MTBLC74129; MTBLC73617; MTBLC73366; MTBLC73571; MTBLC6198; MTBLC116314; MTBLC73421; MTBLC1391; MTBLC74104; MTBLC73349; MTBLC73485; MTBLC73506; MTBLC34726; MTBLC73353; MTBLC73738; MTBLC9173; MTBLC73601; MTBLC73926; MTBLC74438; MTBLC17604; MTBLC34019; MTBLC73394; MTBLC84933; MTBLC2881; MTBLC16968; MTBLC42025; MTBLC73526; MTBLC73397; MTBLC73663; MTBLC73607; MTBLC73411; MTBLC74110; MTBLC73381; MTBLC73318; MTBLC74024; MTBLC15783; MTBLC73528; MTBLC73583; MTBLC74112; MTBLC73685; MTBLC73515; MTBLC73736; MTBLC73529; MTBLC37251; MTBLC73530; MTBLC73585; MTBLC73645; MTBLC17195; MTBLC31071; MTBLC30820; MTBLC73646; MTBLC73632; MTBLC73990; MTBLC74077; MTBLC73579; MTBLC72723; MTBLC35019; MTBLC73444; MTBLC2814; MTBLC73437; MTBLC73580; MTBLC73695; MTBLC73596; MTBLC45171; MTBLC73512; MTBLC73531; MTBLC3206; MTBLC64486; MTBLC74027; MTBLC73634; MTBLC11946; MTBLC73565; MTBLC74533; MTBLC73608; MTBLC73520; MTBLC73794; MTBLC65842; MTBLC74562; MTBLC73566; MTBLC73861; MTBLC73363; MTBLC73443; MTBLC73425; MTBLC73721; MTBLC74044; MTBLC73489; MTBLC64288; MTBLC47914; MTBLC27626; MTBLC73701; MTBLC73858; MTBLC35050; MTBLC44164; MTBLC57885; MTBLC64489; MTBLC73850; MTBLC73869; MTBLC74344; MTBLC73873; MTBLC6253; MTBLC63934; MTBLC36575; MTBLC506227; MTBLC18357; MTBLC17924; MTBLC18397; MTBLC28297; MTBLC28220; MTBLC17697; MTBLC27413; MTBLC27931; MTBLC27592; MTBLC15728; MTBLC28621; MTBLC28004; MTBLC28790; MTBLC18107; MTBLC15760; MTBLC18032; MTBLC17213; MTBLC17724; MTBLC49015; MTBLC28716; MTBLC16576; MTBLC17957; MTBLC15805; MTBLC18373; MTBLC33094; MTBLC17862; MTBLC16742; MTBLC16026; MTBLC15675; MTBLC16660; MTBLC17755; MTBLC15743; MTBLC17645; MTBLC27468; MTBLC17620; MTBLC17294; MTBLC16288; MTBLC10329; MTBLC73780; MTBLC74125; MTBLC73522; MTBLC61346; MTBLC73459; MTBLC338412; MTBLC73490; MTBLC73737; MTBLC73454; MTBLC74323; MTBLC73694; MTBLC1604; MTBLC74049; MTBLC73710; MTBLC74484; MTBLC29010; MTBLC15426; MTBLC74490; MTBLC16020; MTBLC73800; MTBLC73362; MTBLC73643; MTBLC21374; MTBLC73612; MTBLC50601; MTBLC73439; MTBLC73488; MTBLC27419; MTBLC73868; MTBLC74487; MTBLC73865; MTBLC73644; MTBLC73457; MTBLC73696; MTBLC1237; MTBLC74517; MTBLC73740; MTBLC73434; MTBLC17303; MTBLC73393; MTBLC73582; MTBLC73024; MTBLC73384; MTBLC64305; MTBLC73438; MTBLC73344; MTBLC73572; MTBLC73496; MTBLC17702; MTBLC74532; MTBLC15956; MTBLC39585; MTBLC6851; MTBLC73419; MTBLC73448; MTBLC1643; MTBLC73699; MTBLC73461; MTBLC73446; MTBLC73733; MTBLC32963; MTBLC17310; MTBLC73465; MTBLC16531; MTBLC74092; MTBLC73594; MTBLC74404; MTBLC73889; MTBLC73633; MTBLC73563; MTBLC73627; MTBLC73399; MTBLC73412; MTBLC73609; MTBLC30270; MTBLC34900; MTBLC73323; MTBLC73409; MTBLC15424; MTBLC17618; MTBLC73661; MTBLC73970; MTBLC73882; MTBLC5724; MTBLC73981; MTBLC73428; MTBLC73516; MTBLC73402; MTBLC73577; MTBLC73613; MTBLC8067; MTBLC73270; MTBLC17443; MTBLC73329; MTBLC73591; MTBLC73502; MTBLC73979; MTBLC73401; MTBLC73372; MTBLC73341; MTBLC5712; MTBLC73026; MTBLC74430; MTBLC24109; MTBLC73351; MTBLC73611; MTBLC7676; MTBLC73487; MTBLC5858; MTBLC74479; MTBLC73635; MTBLC73499; MTBLC45757; MTBLC73524; MTBLC73342; MTBLC73578; MTBLC73789; MTBLC16357; MTBLC73614; MTBLC16737; MTBLC73517; MTBLC74535; MTBLC45564; MTBLC73705; MTBLC73355; MTBLC7061; MTBLC73326; MTBLC16244; MTBLC10018; MTBLC73610; MTBLC73652; MTBLC73330; MTBLC73376; MTBLC74101; MTBLC7621; MTBLC6631; MTBLC73456; MTBLC73798; MTBLC84834; MTBLC73725; MTBLC73739; MTBLC21557; MTBLC73616; MTBLC74441; MTBLC73660; MTBLC17495; MTBLC73406; MTBLC55458; MTBLC73667; MTBLC73347; MTBLC73692; MTBLC17927; MTBLC73375; MTBLC74475; MTBLC50845; MTBLC73910; MTBLC73430; MTBLC73462; MTBLC73892; MTBLC73404; MTBLC73497; MTBLC5390; MTBLC73697; MTBLC73636; MTBLC73508; MTBLC74437; MTBLC73658; MTBLC73324; MTBLC74123; MTBLC73427; MTBLC73498; MTBLC18255; MTBLC73463; MTBLC73429; MTBLC73562; MTBLC73348; MTBLC73395; MTBLC73494; MTBLC74303; MTBLC45571; MTBLC4117; MTBLC74102; MTBLC73923; MTBLC73391; MTBLC73929; MTBLC73455; MTBLC73659; MTBLC73648; MTBLC73564; MTBLC73392; MTBLC17328; MTBLC73493; MTBLC35280; MTBLC6645; MTBLC132188; MTBLC73503; MTBLC74107; MTBLC73561; MTBLC73484; MTBLC73451; MTBLC73501; MTBLC73711; MTBLC73698; MTBLC16227; MTBLC73655; MTBLC30821; MTBLC73900; MTBLC73615; MTBLC15425; MTBLC73492; MTBLC73314; MTBLC73741; MTBLC73649; MTBLC73927; MTBLC73894; MTBLC73630; MTBLC73435; MTBLC46807; MTBLC73691; MTBLC73638; MTBLC73491; MTBLC73656; MTBLC16213; MTBLC73568; MTBLC17394; MTBLC73382; MTBLC73424; MTBLC73321; MTBLC73628; MTBLC73590; MTBLC73637; MTBLC5757; MTBLC73639; MTBLC73666; MTBLC73575; MTBLC73570; MTBLC70744; MTBLC74096; MTBLC73567; MTBLC61138; MTBLC16533; MTBLC73576; MTBLC73662; MTBLC73569; MTBLC73885; MTBLC73345; MTBLC73797; MTBLC73875; MTBLC73793; MTBLC73751; MTBLC73377; MTBLC16708; MTBLC74356; MTBLC73723; MTBLC73795; MTBLC16027; MTBLC73851; MTBLC73854; MTBLC72737; MTBLC74343; MTBLC74348; MTBLC28610; MTBLC32816; MTBLC16742; MTBLC30852; MTBLC52742; MTBLC17533; MTBLC31991; MTBLC42334; MTBLC17066; MTBLC29069; MTBLC15676; MTBLC16600; MTBLC32805; MTBLC22198; MTBLC30851; MTBLC16530; MTBLC15999; MTBLC15614; MTBLC27823; MTBLC29750; MTBLC30915; MTBLC1427; MTBLC16216; MTBLC18268; MTBLC17140; MTBLC15847; MTBLC15867; MTBLC27891; MTBLC18089; MTBLC17960; MTBLC30797; MTBLC16929; MTBLC15551; MTBLC915; MTBLC18012; MTBLC10565; MTBLC16154; MTBLC28177; MTBLC27625; MTBLC27480; MTBLC30832; MTBLC17764; MTBLC17775; MTBLC15436; MTBLC15908; MTBLC30796; MTBLC30887; MTBLC17802; MTBLC30769; MTBLC18409; MTBLC63934; MTBLC30841; MTBLC18078; MTBLC2024; MTBLC29045; MTBLC8478; MTBLC17415; MTBLC17852; MTBLC17978; MTBLC18042; MTBLC1157; MTBLC74021; MTBLC18426; MTBLC28124; MTBLC50261; MTBLC28695; MTBLC16817; MTBLC74074; MTBLC5810; MTBLC5987; MTBLC74482; MTBLC74324; MTBLC73365; MTBLC5607; MTBLC73992; MTBLC8984; MTBLC73715; MTBLC17506; MTBLC73631; MTBLC73906; MTBLC73510; MTBLC7265; MTBLC73440; MTBLC44976; MTBLC61645; MTBLC74433; MTBLC73433; MTBLC44992; MTBLC74439; MTBLC41865; MTBLC73519; MTBLC61565; MTBLC45564; MTBLC73664; MTBLC10136; MTBLC73665; MTBLC73597; MTBLC73379; MTBLC73640; MTBLC16357; MTBLC74064; MTBLC73407; MTBLC74089; MTBLC5457; MTBLC73509; MTBLC17270; MTBLC20607; MTBLC73752; MTBLC73728; MTBLC9300; MTBLC34837; MTBLC50398; MTBLC73703; MTBLC73753; MTBLC73775; MTBLC74029; MTBLC15892; MTBLC29604; MTBLC845; MTBLC73317; MTBLC73405; MTBLC74407; MTBLC1372; MTBLC74295; MTBLC68846|MTBLC68848; MTBLC74031; MTBLC50519; MTBLC73415; MTBLC73742; MTBLC28724; MTBLC73523; MTBLC34506; MTBLC17515; MTBLC73756; MTBLC5196; MTBLC34372; MTBLC42082; MTBLC9499; MTBLC7567; MTBLC33574; MTBLC32398; MTBLC17710; MTBLC15684; MTBLC17385; MTBLC30745; MTBLC35128; MTBLC2323; MTBLC16583; MTBLC15961; MTBLC371; MTBLC16253; MTBLC17905; MTBLC17405; MTBLC16582; MTBLC30837; MTBLC16992; MTBLC17137; MTBLC17709; MTBLC18427; MTBLC33510; MTBLC30531; MTBLC28376; MTBLC27574; MTBLC16732; MTBLC30849; MTBLC16444; MTBLC16345; MTBLC1438; MTBLC17275; MTBLC15698; MTBLC34498; MTBLC16002; MTBLC18388; MTBLC29864; MTBLC4178; MTBLC16682; MTBLC15637; MTBLC17578; MTBLC74121; MTBLC39567; MTBLC74542; MTBLC23683; MTBLC43580; MTBLC17803; MTBLC10586; MTBLC15741; MTBLC34314; MTBLC73964; MTBLC6951; MTBLC16836; MTBLC521461; MTBLC17409; MTBLC40957; MTBLC16695; MTBLC9008; MTBLC73749; MTBLC74435; MTBLC74357; MTBLC4324; MTBLC73464; MTBLC73961; MTBLC55328; MTBLC73917; MTBLC48031; MTBLC73495; MTBLC9543; MTBLC73455; MTBLC27913; MTBLC73441; MTBLC73460; MTBLC73718; MTBLC34579; MTBLC73941; MTBLC10017; MTBLC15984; MTBLC18129; MTBLC74099; MTBLC28865; MTBLC73713; MTBLC30156; MTBLC16043; MTBLC73967; MTBLC74030; MTBLC73968; MTBLC29600; MTBLC16802; MTBLC1848; MTBLC17691; MTBLC6835; MTBLC73070; MTBLC4676; MTBLC73722; MTBLC73431; MTBLC74501; MTBLC3696; MTBLC27904; MTBLC16525; MTBLC9283; MTBLC34248; MTBLC74452; MTBLC73651; MTBLC73383; MTBLC73408; MTBLC74456; MTBLC72663; MTBLC74092; MTBLC73513; MTBLC3159; MTBLC8883; MTBLC73350; MTBLC74403; MTBLC62193; MTBLC73529; MTBLC16437; MTBLC16948; MTBLC74509; MTBLC74555; MTBLC73657; MTBLC73629; MTBLC3687; MTBLC73707; MTBLC73595; MTBLC73613; MTBLC73650; MTBLC73773; MTBLC74410; MTBLC16471; MTBLC2368; MTBLC73719; MTBLC73782; MTBLC73880; MTBLC73507; MTBLC73642; MTBLC32906; MTBLC73584; MTBLC27905; MTBLC73787; MTBLC28132; MTBLC73778; MTBLC74492; MTBLC73982; MTBLC18025; MTBLC74046; MTBLC73573; MTBLC17322; MTBLC35485; MTBLC73792; MTBLC74330; MTBLC21557</t>
+  </si>
+  <si>
     <t>MTBLS1188</t>
   </si>
   <si>
@@ -487,40 +523,40 @@
     <t>MTBLC15354; MTBLC73858; MTBLC16870; MTBLC34018; MTBLC16002; MTBLC30923; MTBLC89930; MTBLC27404; MTBLC16335; MTBLC16283; MTBLC15354; MTBLC73858; MTBLC16870; MTBLC34018; MTBLC16002; MTBLC30923; MTBLC89930; MTBLC27404; MTBLC16335; MTBLC16283</t>
   </si>
   <si>
-    <t>MTBLS49</t>
-  </si>
-  <si>
-    <t>Metabolomics guides rational development of a simplified cell culture medium for drug screening against Trypanosoma brucei</t>
-  </si>
-  <si>
-    <t>In vitro culture methods underpin many experimental approaches to biology and drug discovery. The modification of established cell culture methods to be more biologically relevant, or to optimise growth, is traditionally a laborious task. Emerging metabolomics technology enables rapid evaluation of intra- and extra-cellular metabolites, and can be applied to the rational development of cell culture medium. In this study, untargeted semi-quantitative, and targeted quantitative, metabolomic analyses of fresh and spent media revealed the major nutritional requirements for growth of bloodstream-form Trypanosoma brucei. The standard culture medium (HMI11) contained unnecessarily high concentrations of 32 nutrients that were subsequently removed to more closely resemble concentrations normally found in blood. Our new minimal medium (CMM) supports in vitro growth equivalent to HMI11, and causes no significant perturbation of metabolite levels for 94% of the detected metabolome (&lt; 3-fold change; a = 0.05). Importantly, improved sensitivity was observed for drug activity studies in whole cell phenotypic screens, and in metabolomics mode of action assays. 400-fold decreases in IC50 were observed for pentamidine and methotrexate, suggesting inhibition of activity by nutrients present in HMI11. CMM is suitable for routine cell culture and offers important advantages for metabolomics studies and drug activity screening.</t>
-  </si>
-  <si>
-    <t>drug screening/evaluation; culture medium; liquid chromatography-mass spectrometry; untargeted metabolites</t>
-  </si>
-  <si>
-    <t>Metabolomics guides rational development of a simplified cell culture medium for drug screening against Trypanosoma brucei. 10.1128/aac.00044-13. PMID:23571546</t>
-  </si>
-  <si>
-    <t>Bloodstream-form Trypanosoma brucei brucei (s427) were cultured in vitro in either HMI11 (Gibco), CMM or modified media with 10% FCS Gold (PAA). Cell culture grade (or high purity) D-glucose, L-cysteine, L-glutamine and all other medium components were purchased from Sigma Aldrich. 5 ml cultures were maintained in 25 ml vented flasks (Corning) at 37 C with 5% CO2. Cultures were grown to a maximum density of 4 x 106 cells/ml and sub-cultured by 1 in 100 or 1 in 1000 dilution, every 2 or 3 days, respectively. Cell counts were obtained by haemocytometer (Neubauer).</t>
-  </si>
-  <si>
-    <t>Metabolite extraction was performed according to previously described methods [1][2]. 25 ml of cell culture was quenched by rapid cooling to 4 C in a dry ice/ethanol bath. Cell pellets were obtained by centrifugation at 1250 x g for 10 minutes, and 5 l spent media was removed and extracted by addition of 100 l chloroform/methanol/water (1:3:1). The remaining cell pellet was washed with 1 ml PBS, and the washed pellet (5  107 cells) was extracted with 100 l chloroform/methanol/water (1:3:1) by mixing for 1 h at 4 C, before centrifugation to remove precipitate. The resulting metabolite solution was stored at -80 C until analysis by liquid chromatography-mass spectrometry (LC-MS). Comparative data from HMI11 and CMM cell pellets and spent media are from 5 independent biological replicates.&lt;/p&gt;Ref:&lt;/br&gt;[1] Saunders EC, Ng WW, Chambers JM, Ng M, Naderer T, Kramer JO, Likic VA, McConville MJ. 2011. Isotopomer profiling of Leishmania mexicana promastigotes reveals important roles for succinate fermentation and aspartate uptake in tricarboxylic acid cycle (TCA) anaplerosis, glutamate synthesis, and growth. J. Biol. Chem. 286:2770627717. doi:10.1074/jbc.M110.213553. PMID:21636575&lt;/br&gt;[2] t'Kindt R, Jankevics A, Scheltema RA, Zheng L, Watson DG, Dujardin JC, Breitling R, Coombs GH, Decuypere S. 2010. Towards an unbiased metabolic profiling of protozoan parasites: optimisation of a Leishmania sampling protocol for HILIC-Orbitrap analysis. Anal. Bioanal. Chem. 398:20592069. doi:10.1007/s00216-010-4139-0. PMID:20824428&lt;/br&gt;</t>
-  </si>
-  <si>
-    <t>The LC separation was performed using hydrophilic interaction chromatography with a ZIC-HILIC 150 mm x 4.6 mm, 5 m column (Merck Sequant), operated by a Dionex UltiMate liquid chromatography system (Dionex, Camberley, Surrey), and coupled to a FAMOS autosampler. The LC mobile phase was a linear gradient from 80% B to 20% B over 30 min, followed by an 8 min wash with 5% B, and 8 min re-equilibration with 80% B, where solvent B is 0.08% formic acid in acetonitrile and solvent A is 0.1% formic acid in water. The flow rate was 300 l/min, column temperature 20 C, injection volume 10 l, and samples were maintained at 4 C.</t>
-  </si>
-  <si>
-    <t>The mass spectrometry was performed using an Orbitrap Exactive (Thermo Fisher Scientific, Hemel Hempstead, U.K.) with a HESI 2 probe. The spectrometer was operated in polarity switching mode, with the following settings: resolution 50,000, AGC 1 x 106, m/z range 701400, sheath gas 40, auxiliary gas 20, sweep gas 1, probe temperature 275 C, and capillary temperature 250 C. For positive mode ionization: source voltage +4 kV, capillary voltage +50 V, tube voltage +70 V, skimmer voltage +20 V. For negative mode ionization: source voltage -3.5 kV, capillary voltage -50 V, tube voltage -70 V, skimmer voltage -20 V. Mass calibration was performed for each polarity immediately before each analysis batch, within 48 h for all samples. The calibration mass range was extended to cover small metabolites by inclusion of low-mass contaminants with the standard Thermo calmix masses (below m/z 1400), acetonitrile dimer for positive ion electrospray ionization (PIESI) mode (m/z 83.0604) and C3H5O3 for negative ion electrospray ionization (NIESI) mode (m/z 89.0244). To enhance calibration stability, lock-mass correction was also applied to each analytical run using these ubiquitous low-mass contaminants.</t>
-  </si>
-  <si>
-    <t>Peak-picking by XCMS - http://metlin.scripps.edu/xcms/ (Centwave), peak matching and annotation by mzMatch, and noise filtering and metabolite identification by IDEOM (http://mzmatch.sourceforge.net/ideom.php), using the default parameters.</t>
-  </si>
-  <si>
-    <t>Metabolite identification is based on accurate mass and predicted retention time, which is accepted as a level 3 standard of identification by the Metabolomics Standards Initiative (MSI), but should be considered as a putative identification. Retention time was verified by authentic standards for the major HMI11 components and other metabolites where possible.</t>
-  </si>
-  <si>
-    <t>MTBLC16235; MTBLC17754; MTBLC17748; MTBLC17712; MTBLC16977; MTBLC17154; MTBLC41531|MTBLC45658; MTBLC16870; MTBLC17509; MTBLC16335; MTBLC17361; MTBLC27596; MTBLC15354; MTBLC17053; MTBLC16467; MTBLC17196; MTBLC17368; MTBLC18385; MTBLC16015; MTBLC15971; MTBLC16704; MTBLC17015; MTBLC17895; MTBLC17115; MTBLC15603; MTBLC17203; MTBLC15729; MTBLC16414; MTBLC17515; MTBLC48950; MTBLC16643; MTBLC18050; MTBLC16349; MTBLC18019; MTBLC16857; MTBLC47977; MTBLC17295; MTBLC17568; MTBLC15940; MTBLC17561; MTBLC17596; MTBLC16750; MTBLC16610; MTBLC16283; MTBLC16319; MTBLC17405; MTBLC18062; MTBLC6151; MTBLC73949; MTBLC17821; MTBLC28474; MTBLC16530; MTBLC16410; MTBLC1606|MTBLC70966|MTBLC74763|MTBLC73087|MTBLC74765|MTBLC74766; MTBLC16671; MTBLC17016; MTBLC16570; MTBLC27248; MTBLC7274; MTBLC27470; MTBLC17232; MTBLC15946; MTBLC28712; MTBLC17884; MTBLC17311; MTBLC27574; MTBLC15428; MTBLC15891; MTBLC37023; MTBLC2198; MTBLC7916; MTBLC30913; MTBLC17374; MTBLC27676; MTBLC18123; MTBLC16946; MTBLC9533; MTBLC16828; MTBLC15887; MTBLC15727; MTBLC48005; MTBLC28123; MTBLC17562; MTBLC16919; MTBLC16668; MTBLC20000; MTBLC16463; MTBLC17752; MTBLC17381; MTBLC17780; MTBLC27713; MTBLC41218; MTBLC51824; MTBLC15420; MTBLC61521; MTBLC43997; MTBLC73960; MTBLC7858; MTBLC73291; MTBLC73292; MTBLC73881; MTBLC73293; MTBLC74085; MTBLC73368; MTBLC17920; MTBLC29136; MTBLC73436; MTBLC17417; MTBLC15870; MTBLC73647; MTBLC17342; MTBLC5277; MTBLC74048; MTBLC73605; MTBLC27578; MTBLC73758; MTBLC73386; MTBLC16437; MTBLC15968; MTBLC73514; MTBLC15997; MTBLC32571; MTBLC74111; MTBLC74321; MTBLC73450; MTBLC28182; MTBLC73600; MTBLC73654; MTBLC73589; MTBLC73700; MTBLC7728; MTBLC6329; MTBLC5649; MTBLC2600; MTBLC73445; MTBLC6988; MTBLC55357; MTBLC73959; MTBLC73581; MTBLC73313; MTBLC45530; MTBLC73527; MTBLC50395; MTBLC28867; MTBLC73422; MTBLC11060; MTBLC73653; MTBLC73331; MTBLC73604; MTBLC27747; MTBLC17929; MTBLC73426; MTBLC73598; MTBLC74135; MTBLC73447; MTBLC73521; MTBLC74521; MTBLC73574; MTBLC73350; MTBLC73671; MTBLC73518; MTBLC73703; MTBLC74079; MTBLC756; MTBLC34237; MTBLC73525; MTBLC5583; MTBLC73704; MTBLC73606; MTBLC73513; MTBLC73414; MTBLC3222; MTBLC15336; MTBLC34792; MTBLC73505; MTBLC29563; MTBLC74516; MTBLC73903; MTBLC74129; MTBLC73617; MTBLC73366; MTBLC73571; MTBLC6198; MTBLC116314; MTBLC73421; MTBLC1391; MTBLC74104; MTBLC73349; MTBLC73485; MTBLC73506; MTBLC34726; MTBLC73353; MTBLC73738; MTBLC9173; MTBLC73601; MTBLC73926; MTBLC74438; MTBLC17604; MTBLC34019; MTBLC73394; MTBLC84933; MTBLC2881; MTBLC16968; MTBLC42025; MTBLC73526; MTBLC73397; MTBLC73663; MTBLC73607; MTBLC73411; MTBLC74110; MTBLC73381; MTBLC73318; MTBLC74024; MTBLC15783; MTBLC73528; MTBLC73583; MTBLC74112; MTBLC73685; MTBLC73515; MTBLC73736; MTBLC73529; MTBLC37251; MTBLC73530; MTBLC73585; MTBLC73645; MTBLC17195; MTBLC31071; MTBLC30820; MTBLC73646; MTBLC73632; MTBLC73990; MTBLC74077; MTBLC73579; MTBLC72723; MTBLC35019; MTBLC73444; MTBLC2814; MTBLC73437; MTBLC73580; MTBLC73695; MTBLC73596; MTBLC45171; MTBLC73512; MTBLC73531; MTBLC3206; MTBLC64486; MTBLC74027; MTBLC73634; MTBLC11946; MTBLC73565; MTBLC74533; MTBLC73608; MTBLC73520; MTBLC73794; MTBLC65842; MTBLC74562; MTBLC73566; MTBLC73861; MTBLC73363; MTBLC73443; MTBLC73425; MTBLC73721; MTBLC74044; MTBLC73489; MTBLC64288; MTBLC47914; MTBLC27626; MTBLC73701; MTBLC73858; MTBLC35050; MTBLC44164; MTBLC57885; MTBLC64489; MTBLC73850; MTBLC73869; MTBLC74344; MTBLC73873; MTBLC6253; MTBLC63934; MTBLC36575; MTBLC506227; MTBLC18357; MTBLC17924; MTBLC18397; MTBLC28297; MTBLC28220; MTBLC17697; MTBLC27413; MTBLC27931; MTBLC27592; MTBLC15728; MTBLC28621; MTBLC28004; MTBLC28790; MTBLC18107; MTBLC15760; MTBLC18032; MTBLC17213; MTBLC17724; MTBLC49015; MTBLC28716; MTBLC16576; MTBLC17957; MTBLC15805; MTBLC18373; MTBLC33094; MTBLC17862; MTBLC16742; MTBLC16026; MTBLC15675; MTBLC16660; MTBLC17755; MTBLC15743; MTBLC17645; MTBLC27468; MTBLC17620; MTBLC17294; MTBLC16288; MTBLC10329; MTBLC73780; MTBLC74125; MTBLC73522; MTBLC61346; MTBLC73459; MTBLC338412; MTBLC73490; MTBLC73737; MTBLC73454; MTBLC74323; MTBLC73694; MTBLC1604; MTBLC74049; MTBLC73710; MTBLC74484; MTBLC29010; MTBLC15426; MTBLC74490; MTBLC16020; MTBLC73800; MTBLC73362; MTBLC73643; MTBLC21374; MTBLC73612; MTBLC50601; MTBLC73439; MTBLC73488; MTBLC27419; MTBLC73868; MTBLC74487; MTBLC73865; MTBLC73644; MTBLC73457; MTBLC73696; MTBLC1237; MTBLC74517; MTBLC73740; MTBLC73434; MTBLC17303; MTBLC73393; MTBLC73582; MTBLC73024; MTBLC73384; MTBLC64305; MTBLC73438; MTBLC73344; MTBLC73572; MTBLC73496; MTBLC17702; MTBLC74532; MTBLC15956; MTBLC39585; MTBLC6851; MTBLC73419; MTBLC73448; MTBLC1643; MTBLC73699; MTBLC73461; MTBLC73446; MTBLC73733; MTBLC32963; MTBLC17310; MTBLC73465; MTBLC16531; MTBLC74092; MTBLC73594; MTBLC74404; MTBLC73889; MTBLC73633; MTBLC73563; MTBLC73627; MTBLC73399; MTBLC73412; MTBLC73609; MTBLC30270; MTBLC34900; MTBLC73323; MTBLC73409; MTBLC15424; MTBLC17618; MTBLC73661; MTBLC73970; MTBLC73882; MTBLC5724; MTBLC73981; MTBLC73428; MTBLC73516; MTBLC73402; MTBLC73577; MTBLC73613; MTBLC8067; MTBLC73270; MTBLC17443; MTBLC73329; MTBLC73591; MTBLC73502; MTBLC73979; MTBLC73401; MTBLC73372; MTBLC73341; MTBLC5712; MTBLC73026; MTBLC74430; MTBLC24109; MTBLC73351; MTBLC73611; MTBLC7676; MTBLC73487; MTBLC5858; MTBLC74479; MTBLC73635; MTBLC73499; MTBLC45757; MTBLC73524; MTBLC73342; MTBLC73578; MTBLC73789; MTBLC16357; MTBLC73614; MTBLC16737; MTBLC73517; MTBLC74535; MTBLC45564; MTBLC73705; MTBLC73355; MTBLC7061; MTBLC73326; MTBLC16244; MTBLC10018; MTBLC73610; MTBLC73652; MTBLC73330; MTBLC73376; MTBLC74101; MTBLC7621; MTBLC6631; MTBLC73456; MTBLC73798; MTBLC84834; MTBLC73725; MTBLC73739; MTBLC21557; MTBLC73616; MTBLC74441; MTBLC73660; MTBLC17495; MTBLC73406; MTBLC55458; MTBLC73667; MTBLC73347; MTBLC73692; MTBLC17927; MTBLC73375; MTBLC74475; MTBLC50845; MTBLC73910; MTBLC73430; MTBLC73462; MTBLC73892; MTBLC73404; MTBLC73497; MTBLC5390; MTBLC73697; MTBLC73636; MTBLC73508; MTBLC74437; MTBLC73658; MTBLC73324; MTBLC74123; MTBLC73427; MTBLC73498; MTBLC18255; MTBLC73463; MTBLC73429; MTBLC73562; MTBLC73348; MTBLC73395; MTBLC73494; MTBLC74303; MTBLC45571; MTBLC4117; MTBLC74102; MTBLC73923; MTBLC73391; MTBLC73929; MTBLC73455; MTBLC73659; MTBLC73648; MTBLC73564; MTBLC73392; MTBLC17328; MTBLC73493; MTBLC35280; MTBLC6645; MTBLC132188; MTBLC73503; MTBLC74107; MTBLC73561; MTBLC73484; MTBLC73451; MTBLC73501; MTBLC73711; MTBLC73698; MTBLC16227; MTBLC73655; MTBLC30821; MTBLC73900; MTBLC73615; MTBLC15425; MTBLC73492; MTBLC73314; MTBLC73741; MTBLC73649; MTBLC73927; MTBLC73894; MTBLC73630; MTBLC73435; MTBLC46807; MTBLC73691; MTBLC73638; MTBLC73491; MTBLC73656; MTBLC16213; MTBLC73568; MTBLC17394; MTBLC73382; MTBLC73424; MTBLC73321; MTBLC73628; MTBLC73590; MTBLC73637; MTBLC5757; MTBLC73639; MTBLC73666; MTBLC73575; MTBLC73570; MTBLC70744; MTBLC74096; MTBLC73567; MTBLC61138; MTBLC16533; MTBLC73576; MTBLC73662; MTBLC73569; MTBLC73885; MTBLC73345; MTBLC73797; MTBLC73875; MTBLC73793; MTBLC73751; MTBLC73377; MTBLC16708; MTBLC74356; MTBLC73723; MTBLC73795; MTBLC16027; MTBLC73851; MTBLC73854; MTBLC72737; MTBLC74343; MTBLC74348; MTBLC28610; MTBLC32816; MTBLC16742; MTBLC30852; MTBLC52742; MTBLC17533; MTBLC31991; MTBLC42334; MTBLC17066; MTBLC29069; MTBLC15676; MTBLC16600; MTBLC32805; MTBLC22198; MTBLC30851; MTBLC16530; MTBLC15999; MTBLC15614; MTBLC27823; MTBLC29750; MTBLC30915; MTBLC1427; MTBLC16216; MTBLC18268; MTBLC17140; MTBLC15847; MTBLC15867; MTBLC27891; MTBLC18089; MTBLC17960; MTBLC30797; MTBLC16929; MTBLC15551; MTBLC915; MTBLC18012; MTBLC10565; MTBLC16154; MTBLC28177; MTBLC27625; MTBLC27480; MTBLC30832; MTBLC17764; MTBLC17775; MTBLC15436; MTBLC15908; MTBLC30796; MTBLC30887; MTBLC17802; MTBLC30769; MTBLC18409; MTBLC63934; MTBLC30841; MTBLC18078; MTBLC2024; MTBLC29045; MTBLC8478; MTBLC17415; MTBLC17852; MTBLC17978; MTBLC18042; MTBLC1157; MTBLC74021; MTBLC18426; MTBLC28124; MTBLC50261; MTBLC28695; MTBLC16817; MTBLC74074; MTBLC5810; MTBLC5987; MTBLC74482; MTBLC74324; MTBLC73365; MTBLC5607; MTBLC73992; MTBLC8984; MTBLC73715; MTBLC17506; MTBLC73631; MTBLC73906; MTBLC73510; MTBLC7265; MTBLC73440; MTBLC44976; MTBLC61645; MTBLC74433; MTBLC73433; MTBLC44992; MTBLC74439; MTBLC41865; MTBLC73519; MTBLC61565; MTBLC45564; MTBLC73664; MTBLC10136; MTBLC73665; MTBLC73597; MTBLC73379; MTBLC73640; MTBLC16357; MTBLC74064; MTBLC73407; MTBLC74089; MTBLC5457; MTBLC73509; MTBLC17270; MTBLC20607; MTBLC73752; MTBLC73728; MTBLC9300; MTBLC34837; MTBLC50398; MTBLC73703; MTBLC73753; MTBLC73775; MTBLC74029; MTBLC15892; MTBLC29604; MTBLC845; MTBLC73317; MTBLC73405; MTBLC74407; MTBLC1372; MTBLC74295; MTBLC68846|MTBLC68848; MTBLC74031; MTBLC50519; MTBLC73415; MTBLC73742; MTBLC28724; MTBLC73523; MTBLC34506; MTBLC17515; MTBLC73756; MTBLC5196; MTBLC34372; MTBLC42082; MTBLC9499; MTBLC7567; MTBLC33574; MTBLC32398; MTBLC17710; MTBLC15684; MTBLC17385; MTBLC30745; MTBLC35128; MTBLC2323; MTBLC16583; MTBLC15961; MTBLC371; MTBLC16253; MTBLC17905; MTBLC17405; MTBLC16582; MTBLC30837; MTBLC16992; MTBLC17137; MTBLC17709; MTBLC18427; MTBLC33510; MTBLC30531; MTBLC28376; MTBLC27574; MTBLC16732; MTBLC30849; MTBLC16444; MTBLC16345; MTBLC1438; MTBLC17275; MTBLC15698; MTBLC34498; MTBLC16002; MTBLC18388; MTBLC29864; MTBLC4178; MTBLC16682; MTBLC15637; MTBLC17578; MTBLC74121; MTBLC39567; MTBLC74542; MTBLC23683; MTBLC43580; MTBLC17803; MTBLC10586; MTBLC15741; MTBLC34314; MTBLC73964; MTBLC6951; MTBLC16836; MTBLC521461; MTBLC17409; MTBLC40957; MTBLC16695; MTBLC9008; MTBLC73749; MTBLC74435; MTBLC74357; MTBLC4324; MTBLC73464; MTBLC73961; MTBLC55328; MTBLC73917; MTBLC48031; MTBLC73495; MTBLC9543; MTBLC73455; MTBLC27913; MTBLC73441; MTBLC73460; MTBLC73718; MTBLC34579; MTBLC73941; MTBLC10017; MTBLC15984; MTBLC18129; MTBLC74099; MTBLC28865; MTBLC73713; MTBLC30156; MTBLC16043; MTBLC73967; MTBLC74030; MTBLC73968; MTBLC29600; MTBLC16802; MTBLC1848; MTBLC17691; MTBLC6835; MTBLC73070; MTBLC4676; MTBLC73722; MTBLC73431; MTBLC74501; MTBLC3696; MTBLC27904; MTBLC16525; MTBLC9283; MTBLC34248; MTBLC74452; MTBLC73651; MTBLC73383; MTBLC73408; MTBLC74456; MTBLC72663; MTBLC74092; MTBLC73513; MTBLC3159; MTBLC8883; MTBLC73350; MTBLC74403; MTBLC62193; MTBLC73529; MTBLC16437; MTBLC16948; MTBLC74509; MTBLC74555; MTBLC73657; MTBLC73629; MTBLC3687; MTBLC73707; MTBLC73595; MTBLC73613; MTBLC73650; MTBLC73773; MTBLC74410; MTBLC16471; MTBLC2368; MTBLC73719; MTBLC73782; MTBLC73880; MTBLC73507; MTBLC73642; MTBLC32906; MTBLC73584; MTBLC27905; MTBLC73787; MTBLC28132; MTBLC73778; MTBLC74492; MTBLC73982; MTBLC18025; MTBLC74046; MTBLC73573; MTBLC17322; MTBLC35485; MTBLC73792; MTBLC74330; MTBLC21557</t>
+    <t>MTBLS804</t>
+  </si>
+  <si>
+    <t>Rapid UHPLC-MS metabolite profiling and phenotypic assays reveal genotypic impacts of nitrogen supplementation in oats</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;&lt;b&gt;INTRODUCTION:&lt;/b&gt; Oats (Avena sativa L.) are a whole grain cereal recognised for their health benefits and which are cultivated largely in temperate regions providing both a source of food for humans and animals, as well as being used in cosmetics and as a potential treatment for a number of diseases. Oats are known as being a cereal source high in dietary fibre (e.g. beta-glucans), as well as being high in antioxidants, minerals and vitamins. Recently, oats have been gaining increased global attention due to their large number of beneficial health effects. Consumption of oats has been proven to lower blood LDL cholesterol levels and blood pressure, thus reducing the risk of heart disease, as well as reducing blood-sugar and insulin levels.&lt;/div&gt;&lt;div&gt;&lt;b&gt;OBJECTIVES:&lt;/b&gt; Oats are seen as a low input cereal. Current agricultural guidelines on nitrogen application are believed to be suboptimal and only consider the effect of nitrogen on grain yield. It is important to understand the role of both variety and of crop management in determining nutritional quality of oats. In this study the response of yield, grain quality and grain metabolites to increasing nitrogen application to levels greater than current guidelines were investigated.&lt;/div&gt;&lt;div&gt;&lt;b&gt;METHODS:&lt;/b&gt; Four winter oat varieties (Mascani, Tardis, Balado and Gerald) were grown in a replicated nitrogen response trial consisting of a no added nitrogen control and four added nitrogen treatments between 50 and 200&amp;nbsp;kg&amp;nbsp;N&amp;nbsp;ha-1 in a randomised split-plot design. Grain yield, milling quality traits, beta-glucan, total protein and oil content were assessed. The de-hulled oats (groats) were also subjected to a rapid Ultra High Performance Liquid Chromatography-Mass Spectrometry (UHPLC-MS) metabolomic screening approach.&lt;/div&gt;&lt;div&gt;&lt;b&gt;RESULTS:&lt;/b&gt; Application of nitrogen had a significant effect on grain yield but there was no significant difference between the response of the four varieties. Grain quality traits however displayed significant differences both between varieties and nitrogen application level. beta-glucan content significantly increased with nitrogen application. The UHPLC-MS approach has provided a rapid, sub 15&amp;nbsp;min per sample, metabolite profiling method that is repeatable and appropriate for the screening of large numbers of cereal samples. The method captured a wide range of compounds, inclusive of primary metabolites such as the amino acids, organic acids, vitamins and lipids, as well as a number of key secondary metabolites, including the avenanthramides, caffeic acid, and sinapic acid and its derivatives and was able to identify distinct metabolic phenotypes for the varieties studied. Amino acid metabolism was massively upregulated by nitrogen supplementation as were total protein levels, whilst the levels of organic acids were decreased, likely due to them acting as a carbon skeleton source. Several TCA cycle intermediates were also impacted, potentially indicating increased TCA cycle turn over, thus providing the plant with a source of energy and reductant power to aid elevated nitrogen assimilation. Elevated nitrogen availability was also directed towards the increased production of nitrogen containing phospholipids. A number of both positive and negative impacts on the metabolism of phenolic compounds that have influence upon the health beneficial value of oats and their products were also observed.&lt;/div&gt;&lt;div&gt;&lt;b&gt;CONCLUSIONS:&lt;/b&gt; Although the developed method has broad applicability as a rapid screening method or a rapid metabolite profiling method and in this study has provided valuable metabolic insights, it still must be considered that much greater confidence in metabolite identification, as well as quantitative precision, will be gained by the application of higher resolution chromatography methods, although at a large expense to sample throughput. Follow up studies will apply higher resolution GC (gas chromatography) and LC (reversed phase and HILIC) approaches, oats will be also analysed from across multiple growth locations and growth seasons, effectively providing a cross validation for the results obtained within this preliminary study. It will also be fascinating to perform more controlled experiments with sampling of green tissues, as well as oat grains, throughout the plants and grains development, to reveal greater insight of carbon and nitrogen metabolism balance, as well as resource partitioning into lipid and secondary metabolism.&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>ultra-performance liquid chromatography-mass spectrometry; nitrogen molecular entity; bio-variety; grain quality trait; beta-D-glucan; amino acid; Lipidomics; Avenanthramides</t>
+  </si>
+  <si>
+    <t>Rapid UHPLC-MS metabolite profiling and phenotypic assays reveal genotypic impacts of nitrogen supplementation in oats. 10.1007/s11306-019-1501-x. PMID:30868357</t>
+  </si>
+  <si>
+    <t>The trial was conducted at Lydbury North, Shropshire, UK (latitude 52.45, longitude 2.94, medium soil type) in a split plot design with 3 replicates using 5 levels of nitrogen application (main plot treatment) and 4 commercially available winter oat varieties (sub-plot treatment) from the Aberystwyth University winter oat breeding programme. These included 2 of the most widely grown winter oat varieties in the UK over the last 20 years, Gerald and Mascani (AHDB 2015). 3 varieties were of conventional height (Mascani, Gerald and Tardis) and the fourth was a dwarf variety (Balado). Plots (1.8 x 6 m) were sown on the 9th October 2013 at a sowing rate of 300 seeds/m^2 and harvested on the 7th August 2014 using a small plot combine. Fungicides and weed control followed standard practise for winter oats including the use of a plant growth regulator (Cycocel 5C). Soils were sampled to a depth of 90 cm in early spring and residual soil nitrogen was determined to be 58 kg N/ha. Nitrogen (ammonium nitrate) doses were split between 3 different developmental stages in early to late spring as indicated in Table S1 in the paper associated with this study, to provide 5 final doses: Control, no applied nitrogen; level 1, 50 kg N/ha applied; level 2, 100 kg N/ha applied; level 3, 150 kg N/ha applied; level 4, 200 kg N/ha applied. The 17th April application date corresponded to growth stage 31 (early stem elongation, Zadoks et al. 1974). Prior to harvest the number of fertile shoots (panicles) per m2 were counted and plant heights from soil surface to panicle tip measured.&lt;/br&gt;&lt;/br&gt;Ref:&lt;/br&gt;[1] Zadoks JC, Chang TT, Konzak CF. Decimal code for growth stages of cereals. Weed Research. 1974;14:415421. doi:10.1111/j.1365-3180.1974.tb01084.x&lt;/br&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;The dehulled oat samples were first homogenised using a Retsch Cyclone Mill-Twister with the following settings: speed 12,000 rpm/min; 62 ms peripheral rotor speed; 1 mm sieve; 1 min cycle. 100 mg  2 mg FW of oats were weighed into 2 ml safe-lock Eppendorf microcentrifuge tubes, 1.5 ml of extraction buffer (10 uM reserpine and 10 M morin in 75% methanol 24.9% water 0.1% formic acid) was added, the sample was vortexed for 15 s, ultrasonicated for 15 min with an Elma S40 ultrasonicator, vortexed for 15 s, agitated on an IKA VXR basic vibrax fitted with the VX2E.n Eppendorf tube adapter set on speed 8 for 30 min, and centrifuged for 10 min at 3 C and 18,407 x g with an Eppendorf 5424R (rotor FA-45-24-11). The extract supernatants were next filtered with 0.45um PTFE filter vials (Thomson single step) and transferred to 2 ml HPLC vials with pre-slit caps (Thermo-Fisher, Chromacol 2SVW and 9-SCK(B)-ST1 X, respectively). A quality assurance (QA) sample was prepared by mixing equal quantities of each sample extract, thus providing a QA sample representative of the average of the entire sample set. A number of representative samples were also extracted and analysed in triplicate (denoted as a, b, and c, within the sample number) to serve as reference samples to define extraction and analytical repeatability. The samples were stored in the HPLC autosampler at 10 C and analysed within 72 h of extraction in positive and negative electrospray ionisation (ESI) modes. The ESI source spray cone and ion tube were cleaned between running the sample set in each ionisation mode.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>UHPLC separations were performed with a Thermo Accela 600 HPLC system coupled with an Accela PDA detector (Thermo-Fisher Ltd. U.K). The HPLC was operated at a flow rate of 400 l/min, the column and guard column (Thermo Hypersil Gold C18 50 x 2.1 mm, 1.9 m particle size; Hypersil Gold C18 Guard 10 x 2.1 mm, 3 m particle size; Thermo Universal Uniguard guard holder 2.1/3 mm) were maintained at a temperature of 40 C. The solvent A, HPLC grade water, and solvent B, HPLC grade acetonitrile, were acidified with 0.1% [v/v] MS grade formic acid. Prior to sample analysis a new UHPLC column and guard column were conditioned with solvents A and B for a minimum of 40 min at a flow rate of 400 l/min. A sample injection volume of 5 l was employed in full-loop mode. The gradient programme was as follows: hold 5% B 01 min, 5100% B 18 min, hold 100% B 811 min, 1005% B 1111.1 min, hold 5% B 11.115 min. Autosampler syringe and line washes were performed with 80% HPLC grade acetonitrile 20% HPLC grade water. The UHPLC column eluent was first monitored by the Accela PDA detector where spectra were collected in wavelength/absorbance mode from 200 to 600 nm with a filter bandwidth and wavelength step of 1 nm, the filter rise time was 1 s, the sample rate was 10 Hz. Additionally three channel set points were employed, Channel A 280 nm, Channel B 365 nm, Channel C 520 nm, with a bandwidth of 9 nm and a sample rate of 10 Hz.</t>
+  </si>
+  <si>
+    <t>The PDA detector eluent was next transfered to a Thermo LTQ-Orbitrap XL mass spectrometry system operated under Xcalibur software (Thermo-Fisher Ltd. UK). Mass spectra were primarilly collected in full scan mode (m/z 1001200) at a mass resolution of 30,000 (FWHM defined at m/z 400) within the FT detector for all samples. An additional method was applied to obtain ion trees by performing data-dependent analysis (DDA) MS2 on the top 3 most intense ions for the mixed QA sample[1]. The DDA method applied a primary full scan event within the FT, followed by a secondary scan event within the LTQ-IT to collect MS2 CID fragmentation spectra for the top 3 most intense ions as defined within the preliminary full MS scan. Helium was applied as a collision gas for CID at a normalised collision energy of 45%, a trapping window width of 2 ( 1) m/z was applied, an activation time of 30 ms and activation Q of 0.25 were applied, only singly charged ions were selected for DDA, isotopic ions were also excluded. The preliminary full scan event within the FT generated profile mode data, whereas the LTQ-IT MS2 data were collected in 'centroid' mode.&lt;/br&gt;&lt;/br&gt;A scan speed of 0.1 s and 0.4 s were applied in the LTQ-IT and FT-MS respectively. The Automatic Gain Control was set to 1 x 10^5 and 1 x 10^6 for the LTQ-IT and FT-MS respectively. Prior to the analytical run the LTQ-IT and FT-MS were tuned to optimise conditions for the detection of ions in the mid detection range of m/z 1001200, as well as being calibrated with the manufacturers recommended calibration mixture and procedures. The ESI conditions were optimised to allow efficient ionisation and ion transmission whilst limiting insource fragmentation. The following settings were applied to ESI: Spray voltage 3.5 kV (ESI) and +4.5 kV (ESI+); Sheath gas 60; Auxiliary gas 30; Capillary voltage 35 V (ESI)+35 V (ESI+); Tube lens voltage 100 V (ESI) and +100 V (ESI+); Capillary temperature 280 C; ESI probe temperature 100 C.&lt;/br&gt;&lt;/br&gt;The samples were analysed in a completely randomised order as 2 independent analytical blocks, each of approximately 100 injections, respective of ESI positive and ESI negative polarities. For each analytical block, initially 8 injections of QA sample were performed for LC-MS system conditioning, after which 3 further injections of QA sample were performed, followed by 6 injections of experimental samples and a further QA injection. This was repeated until all samples were analysed, finally the analytical block was concluded with a further 3 QA injections. A control blank sample was analysed at the start and end of the analytical block, thus providing a measure of the sample background and also a measure of compound carry over resulting from dirtying of the ESI source. Each analytical block was finally concluded by collection of the DDA MS2 profiles for the QA sample.&lt;/br&gt;&lt;/br&gt;Ref:&lt;/br&gt;[1] Mullard G, Allwood JW, Webber RJM, Brown M, Begley P, Hollywood KA, Jones M, Unwin RD, Bishop PN, Cooper GJS, Dunn WB. A new strategy for MS/MS data acquisition applying multiple data dependent experiments on Orbitrap mass spectrometers in non-targeted metabolomics applications. Metabolomics. 2015;11(5):10681080. doi:10.1007/s11306-014-0763-6.&lt;/br&gt;</t>
+  </si>
+  <si>
+    <t>The UHPLC-PDA-MS raw data profiles were first converted into an MZML centroid format within the Proteowizard (http://proteowizard.sourceforge.net/) MSConvert software package. Each MZML based three-dimensional data matrix (intensityxm/zxtime1 per sample) was converted (or deconvolved) into a vector of peak responses, where a peak response is defined as the sum of intensities over a window of specified mass and time range (e.g. m/z = 102.1  0.01 and time = 130  10 s). In this experiment the deconvolution was performed using the freely available XCMS online package (https://xcmsonline.scripps.edu/). XCMS online was operated with the following parameter set points: Feature detection; methodCentWave; mass error 5 ppm, minimum and maximum peak width 5 and 30 s respectively, mzdiff 0.01, S/N threshold 10, integration method 1, prefilter peaks 3, prefilter intensity 40,000, noise filter 100,000: RT correction; method  Obiwarp, profstep 1: Alignment; minfrac 0.5, mz width 0.015, bw 5, min samp 1, max samp 100: Annotation; Search for isotopes + adducts, mz absolute error 0.015, ppm error 5.&lt;/br&gt;&lt;/br&gt;The XCMS deconvolution results in the production of a Microsoft Excel based XY matrix containing the paired RT and m/z of each feature, along with the peak area in each profiled sample, and where provided, adduct and isotope annotations for each m/z. The XY matrix was trimmed of peaks that eluted within the first 0.3 min and final 4 min of chromatography (the void and equilibration periods), as well as removal of peaks that were dominant within blank sample extracts (more than 2 more intense than the peaks highest intensity within a biological sample)[1]. &lt;/br&gt;&lt;/br&gt;Ref:&lt;/br&gt;[1] Di Guida R, Engel J, Allwood JW, Weber RJ, Jones MR, Sommer U, Viant MR, Dunn WB. Non-targeted UHPLC-MS metabolomic data processing methods: a comparative investigation of normalisation, missing value imputation, transformation and scaling. Metabolomics. 2016;12:93. Epub 2016 Apr 15. doi:10.1007/s11306-016-1030-9. PMID:27123000&lt;/br&gt;</t>
+  </si>
+  <si>
+    <t>Applying a set of workflows known as PutMedID which are operated within the Taverna Workbench 1.7.2 software package[1]-[3], peak to peak Pearson correlations were first calculated within a 5 s moving RT window, peaks that show a high level of Pearson correlation (greater than 0.8) within the same RT window were grouped as m/z features that were likely associated with the same compound (i.e. an m/z group). As a second step, accurate mass differences between m/z within each peak group were calculated to allow the annotation of the parent m/z from isotopic and adduct ions. Consensus was drawn between the two methods of peak annotation performed within XCMS online and PutMedID. Once the parent ion, adducts and isotopes are annotated within each peak group, the neutral accurate mass is calculated for each ion (5 ppm mass error) and in turn matched to possible molecular formula(s), which are then matched to metabolite name(s). Molecular formula and metabolite matching were based upon a library of known plant metabolites obtained from the Plant Metabolic Network PlantCyc database (http://www.plantcyc.org) in addition to the Manchester Metabolomics Database (MMD: http://dbkgroup.org/MMD/), thus in most cases providing an MSI level 2 or 3 identification[4]. Where multiple putative molecular formula or metabolite identifications were obtained by the peak annotation approach, the identifications were also manually checked for having been previously reported as an oat metabolite (FooDB: http://foodb.ca/), thus increasing confidence in the assigned putative identification(s). In the case of lipids where multiple isomeric species could be assigned to a given accurate mass, the lipids fatty acid chain lengths and numbers of unsaturated bonds were summed in order to condense the high numbers of isomeric identifications.&lt;/br&gt;&lt;/br&gt;Ref:&lt;/br&gt;[1] Brown M, Dunn WB, Dobson P, Patel Y, Winder CL, Francis-McIntyre S, Begley P, Carroll K, Broadhurst D, Tseng A, Swainston N, Spasic I, Goodacre R, Kell DB. Mass spectrometry tools and metabolite-specific databases for molecular identification in metabolomics. Analyst. 2009 Jul;134(7):1322-32. doi:10.1039/b901179j. PMID:19562197&lt;/br&gt;[2] Brown M, Wedge DC, Goodacre R, Kell DB, Baker PN, Kenny LC, Mamas MA, Neyses L, Dunn WB. Automated workflows for accurate mass-based putative metabolite identification in LC/MS-derived metabolomic datasets. Bioinformatics. 2011 Apr 15;27(8):1108-12. doi: 0.1093/bioinformatics/btr079. PMID:21325300&lt;/br&gt;[3] Allwood JW, Weber RJ, Zhou J, He S, Viant MR, Dunn WB. CASMI-The Small Molecule Identification Process from a Birmingham Perspective. Metabolites. 2013 May 21;3(2):397-411. doi:10.3390/metabo3020397. PMID:24957998&gt;/br&gt;[4] Sumner LW, Amberg A, Barrett D, Beale MH, Beger R, Daykin CA, Fan TW et al. Proposed minimum reporting standards for chemical analysis Chemical Analysis Working Group (CAWG) Metabolomics Standards Initiative (MSI). Metabolomics. 2007 Sep;3(3):211-221. doi:10.1007/s11306-007-0082-2. PMID:24039616&lt;/br&gt;</t>
+  </si>
+  <si>
+    <t>MTBLC34262; MTBLC27951; MTBLC27797; MTBLC16713; MTBLC34454; MTBLC47220; MTBLC28967; MTBLC37144; MTBLC28960; MTBLC28905; MTBLC15368; MTBLC1217; MTBLC44692; MTBLC45285; MTBLC1467; MTBLC72700; MTBLC16119; MTBLC16199; MTBLC16607; MTBLC16610; MTBLC4614; MTBLC19092; MTBLC28638; MTBLC30322; MTBLC17203; MTBLC1439; MTBLC37600; MTBLC27371; MTBLC16070; MTBLC74863; MTBLC27411; MTBLC15866; MTBLC28847; MTBLC28140; MTBLC18287; MTBLC42606; MTBLC27907; MTBLC27442; MTBLC27586; MTBLC137774; MTBLC63150; MTBLC17617; MTBLC16935; MTBLC62345; MTBLC17897; MTBLC27708; MTBLC9652; MTBLC17059; MTBLC16357; MTBLC15971; MTBLC17064; MTBLC30818; MTBLC89640; MTBLC27248; MTBLC31042; MTBLC16572; MTBLC1580; MTBLC1879; MTBLC26797; MTBLC17578; MTBLC34213; MTBLC27869; MTBLC15767; MTBLC16089; MTBLC2319; MTBLC5966; MTBLC16380; MTBLC17143; MTBLC31173; MTBLC31278; MTBLC64977; MTBLC5320; MTBLC71166; MTBLC27480; MTBLC16355; MTBLC2600; MTBLC133351; MTBLC17881; MTBLC28928; MTBLC27616; MTBLC16100; MTBLC17641; MTBLC90886; MTBLC1139; MTBLC1387; MTBLC17095; MTBLC76163; MTBLC114204; MTBLC34252; MTBLC34256; MTBLC79445; MTBLC34876; MTBLC34877; MTBLC3007; MTBLC8986; MTBLC31054; MTBLC2932; MTBLC31435; MTBLC6945; MTBLC8616; MTBLC9183; MTBLC5959; MTBLC5708; MTBLC7468; MTBLC88104; MTBLC139134; MTBLC73926; MTBLC139133; MTBLC82679; MTBLC137760; MTBLC82678; MTBLC79877; MTBLC17747; MTBLC34710; MTBLC34679; MTBLC34097; MTBLC16323; MTBLC18385; MTBLC43997; MTBLC80424; MTBLC134287; MTBLC16929; MTBLC508; MTBLC60872; MTBLC70824; MTBLC68451; MTBLC16852; MTBLC134850; MTBLC9008; MTBLC16181; MTBLC28393; MTBLC28328; MTBLC47977; MTBLC62324; MTBLC24103; MTBLC31747; MTBLC28945; MTBLC31997; MTBLC19332; MTBLC16467; MTBLC10454; MTBLC5121; MTBLC5139; MTBLC5356; MTBLC5358; MTBLC69039; MTBLC93403; MTBLC63112; MTBLC16870; MTBLC17874; MTBLC28057; MTBLC28586; MTBLC62976; MTBLC62006; MTBLC17321; MTBLC3017; MTBLC51805; MTBLC2302; MTBLC2304; MTBLC17913; MTBLC3766; MTBLC79576; MTBLC38159; MTBLC25426; MTBLC16060; MTBLC3703; MTBLC27509; MTBLC4740; MTBLC6931; MTBLC7906; MTBLC5578; MTBLC59560; MTBLC15372; MTBLC80385; MTBLC952; MTBLC1141; MTBLC27852; MTBLC41941; MTBLC86553; MTBLC30816; MTBLC16388; MTBLC20415; MTBLC1881; MTBLC89830; MTBLC44747; MTBLC32807; MTBLC17151; MTBLC18403; MTBLC15963; MTBLC16207; MTBLC17597; MTBLC30746; MTBLC16008; MTBLC79966; MTBLC46807; MTBLC133314; MTBLC19891; MTBLC16138; MTBLC57653; MTBLC33917; MTBLC22357; MTBLC37690; MTBLC28061; MTBLC17925; MTBLC28729; MTBLC10295; MTBLC28645; MTBLC27667; MTBLC15903; MTBLC28994; MTBLC28563; MTBLC17393; MTBLC28385; MTBLC15824; MTBLC16824; MTBLC4139; MTBLC4167; MTBLC27611; MTBLC18004; MTBLC4194; MTBLC28014; MTBLC16024; MTBLC27605; MTBLC17317; MTBLC16443; MTBLC28458; MTBLC48095; MTBLC17234; MTBLC24978; MTBLC17357; MTBLC27987; MTBLC17268; MTBLC10642; MTBLC27922; MTBLC25858; MTBLC28946; MTBLC28177; MTBLC17605; MTBLC18280; MTBLC8240; MTBLC28354; MTBLC27806; MTBLC27816; MTBLC28816; MTBLC40274; MTBLC30156; MTBLC44842; MTBLC17807; MTBLC20106; MTBLC68329; MTBLC16899; MTBLC17924; MTBLC17505; MTBLC18202; MTBLC28789; MTBLC29864; MTBLC6259; MTBLC17656; MTBLC32800; MTBLC18414; MTBLC28478; MTBLC19868; MTBLC27978; MTBLC17445; MTBLC1581; MTBLC18346; MTBLC85239; MTBLC20414; MTBLC35164; MTBLC18101; MTBLC40813; MTBLC20450; MTBLC17637; MTBLC31835; MTBLC31832; MTBLC8075; MTBLC29672; MTBLC17702; MTBLC28889; MTBLC17631; MTBLC64835; MTBLC27603; MTBLC1683; MTBLC62974; MTBLC28087; MTBLC28460; MTBLC17164; MTBLC15354; MTBLC16182; MTBLC16638; MTBLC16133; MTBLC16472; MTBLC87755; MTBLC84069; MTBLC16019; MTBLC46941; MTBLC53608; MTBLC79569; MTBLC17243; MTBLC134341; MTBLC88427; MTBLC34687; MTBLC79053; MTBLC4316; MTBLC10607; MTBLC88526; MTBLC32337; MTBLC10525; MTBLC27801; MTBLC29732; MTBLC2959; MTBLC52859; MTBLC80420; MTBLC2818; MTBLC17929; MTBLC25682; MTBLC81297; MTBLC17417; MTBLC144066; MTBLC142578; MTBLC18037; MTBLC3210; MTBLC3474; MTBLC8613; MTBLC2247; MTBLC17311; MTBLC35619; MTBLC138425; MTBLC27971; MTBLC27389; MTBLC16865; MTBLC33094; MTBLC28797; MTBLC37081; MTBLC5588; MTBLC17724; MTBLC15620; MTBLC138669; MTBLC17519; MTBLC37581; MTBLC17217; MTBLC16413; MTBLC23500; MTBLC16583; MTBLC36253; MTBLC46916; MTBLC478164; MTBLC17765; MTBLC15754; MTBLC24168; MTBLC4728; MTBLC134255; MTBLC77131; MTBLC15643; MTBLC33098; MTBLC39931; MTBLC86390; MTBLC30753; MTBLC35227; MTBLC30754; MTBLC42682; MTBLC134761; MTBLC18123; MTBLC32114; MTBLC47564; MTBLC139; MTBLC16703; MTBLC531; MTBLC27380; MTBLC16885; MTBLC17332; MTBLC64833; MTBLC28782; MTBLC28793; MTBLC3528; MTBLC31005; MTBLC27680; MTBLC27649; MTBLC6364; MTBLC27931; MTBLC6731; MTBLC7912; MTBLC18154; MTBLC16634; MTBLC9859; MTBLC32059; MTBLC83804; MTBLC16546; MTBLC18428; MTBLC28102; MTBLC37165; MTBLC28808; MTBLC90185; MTBLC141517; MTBLC50663; MTBLC4954; MTBLC135681; MTBLC73275; MTBLC140748; MTBLC7982; MTBLC31576; MTBLC135209; MTBLC137782; MTBLC23875; MTBLC73892; MTBLC33020; MTBLC1230; MTBLC16551; MTBLC39244; MTBLC28676; MTBLC18260; MTBLC27554; MTBLC77436; MTBLC18167; MTBLC36217; MTBLC71422; MTBLC36218; MTBLC18147; MTBLC17057; MTBLC4125; MTBLC21010; MTBLC17306; MTBLC4808; MTBLC133330; MTBLC28066; MTBLC16751; MTBLC28189; MTBLC17716; MTBLC6359; MTBLC18411; MTBLC6435; MTBLC25164; MTBLC28053; MTBLC7570; MTBLC18394; MTBLC17992; MTBLC5105; MTBLC143968; MTBLC17705; MTBLC16708; MTBLC16347; MTBLC73707; MTBLC89341; MTBLC16817; MTBLC6907; MTBLC80354; MTBLC31085; MTBLC2089; MTBLC4055; MTBLC48294; MTBLC35090; MTBLC6415; MTBLC75627; MTBLC16246; MTBLC16772; MTBLC20582; MTBLC111; MTBLC18427; MTBLC28310; MTBLC18266; MTBLC15975; MTBLC28762; MTBLC28548; MTBLC43943; MTBLC17540; MTBLC320055; MTBLC27732; MTBLC126237; MTBLC36090; MTBLC137825; MTBLC36633; MTBLC28323; MTBLC28873; MTBLC23401; MTBLC32815; MTBLC30851; MTBLC18125; MTBLC32374; MTBLC18697; MTBLC882; MTBLC15980; MTBLC1416; MTBLC27778; MTBLC59052; MTBLC25351; MTBLC6933; MTBLC15607; MTBLC52222; MTBLC36458; MTBLC30835; MTBLC25311; MTBLC30314; MTBLC5958; MTBLC29717; MTBLC27645; MTBLC30906; MTBLC30940; MTBLC29722; MTBLC28176; MTBLC29724; MTBLC15798; MTBLC18128; MTBLC16590; MTBLC3693; MTBLC17989; MTBLC4853; MTBLC139533; MTBLC17618; MTBLC4117; MTBLC82348; MTBLC5673; MTBLC64305; MTBLC3337; MTBLC138529; MTBLC15567; MTBLC17275; MTBLC4607; MTBLC87897; MTBLC37331; MTBLC16939; MTBLC44303; MTBLC82573; MTBLC134821; MTBLC16795; MTBLC17895; MTBLC89461; MTBLC134820; MTBLC34019; MTBLC74516; MTBLC2628; MTBLC3244; MTBLC28709; MTBLC5989; MTBLC7502; MTBLC3546; MTBLC137728; MTBLC27468; MTBLC27578; MTBLC28474; MTBLC16364; MTBLC17681; MTBLC29053; MTBLC28630; MTBLC36751; MTBLC52143; MTBLC62768; MTBLC62770; MTBLC27747; MTBLC28229; MTBLC139383; MTBLC17115; MTBLC29480; MTBLC17960; MTBLC32816; MTBLC6604; MTBLC34867; MTBLC2196; MTBLC39564; MTBLC94764; MTBLC139388; MTBLC74076; MTBLC73580; MTBLC6257; MTBLC28346; MTBLC6792; MTBLC6839; MTBLC18106; MTBLC17286; MTBLC87407; MTBLC4683; MTBLC7797; MTBLC10044; MTBLC3697; MTBLC6765; MTBLC31030; MTBLC28462; MTBLC5792; MTBLC5979; MTBLC31827; MTBLC109895; MTBLC1927; MTBLC46295; MTBLC16009; MTBLC16335; MTBLC17172; MTBLC24088; MTBLC10110; MTBLC8674; MTBLC90721; MTBLC32; MTBLC134766; MTBLC135744; MTBLC63616; MTBLC5384; MTBLC79587; MTBLC44616; MTBLC34731; MTBLC2376; MTBLC64020; MTBLC4071; MTBLC3748; MTBLC23359; MTBLC50540; MTBLC16512; MTBLC6739; MTBLC137234; MTBLC27441; MTBLC28309; MTBLC19065; MTBLC70971; MTBLC16299; MTBLC490877; MTBLC37754; MTBLC27748; MTBLC6520; MTBLC107635; MTBLC84500; MTBLC15781; MTBLC81545; MTBLC81546; MTBLC27478; MTBLC29012; MTBLC9200; MTBLC8245; MTBLC9173; MTBLC32322; MTBLC31311; MTBLC171741; MTBLC92675; MTBLC138493; MTBLC74112; MTBLC61138; MTBLC37079; MTBLC33033; MTBLC16530; MTBLC27401; MTBLC39153; MTBLC45630; MTBLC38531; MTBLC8882; MTBLC6521; MTBLC50973; MTBLC8774; MTBLC137248; MTBLC2819; MTBLC27713; MTBLC19450; MTBLC17645; MTBLC58183; MTBLC17027; MTBLC70979; MTBLC17917; MTBLC724125; MTBLC89963; MTBLC28998; MTBLC1142; MTBLC18395; MTBLC16370; MTBLC15847; MTBLC71429; MTBLC88455; MTBLC42654; MTBLC17596; MTBLC17901; MTBLC87248; MTBLC9447; MTBLC28715; MTBLC21412; MTBLC143078; MTBLC8665; MTBLC55344; MTBLC37755; MTBLC15887; MTBLC17750; MTBLC58441; MTBLC18314; MTBLC16414; MTBLC138668; MTBLC77042; MTBLC134261; MTBLC41139; MTBLC2540; MTBLC10226; MTBLC10364; MTBLC3900; MTBLC4817; MTBLC5177; MTBLC5379; MTBLC5981; MTBLC6070; MTBLC8216; MTBLC73719; MTBLC50178; MTBLC135187; MTBLC17144; MTBLC6407; MTBLC73880; MTBLC79449; MTBLC7575; MTBLC11946; MTBLC3926; MTBLC35280; MTBLC29565; MTBLC15565; MTBLC16856; MTBLC32153; MTBLC6413; MTBLC8426; MTBLC80592; MTBLC51032; MTBLC28598; MTBLC17799; MTBLC57630; MTBLC28718; MTBLC15699; MTBLC16857; MTBLC16256; MTBLC30831; MTBLC137232; MTBLC15344; MTBLC51850; MTBLC16265; MTBLC28867; MTBLC18261; MTBLC17201; MTBLC17196; MTBLC15737; MTBLC29045; MTBLC16770; MTBLC17374; MTBLC28376; MTBLC2165; MTBLC29637; MTBLC39501; MTBLC32069; MTBLC6874; MTBLC5044; MTBLC37628; MTBLC64366; MTBLC17053; MTBLC29990; MTBLC5159; MTBLC18012; MTBLC18300; MTBLC17257; MTBLC135747; MTBLC31785; MTBLC10556; MTBLC5511; MTBLC5534; MTBLC2532; MTBLC2821; MTBLC3287; MTBLC6511; MTBLC1670; MTBLC73757; MTBLC21305; MTBLC18050; MTBLC16352; MTBLC37011; MTBLC16010; MTBLC94613; MTBLC6151; MTBLC139123; MTBLC1241; MTBLC28791; MTBLC62637; MTBLC16015; MTBLC16439; MTBLC45441; MTBLC31882; MTBLC17981; MTBLC36461; MTBLC17415; MTBLC17626; MTBLC17204; MTBLC2424; MTBLC15670; MTBLC30838; MTBLC16600; MTBLC51330; MTBLC75984; MTBLC3734; MTBLC7856; MTBLC9196; MTBLC7959; MTBLC16643; MTBLC50868; MTBLC9384; MTBLC15604; MTBLC89185; MTBLC57826; MTBLC28825; MTBLC18347; MTBLC17191; MTBLC15603; MTBLC64348; MTBLC17878; MTBLC17611; MTBLC17915; MTBLC85235; MTBLC38355; MTBLC49283; MTBLC143856; MTBLC61206; MTBLC79634; MTBLC79456; MTBLC79768; MTBLC79876; MTBLC34930; MTBLC6536; MTBLC17472; MTBLC73740; MTBLC7034; MTBLC5158; MTBLC30845; MTBLC30846; MTBLC74104; MTBLC19274; MTBLC85162; MTBLC23757; MTBLC5826; MTBLC62069; MTBLC223316; MTBLC44934; MTBLC10018; MTBLC135072; MTBLC34405; MTBLC34788; MTBLC31268; MTBLC34756; MTBLC3391; MTBLC53490; MTBLC5847; MTBLC5597; MTBLC79439; MTBLC34619; MTBLC135714; MTBLC7807; MTBLC78549; MTBLC1957; MTBLC20013; MTBLC40521; MTBLC31111; MTBLC34522; MTBLC16079; MTBLC37287; MTBLC37291; MTBLC29064; MTBLC2128; MTBLC9212; MTBLC53763; MTBLC86455; MTBLC45652; MTBLC30449; MTBLC34291; MTBLC17397; MTBLC24814; MTBLC74018; MTBLC52172; MTBLC28682; MTBLC66876; MTBLC9741; MTBLC5515; MTBLC47899; MTBLC8397; MTBLC695; MTBLC9403; MTBLC34307; MTBLC3767; MTBLC68428; MTBLC27527; MTBLC27588; MTBLC29573; MTBLC7599; MTBLC61645; MTBLC79626; MTBLC79729; MTBLC134923; MTBLC16043; MTBLC5457; MTBLC34048; MTBLC48541; MTBLC137772; MTBLC16547; MTBLC9957; MTBLC10366; MTBLC10423; MTBLC15582; MTBLC15583; MTBLC49076; MTBLC18104; MTBLC18078; MTBLC17023; MTBLC27861; MTBLC27550; MTBLC15591; MTBLC16831; MTBLC89205; MTBLC138367; MTBLC28381; MTBLC59051; MTBLC30997; MTBLC6452; MTBLC17937; MTBLC62112; MTBLC3207; MTBLC66913; MTBLC50131; MTBLC31989; MTBLC8097; MTBLC2705; MTBLC137310; MTBLC28502; MTBLC16765; MTBLC31993; MTBLC3085; MTBLC59020; MTBLC28948; MTBLC28136; MTBLC132335; MTBLC31584; MTBLC31952; MTBLC3112; MTBLC15676; MTBLC21860; MTBLC79347; MTBLC68606; MTBLC610092; MTBLC139380; MTBLC34598; MTBLC80544; MTBLC23812; MTBLC87166; MTBLC37245; MTBLC35460; MTBLC16093; MTBLC16558; MTBLC28568; MTBLC218; MTBLC18297; MTBLC2559; MTBLC17973; MTBLC27818; MTBLC17665; MTBLC12350; MTBLC16084; MTBLC27973; MTBLC78736; MTBLC78697; MTBLC37480; MTBLC12937; MTBLC16077; MTBLC14314; MTBLC16588; MTBLC35374; MTBLC17369; MTBLC17837; MTBLC78737; MTBLC24588; MTBLC25448; MTBLC80181; MTBLC28173; MTBLC18365; MTBLC28992; MTBLC1369; MTBLC67375; MTBLC2373; MTBLC17488; MTBLC59353; MTBLC43468; MTBLC35128; MTBLC28652; MTBLC28635; MTBLC30850; MTBLC8809; MTBLC69440; MTBLC4910; MTBLC27429; MTBLC32506; MTBLC79659; MTBLC45980; MTBLC6375; MTBLC3534; MTBLC4997; MTBLC73873; MTBLC9735; MTBLC16927; MTBLC31657; MTBLC135111; MTBLC136292; MTBLC6758; MTBLC16734; MTBLC102524; MTBLC134922; MTBLC17409; MTBLC133172; MTBLC132983; MTBLC78951; MTBLC16445; MTBLC151; MTBLC160; MTBLC15622; MTBLC35453; MTBLC18281; MTBLC17305; MTBLC41893; MTBLC42819; MTBLC30769; MTBLC30887; MTBLC30915; MTBLC17803; MTBLC6885; MTBLC4488; MTBLC27837; MTBLC86556; MTBLC84058; MTBLC3805; MTBLC4520; MTBLC73026; MTBLC73025; MTBLC34923; MTBLC64; MTBLC4628; MTBLC31585; MTBLC76160; MTBLC31981; MTBLC17802; MTBLC16704; MTBLC73715; MTBLC70353; MTBLC34698; MTBLC70453; MTBLC134913; MTBLC90038; MTBLC86004; MTBLC9274; MTBLC9275; MTBLC89730; MTBLC11222; MTBLC34447; MTBLC31402; MTBLC4895; MTBLC6347; MTBLC35796; MTBLC137768; MTBLC3158; MTBLC29513; MTBLC58556; MTBLC17533; MTBLC36554; MTBLC28249; MTBLC1162; MTBLC1243; MTBLC87507; MTBLC48061; MTBLC30918; MTBLC17902; MTBLC17568; MTBLC28942; MTBLC22099; MTBLC13497; MTBLC32275; MTBLC135817; MTBLC49026; MTBLC17012; MTBLC28879; MTBLC91807; MTBLC15809; MTBLC6381; MTBLC9605; MTBLC79471; MTBLC79566; MTBLC6851; MTBLC38546; MTBLC10561; MTBLC3146; MTBLC49260; MTBLC144027; MTBLC27574; MTBLC49004; MTBLC9308; MTBLC27407; MTBLC40304; MTBLC3927; MTBLC16750; MTBLC27427; MTBLC17643; MTBLC31552; MTBLC43755; MTBLC3088; MTBLC50271; MTBLC69499; MTBLC4994; MTBLC6008; MTBLC7161; MTBLC94381; MTBLC116; MTBLC4962; MTBLC29474; MTBLC17693; MTBLC16409; MTBLC17405; MTBLC2085; MTBLC34334; MTBLC20367; MTBLC28719; MTBLC137246; MTBLC29069; MTBLC29009; MTBLC74321; MTBLC2685; MTBLC3082; MTBLC135310; MTBLC116735; MTBLC17295; MTBLC46209; MTBLC28438; MTBLC28170; MTBLC28353; MTBLC16151; MTBLC35697; MTBLC4888; MTBLC134865; MTBLC5862; MTBLC16828; MTBLC79441; MTBLC9935; MTBLC9962; MTBLC135165; MTBLC3845; MTBLC135386; MTBLC15637; MTBLC63606; MTBLC45981; MTBLC8772; MTBLC4708; MTBLC9259; MTBLC51141; MTBLC17509; MTBLC53727; MTBLC32162; MTBLC102516; MTBLC32164; MTBLC9593; MTBLC7209; MTBLC24479; MTBLC4822; MTBLC6617; MTBLC4724; MTBLC10026; MTBLC35028; MTBLC10022; MTBLC69088; MTBLC17501; MTBLC28523; MTBLC89486; MTBLC2108; MTBLC2336; MTBLC4774; MTBLC34712; MTBLC60069; MTBLC6891; MTBLC16389; MTBLC8418; MTBLC8419; MTBLC18082; MTBLC28334; MTBLC88677; MTBLC15490; MTBLC34041; MTBLC60076; MTBLC16305; MTBLC31682; MTBLC73970; MTBLC3695; MTBLC132058; MTBLC74533; MTBLC137196; MTBLC2978; MTBLC80227; MTBLC34087; MTBLC89521; MTBLC86095; MTBLC88906; MTBLC89602; MTBLC89539; MTBLC89536; MTBLC73739; MTBLC75145; MTBLC64356; MTBLC86544; MTBLC29564; MTBLC31447; MTBLC4512; MTBLC6001; MTBLC32771; MTBLC37108; MTBLC29019; MTBLC86618; MTBLC82864; MTBLC135383; MTBLC4682; MTBLC76258; MTBLC135151; MTBLC36665; MTBLC18094; MTBLC4718; MTBLC9239; MTBLC25357; MTBLC27504; MTBLC2699; MTBLC8837; MTBLC9198; MTBLC9524; MTBLC9601; MTBLC9770; MTBLC9969; MTBLC2697; MTBLC2722; MTBLC6080; MTBLC8822; MTBLC52070; MTBLC9912; MTBLC8247; MTBLC32003; MTBLC10329; MTBLC135757; MTBLC42; MTBLC6066; MTBLC7458; MTBLC9519; MTBLC4856; MTBLC9120; MTBLC79434; MTBLC16684; MTBLC6140; MTBLC58164; MTBLC6506; MTBLC31789; MTBLC6778; MTBLC79600; MTBLC137783; MTBLC51211; MTBLC135016; MTBLC6535; MTBLC5990; MTBLC3094; MTBLC16112; MTBLC16065; MTBLC16952; MTBLC74725; MTBLC16475; MTBLC28155; MTBLC4732; MTBLC79423; MTBLC79564; MTBLC9291; MTBLC62431; MTBLC2365; MTBLC22152; MTBLC2620; MTBLC2851; MTBLC2870; MTBLC2982; MTBLC3574; MTBLC3888; MTBLC5095; MTBLC5281; MTBLC5536; MTBLC5727; MTBLC5867; MTBLC6560; MTBLC6921; MTBLC8115; MTBLC8267; MTBLC8268; MTBLC8856; MTBLC9013; MTBLC9956; MTBLC10024; MTBLC79890; MTBLC6863; MTBLC29612; MTBLC93369; MTBLC30805; MTBLC140088; MTBLC74966; MTBLC43966; MTBLC85252; MTBLC63924; MTBLC4973; MTBLC6419; MTBLC16725; MTBLC27769; MTBLC86068; MTBLC2404; MTBLC133419; MTBLC10070; MTBLC93847; MTBLC28708; MTBLC29458; MTBLC15830; MTBLC134834; MTBLC34769; MTBLC139312; MTBLC3061; MTBLC10099; MTBLC6738; MTBLC3005; MTBLC135349; MTBLC92338; MTBLC7789; MTBLC7640; MTBLC8597; MTBLC93626; MTBLC28865; MTBLC38258; MTBLC5859; MTBLC8021; MTBLC636; MTBLC67547; MTBLC137192; MTBLC88935; MTBLC86119; MTBLC86121; MTBLC89734; MTBLC86117; MTBLC78022; MTBLC89691; MTBLC84831; MTBLC74670; MTBLC89599; MTBLC89597; MTBLC89548; MTBLC89438; MTBLC89078; MTBLC89127; MTBLC89177; MTBLC88712; MTBLC21484; MTBLC15874; MTBLC17976; MTBLC5093; MTBLC63630; MTBLC2294; MTBLC2425; MTBLC16363; MTBLC2629; MTBLC69335; MTBLC28356; MTBLC4441; MTBLC135002; MTBLC10058; MTBLC10076; MTBLC10103; MTBLC28714; MTBLC43415; MTBLC5855; MTBLC28325; MTBLC74405; MTBLC3300; MTBLC9515; MTBLC41509; MTBLC2156; MTBLC2368; MTBLC9439; MTBLC74274; MTBLC8386; MTBLC18278; MTBLC27993; MTBLC82684; MTBLC9997; MTBLC80033; MTBLC29527; MTBLC29536; MTBLC135701; MTBLC16778; MTBLC18330; MTBLC4783; MTBLC27514; MTBLC5304; MTBLC31967; MTBLC16954; MTBLC8028; MTBLC133473; MTBLC29043; MTBLC38266; MTBLC80494; MTBLC72609; MTBLC62881; MTBLC135932; MTBLC9943; MTBLC58552; MTBLC42797; MTBLC31871; MTBLC82763; MTBLC31922; MTBLC135703; MTBLC64210; MTBLC135483; MTBLC32181; MTBLC474014; MTBLC3825; MTBLC34668; MTBLC7736; MTBLC17713; MTBLC10037; MTBLC8922; MTBLC7471; MTBLC31563; MTBLC3740; MTBLC4320; MTBLC24293; MTBLC80538; MTBLC79465; MTBLC4773; MTBLC5527; MTBLC9959; MTBLC131852; MTBLC9665; MTBLC473990; MTBLC17433; MTBLC80393; MTBLC3162; MTBLC5970; MTBLC44492; MTBLC79394; MTBLC15430; MTBLC2341; MTBLC34163; MTBLC31561; MTBLC135525; MTBLC8039; MTBLC79655; MTBLC79502; MTBLC34461; MTBLC79892; MTBLC34353; MTBLC34355; MTBLC79657; MTBLC17457; MTBLC4453; MTBLC9261; MTBLC79432; MTBLC79620; MTBLC29510; MTBLC52075; MTBLC15416; MTBLC31578; MTBLC52484; MTBLC29611; MTBLC52482; MTBLC29654; MTBLC81594; MTBLC30038; MTBLC31896; MTBLC9108; MTBLC9946; MTBLC847; MTBLC9205; MTBLC15735; MTBLC3745; MTBLC82461; MTBLC27796; MTBLC34580; MTBLC6147; MTBLC135451; MTBLC2565; MTBLC4038; MTBLC28833; MTBLC29592; MTBLC29594; MTBLC29602; MTBLC5606; MTBLC6962; MTBLC8330; MTBLC9042; MTBLC9290; MTBLC2534; MTBLC799; MTBLC34139; MTBLC79668; MTBLC79797; MTBLC136980; MTBLC1189; MTBLC136972; MTBLC79907; MTBLC63641; MTBLC79715; MTBLC2495; MTBLC79887; MTBLC9460; MTBLC17078; MTBLC141472; MTBLC28192; MTBLC135231; MTBLC79496; MTBLC79601; MTBLC5887; MTBLC59788; MTBLC31086; MTBLC2626; MTBLC8402; MTBLC32185; MTBLC4417; MTBLC31298; MTBLC31497; MTBLC8713; MTBLC31459; MTBLC113542; MTBLC40070; MTBLC27510; MTBLC17148; MTBLC716; MTBLC2327; MTBLC2544; MTBLC3614; MTBLC89837; MTBLC89829; MTBLC89824; MTBLC90028; MTBLC90034; MTBLC90021; MTBLC77677; MTBLC88798; MTBLC88446; MTBLC41847; MTBLC89028; MTBLC90068; MTBLC64793; MTBLC84266; MTBLC5674; MTBLC142272; MTBLC2939; MTBLC6798; MTBLC1749; MTBLC8602; MTBLC17467; MTBLC34605; MTBLC9425; MTBLC2725; MTBLC9923; MTBLC73; MTBLC30725; MTBLC34968; MTBLC31753; MTBLC2934; MTBLC7948; MTBLC86251; MTBLC30248; MTBLC34227; MTBLC142243; MTBLC136795; MTBLC2504; MTBLC3081; MTBLC16188; MTBLC16011; MTBLC85158; MTBLC79925; MTBLC79522; MTBLC34175; MTBLC79455; MTBLC80656; MTBLC79735; MTBLC135981; MTBLC6085; MTBLC49191; MTBLC9419; MTBLC89642; MTBLC16374; MTBLC10136; MTBLC4778; MTBLC8196; MTBLC28794; MTBLC90355; MTBLC79553; MTBLC28090; MTBLC2197; MTBLC3163; MTBLC28436; MTBLC5837; MTBLC6006; MTBLC75092; MTBLC16243; MTBLC8876; MTBLC507499; MTBLC204; MTBLC214; MTBLC241; MTBLC242; MTBLC78668; MTBLC138752; MTBLC17130; MTBLC34301; MTBLC37157; MTBLC78853; MTBLC61024; MTBLC8607; MTBLC4389; MTBLC5528; MTBLC89343; MTBLC89314; MTBLC89088; MTBLC89075; MTBLC89076; MTBLC89371; MTBLC89333; MTBLC89334; MTBLC89311; MTBLC89316; MTBLC138499; MTBLC18227; MTBLC94661; MTBLC36108; MTBLC80383; MTBLC8273; MTBLC8773; MTBLC31049; MTBLC18393; MTBLC137750; MTBLC17224; MTBLC5679; MTBLC18127; MTBLC17166; MTBLC28091; MTBLC36466; MTBLC36106; MTBLC4366; MTBLC28869; MTBLC28925; MTBLC9185; MTBLC9188; MTBLC86162; MTBLC88930; MTBLC88929; MTBLC89739; MTBLC89576; MTBLC89557; MTBLC89559; MTBLC89441; MTBLC86161; MTBLC89419; MTBLC88925; MTBLC88841; MTBLC88430; MTBLC88654; MTBLC10219; MTBLC86344; MTBLC84549; MTBLC84837; MTBLC78268; MTBLC7492; MTBLC91712; MTBLC4974; MTBLC4572; MTBLC6414; MTBLC81785; MTBLC135138; MTBLC60656; MTBLC16312; MTBLC16390; MTBLC138401; MTBLC88108; MTBLC2812; MTBLC79833; MTBLC47818; MTBLC79918; MTBLC34838; MTBLC31523; MTBLC138422; MTBLC47214; MTBLC28818; MTBLC32176; MTBLC15578; MTBLC89324; MTBLC89079; MTBLC19290; MTBLC79996; MTBLC28477; MTBLC81013; MTBLC17823; MTBLC86378; MTBLC7931; MTBLC28933; MTBLC9595; MTBLC34667; MTBLC31648; MTBLC4819; MTBLC32645; MTBLC8764; MTBLC4921; MTBLC9165; MTBLC31857; MTBLC31174; MTBLC34831; MTBLC31894; MTBLC9316; MTBLC27617; MTBLC80461; MTBLC80167; MTBLC1107; MTBLC82949; MTBLC88480; MTBLC88479; MTBLC88547; MTBLC89218; MTBLC89203; MTBLC89202; MTBLC89162; MTBLC89160; MTBLC89238; MTBLC89237; MTBLC88966; MTBLC89040; MTBLC89780; MTBLC89784; MTBLC89799; MTBLC89797; MTBLC89684; MTBLC89669; MTBLC89670; MTBLC89671; MTBLC89433; MTBLC89322; MTBLC89337; MTBLC136371; MTBLC64396; MTBLC88779; MTBLC28517; MTBLC18171; MTBLC32086; MTBLC5206; MTBLC15575; MTBLC2513; MTBLC50749; MTBLC31893; MTBLC9463; MTBLC15574; MTBLC90980; MTBLC47812; MTBLC80533; MTBLC3863; MTBLC5633; MTBLC8913; MTBLC6145; MTBLC64668; MTBLC7800; MTBLC9039; MTBLC8621; MTBLC80017; MTBLC34042; MTBLC7752; MTBLC28285; MTBLC18010; MTBLC3719; MTBLC5718; MTBLC6674; MTBLC59979; MTBLC34499; MTBLC34503; MTBLC34506; MTBLC91217; MTBLC138082; MTBLC15658; MTBLC15655; MTBLC15657; MTBLC64008; MTBLC138786; MTBLC88461; MTBLC34148; MTBLC91272; MTBLC34485; MTBLC34498; MTBLC34500; MTBLC88440; MTBLC34504; MTBLC143972; MTBLC88465; MTBLC89257; MTBLC3403; MTBLC3898; MTBLC79904; MTBLC34352; MTBLC1689; MTBLC89328; MTBLC79870; MTBLC9481; MTBLC93; MTBLC1941; MTBLC8603; MTBLC134767; MTBLC74562; MTBLC61725; MTBLC142079; MTBLC16310; MTBLC42471; MTBLC7567; MTBLC16147; MTBLC85232; MTBLC90230; MTBLC133979; MTBLC137172; MTBLC85166; MTBLC133325; MTBLC135350; MTBLC545687; MTBLC7496; MTBLC34322; MTBLC79177; MTBLC84854; MTBLC34295; MTBLC29479; MTBLC17903; MTBLC4045; MTBLC10445; MTBLC6706; MTBLC79519; MTBLC34293; MTBLC34294; MTBLC135489; MTBLC9238; MTBLC137712; MTBLC19143; MTBLC18446; MTBLC8648; MTBLC19144; MTBLC49265; MTBLC15654; MTBLC88462; MTBLC80442; MTBLC84441; MTBLC72641; MTBLC136531; MTBLC72815; MTBLC80463; MTBLC76234; MTBLC34491; MTBLC88441; MTBLC80447; MTBLC88438; MTBLC72843; MTBLC72842; MTBLC88460; MTBLC60956; MTBLC133329; MTBLC80413; MTBLC63067; MTBLC18230; MTBLC65247; MTBLC3705; MTBLC31352; MTBLC76334; MTBLC9510; MTBLC3128; MTBLC61726; MTBLC89365; MTBLC89339; MTBLC89342; MTBLC89318; MTBLC89313; MTBLC60273; MTBLC65211; MTBLC138212; MTBLC78700; MTBLC55523; MTBLC27706; MTBLC38299; MTBLC137495; MTBLC34154; MTBLC72639; MTBLC133357; MTBLC34494; MTBLC78730; MTBLC34496; MTBLC72651; MTBLC131659; MTBLC5833; MTBLC73074; MTBLC2366; MTBLC1019; MTBLC88696; MTBLC52897; MTBLC79575; MTBLC135210; MTBLC132495; MTBLC73751; MTBLC34828; MTBLC88667; MTBLC9778; MTBLC28919; MTBLC10088; MTBLC69081; MTBLC75542; MTBLC95216; MTBLC134424; MTBLC134423; MTBLC29627; MTBLC10120; MTBLC34034; MTBLC34443; MTBLC40131; MTBLC4918; MTBLC14469; MTBLC2492; MTBLC5166; MTBLC88808; MTBLC88807; MTBLC88782; MTBLC89214; MTBLC89189; MTBLC89149; MTBLC1418; MTBLC27867; MTBLC80419; MTBLC3375; MTBLC5087; MTBLC27448; MTBLC80177; MTBLC19793; MTBLC28485; MTBLC88765; MTBLC28810; MTBLC32157; MTBLC31279; MTBLC7720; MTBLC73728; MTBLC133875; MTBLC34920; MTBLC6088; MTBLC137139; MTBLC138782; MTBLC34652; MTBLC34680; MTBLC33913; MTBLC75219; MTBLC133456; MTBLC88698; MTBLC88697; MTBLC79838; MTBLC50106; MTBLC34229; MTBLC138081; MTBLC38833; MTBLC22469; MTBLC28093; MTBLC15405; MTBLC17580; MTBLC36503; MTBLC15393; MTBLC36492; MTBLC98; MTBLC31; MTBLC60; MTBLC61; MTBLC149; MTBLC150; MTBLC152; MTBLC153; MTBLC50232; MTBLC158; MTBLC50233; MTBLC50235; MTBLC300; MTBLC299; MTBLC368; MTBLC27961; MTBLC61727; MTBLC47856; MTBLC17447; MTBLC29452; MTBLC28071; MTBLC692; MTBLC35002; MTBLC9602; MTBLC137135; MTBLC34537; MTBLC79794; MTBLC79879; MTBLC28125; MTBLC79767; MTBLC79635; MTBLC34476; MTBLC79801; MTBLC135402; MTBLC32095; MTBLC79581; MTBLC76937; MTBLC39567; MTBLC36206; MTBLC36214; MTBLC85510; MTBLC36211; MTBLC7989; MTBLC79096; MTBLC75103; MTBLC32411; MTBLC138778; MTBLC36412; MTBLC86135; MTBLC142250; MTBLC86506; MTBLC32409; MTBLC32389; MTBLC37810; MTBLC2905; MTBLC135532; MTBLC79179; MTBLC84855; MTBLC80050; MTBLC48635; MTBLC5644; MTBLC63916; MTBLC79523; MTBLC79689; MTBLC80001; MTBLC52421; MTBLC448; MTBLC72665; MTBLC138258; MTBLC138255; MTBLC72663; MTBLC133381; MTBLC133086; MTBLC131762; MTBLC73882; MTBLC84067; MTBLC86403; MTBLC31850; MTBLC132479; MTBLC92833; MTBLC34370; MTBLC135041; MTBLC134981; MTBLC31547; MTBLC79883; MTBLC79939; MTBLC6645; MTBLC84094; MTBLC116278; MTBLC9232; MTBLC28661; MTBLC10275; MTBLC27432; MTBLC44602; MTBLC79716; MTBLC86136; MTBLC86148; MTBLC38384; MTBLC16423; MTBLC61676; MTBLC8638; MTBLC88809; MTBLC75465; MTBLC88786; MTBLC84394; MTBLC88471; MTBLC88536; MTBLC88367; MTBLC75446; MTBLC138077; MTBLC28627; MTBLC80415; MTBLC88796; MTBLC88725; MTBLC82927; MTBLC88501; MTBLC88500; MTBLC88364; MTBLC89229; MTBLC89211; MTBLC88942; MTBLC89034; MTBLC89029; MTBLC50585; MTBLC138489; MTBLC31571; MTBLC45571; MTBLC31725; MTBLC144339; MTBLC9194; MTBLC89605; MTBLC15843; MTBLC79754; MTBLC79694; MTBLC1182; MTBLC79480; MTBLC79869; MTBLC82835; MTBLC2451; MTBLC36033; MTBLC31825; MTBLC135293; MTBLC34834; MTBLC30041; MTBLC10419; MTBLC3425; MTBLC8996; MTBLC6991; MTBLC32345; MTBLC137651; MTBLC641; MTBLC1784; MTBLC4640; MTBLC72800; MTBLC20096; MTBLC72758; MTBLC73889; MTBLC3456; MTBLC9242; MTBLC44526; MTBLC83063; MTBLC38394; MTBLC142447; MTBLC24993; MTBLC138083; MTBLC38362; MTBLC82749; MTBLC32798; MTBLC88464; MTBLC86141; MTBLC27939; MTBLC75108; MTBLC6673; MTBLC28801; MTBLC84299; MTBLC4650; MTBLC46979; MTBLC136623; MTBLC46859; MTBLC83058; MTBLC9189; MTBLC86570; MTBLC31542; MTBLC89519; MTBLC85028; MTBLC74971; MTBLC4021; MTBLC48923; MTBLC64483; MTBLC131738; MTBLC64489; MTBLC78103; MTBLC63959; MTBLC31000; MTBLC75454; MTBLC75536; MTBLC31831; MTBLC75565; MTBLC137215; MTBLC135498; MTBLC3961; MTBLC71025; MTBLC73792; MTBLC137845; MTBLC9011; MTBLC33276; MTBLC80541; MTBLC137134; MTBLC47805; MTBLC79517; MTBLC4629; MTBLC31826; MTBLC10086; MTBLC64124; MTBLC46961; MTBLC15913; MTBLC18129; MTBLC79182; MTBLC143095; MTBLC85208; MTBLC136406; MTBLC50578; MTBLC136819; MTBLC136638; MTBLC74789; MTBLC79951; MTBLC5382; MTBLC69833; MTBLC80540; MTBLC3450; MTBLC37779; MTBLC37537; MTBLC49254; MTBLC28724; MTBLC136767; MTBLC85633; MTBLC34004; MTBLC85639; MTBLC45478; MTBLC79312; MTBLC30820; MTBLC50576; MTBLC138260; MTBLC82464; MTBLC28592; MTBLC84874; MTBLC70850; MTBLC85057; MTBLC32365; MTBLC90027; MTBLC3433; MTBLC9184; MTBLC74330; MTBLC62834; MTBLC73741; MTBLC79501; MTBLC34464; MTBLC11152; MTBLC29644; MTBLC84519; MTBLC34726; MTBLC133741; MTBLC46703; MTBLC73829; MTBLC34402; MTBLC137126; MTBLC81246; MTBLC67061; MTBLC73851; MTBLC84752; MTBLC79723; MTBLC33216; MTBLC6689; MTBLC7443; MTBLC79824; MTBLC135488; MTBLC88790; MTBLC77096; MTBLC88474; MTBLC88495; MTBLC88490; MTBLC88520; MTBLC88371; MTBLC88395; MTBLC89225; MTBLC75475; MTBLC77127; MTBLC89169; MTBLC89168; MTBLC89260; MTBLC75578; MTBLC88989; MTBLC89046; MTBLC89795; MTBLC89682; MTBLC89665; MTBLC89811; MTBLC80207; MTBLC131692; MTBLC17862; MTBLC71464; MTBLC16393; MTBLC28727; MTBLC28194; MTBLC27997; MTBLC16196; MTBLC82617; MTBLC50575; MTBLC32375; MTBLC50464; MTBLC29735; MTBLC30829; MTBLC28193; MTBLC50572; MTBLC36023; MTBLC35517; MTBLC79612; MTBLC18054; MTBLC3430; MTBLC6965; MTBLC82985; MTBLC10087; MTBLC9916; MTBLC35464; MTBLC142241; MTBLC28716; MTBLC35465; MTBLC76244; MTBLC37252; MTBLC76090; MTBLC9199; MTBLC9951; MTBLC77148; MTBLC31872; MTBLC3944; MTBLC5933; MTBLC72828; MTBLC72952; MTBLC27620; MTBLC91006; MTBLC67309; MTBLC3940; MTBLC7909; MTBLC79407; MTBLC79791; MTBLC79792; MTBLC66666; MTBLC135355; MTBLC88112; MTBLC135566; MTBLC79513; MTBLC73092; MTBLC31501; MTBLC88109; MTBLC31297; MTBLC28941; MTBLC84901; MTBLC28733; MTBLC6144; MTBLC75612; MTBLC52392; MTBLC3427; MTBLC137833; MTBLC16566; MTBLC84896; MTBLC28842; MTBLC88686; MTBLC29702; MTBLC34478; MTBLC137844; MTBLC53154; MTBLC72736; MTBLC133144; MTBLC75036; MTBLC131924; MTBLC8416; MTBLC9190; MTBLC18318; MTBLC86422; MTBLC89413; MTBLC89431; MTBLC89391; MTBLC89140; MTBLC89196; MTBLC89294; MTBLC88904; MTBLC88905; MTBLC88760; MTBLC88761; MTBLC88731; MTBLC88729; MTBLC88871; MTBLC88869; MTBLC88587; MTBLC89500; MTBLC89501; MTBLC34542; MTBLC61473; MTBLC3249; MTBLC4746; MTBLC80169; MTBLC34121; MTBLC52971; MTBLC93175; MTBLC137734; MTBLC73854; MTBLC90040; MTBLC89382; MTBLC89352; MTBLC89368; MTBLC89366; MTBLC89340; MTBLC89317; MTBLC137279; MTBLC137293; MTBLC134075; MTBLC90459; MTBLC134076; MTBLC134077; MTBLC134078; MTBLC39934; MTBLC134227; MTBLC134228; MTBLC16038; MTBLC9970; MTBLC4592; MTBLC79643; MTBLC34554; MTBLC2927; MTBLC27722; MTBLC28277; MTBLC80014; MTBLC77258; MTBLC4915; MTBLC5746; MTBLC28468; MTBLC64563; MTBLC76078; MTBLC72998; MTBLC78101; MTBLC73721; MTBLC73134; MTBLC73004; MTBLC62837; MTBLC78270; MTBLC79536; MTBLC73894; MTBLC31676; MTBLC50782; MTBLC31650; MTBLC6574; MTBLC31940; MTBLC44247; MTBLC79899; MTBLC27965; MTBLC79098; MTBLC75038; MTBLC133623; MTBLC84577; MTBLC84234; MTBLC64032; MTBLC53486; MTBLC53460; MTBLC79878; MTBLC79900; MTBLC525464; MTBLC79409; MTBLC79578; MTBLC82832; MTBLC71589; MTBLC32023; MTBLC34349; MTBLC32068; MTBLC31020; MTBLC2502; MTBLC28593; MTBLC15854; MTBLC309594; MTBLC84116; MTBLC3560; MTBLC79190; MTBLC76992; MTBLC52347; MTBLC18164; MTBLC32027; MTBLC135857; MTBLC88780; MTBLC88468; MTBLC75342; MTBLC744; MTBLC34115; MTBLC84911; MTBLC32154; MTBLC131508; MTBLC32906; MTBLC29596; MTBLC28211; MTBLC6927; MTBLC7603; MTBLC80537; MTBLC10137; MTBLC80732; MTBLC79113; MTBLC90041; MTBLC133599; MTBLC133617; MTBLC84845; MTBLC84844; MTBLC74986; MTBLC143985; MTBLC80203; MTBLC143980; MTBLC134453; MTBLC34126; MTBLC34130; MTBLC79851; MTBLC72606; MTBLC19138; MTBLC137345; MTBLC34157; MTBLC88823; MTBLC78837; MTBLC64017; MTBLC34162; MTBLC79557; MTBLC79656; MTBLC63995; MTBLC79561; MTBLC63579; MTBLC34185; MTBLC34306; MTBLC79485; MTBLC34450; MTBLC60943; MTBLC137344; MTBLC34490; MTBLC72643; MTBLC72786; MTBLC36275; MTBLC86031; MTBLC73733; MTBLC89091; MTBLC75646; MTBLC89387; MTBLC89392; MTBLC89395; MTBLC89394; MTBLC53081; MTBLC76284; MTBLC137704; MTBLC34438; MTBLC32319; MTBLC32325; MTBLC34711; MTBLC4676; MTBLC34136; MTBLC39449; MTBLC39451; MTBLC39453; MTBLC39454; MTBLC31406; MTBLC10580; MTBLC39448; MTBLC4722; MTBLC19287; MTBLC31164; MTBLC27655; MTBLC5715; MTBLC6567; MTBLC6586; MTBLC34883; MTBLC88902; MTBLC8034; MTBLC10045; MTBLC10089; MTBLC80194; MTBLC79956; MTBLC79588; MTBLC81561; MTBLC2296; MTBLC3321; MTBLC65585; MTBLC134353; MTBLC143960; MTBLC30088; MTBLC29589; MTBLC29601; MTBLC6696; MTBLC134511; MTBLC140267; MTBLC8390; MTBLC5783; MTBLC80531; MTBLC16688; MTBLC28135; MTBLC137137; MTBLC139534; MTBLC31731; MTBLC73923; MTBLC31801; MTBLC35459; MTBLC135729; MTBLC135684; MTBLC86197; MTBLC86196; MTBLC86189; MTBLC86190; MTBLC86188; MTBLC80532; MTBLC18531; MTBLC18532; MTBLC46739; MTBLC79839; MTBLC28033; MTBLC17168; MTBLC16608; MTBLC17762; MTBLC16074; MTBLC16113; MTBLC143982; MTBLC28610; MTBLC86255; MTBLC76071; MTBLC143713; MTBLC72589; MTBLC131658; MTBLC31025; MTBLC17390; MTBLC27808; MTBLC5191; MTBLC31123; MTBLC82648; MTBLC135276; MTBLC4670; MTBLC143989; MTBLC9669; MTBLC52672; MTBLC37945; MTBLC34899; MTBLC37923; MTBLC8710; MTBLC31550; MTBLC3156; MTBLC48742; MTBLC135719; MTBLC8036; MTBLC7352; MTBLC90970; MTBLC47834; MTBLC63911; MTBLC137141; MTBLC47799; MTBLC72727; MTBLC80530; MTBLC5363; MTBLC52348; MTBLC17314; MTBLC76980; MTBLC76304; MTBLC6113; MTBLC143987; MTBLC143990; MTBLC9911; MTBLC135737; MTBLC28700; MTBLC79923; MTBLC73794; MTBLC62736; MTBLC62737; MTBLC84958; MTBLC86418; MTBLC89703; MTBLC89592; MTBLC89589; MTBLC89384; MTBLC89098; MTBLC89143; MTBLC89070; MTBLC88726; MTBLC88872; MTBLC88588; MTBLC89498; MTBLC89502; MTBLC143981; MTBLC143983; MTBLC71466; MTBLC9453; MTBLC31264; MTBLC131689; MTBLC74340; MTBLC131668; MTBLC131687; MTBLC131688; MTBLC52639; MTBLC85403; MTBLC29613; MTBLC79453; MTBLC28047; MTBLC132620; MTBLC31257; MTBLC29677; MTBLC31222; MTBLC5197; MTBLC135094; MTBLC32277; MTBLC15929; MTBLC25242; MTBLC28258; MTBLC134924; MTBLC86975; MTBLC88529; MTBLC89026; MTBLC137784; MTBLC32002; MTBLC125; MTBLC46734; MTBLC141283; MTBLC16774; MTBLC35966; MTBLC16619; MTBLC10217; MTBLC10278; MTBLC10417; MTBLC3431; MTBLC4001; MTBLC5552; MTBLC5719; MTBLC6401; MTBLC7524; MTBLC7940; MTBLC64792; MTBLC137092; MTBLC144025; MTBLC10274; MTBLC3087; MTBLC37659; MTBLC135741; MTBLC9908; MTBLC18067; MTBLC89279; MTBLC89380; MTBLC89383; MTBLC89360; MTBLC89359; MTBLC89370; MTBLC84566; MTBLC137216; MTBLC85680; MTBLC18168; MTBLC52350; MTBLC73731; MTBLC78706; MTBLC31572; MTBLC36036; MTBLC9053; MTBLC89090; MTBLC89089; MTBLC89074; MTBLC89390; MTBLC89357; MTBLC89374; MTBLC89373; MTBLC90454; MTBLC75376; MTBLC17058; MTBLC28688; MTBLC34184; MTBLC3941; MTBLC53424; MTBLC1309; MTBLC1310; MTBLC79897; MTBLC63065; MTBLC143013; MTBLC4813; MTBLC134507; MTBLC84759; MTBLC34835; MTBLC84877; MTBLC39248; MTBLC34122; MTBLC84386; MTBLC88781; MTBLC88757; MTBLC88469; MTBLC75550; MTBLC83055; MTBLC27423; MTBLC37998; MTBLC2944; MTBLC132949; MTBLC137858; MTBLC137136; MTBLC79992; MTBLC9948; MTBLC135723; MTBLC90233; MTBLC137178; MTBLC73736; MTBLC39826; MTBLC50158; MTBLC17177; MTBLC16697; MTBLC52052; MTBLC16101; MTBLC28488; MTBLC28063; MTBLC27417; MTBLC84341; MTBLC88756; MTBLC3663; MTBLC59912; MTBLC80083; MTBLC94686; MTBLC137229; MTBLC82836; MTBLC77525; MTBLC34743; MTBLC133914; MTBLC89451; MTBLC135440; MTBLC72844; MTBLC79787; MTBLC79494; MTBLC88359; MTBLC140473; MTBLC137304; MTBLC63836; MTBLC73135; MTBLC48131; MTBLC79444; MTBLC2696; MTBLC46750; MTBLC7952; MTBLC8186; MTBLC32249; MTBLC15884; MTBLC41872; MTBLC33275; MTBLC33277; MTBLC135704; MTBLC4429; MTBLC15414; MTBLC88735; MTBLC17685; MTBLC4391; MTBLC8038; MTBLC17858; MTBLC2669; MTBLC5762; MTBLC9122; MTBLC79874; MTBLC34141; MTBLC73773; MTBLC79786; MTBLC79448; MTBLC5120; MTBLC16264; MTBLC16650; MTBLC16287; MTBLC3421; MTBLC7500; MTBLC135923; MTBLC40957; MTBLC41938; MTBLC79970; MTBLC4289; MTBLC59276; MTBLC16654; MTBLC86537; MTBLC982; MTBLC17094; MTBLC28710; MTBLC37032; MTBLC27530; MTBLC30832; MTBLC68566; MTBLC17646; MTBLC86396; MTBLC89760; MTBLC137770; MTBLC32350; MTBLC17400; MTBLC28870; MTBLC3354; MTBLC2310; MTBLC31759; MTBLC45951; MTBLC28657; MTBLC27520; MTBLC42976; MTBLC16802; MTBLC3014; MTBLC2155; MTBLC2185; MTBLC2321; MTBLC135989; MTBLC6709; MTBLC6888; MTBLC79546; MTBLC79481; MTBLC81712; MTBLC6995; MTBLC6960; MTBLC35040; MTBLC3533; MTBLC35421; MTBLC33509; MTBLC48093; MTBLC33510; MTBLC33511; MTBLC34237; MTBLC80471; MTBLC43996; MTBLC18226; MTBLC17532; MTBLC30734; MTBLC134814; MTBLC37753; MTBLC27469; MTBLC16142; MTBLC17426; MTBLC28860; MTBLC20937; MTBLC47962; MTBLC4178; MTBLC16224; MTBLC21099; MTBLC24113; MTBLC33830; MTBLC24769; MTBLC28378; MTBLC85187; MTBLC17077; MTBLC46644; MTBLC33198; MTBLC24149; MTBLC24266; MTBLC24462; MTBLC18246; MTBLC681850; MTBLC32709; MTBLC31677; MTBLC8871; MTBLC27513; MTBLC613; MTBLC1945; MTBLC15937; MTBLC9513; MTBLC63624; MTBLC17748; MTBLC17293; MTBLC2555; MTBLC7785; MTBLC8256; MTBLC7821; MTBLC135842; MTBLC66773; MTBLC2913; MTBLC6076; MTBLC15532; MTBLC6791; MTBLC87625; MTBLC6859; MTBLC30860; MTBLC15741; MTBLC30347; MTBLC77780; MTBLC89639; MTBLC254496; MTBLC35034; MTBLC4364; MTBLC17506; MTBLC18321; MTBLC15934; MTBLC6819; MTBLC30527; MTBLC2653; MTBLC39462; MTBLC79807; MTBLC3897; MTBLC8380; MTBLC15362; MTBLC8478; MTBLC48058; MTBLC27444; MTBLC41607; MTBLC705; MTBLC5954; MTBLC50885; MTBLC135324; MTBLC836; MTBLC3276; MTBLC89060; MTBLC89499; MTBLC6650; MTBLC32242; MTBLC2431; MTBLC34801; MTBLC63622; MTBLC79719; MTBLC34321; MTBLC5810; MTBLC17871; MTBLC30966; MTBLC27957; MTBLC18419; MTBLC30768; MTBLC137814; MTBLC86348; MTBLC86391; MTBLC36532; MTBLC27904; MTBLC16023; MTBLC27378; MTBLC28587; MTBLC3641; MTBLC9653; MTBLC135517; MTBLC3918; MTBLC79692; MTBLC79988; MTBLC9961; MTBLC6838; MTBLC1547; MTBLC2076; MTBLC63581; MTBLC141154; MTBLC8049; MTBLC16992; MTBLC30841; MTBLC30794; MTBLC135928; MTBLC6628; MTBLC8341; MTBLC73758; MTBLC15436; MTBLC27630; MTBLC32398; MTBLC15366; MTBLC17071; MTBLC15586; MTBLC29003; MTBLC17647; MTBLC17084; MTBLC58511; MTBLC15584; MTBLC16292; MTBLC27736; MTBLC16392; MTBLC15867; MTBLC6177; MTBLC37434; MTBLC47518; MTBLC31441; MTBLC75988; MTBLC80438; MTBLC3978; MTBLC80441; MTBLC133224; MTBLC31743; MTBLC80528; MTBLC6553; MTBLC133244; MTBLC28527; MTBLC135754; MTBLC27994; MTBLC66905; MTBLC3439; MTBLC27475; MTBLC28426; MTBLC80434; MTBLC5065; MTBLC17965; MTBLC31742; MTBLC30200; MTBLC75790; MTBLC7781; MTBLC17558; MTBLC43136; MTBLC17456; MTBLC18320; MTBLC31784; MTBLC101278; MTBLC31901; MTBLC34474; MTBLC34511; MTBLC79863; MTBLC57681; MTBLC16211; MTBLC16773; MTBLC16898; MTBLC44932; MTBLC53770; MTBLC79369; MTBLC13714; MTBLC63609; MTBLC79929; MTBLC10285; MTBLC2883; MTBLC135745; MTBLC34574; MTBLC31359; MTBLC31849; MTBLC7814; MTBLC33138; MTBLC18043; MTBLC28459; MTBLC17798; MTBLC10072; MTBLC35014; MTBLC73688; MTBLC135289; MTBLC2506; MTBLC2769; MTBLC9045; MTBLC141; MTBLC89487; MTBLC30821; MTBLC79630; MTBLC1734; MTBLC12257; MTBLC133809; MTBLC135613; MTBLC50742; MTBLC15623; MTBLC15624; MTBLC16715; MTBLC27583; MTBLC16278; MTBLC17782; MTBLC22652; MTBLC17039; MTBLC18268; MTBLC73681; MTBLC17801; MTBLC45969; MTBLC21241; MTBLC30923; MTBLC4083; MTBLC28411; MTBLC36622; MTBLC58468; MTBLC18383; MTBLC135643; MTBLC34170; MTBLC87820; MTBLC79702; MTBLC31215; MTBLC4919; MTBLC8880; MTBLC1656; MTBLC49003; MTBLC17032; MTBLC16609; MTBLC27972; MTBLC16622; MTBLC27453; MTBLC17011; MTBLC16222; MTBLC15895; MTBLC15945; MTBLC16165; MTBLC16217; MTBLC28991; MTBLC24150; MTBLC5571; MTBLC5711; MTBLC48657; MTBLC8355; MTBLC29484; MTBLC17413; MTBLC16444; MTBLC17281; MTBLC17667; MTBLC17655; MTBLC111517; MTBLC741548; MTBLC17859; MTBLC91315; MTBLC75146; MTBLC76138; MTBLC80222; MTBLC30751; MTBLC28624; MTBLC135926; MTBLC57303; MTBLC15426; MTBLC6049; MTBLC7851; MTBLC3364; MTBLC7564; MTBLC16719; MTBLC31046; MTBLC34288; MTBLC86365; MTBLC17308; MTBLC35932; MTBLC28422; MTBLC48430; MTBLC15888; MTBLC17075; MTBLC29024; MTBLC4893; MTBLC15825; MTBLC16486; MTBLC89540; MTBLC89917; MTBLC9603; MTBLC2801; MTBLC92373; MTBLC2724; MTBLC90086; MTBLC16820; MTBLC7986; MTBLC82603; MTBLC3746; MTBLC8955; MTBLC34596; MTBLC34597; MTBLC50729; MTBLC28463; MTBLC135497; MTBLC34379; MTBLC5138; MTBLC81321; MTBLC5321; MTBLC58778; MTBLC8982; MTBLC9783; MTBLC31113; MTBLC8393; MTBLC44185; MTBLC79670; MTBLC7577; MTBLC79483; MTBLC135464; MTBLC27683; MTBLC15999; MTBLC16433; MTBLC15365; MTBLC17395; MTBLC89749; MTBLC137819; MTBLC88868; MTBLC70851; MTBLC15566; MTBLC68502; MTBLC68503; MTBLC7773; MTBLC17990; MTBLC15711; MTBLC18412; MTBLC94706; MTBLC7470; MTBLC31592; MTBLC16252; MTBLC27949; MTBLC9725; MTBLC40947; MTBLC32019; MTBLC3154; MTBLC8682; MTBLC6737; MTBLC8205; MTBLC16279; MTBLC15645; MTBLC2735; MTBLC17340; MTBLC3868; MTBLC6563; MTBLC8339; MTBLC59583; MTBLC45257; MTBLC10003; MTBLC3451; MTBLC141529; MTBLC137236; MTBLC18026; MTBLC17189; MTBLC68465; MTBLC36062; MTBLC17253; MTBLC16509; MTBLC133083; MTBLC86542; MTBLC131434; MTBLC17869; MTBLC59783; MTBLC55534; MTBLC28707; MTBLC27909; MTBLC134808; MTBLC64390; MTBLC136818; MTBLC136917; MTBLC17786; MTBLC9367; MTBLC138495; MTBLC43533; MTBLC17945; MTBLC37419; MTBLC75; MTBLC2702; MTBLC27920; MTBLC5557; MTBLC2527; MTBLC67461; MTBLC17727; MTBLC34921; MTBLC15932; MTBLC7513; MTBLC9047; MTBLC31433; MTBLC80391; MTBLC3384; MTBLC6003; MTBLC79609; MTBLC135445; MTBLC7628; MTBLC133152; MTBLC80000; MTBLC7421; MTBLC71498; MTBLC17335; MTBLC3103; MTBLC62251; MTBLC17531; MTBLC2469; MTBLC34550; MTBLC2515; MTBLC79698; MTBLC8173; MTBLC18328; MTBLC2672; MTBLC6369; MTBLC7659; MTBLC9468; MTBLC82542; MTBLC63628; MTBLC6109; MTBLC7609; MTBLC28064; MTBLC16726; MTBLC28596; MTBLC17379; MTBLC31788; MTBLC7910; MTBLC134007; MTBLC7951; MTBLC133365; MTBLC75439; MTBLC69814; MTBLC16631; MTBLC79936; MTBLC34236; MTBLC51016; MTBLC3419; MTBLC136949; MTBLC135542; MTBLC135408; MTBLC17249; MTBLC614; MTBLC3293; MTBLC34715; MTBLC9300; MTBLC39618; MTBLC663; MTBLC20092; MTBLC35057; MTBLC36152; MTBLC35067; MTBLC3245; MTBLC38363; MTBLC4892; MTBLC4352; MTBLC80493; MTBLC28766; MTBLC15437; MTBLC6090; MTBLC8198; MTBLC8333; MTBLC49005; MTBLC3251; MTBLC32061; MTBLC75529; MTBLC79637; MTBLC3302; MTBLC4409; MTBLC4748; MTBLC32288; MTBLC5178; MTBLC79484; MTBLC59781; MTBLC567361; MTBLC31184; MTBLC3002; MTBLC5944; MTBLC135161; MTBLC2538; MTBLC5980; MTBLC38545; MTBLC59297; MTBLC136009; MTBLC15641; MTBLC3190; MTBLC5988; MTBLC7889; MTBLC3205; MTBLC32047; MTBLC3189; MTBLC22584; MTBLC38209; MTBLC89227; MTBLC89226; MTBLC89265; MTBLC89264; MTBLC89386; MTBLC89404; MTBLC89349; MTBLC89348; MTBLC89329; MTBLC89346; MTBLC7751; MTBLC18144; MTBLC89312; MTBLC89182; MTBLC4575; MTBLC4909; MTBLC42944; MTBLC6777; MTBLC8872; MTBLC32309; MTBLC31969; MTBLC8878; MTBLC71003; MTBLC16874; MTBLC71981; MTBLC4877; MTBLC73713; MTBLC135149; MTBLC30764; MTBLC30763; MTBLC28508; MTBLC50205; MTBLC16914; MTBLC9126; MTBLC73752; MTBLC78774; MTBLC79112; MTBLC141205; MTBLC89206; MTBLC89891; MTBLC17998; MTBLC28857; MTBLC18099; MTBLC89215; MTBLC88528; MTBLC82344; MTBLC9878; MTBLC28276; MTBLC131951; MTBLC27540; MTBLC748; MTBLC34311; MTBLC2429; MTBLC5831; MTBLC29491; MTBLC3299; MTBLC3329; MTBLC8891; MTBLC31070; MTBLC138195; MTBLC137853; MTBLC34697; MTBLC41865; MTBLC73112; MTBLC143910; MTBLC142593; MTBLC3570; MTBLC10575; MTBLC16111; MTBLC3555; MTBLC6372; MTBLC35038; MTBLC63610; MTBLC79675; MTBLC79848; MTBLC34114; MTBLC64496; MTBLC143715; MTBLC135277; MTBLC5541; MTBLC135317; MTBLC6565; MTBLC29544; MTBLC138814; MTBLC79429; MTBLC34866; MTBLC78661; MTBLC80148; MTBLC79962; MTBLC137230; MTBLC83030; MTBLC10225; MTBLC75097; MTBLC75094; MTBLC78448; MTBLC80550; MTBLC29736; MTBLC32110; MTBLC60723; MTBLC77122; MTBLC80188; MTBLC6357; MTBLC28838; MTBLC138919; MTBLC80411; MTBLC27325; MTBLC27547; MTBLC29526; MTBLC29535; MTBLC70549; MTBLC3953; MTBLC16587; MTBLC80534; MTBLC2528; MTBLC27495; MTBLC8629; MTBLC27471; MTBLC36274; MTBLC89929; MTBLC7190; MTBLC79995; MTBLC6426; MTBLC39251; MTBLC39250; MTBLC42504; MTBLC79074; MTBLC247956; MTBLC72715; MTBLC73072; MTBLC9250; MTBLC27752; MTBLC31116; MTBLC94461; MTBLC37550; MTBLC34120; MTBLC4648; MTBLC5016; MTBLC51963; MTBLC81262; MTBLC81252; MTBLC81249; MTBLC81245; MTBLC89219; MTBLC136724; MTBLC81299; MTBLC81298; MTBLC36240; MTBLC81308; MTBLC16359; MTBLC138876; MTBLC81261; MTBLC88105; MTBLC137810; MTBLC22868; MTBLC81244; MTBLC134216; MTBLC81240; MTBLC137147; MTBLC87823; MTBLC3216; MTBLC75029; MTBLC34086; MTBLC75106; MTBLC136790; MTBLC73121; MTBLC73008; MTBLC78810; MTBLC76151; MTBLC15889; MTBLC136361; MTBLC64153; MTBLC52979; MTBLC582124; MTBLC84883; MTBLC53488; MTBLC79914; MTBLC79922; MTBLC61204; MTBLC30042; MTBLC2740; MTBLC17034; MTBLC73504; MTBLC79961; MTBLC137717; MTBLC135699; MTBLC89608; MTBLC137921; MTBLC20538; MTBLC64023; MTBLC2625; MTBLC135865; MTBLC37658; MTBLC80134; MTBLC62481; MTBLC10223; MTBLC27793; MTBLC10362; MTBLC6602; MTBLC7037; MTBLC8907; MTBLC65244; MTBLC27776; MTBLC52649; MTBLC31602; MTBLC80020; MTBLC4787; MTBLC75062; MTBLC86088; MTBLC75304; MTBLC138215; MTBLC136139; MTBLC3902; MTBLC29532; MTBLC29541; MTBLC65657; MTBLC9612; MTBLC732; MTBLC27783; MTBLC1684; MTBLC9901; MTBLC135424; MTBLC28371; MTBLC4384; MTBLC4747; MTBLC5540; MTBLC66682; MTBLC28373; MTBLC3115; MTBLC27799; MTBLC9455; MTBLC9644; MTBLC81242; MTBLC28834; MTBLC88098; MTBLC88102; MTBLC72724; MTBLC81258; MTBLC81276; MTBLC16755; MTBLC52023; MTBLC81256; MTBLC43419; MTBLC9907; MTBLC2364; MTBLC83267; MTBLC67554; MTBLC80214; MTBLC80215; MTBLC4851; MTBLC28753; MTBLC16835; MTBLC89266; MTBLC89273; MTBLC89275; MTBLC84525; MTBLC89410; MTBLC75385; MTBLC89353; MTBLC18197; MTBLC53042; MTBLC84372; MTBLC72797; MTBLC138421; MTBLC8484; MTBLC62739; MTBLC84875; MTBLC85058; MTBLC133136; MTBLC144310; MTBLC84262; MTBLC39246; MTBLC51340; MTBLC68565; MTBLC29582; MTBLC80164; MTBLC80133; MTBLC62505; MTBLC35331; MTBLC5760; MTBLC89656; MTBLC137056; MTBLC2440; MTBLC3948; MTBLC70548; MTBLC53041; MTBLC137855; MTBLC73858; MTBLC64561; MTBLC76076; MTBLC44811; MTBLC18081; MTBLC17495; MTBLC76325; MTBLC76986; MTBLC76218; MTBLC136990; MTBLC136991; MTBLC136988; MTBLC136989; MTBLC4356; MTBLC132492; MTBLC132493; MTBLC80086; MTBLC137161; MTBLC50108; MTBLC135810; MTBLC32065; MTBLC28292; MTBLC73060; MTBLC80206; MTBLC2987; MTBLC43602; MTBLC79548; MTBLC77254; MTBLC73262; MTBLC3946; MTBLC4668; MTBLC4669; MTBLC7522; MTBLC134518; MTBLC136105; MTBLC136110; MTBLC80082; MTBLC80079; MTBLC77996; MTBLC34979; MTBLC8711; MTBLC79875; MTBLC53487; MTBLC88685; MTBLC34031; MTBLC28805; MTBLC29027; MTBLC15577; MTBLC16286; MTBLC87046; MTBLC87289; MTBLC78242; MTBLC84863; MTBLC73215; MTBLC84945; MTBLC72714; MTBLC52717; MTBLC34894; MTBLC84392; MTBLC88784; MTBLC88783; MTBLC84417; MTBLC88368; MTBLC89231; MTBLC89212; MTBLC3441; MTBLC18430; MTBLC70069; MTBLC7868; MTBLC583; MTBLC2888; MTBLC3887; MTBLC4804; MTBLC39; MTBLC29457; MTBLC28364; MTBLC79531; MTBLC79820; MTBLC79590; MTBLC79957; MTBLC79761; MTBLC79913; MTBLC79540; MTBLC79701; MTBLC79417; MTBLC34183; MTBLC79526; MTBLC79705; MTBLC79558; MTBLC132927; MTBLC28987; MTBLC15417; MTBLC6039; MTBLC29615; MTBLC135283; MTBLC27436; MTBLC34849; MTBLC29653; MTBLC135282; MTBLC78258; MTBLC31946; MTBLC29660; MTBLC16179; MTBLC34980; MTBLC139131; MTBLC73676; MTBLC81253; MTBLC16325; MTBLC63598; MTBLC7731; MTBLC135233; MTBLC36461; MTBLC17415; MTBLC17626; MTBLC17204; MTBLC2424; MTBLC15670; MTBLC30838; MTBLC16600; MTBLC135704; MTBLC4429; MTBLC15414; MTBLC88735; MTBLC51805; MTBLC17685; MTBLC4391; MTBLC8038; MTBLC17858; MTBLC2669; MTBLC17631; MTBLC64835; MTBLC27603; MTBLC1683; MTBLC62974; MTBLC28087; MTBLC28460; MTBLC17164; MTBLC8809; MTBLC5762; MTBLC18261; MTBLC17201; MTBLC17196; MTBLC15737; MTBLC29045; MTBLC134287; MTBLC16929; MTBLC17143; MTBLC31173; MTBLC31278; MTBLC64977; MTBLC5320; MTBLC71166; MTBLC27480; MTBLC30449; MTBLC34291; MTBLC17397; MTBLC24814; MTBLC15604; MTBLC89185; MTBLC57826; MTBLC28825; MTBLC18347; MTBLC17191; MTBLC15603; MTBLC64348; MTBLC9122; MTBLC79874; MTBLC34141; MTBLC73773; MTBLC79786; MTBLC79448; MTBLC5120; MTBLC16899; MTBLC17924; MTBLC17505; MTBLC18202; MTBLC28789; MTBLC29864; MTBLC17702; MTBLC17151; MTBLC18403; MTBLC15963; MTBLC16138; MTBLC57653; MTBLC33917; MTBLC22357; MTBLC37690; MTBLC28061; MTBLC17925; MTBLC28729; MTBLC10295; MTBLC28645; MTBLC27667; MTBLC15903; MTBLC28994; MTBLC28563; MTBLC17393; MTBLC28385; MTBLC15824; MTBLC16824; MTBLC4139; MTBLC4167; MTBLC27611; MTBLC18004; MTBLC4194; MTBLC28014; MTBLC16024; MTBLC27605; MTBLC17317; MTBLC16443; MTBLC28458; MTBLC48095; MTBLC17234; MTBLC24978; MTBLC17357; MTBLC27987; MTBLC17268; MTBLC10642; MTBLC27922; MTBLC28354; MTBLC11424; MTBLC27806; MTBLC27816; MTBLC28816; MTBLC17053; MTBLC29990; MTBLC5159; MTBLC18012; MTBLC18300; MTBLC1241; MTBLC28791; MTBLC62637; MTBLC16015; MTBLC58724; MTBLC16439; MTBLC45441; MTBLC31882; MTBLC17981; MTBLC16264; MTBLC16650; MTBLC16287; MTBLC3421; MTBLC7500; MTBLC32059; MTBLC135923; MTBLC40957; MTBLC41938; MTBLC79970; MTBLC4289; MTBLC59276; MTBLC133622; MTBLC16654; MTBLC86537; MTBLC982; MTBLC17094; MTBLC28710; MTBLC37032; MTBLC27530; MTBLC30832; MTBLC68566; MTBLC17646; MTBLC86396; MTBLC89760; MTBLC79634; MTBLC79456; MTBLC79768; MTBLC79876; MTBLC34930; MTBLC137770; MTBLC32350; MTBLC33020; MTBLC1230; MTBLC16551; MTBLC39244; MTBLC28676; MTBLC18260; MTBLC27554; MTBLC77436; MTBLC18167; MTBLC36217; MTBLC71422; MTBLC36218; MTBLC18147; MTBLC17057; MTBLC4125; MTBLC21010; MTBLC17306; MTBLC4808; MTBLC133330; MTBLC28066; MTBLC16751; MTBLC28189; MTBLC17716; MTBLC6359; MTBLC18411; MTBLC6435; MTBLC25164; MTBLC28053; MTBLC7570; MTBLC18394; MTBLC17992; MTBLC17400; MTBLC28870; MTBLC3354; MTBLC5158; MTBLC2310; MTBLC89730; MTBLC11222; MTBLC53490; MTBLC5847; MTBLC31759; MTBLC5597; MTBLC79439; MTBLC45951; MTBLC34619; MTBLC28657; MTBLC27520; MTBLC42976; MTBLC16802; MTBLC3014; MTBLC2155; MTBLC2185; MTBLC2321; MTBLC135989; MTBLC6709; MTBLC6888; MTBLC79546; MTBLC79481; MTBLC81712; MTBLC6995; MTBLC6960; MTBLC35040; MTBLC3533; MTBLC35421; MTBLC33509; MTBLC48093; MTBLC33510; MTBLC33511; MTBLC34237; MTBLC15847; MTBLC57541; MTBLC71429; MTBLC102524; MTBLC134923; MTBLC134922; MTBLC80471; MTBLC43996; MTBLC18226; MTBLC17532; MTBLC30734; MTBLC134814; MTBLC37753; MTBLC27469; MTBLC16142; MTBLC17426; MTBLC28860; MTBLC20937; MTBLC47962; MTBLC4178; MTBLC16224; MTBLC21099; MTBLC24113; MTBLC33830; MTBLC24769; MTBLC28378; MTBLC85187; MTBLC15676; MTBLC29474; MTBLC17693; MTBLC16409; MTBLC17405; MTBLC2085; MTBLC34334; MTBLC20367; MTBLC28719; MTBLC137246; MTBLC29069; MTBLC30801; MTBLC29009; MTBLC17077; MTBLC46644; MTBLC33198; MTBLC24149; MTBLC24266; MTBLC24462; MTBLC18246; MTBLC681850; MTBLC9669; MTBLC52672; MTBLC32709; MTBLC31677; MTBLC8871; MTBLC27513; MTBLC77872; MTBLC60076; MTBLC613; MTBLC1945; MTBLC15937; MTBLC9513; MTBLC63624; MTBLC17748; MTBLC17293; MTBLC2555; MTBLC137768; MTBLC3158; MTBLC7785; MTBLC8256; MTBLC7821; MTBLC135842; MTBLC66773; MTBLC139; MTBLC16703; MTBLC531; MTBLC27380; MTBLC16885; MTBLC17332; MTBLC64833; MTBLC28782; MTBLC28793; MTBLC3528; MTBLC31005; MTBLC27680; MTBLC27649; MTBLC6364; MTBLC27931; MTBLC6731; MTBLC7912; MTBLC18154; MTBLC16634; MTBLC9859; MTBLC2913; MTBLC6076; MTBLC135714; MTBLC15532; MTBLC57385; MTBLC16043; MTBLC5457; MTBLC134255; MTBLC77131; MTBLC6791; MTBLC34048; MTBLC48541; MTBLC137772; MTBLC16547; MTBLC9957; MTBLC10366; MTBLC10423; MTBLC87625; MTBLC6859; MTBLC30860; MTBLC15741; MTBLC30347; MTBLC77780; MTBLC89639; MTBLC9735; MTBLC135111; MTBLC136292; MTBLC254496; MTBLC35034; MTBLC4364; MTBLC17506; MTBLC57874; MTBLC58330; MTBLC18321; MTBLC15934; MTBLC6819; MTBLC30527; MTBLC2653; MTBLC39462; MTBLC79807; MTBLC3897; MTBLC8380; MTBLC57831; MTBLC15362; MTBLC8478; MTBLC37079; MTBLC33033; MTBLC16530; MTBLC27401; MTBLC39153; MTBLC45630; MTBLC48058; MTBLC27444; MTBLC41607; MTBLC705; MTBLC5954; MTBLC50885; MTBLC135324; MTBLC78158; MTBLC836; MTBLC3276; MTBLC3614; MTBLC89060; MTBLC89499; MTBLC799; MTBLC34139; MTBLC79668; MTBLC79797; MTBLC136980; MTBLC1189; MTBLC136972; MTBLC79907; MTBLC63641; MTBLC79715; MTBLC2495; MTBLC79887; MTBLC9460; MTBLC57958; MTBLC6650; MTBLC32242; MTBLC2431; MTBLC34801; MTBLC63622; MTBLC79719; MTBLC34321; MTBLC5810; MTBLC17871; MTBLC30966; MTBLC27957; MTBLC18419; MTBLC30768; MTBLC137814; MTBLC86348; MTBLC86391; MTBLC36532; MTBLC27904; MTBLC16023; MTBLC27378; MTBLC28587; MTBLC3641; MTBLC9653; MTBLC135517; MTBLC3918; MTBLC79692; MTBLC79988; MTBLC9961; MTBLC16546; MTBLC18428; MTBLC28102; MTBLC37165; MTBLC28808; MTBLC90185; MTBLC6838; MTBLC1547; MTBLC2076; MTBLC63581; MTBLC141154; MTBLC8049; MTBLC16992; MTBLC30841; MTBLC30794; MTBLC135928; MTBLC6628; MTBLC57905; MTBLC84094; MTBLC8341; MTBLC79347; MTBLC68606; MTBLC610092; MTBLC139380; MTBLC73758; MTBLC15436; MTBLC27630; MTBLC32398; MTBLC15366; MTBLC17071; MTBLC15586; MTBLC29003; MTBLC16699; MTBLC17647; MTBLC35173; MTBLC17084; MTBLC58511; MTBLC15584; MTBLC16292; MTBLC27736; MTBLC16392; MTBLC15867; MTBLC6177; MTBLC37434; MTBLC47518; MTBLC31441; MTBLC75988; MTBLC80438; MTBLC3978; MTBLC80441; MTBLC133224; MTBLC31743; MTBLC80528; MTBLC6553; MTBLC133244; MTBLC28527; MTBLC135754; MTBLC27994; MTBLC66905; MTBLC3439; MTBLC27475; MTBLC28426; MTBLC80434; MTBLC5065; MTBLC17965; MTBLC31742; MTBLC30200; MTBLC75790; MTBLC7781; MTBLC17558; MTBLC43136; MTBLC17456; MTBLC18320; MTBLC31784; MTBLC2905; MTBLC101278; MTBLC31901; MTBLC34474; MTBLC34511; MTBLC79863; MTBLC57681; MTBLC16211; MTBLC16773; MTBLC16898; MTBLC3697; MTBLC44932; MTBLC53770; MTBLC31682; MTBLC79369; MTBLC13714; MTBLC63609; MTBLC16856; MTBLC32153; MTBLC6413; MTBLC80592; MTBLC51032; MTBLC79929; MTBLC10285; MTBLC2883; MTBLC135745; MTBLC34574; MTBLC31359; MTBLC31849; MTBLC4708; MTBLC5384; MTBLC151; MTBLC160; MTBLC15622; MTBLC35453; MTBLC18281; MTBLC17305; MTBLC41893; MTBLC42819; MTBLC57992; MTBLC30769; MTBLC30887; MTBLC7814; MTBLC1670; MTBLC73757; MTBLC21305; MTBLC18050; MTBLC33138; MTBLC15607; MTBLC52222; MTBLC36458; MTBLC30835; MTBLC36455; MTBLC25311; MTBLC30314; MTBLC18043; MTBLC16352; MTBLC37011; MTBLC16010; MTBLC94613; MTBLC6151; MTBLC139123; MTBLC30845; MTBLC30846; MTBLC28459; MTBLC58560; MTBLC17798; MTBLC10072; MTBLC29513; MTBLC58556; MTBLC17533; MTBLC52859; MTBLC17802; MTBLC16704; MTBLC86004; MTBLC9274; MTBLC9275; MTBLC35014; MTBLC73688; MTBLC135289; MTBLC2506; MTBLC2769; MTBLC9045; MTBLC141; MTBLC89487; MTBLC30821; MTBLC79630; MTBLC1734; MTBLC12257; MTBLC133809; MTBLC135613; MTBLC50742; MTBLC131508; MTBLC34262; MTBLC27951; MTBLC15623; MTBLC15624; MTBLC16715; MTBLC27583; MTBLC16278; MTBLC17782; MTBLC22652; MTBLC17039; MTBLC18268; MTBLC73681; MTBLC17801; MTBLC45969; MTBLC21241; MTBLC27797; MTBLC30923; MTBLC4083; MTBLC28411; MTBLC36622; MTBLC58468; MTBLC18383; MTBLC135643; MTBLC34170; MTBLC87820; MTBLC79702; MTBLC31215; MTBLC4919; MTBLC8880; MTBLC1656; MTBLC49003; MTBLC17032; MTBLC16609; MTBLC27972; MTBLC16622; MTBLC27453; MTBLC16669; MTBLC17011; MTBLC16222; MTBLC15895; MTBLC15945; MTBLC16165; MTBLC16217; MTBLC28991; MTBLC24150; MTBLC5571; MTBLC5711; MTBLC48657; MTBLC8355; MTBLC29484; MTBLC17413; MTBLC16444; MTBLC17281; MTBLC17667; MTBLC17655; MTBLC111517; MTBLC741548; MTBLC17859; MTBLC91315; MTBLC75146; MTBLC76138; MTBLC15582; MTBLC15583; MTBLC57424; MTBLC49076; MTBLC18104; MTBLC18078; MTBLC17023; MTBLC27861; MTBLC27550; MTBLC15591; MTBLC16831; MTBLC89205; MTBLC138367; MTBLC28381; MTBLC59051; MTBLC30997; MTBLC6452; MTBLC17937; MTBLC3088; MTBLC50271; MTBLC69499; MTBLC4994; MTBLC6008; MTBLC7161; MTBLC80222; MTBLC473990; MTBLC17433; MTBLC30751; MTBLC28624; MTBLC135926; MTBLC143968; MTBLC17705; MTBLC57303; MTBLC15426; MTBLC6049; MTBLC7851; MTBLC3364; MTBLC4888; MTBLC134865; MTBLC5862; MTBLC16828; MTBLC79441; MTBLC9935; MTBLC7564; MTBLC16719; MTBLC31046; MTBLC34288; MTBLC86365; MTBLC17308; MTBLC35932; MTBLC28422; MTBLC48430; MTBLC15888; MTBLC17075; MTBLC18322; MTBLC29024; MTBLC4893; MTBLC15825; MTBLC16486; MTBLC89540; MTBLC15637; MTBLC63606; MTBLC45981; MTBLC8772; MTBLC4071; MTBLC3748; MTBLC51141; MTBLC89917; MTBLC9603; MTBLC2801; MTBLC92373; MTBLC2724; MTBLC90086; MTBLC16820; MTBLC7986; MTBLC82603; MTBLC3746; MTBLC8955; MTBLC37923; MTBLC10026; MTBLC35028; MTBLC10022; MTBLC34712; MTBLC60069; MTBLC6891; MTBLC16389; MTBLC43468; MTBLC35128; MTBLC28652; MTBLC35121; MTBLC28635; MTBLC30850; MTBLC4822; MTBLC6617; MTBLC34596; MTBLC34597; MTBLC50729; MTBLC28463; MTBLC135497; MTBLC34379; MTBLC25357; MTBLC27504; MTBLC5138; MTBLC81321; MTBLC5321; MTBLC58778; MTBLC8982; MTBLC9783; MTBLC31113; MTBLC8393; MTBLC44185; MTBLC79670; MTBLC7577; MTBLC79483; MTBLC60078; MTBLC135464; MTBLC82864; MTBLC135383; MTBLC4682; MTBLC76258; MTBLC135151; MTBLC27683; MTBLC15999; MTBLC16433; MTBLC15365; MTBLC58129; MTBLC17395; MTBLC89749; MTBLC58642; MTBLC137819; MTBLC88868; MTBLC70851; MTBLC15566; MTBLC68502; MTBLC68503; MTBLC36165; MTBLC17878; MTBLC17611; MTBLC17915; MTBLC85235; MTBLC38355; MTBLC49283; MTBLC143856; MTBLC61206; MTBLC7773; MTBLC17990; MTBLC15711; MTBLC18412; MTBLC94706; MTBLC40521; MTBLC7470; MTBLC31592; MTBLC16252; MTBLC57621; MTBLC27949; MTBLC9725; MTBLC40947; MTBLC32019; MTBLC3154; MTBLC8682; MTBLC6737; MTBLC8205; MTBLC16279; MTBLC2697; MTBLC2722; MTBLC6080; MTBLC8822; MTBLC52070; MTBLC9912; MTBLC8247; MTBLC32003; MTBLC15645; MTBLC2735; MTBLC17340; MTBLC3868; MTBLC6563; MTBLC8339; MTBLC59583; MTBLC45257; MTBLC3451; MTBLC141529; MTBLC137236; MTBLC18026; MTBLC17189; MTBLC68465; MTBLC36062; MTBLC17253; MTBLC16509; MTBLC133083; MTBLC86542; MTBLC131434; MTBLC17869; MTBLC59783; MTBLC55534; MTBLC28707; MTBLC27909; MTBLC16182; MTBLC16638; MTBLC16133; MTBLC16472; MTBLC87755; MTBLC84069; MTBLC16019; MTBLC46941; MTBLC134808; MTBLC64390; MTBLC136818; MTBLC136917; MTBLC17786; MTBLC9367; MTBLC138495; MTBLC43533; MTBLC17945; MTBLC37419; MTBLC85162; MTBLC23757; MTBLC5826; MTBLC62069; MTBLC223316; MTBLC135072; MTBLC75; MTBLC2702; MTBLC27920; MTBLC5557; MTBLC34405; MTBLC34788; MTBLC2527; MTBLC67461; MTBLC17727; MTBLC34921; MTBLC15932; MTBLC7513; MTBLC9047; MTBLC31433; MTBLC80391; MTBLC3384; MTBLC2156; MTBLC2368; MTBLC6003; MTBLC2532; MTBLC2821; MTBLC3287; MTBLC6511; MTBLC79609; MTBLC135445; MTBLC7628; MTBLC133152; MTBLC80000; MTBLC7421; MTBLC71498; MTBLC17335; MTBLC3103; MTBLC62251; MTBLC17531; MTBLC29458; MTBLC15830; MTBLC134834; MTBLC34769; MTBLC46750; MTBLC7952; MTBLC8186; MTBLC32249; MTBLC15884; MTBLC28865; MTBLC21484; MTBLC15874; MTBLC2469; MTBLC5093; MTBLC63630; MTBLC2294; MTBLC2425; MTBLC16363; MTBLC2629; MTBLC69335; MTBLC28356; MTBLC4441; MTBLC135002; MTBLC10058; MTBLC10076; MTBLC10103; MTBLC28714; MTBLC34550; MTBLC2515; MTBLC79698; MTBLC8173; MTBLC18328; MTBLC2672; MTBLC6369; MTBLC7659; MTBLC9468; MTBLC82542; MTBLC63628; MTBLC6109; MTBLC7609; MTBLC28064; MTBLC16726; MTBLC28596; MTBLC17379; MTBLC31788; MTBLC7910; MTBLC134007; MTBLC7951; MTBLC133365; MTBLC75439; MTBLC69814; MTBLC16631; MTBLC135701; MTBLC16778; MTBLC18330; MTBLC4783; MTBLC27514; MTBLC5304; MTBLC31967; MTBLC16954; MTBLC3740; MTBLC4320; MTBLC24293; MTBLC79936; MTBLC34236; MTBLC51016; MTBLC3419; MTBLC136949; MTBLC135542; MTBLC135408; MTBLC17249; MTBLC614; MTBLC3293; MTBLC34715; MTBLC9300; MTBLC39618; MTBLC663; MTBLC20092; MTBLC35057; MTBLC36152; MTBLC35067; MTBLC3245; MTBLC27804; MTBLC38363; MTBLC4892; MTBLC4352; MTBLC34580; MTBLC27993; MTBLC82684; MTBLC135703; MTBLC80493; MTBLC87947; MTBLC28766; MTBLC15437; MTBLC6090; MTBLC8198; MTBLC8333; MTBLC49005; MTBLC3251; MTBLC32061; MTBLC75529; MTBLC79637; MTBLC3302; MTBLC4409; MTBLC4748; MTBLC32288; MTBLC5178; MTBLC79484; MTBLC17713; MTBLC10037; MTBLC8922; MTBLC7471; MTBLC59781; MTBLC31563; MTBLC6863; MTBLC567361; MTBLC31184; MTBLC3002; MTBLC5944; MTBLC135161; MTBLC2538; MTBLC5980; MTBLC38545; MTBLC59297; MTBLC136009; MTBLC15641; MTBLC3190; MTBLC5988; MTBLC7889; MTBLC3205; MTBLC32047; MTBLC3189; MTBLC22584; MTBLC38209; MTBLC89227; MTBLC89226; MTBLC89265; MTBLC89264; MTBLC89386; MTBLC89404; MTBLC89349; MTBLC89348; MTBLC89329; MTBLC89346; MTBLC7751; MTBLC18144; MTBLC89312; MTBLC89182; MTBLC78700; MTBLC55523; MTBLC31896; MTBLC9108; MTBLC9946; MTBLC847; MTBLC9205; MTBLC4575; MTBLC4909; MTBLC42944; MTBLC6777; MTBLC8872; MTBLC32309; MTBLC31969; MTBLC8878; MTBLC79612; MTBLC18054; MTBLC3430; MTBLC6965; MTBLC71003; MTBLC16874; MTBLC71981; MTBLC4877; MTBLC73713; MTBLC4417; MTBLC31298; MTBLC8713; MTBLC79465; MTBLC4773; MTBLC5527; MTBLC9959; MTBLC31086; MTBLC2626; MTBLC8402; MTBLC32185; MTBLC48131; MTBLC86544; MTBLC29564; MTBLC31447; MTBLC73; MTBLC30725; MTBLC34968; MTBLC135149; MTBLC6798; MTBLC91807; MTBLC2939; MTBLC30764; MTBLC30763; MTBLC28508; MTBLC50205; MTBLC16914; MTBLC9126; MTBLC73752; MTBLC78774; MTBLC79112; MTBLC141205; MTBLC89206; MTBLC89891; MTBLC17998; MTBLC28857; MTBLC18099; MTBLC89215; MTBLC88528; MTBLC82344; MTBLC9878; MTBLC28276; MTBLC1749; MTBLC8602; MTBLC17467; MTBLC34605; MTBLC9425; MTBLC34252; MTBLC34256; MTBLC79445; MTBLC131951; MTBLC27540; MTBLC31049; MTBLC748; MTBLC34311; MTBLC2429; MTBLC5831; MTBLC29491; MTBLC3299; MTBLC3329; MTBLC8891; MTBLC18227; MTBLC94661; MTBLC31070; MTBLC138195; MTBLC137853; MTBLC142272; MTBLC34697; MTBLC41865; MTBLC73112; MTBLC143910; MTBLC142593; MTBLC3570; MTBLC10575; MTBLC16111; MTBLC138422; MTBLC3555; MTBLC6372; MTBLC3284; MTBLC15809; MTBLC135723; MTBLC90233; MTBLC137178; MTBLC82985; MTBLC35038; MTBLC79471; MTBLC79566; MTBLC63610; MTBLC79675; MTBLC79848; MTBLC34114; MTBLC64496; MTBLC143715; MTBLC135277; MTBLC4819; MTBLC5541; MTBLC18171; MTBLC32086; MTBLC5206; MTBLC135317; MTBLC6565; MTBLC8621; MTBLC89382; MTBLC89352; MTBLC89368; MTBLC89366; MTBLC89340; MTBLC89317; MTBLC29544; MTBLC138814; MTBLC136905; MTBLC133325; MTBLC135350; MTBLC79177; MTBLC84854; MTBLC34295; MTBLC29479; MTBLC17903; MTBLC4045; MTBLC10445; MTBLC6706; MTBLC79429; MTBLC34866; MTBLC34499; MTBLC34503; MTBLC34506; MTBLC91217; MTBLC138082; MTBLC79519; MTBLC34293; MTBLC34294; MTBLC78661; MTBLC73794; MTBLC80148; MTBLC34229; MTBLC138081; MTBLC79962; MTBLC137230; MTBLC83030; MTBLC10225; MTBLC448; MTBLC72665; MTBLC138258; MTBLC138255; MTBLC72663; MTBLC133381; MTBLC133086; MTBLC75097; MTBLC75094; MTBLC78448; MTBLC80550; MTBLC29736; MTBLC15658; MTBLC15655; MTBLC15657; MTBLC64008; MTBLC138786; MTBLC88461; MTBLC34148; MTBLC91272; MTBLC34485; MTBLC34498; MTBLC34500; MTBLC88440; MTBLC34504; MTBLC143972; MTBLC88465; MTBLC32110; MTBLC16089; MTBLC60723; MTBLC77122; MTBLC80188; MTBLC6357; MTBLC28838; MTBLC138919; MTBLC80411; MTBLC27325; MTBLC27547; MTBLC82763; MTBLC29526; MTBLC29535; MTBLC70549; MTBLC131659; MTBLC15575; MTBLC2513; MTBLC2492; MTBLC5166; MTBLC3953; MTBLC16587; MTBLC80534; MTBLC2528; MTBLC27495; MTBLC8629; MTBLC63916; MTBLC27471; MTBLC36274; MTBLC89929; MTBLC34920; MTBLC6088; MTBLC7190; MTBLC79995; MTBLC6426; MTBLC692; MTBLC39251; MTBLC39250; MTBLC42504; MTBLC75219; MTBLC30805; MTBLC140088; MTBLC74966; MTBLC34163; MTBLC31561; MTBLC135525; MTBLC8039; MTBLC17457; MTBLC4453; MTBLC9261; MTBLC48742; MTBLC52421; MTBLC79074; MTBLC474014; MTBLC247956; MTBLC83058; MTBLC2366; MTBLC72715; MTBLC73072; MTBLC64483; MTBLC131738; MTBLC64489; MTBLC78103; MTBLC58206; MTBLC9250; MTBLC1418; MTBLC27752; MTBLC31116; MTBLC84299; MTBLC58303; MTBLC46979; MTBLC136623; MTBLC94461; MTBLC37550; MTBLC64124; MTBLC46961; MTBLC65247; MTBLC32345; MTBLC4746; MTBLC80169; MTBLC34120; MTBLC85403; MTBLC74971; MTBLC4648; MTBLC5016; MTBLC51963; MTBLC71025; MTBLC73792; MTBLC137845; MTBLC81262; MTBLC81252; MTBLC81249; MTBLC81245; MTBLC89219; MTBLC136724; MTBLC81299; MTBLC81298; MTBLC36240; MTBLC81308; MTBLC16359; MTBLC138876; MTBLC81261; MTBLC88105; MTBLC137810; MTBLC22868; MTBLC81244; MTBLC134216; MTBLC81240; MTBLC28468; MTBLC64563; MTBLC76078; MTBLC72998; MTBLC78101; MTBLC134424; MTBLC134423; MTBLC133456; MTBLC88698; MTBLC88697; MTBLC137147; MTBLC87823; MTBLC3216; MTBLC76334; MTBLC73135; MTBLC34097; MTBLC75029; MTBLC34086; MTBLC75106; MTBLC136790; MTBLC73121; MTBLC73008; MTBLC78810; MTBLC49265; MTBLC15654; MTBLC88462; MTBLC80442; MTBLC84441; MTBLC72641; MTBLC136531; MTBLC72815; MTBLC80463; MTBLC76234; MTBLC34491; MTBLC88441; MTBLC80447; MTBLC88438; MTBLC72843; MTBLC72842; MTBLC88460; MTBLC60956; MTBLC133329; MTBLC76151; MTBLC15889; MTBLC136361; MTBLC64153; MTBLC1309; MTBLC1310; MTBLC52979; MTBLC49254; MTBLC28724; MTBLC136767; MTBLC85633; MTBLC84874; MTBLC70850; MTBLC85057; MTBLC32365; MTBLC90027; MTBLC582124; MTBLC84883; MTBLC53488; MTBLC79914; MTBLC79922; MTBLC61204; MTBLC30042; MTBLC79179; MTBLC84855; MTBLC2740; MTBLC17034; MTBLC73504; MTBLC131692; MTBLC74330; MTBLC62834; MTBLC77492; MTBLC73741; MTBLC10087; MTBLC73851; MTBLC84752; MTBLC27706; MTBLC38299; MTBLC137495; MTBLC34154; MTBLC72639; MTBLC133357; MTBLC34494; MTBLC78730; MTBLC34496; MTBLC72651; MTBLC79961; MTBLC79513; MTBLC137717; MTBLC135699; MTBLC75612; MTBLC52392; MTBLC89608; MTBLC67309; MTBLC3940; MTBLC137921; MTBLC7909; MTBLC20538; MTBLC73092; MTBLC31501; MTBLC88109; MTBLC31297; MTBLC64023; MTBLC2625; MTBLC135865; MTBLC37658; MTBLC80134; MTBLC62481; MTBLC10223; MTBLC27793; MTBLC10362; MTBLC6602; MTBLC7037; MTBLC8907; MTBLC65244; MTBLC27776; MTBLC90454; MTBLC75376; MTBLC32157; MTBLC31279; MTBLC17058; MTBLC28688; MTBLC7720; MTBLC34835; MTBLC76090; MTBLC37998; MTBLC9951; MTBLC52649; MTBLC31602; MTBLC80020; MTBLC72828; MTBLC72952; MTBLC72736; MTBLC133144; MTBLC75036; MTBLC131924; MTBLC4787; MTBLC75062; MTBLC86088; MTBLC75304; MTBLC138215; MTBLC136139; MTBLC89521; MTBLC86095; MTBLC88906; MTBLC89602; MTBLC89539; MTBLC89536; MTBLC3902; MTBLC29532; MTBLC29541; MTBLC65657; MTBLC9612; MTBLC90040; MTBLC732; MTBLC27783; MTBLC1684; MTBLC9901; MTBLC135424; MTBLC89091; MTBLC75646; MTBLC89387; MTBLC89392; MTBLC89395; MTBLC89394; MTBLC134075; MTBLC90459; MTBLC134076; MTBLC134077; MTBLC134078; MTBLC39934; MTBLC134227; MTBLC134228; MTBLC16038; MTBLC137279; MTBLC137293; MTBLC28733; MTBLC28371; MTBLC4384; MTBLC28610; MTBLC86255; MTBLC76071; MTBLC143713; MTBLC72589; MTBLC131658; MTBLC4747; MTBLC5540; MTBLC66682; MTBLC28373; MTBLC3115; MTBLC27799; MTBLC73134; MTBLC73004; MTBLC62837; MTBLC78270; MTBLC36476; MTBLC79536; MTBLC73894; MTBLC9455; MTBLC9644; MTBLC1107; MTBLC31676; MTBLC50782; MTBLC31650; MTBLC6574; MTBLC31940; MTBLC81242; MTBLC28834; MTBLC88098; MTBLC88102; MTBLC72724; MTBLC58876; MTBLC81258; MTBLC81276; MTBLC16755; MTBLC52023; MTBLC81256; MTBLC43419; MTBLC9907; MTBLC27965; MTBLC744; MTBLC2364; MTBLC83267; MTBLC67554; MTBLC80214; MTBLC80215; MTBLC4851; MTBLC28753; MTBLC16835; MTBLC84519; MTBLC89266; MTBLC89273; MTBLC89275; MTBLC84525; MTBLC89410; MTBLC75385; MTBLC89353; MTBLC75038; MTBLC133623; MTBLC84577; MTBLC84234; MTBLC143985; MTBLC18197; MTBLC53042; MTBLC143980; MTBLC84372; MTBLC72797; MTBLC138421; MTBLC34004; MTBLC85639; MTBLC45478; MTBLC79312; MTBLC30820; MTBLC50576; MTBLC138260; MTBLC82464; MTBLC28592; MTBLC8484; MTBLC62739; MTBLC3427; MTBLC86197; MTBLC86196; MTBLC86189; MTBLC86190; MTBLC86188; MTBLC29613; MTBLC79453; MTBLC28047; MTBLC132620; MTBLC5783; MTBLC80531; MTBLC16688; MTBLC28135; MTBLC137137; MTBLC139534; MTBLC31731; MTBLC73923; MTBLC31801; MTBLC35459; MTBLC144339; MTBLC9194; MTBLC84875; MTBLC85058; MTBLC133136; MTBLC144310; MTBLC84262; MTBLC39246; MTBLC51340; MTBLC68565; MTBLC29582; MTBLC80164; MTBLC80133; MTBLC62505; MTBLC35331; MTBLC5760; MTBLC89656; MTBLC137056; MTBLC86418; MTBLC89703; MTBLC89592; MTBLC89589; MTBLC89384; MTBLC89098; MTBLC89143; MTBLC89070; MTBLC88726; MTBLC88872; MTBLC88588; MTBLC89498; MTBLC89502; MTBLC143982; MTBLC34041; MTBLC2440; MTBLC3948; MTBLC70548; MTBLC53041; MTBLC143989; MTBLC143981; MTBLC143983; MTBLC143987; MTBLC143990; MTBLC137855; MTBLC73858; MTBLC64561; MTBLC76076; MTBLC44811; MTBLC18081; MTBLC17495; MTBLC76325; MTBLC76986; MTBLC76218; MTBLC84566; MTBLC137216; MTBLC85680; MTBLC136990; MTBLC136991; MTBLC136988; MTBLC136989; MTBLC4356; MTBLC84877; MTBLC39248; MTBLC132492; MTBLC132493; MTBLC131689; MTBLC74340; MTBLC131668; MTBLC131687; MTBLC131688; MTBLC83055; MTBLC80086; MTBLC137161; MTBLC11152; MTBLC50108; MTBLC135810; MTBLC32065; MTBLC28292; MTBLC31550; MTBLC73060; MTBLC6991; MTBLC64032; MTBLC73736; MTBLC80206; MTBLC3300; MTBLC9515; MTBLC2987; MTBLC43602; MTBLC3249; MTBLC52897; MTBLC79548; MTBLC77254; MTBLC73262; MTBLC3944; MTBLC3946; MTBLC4668; MTBLC4669; MTBLC7522; MTBLC5933; MTBLC73854; MTBLC134518; MTBLC136105; MTBLC136110; MTBLC80082; MTBLC80079; MTBLC77996; MTBLC8774; MTBLC137248; MTBLC34979; MTBLC8711; MTBLC79875; MTBLC53487; MTBLC135165; MTBLC3845; MTBLC31831; MTBLC75565; MTBLC137215; MTBLC135498; MTBLC88685; MTBLC34031; MTBLC28805; MTBLC29027; MTBLC15577; MTBLC16286; MTBLC87046; MTBLC87289; MTBLC78242; MTBLC84863; MTBLC72837; MTBLC73215; MTBLC69081; MTBLC75542; MTBLC74274; MTBLC84945; MTBLC72714; MTBLC52717; MTBLC34894; MTBLC84392; MTBLC88784; MTBLC88783; MTBLC84417; MTBLC88368; MTBLC89231; MTBLC89212; MTBLC3441; MTBLC18430; MTBLC70069; MTBLC34322; MTBLC7868; MTBLC583; MTBLC2888; MTBLC3887; MTBLC4804; MTBLC39; MTBLC60025; MTBLC29457; MTBLC28364; MTBLC79531; MTBLC79820; MTBLC79590; MTBLC79957; MTBLC79761; MTBLC79913; MTBLC79540; MTBLC79701; MTBLC79417; MTBLC34183; MTBLC79526; MTBLC79705; MTBLC79558; MTBLC132927; MTBLC28987; MTBLC61330; MTBLC15417; MTBLC6039; MTBLC29615; MTBLC135283; MTBLC27436; MTBLC34849; MTBLC29653; MTBLC135282; MTBLC78258; MTBLC31946; MTBLC29660; MTBLC16179; MTBLC34980; MTBLC75342; MTBLC139131; MTBLC29744; MTBLC73676; MTBLC81253; MTBLC16325; MTBLC44526; MTBLC83063; MTBLC38394; MTBLC142447; MTBLC24993; MTBLC138083; MTBLC38362; MTBLC82749; MTBLC32798; MTBLC88464; MTBLC86141; MTBLC27939; MTBLC75108; MTBLC6673; MTBLC28801; MTBLC52639; MTBLC86455; MTBLC63598; MTBLC7731; MTBLC15843; MTBLC79754; MTBLC79694; MTBLC1182; MTBLC79480; MTBLC79869; MTBLC82835; MTBLC2451; MTBLC36033; MTBLC31825; MTBLC135293; MTBLC34834; MTBLC34838; MTBLC30041; MTBLC135233; MTBLC9738; MTBLC6389; MTBLC7454; MTBLC79582; MTBLC34530; MTBLC70708; MTBLC9234; MTBLC4724; MTBLC8411; MTBLC62439; MTBLC73358; MTBLC5613; MTBLC6414; MTBLC63607; MTBLC84701; MTBLC28727; MTBLC28194; MTBLC27997; MTBLC16196; MTBLC82617; MTBLC50575; MTBLC32375; MTBLC50464; MTBLC29735; MTBLC30829; MTBLC28193; MTBLC50572; MTBLC36023; MTBLC80539; MTBLC7954; MTBLC53486; MTBLC53460; MTBLC79878; MTBLC79900; MTBLC525464; MTBLC79409; MTBLC79578; MTBLC82832; MTBLC71589; MTBLC32023; MTBLC134218; MTBLC73000; MTBLC140861; MTBLC75026; MTBLC134231; MTBLC134232; MTBLC137779; MTBLC134229; MTBLC88935; MTBLC86119; MTBLC86121; MTBLC89734; MTBLC86117; MTBLC78022; MTBLC89691; MTBLC84831; MTBLC74670; MTBLC89599; MTBLC89597; MTBLC89548; MTBLC89438; MTBLC89078; MTBLC89127; MTBLC89177; MTBLC88712; MTBLC9916; MTBLC75092; MTBLC34262; MTBLC27951; MTBLC27797; MTBLC16713; MTBLC57999; MTBLC34454; MTBLC47220; MTBLC28967; MTBLC37144; MTBLC28960; MTBLC28905; MTBLC15368; MTBLC57841; MTBLC1217; MTBLC44692; MTBLC45285; MTBLC1467; MTBLC17214; MTBLC72700; MTBLC16119; MTBLC16199; MTBLC16607; MTBLC16610; MTBLC4614; MTBLC19092; MTBLC28638; MTBLC30322; MTBLC17203; MTBLC1439; MTBLC37600; MTBLC27371; MTBLC16070; MTBLC74863; MTBLC27411; MTBLC15866; MTBLC28847; MTBLC28140; MTBLC18287; MTBLC42606; MTBLC27907; MTBLC27442; MTBLC27586; MTBLC137774; MTBLC63150; MTBLC17617; MTBLC16935; MTBLC62345; MTBLC17897; MTBLC27708; MTBLC9652; MTBLC17059; MTBLC58286; MTBLC16357; MTBLC15971; MTBLC17064; MTBLC30818; MTBLC89640; MTBLC27248; MTBLC31042; MTBLC16572; MTBLC1580; MTBLC1879; MTBLC26797; MTBLC17578; MTBLC34213; MTBLC27869; MTBLC15767; MTBLC16089; MTBLC2319; MTBLC5966; MTBLC16380; MTBLC17143; MTBLC31173; MTBLC31278; MTBLC64977; MTBLC5320; MTBLC71166; MTBLC27480; MTBLC16355; MTBLC2600; MTBLC133351; MTBLC17881; MTBLC28928; MTBLC27616; MTBLC16100; MTBLC17641; MTBLC90886; MTBLC1139; MTBLC1387; MTBLC17095; MTBLC76163; MTBLC114204; MTBLC34252; MTBLC34256; MTBLC79445; MTBLC34876; MTBLC34877; MTBLC3007; MTBLC8986; MTBLC31054; MTBLC2932; MTBLC60078; MTBLC31435; MTBLC6945; MTBLC8616; MTBLC9183; MTBLC5959; MTBLC5708; MTBLC7468; MTBLC88104; MTBLC139134; MTBLC73926; MTBLC139133; MTBLC82679; MTBLC137760; MTBLC82678; MTBLC79877; MTBLC17747; MTBLC34710; MTBLC34679; MTBLC34097; MTBLC16323; MTBLC18385; MTBLC43997; MTBLC80424; MTBLC134287; MTBLC16929; MTBLC508; MTBLC60872; MTBLC70824; MTBLC68451; MTBLC16852; MTBLC134850; MTBLC9008; MTBLC16181; MTBLC28393; MTBLC28328; MTBLC47977; MTBLC62324; MTBLC24103; MTBLC31747; MTBLC28945; MTBLC31997; MTBLC19332; MTBLC16467; MTBLC10454; MTBLC5121; MTBLC5139; MTBLC5356; MTBLC5358; MTBLC69039; MTBLC93403; MTBLC63112; MTBLC16870; MTBLC17874; MTBLC28057; MTBLC28586; MTBLC62976; MTBLC62006; MTBLC17321; MTBLC3017; MTBLC51805; MTBLC2302; MTBLC2304; MTBLC136582; MTBLC17913; MTBLC3766; MTBLC79576; MTBLC38159; MTBLC25426; MTBLC16060; MTBLC3703; MTBLC27509; MTBLC4740; MTBLC6931; MTBLC7906; MTBLC5578; MTBLC59560; MTBLC15372; MTBLC80385; MTBLC952; MTBLC1141; MTBLC27852; MTBLC41941; MTBLC86553; MTBLC30816; MTBLC16388; MTBLC20415; MTBLC1881; MTBLC89830; MTBLC44747; MTBLC32807; MTBLC17151; MTBLC18403; MTBLC15963; MTBLC16207; MTBLC17597; MTBLC30746; MTBLC16008; MTBLC79966; MTBLC46807; MTBLC133314; MTBLC19891; MTBLC16138; MTBLC57653; MTBLC33917; MTBLC22357; MTBLC37690; MTBLC28061; MTBLC17925; MTBLC28729; MTBLC10295; MTBLC28645; MTBLC27667; MTBLC15903; MTBLC28994; MTBLC28563; MTBLC17393; MTBLC28385; MTBLC15824; MTBLC16824; MTBLC4139; MTBLC4167; MTBLC27611; MTBLC18004; MTBLC4194; MTBLC28014; MTBLC16024; MTBLC27605; MTBLC17317; MTBLC16443; MTBLC28458; MTBLC48095; MTBLC17234; MTBLC24978; MTBLC17357; MTBLC27987; MTBLC17268; MTBLC10642; MTBLC27922; MTBLC25858; MTBLC28946; MTBLC28177; MTBLC17605; MTBLC18280; MTBLC8240; MTBLC28354; MTBLC11424; MTBLC27806; MTBLC27816; MTBLC28816; MTBLC40274; MTBLC30156; MTBLC44842; MTBLC17807; MTBLC20106; MTBLC68329; MTBLC16899; MTBLC17924; MTBLC17505; MTBLC18202; MTBLC28789; MTBLC29864; MTBLC6259; MTBLC17656; MTBLC32800; MTBLC18414; MTBLC28478; MTBLC19868; MTBLC27978; MTBLC17445; MTBLC1581; MTBLC18346; MTBLC85239; MTBLC20414; MTBLC35164; MTBLC18101; MTBLC40813; MTBLC20450; MTBLC17637; MTBLC31835; MTBLC31832; MTBLC8075; MTBLC29672; MTBLC17702; MTBLC28889; MTBLC17631; MTBLC64835; MTBLC27603; MTBLC1683; MTBLC62974; MTBLC28087; MTBLC28460; MTBLC17164; MTBLC15354; MTBLC16182; MTBLC16638; MTBLC16133; MTBLC16472; MTBLC87755; MTBLC84069; MTBLC16019; MTBLC46941; MTBLC53608; MTBLC79569; MTBLC17243; MTBLC134341; MTBLC88427; MTBLC34687; MTBLC79053; MTBLC4316; MTBLC10607; MTBLC88526; MTBLC32337; MTBLC10525; MTBLC27801; MTBLC29732; MTBLC2959; MTBLC52859; MTBLC80420; MTBLC2818; MTBLC17929; MTBLC25682; MTBLC81297; MTBLC17417; MTBLC144066; MTBLC142578; MTBLC18037; MTBLC3210; MTBLC3474; MTBLC8613; MTBLC2247; MTBLC17311; MTBLC35619; MTBLC138425; MTBLC27971; MTBLC27389; MTBLC16865; MTBLC33094; MTBLC28797; MTBLC37081; MTBLC5588; MTBLC17724; MTBLC15620; MTBLC138669; MTBLC17519; MTBLC37581; MTBLC17217; MTBLC16413; MTBLC23500; MTBLC16583; MTBLC36253; MTBLC46916; MTBLC478164; MTBLC17765; MTBLC15754; MTBLC24168; MTBLC4728; MTBLC134255; MTBLC77131; MTBLC15643; MTBLC33098; MTBLC39931; MTBLC86390; MTBLC30753; MTBLC35227; MTBLC30754; MTBLC42682; MTBLC134761; MTBLC18123; MTBLC32114; MTBLC47564; MTBLC139; MTBLC16703; MTBLC531; MTBLC27380; MTBLC16885; MTBLC17332; MTBLC64833; MTBLC28782; MTBLC28793; MTBLC3528; MTBLC31005; MTBLC27680; MTBLC27649; MTBLC6364; MTBLC27931; MTBLC6731; MTBLC7912; MTBLC18154; MTBLC16634; MTBLC9859; MTBLC32059; MTBLC83804; MTBLC16546; MTBLC18428; MTBLC28102; MTBLC37165; MTBLC28808; MTBLC90185; MTBLC141517; MTBLC50663; MTBLC4954; MTBLC135681; MTBLC73275; MTBLC140748; MTBLC7982; MTBLC31576; MTBLC135209; MTBLC137782; MTBLC23875; MTBLC73892; MTBLC33020; MTBLC1230; MTBLC16551; MTBLC39244; MTBLC28676; MTBLC18260; MTBLC27554; MTBLC77436; MTBLC18167; MTBLC36217; MTBLC71422; MTBLC36218; MTBLC18147; MTBLC17057; MTBLC4125; MTBLC21010; MTBLC17306; MTBLC4808; MTBLC133330; MTBLC28066; MTBLC16751; MTBLC28189; MTBLC17716; MTBLC6359; MTBLC18411; MTBLC6435; MTBLC25164; MTBLC28053; MTBLC7570; MTBLC18394; MTBLC17992; MTBLC5105; MTBLC143968; MTBLC17705; MTBLC16708; MTBLC16347; MTBLC73707; MTBLC89341; MTBLC16817; MTBLC6907; MTBLC80354; MTBLC31085; MTBLC2089; MTBLC4055; MTBLC48294; MTBLC35090; MTBLC6415; MTBLC75627; MTBLC16246; MTBLC16772; MTBLC20582; MTBLC111; MTBLC18427; MTBLC28310; MTBLC18266; MTBLC15975; MTBLC28762; MTBLC28548; MTBLC43943; MTBLC17540; MTBLC320055; MTBLC27732; MTBLC126237; MTBLC36090; MTBLC137825; MTBLC36633; MTBLC28323; MTBLC28873; MTBLC58152; MTBLC23401; MTBLC32815; MTBLC30851; MTBLC18125; MTBLC47928; MTBLC32374; MTBLC18697; MTBLC882; MTBLC15980; MTBLC1416; MTBLC27778; MTBLC59052; MTBLC25351; MTBLC6933; MTBLC15607; MTBLC52222; MTBLC36458; MTBLC30835; MTBLC36455; MTBLC25311; MTBLC30314; MTBLC5958; MTBLC29717; MTBLC27645; MTBLC30906; MTBLC30940; MTBLC29722; MTBLC28176; MTBLC29724; MTBLC15798; MTBLC77671; MTBLC18128; MTBLC16590; MTBLC3693; MTBLC17989; MTBLC4853; MTBLC139533; MTBLC17618; MTBLC4117; MTBLC82348; MTBLC5673; MTBLC64305; MTBLC3337; MTBLC138529; MTBLC15567; MTBLC17275; MTBLC4607; MTBLC87897; MTBLC37331; MTBLC16939; MTBLC44303; MTBLC82573; MTBLC134821; MTBLC16795; MTBLC17895; MTBLC89461; MTBLC134820; MTBLC34019; MTBLC74516; MTBLC2628; MTBLC3244; MTBLC28709; MTBLC5989; MTBLC7502; MTBLC3546; MTBLC137728; MTBLC27468; MTBLC27578; MTBLC28474; MTBLC16364; MTBLC17681; MTBLC29053; MTBLC28630; MTBLC36751; MTBLC52143; MTBLC62768; MTBLC62770; MTBLC27747; MTBLC28229; MTBLC139383; MTBLC17115; MTBLC29480; MTBLC17960; MTBLC32816; MTBLC6604; MTBLC34867; MTBLC2196; MTBLC39564; MTBLC94764; MTBLC139388; MTBLC74076; MTBLC73580; MTBLC6257; MTBLC28346; MTBLC6792; MTBLC6839; MTBLC18106; MTBLC17286; MTBLC87407; MTBLC4683; MTBLC7797; MTBLC10044; MTBLC3697; MTBLC6765; MTBLC31030; MTBLC28462; MTBLC5792; MTBLC5979; MTBLC31827; MTBLC109895; MTBLC1927; MTBLC46295; MTBLC16009; MTBLC16335; MTBLC17172; MTBLC24088; MTBLC10110; MTBLC8674; MTBLC90721; MTBLC32; MTBLC134766; MTBLC135744; MTBLC63616; MTBLC5384; MTBLC79587; MTBLC44616; MTBLC34731; MTBLC2376; MTBLC64020; MTBLC4071; MTBLC3748; MTBLC23359; MTBLC50540; MTBLC16512; MTBLC6739; MTBLC137234; MTBLC27441; MTBLC28309; MTBLC19065; MTBLC70971; MTBLC16299; MTBLC490877; MTBLC37754; MTBLC27748; MTBLC6520; MTBLC107635; MTBLC84500; MTBLC15781; MTBLC81545; MTBLC81546; MTBLC27478; MTBLC29012; MTBLC9200; MTBLC8245; MTBLC9173; MTBLC32322; MTBLC31311; MTBLC171741; MTBLC92675; MTBLC138493; MTBLC74112; MTBLC61138; MTBLC37079; MTBLC33033; MTBLC16530; MTBLC27401; MTBLC39153; MTBLC45630; MTBLC38531; MTBLC8882; MTBLC6521; MTBLC50973; MTBLC8774; MTBLC137248; MTBLC2819; MTBLC27713; MTBLC19450; MTBLC17645; MTBLC58183; MTBLC17027; MTBLC70979; MTBLC17917; MTBLC724125; MTBLC89963; MTBLC28998; MTBLC1142; MTBLC18395; MTBLC16370; MTBLC15847; MTBLC57541; MTBLC71429; MTBLC88455; MTBLC42654; MTBLC17596; MTBLC17901; MTBLC87248; MTBLC9447; MTBLC28715; MTBLC21412; MTBLC143078; MTBLC8665; MTBLC55344; MTBLC37755; MTBLC15887; MTBLC17750; MTBLC58441; MTBLC18314; MTBLC16414; MTBLC138668; MTBLC77042; MTBLC134261; MTBLC41139; MTBLC2540; MTBLC10226; MTBLC10364; MTBLC3900; MTBLC4817; MTBLC5177; MTBLC5379; MTBLC5981; MTBLC6070; MTBLC8216; MTBLC73719; MTBLC50178; MTBLC135187; MTBLC17144; MTBLC6407; MTBLC73880; MTBLC79449; MTBLC7575; MTBLC11946; MTBLC3926; MTBLC35280; MTBLC29565; MTBLC15565; MTBLC16856; MTBLC32153; MTBLC6413; MTBLC8426; MTBLC80592; MTBLC51032; MTBLC28598; MTBLC17799; MTBLC57630; MTBLC28718; MTBLC15699; MTBLC16857; MTBLC62413; MTBLC16256; MTBLC30831; MTBLC137232; MTBLC15344; MTBLC51850; MTBLC16265; MTBLC28867; MTBLC18261; MTBLC17201; MTBLC17196; MTBLC15737; MTBLC29045; MTBLC16770; MTBLC17374; MTBLC28376; MTBLC2165; MTBLC29637; MTBLC61511; MTBLC39501; MTBLC32069; MTBLC6874; MTBLC5044; MTBLC37628; MTBLC64366; MTBLC17053; MTBLC29990; MTBLC5159; MTBLC18012; MTBLC18300; MTBLC17257; MTBLC135747; MTBLC31785; MTBLC10556; MTBLC5511; MTBLC5534; MTBLC2532; MTBLC2821; MTBLC3287; MTBLC6511; MTBLC1670; MTBLC73757; MTBLC21305; MTBLC18050; MTBLC16352; MTBLC37011; MTBLC16010; MTBLC94613; MTBLC6151; MTBLC139123; MTBLC1241; MTBLC28791; MTBLC62637; MTBLC16015; MTBLC58724; MTBLC16439; MTBLC45441; MTBLC31882; MTBLC17981; MTBLC36461; MTBLC17415; MTBLC17626; MTBLC17204; MTBLC2424; MTBLC15670; MTBLC30838; MTBLC16600; MTBLC51330; MTBLC75984; MTBLC3734; MTBLC7856; MTBLC9196; MTBLC7959; MTBLC16643; MTBLC50868; MTBLC9384; MTBLC15604; MTBLC89185; MTBLC57826; MTBLC28825; MTBLC18347; MTBLC17191; MTBLC15603; MTBLC64348; MTBLC17878; MTBLC17611; MTBLC17915; MTBLC85235; MTBLC38355; MTBLC49283; MTBLC143856; MTBLC61206; MTBLC79634; MTBLC79456; MTBLC79768; MTBLC79876; MTBLC34930; MTBLC6536; MTBLC17472; MTBLC73740; MTBLC7034; MTBLC5158; MTBLC30845; MTBLC30846; MTBLC74104; MTBLC19274; MTBLC85162; MTBLC23757; MTBLC5826; MTBLC62069; MTBLC223316; MTBLC44934; MTBLC10018; MTBLC135072; MTBLC34405; MTBLC34788; MTBLC31268; MTBLC34756; MTBLC3391; MTBLC53490; MTBLC5847; MTBLC5597; MTBLC79439; MTBLC34619; MTBLC135714; MTBLC7807; MTBLC78549; MTBLC1957; MTBLC20013; MTBLC40521; MTBLC31111; MTBLC34522; MTBLC16079; MTBLC37287; MTBLC37291; MTBLC29064; MTBLC2128; MTBLC9212; MTBLC53763; MTBLC86455; MTBLC45652; MTBLC30449; MTBLC34291; MTBLC17397; MTBLC24814; MTBLC74018; MTBLC52172; MTBLC28682; MTBLC66876; MTBLC9741; MTBLC5515; MTBLC47899; MTBLC8397; MTBLC695; MTBLC9403; MTBLC34307; MTBLC3767; MTBLC68428; MTBLC27527; MTBLC27588; MTBLC29573; MTBLC7599; MTBLC61645; MTBLC79626; MTBLC79729; MTBLC134923; MTBLC16043; MTBLC5457; MTBLC34048; MTBLC48541; MTBLC137772; MTBLC16547; MTBLC9957; MTBLC10366; MTBLC10423; MTBLC15582; MTBLC15583; MTBLC57424; MTBLC49076; MTBLC18104; MTBLC18078; MTBLC17023; MTBLC27861; MTBLC27550; MTBLC15591; MTBLC16831; MTBLC89205; MTBLC138367; MTBLC28381; MTBLC59051; MTBLC30997; MTBLC6452; MTBLC17937; MTBLC62112; MTBLC3207; MTBLC66913; MTBLC50131; MTBLC31989; MTBLC8097; MTBLC2705; MTBLC137310; MTBLC28502; MTBLC16765; MTBLC31993; MTBLC3085; MTBLC59020; MTBLC28948; MTBLC28136; MTBLC132335; MTBLC31584; MTBLC31952; MTBLC3112; MTBLC15676; MTBLC21860; MTBLC79347; MTBLC68606; MTBLC610092; MTBLC139380; MTBLC34598; MTBLC80544; MTBLC23812; MTBLC58056; MTBLC87166; MTBLC37245; MTBLC35460; MTBLC16093; MTBLC16558; MTBLC28568; MTBLC218; MTBLC18297; MTBLC2559; MTBLC17973; MTBLC27818; MTBLC17665; MTBLC57734; MTBLC12350; MTBLC16084; MTBLC57684; MTBLC58247; MTBLC58328; MTBLC27973; MTBLC78736; MTBLC78697; MTBLC37480; MTBLC12937; MTBLC16077; MTBLC14314; MTBLC57828; MTBLC16588; MTBLC35374; MTBLC17369; MTBLC138150; MTBLC17837; MTBLC78737; MTBLC24588; MTBLC25448; MTBLC80181; MTBLC84141; MTBLC137409; MTBLC28173; MTBLC18365; MTBLC28992; MTBLC1369; MTBLC67375; MTBLC2373; MTBLC17488; MTBLC59353; MTBLC43468; MTBLC35128; MTBLC28652; MTBLC35121; MTBLC28635; MTBLC30850; MTBLC8809; MTBLC69440; MTBLC4910; MTBLC27429; MTBLC32506; MTBLC79659; MTBLC45980; MTBLC6375; MTBLC3534; MTBLC4997; MTBLC73873; MTBLC9735; MTBLC16927; MTBLC31657; MTBLC135111; MTBLC136292; MTBLC6758; MTBLC16734; MTBLC102524; MTBLC134922; MTBLC17409; MTBLC133172; MTBLC132983; MTBLC78951; MTBLC16445; MTBLC151; MTBLC160; MTBLC15622; MTBLC35453; MTBLC18281; MTBLC17305; MTBLC41893; MTBLC42819; MTBLC57992; MTBLC30769; MTBLC30887; MTBLC30915; MTBLC17803; MTBLC6885; MTBLC57927; MTBLC4488; MTBLC27837; MTBLC86556; MTBLC84058; MTBLC3805; MTBLC4520; MTBLC73026; MTBLC73025; MTBLC34923; MTBLC64; MTBLC4628; MTBLC31585; MTBLC76160; MTBLC31981; MTBLC17802; MTBLC16704; MTBLC73715; MTBLC70353; MTBLC34698; MTBLC70453; MTBLC134913; MTBLC90038; MTBLC86004; MTBLC9274; MTBLC9275; MTBLC89730; MTBLC11222; MTBLC34447; MTBLC31402; MTBLC4895; MTBLC6347; MTBLC35796; MTBLC137768; MTBLC3158; MTBLC29513; MTBLC58556; MTBLC17533; MTBLC36554; MTBLC28249; MTBLC1162; MTBLC1243; MTBLC87507; MTBLC48061; MTBLC30918; MTBLC16630; MTBLC17902; MTBLC17568; MTBLC28942; MTBLC22099; MTBLC13497; MTBLC32275; MTBLC135817; MTBLC49026; MTBLC17012; MTBLC28879; MTBLC91807; MTBLC15809; MTBLC6381; MTBLC9605; MTBLC79471; MTBLC79566; MTBLC6851; MTBLC38546; MTBLC10561; MTBLC58800; MTBLC3146; MTBLC49260; MTBLC144027; MTBLC27574; MTBLC58767; MTBLC49004; MTBLC9308; MTBLC27407; MTBLC40304; MTBLC3927; MTBLC16750; MTBLC27427; MTBLC17643; MTBLC31552; MTBLC43755; MTBLC3088; MTBLC50271; MTBLC69499; MTBLC4994; MTBLC6008; MTBLC7161; MTBLC94381; MTBLC116; MTBLC4962; MTBLC29474; MTBLC17693; MTBLC16409; MTBLC17405; MTBLC2085; MTBLC34334; MTBLC20367; MTBLC28719; MTBLC137246; MTBLC29069; MTBLC30801; MTBLC29009; MTBLC74321; MTBLC2685; MTBLC3082; MTBLC135310; MTBLC116735; MTBLC17295; MTBLC46209; MTBLC28438; MTBLC28170; MTBLC28353; MTBLC16151; MTBLC35697; MTBLC4888; MTBLC134865; MTBLC5862; MTBLC16828; MTBLC79441; MTBLC9935; MTBLC9962; MTBLC135165; MTBLC3845; MTBLC135386; MTBLC15637; MTBLC63606; MTBLC45981; MTBLC8772; MTBLC4708; MTBLC9259; MTBLC51141; MTBLC17509; MTBLC53727; MTBLC32162; MTBLC102516; MTBLC32164; MTBLC9593; MTBLC7209; MTBLC24479; MTBLC4822; MTBLC6617; MTBLC4724; MTBLC10026; MTBLC35028; MTBLC10022; MTBLC69088; MTBLC17501; MTBLC28523; MTBLC89486; MTBLC2108; MTBLC2336; MTBLC4774; MTBLC34712; MTBLC60069; MTBLC6891; MTBLC16389; MTBLC8418; MTBLC8419; MTBLC18082; MTBLC28334; MTBLC88677; MTBLC15490; MTBLC34041; MTBLC60076; MTBLC16305; MTBLC31682; MTBLC73970; MTBLC3695; MTBLC132058; MTBLC74533; MTBLC137196; MTBLC2978; MTBLC80227; MTBLC34087; MTBLC89521; MTBLC86095; MTBLC88906; MTBLC89602; MTBLC89539; MTBLC89536; MTBLC73739; MTBLC75145; MTBLC64356; MTBLC86544; MTBLC29564; MTBLC31447; MTBLC4512; MTBLC6001; MTBLC32771; MTBLC37108; MTBLC29019; MTBLC86618; MTBLC82864; MTBLC135383; MTBLC4682; MTBLC76258; MTBLC135151; MTBLC36665; MTBLC18094; MTBLC4718; MTBLC9239; MTBLC25357; MTBLC27504; MTBLC2699; MTBLC8837; MTBLC9198; MTBLC9524; MTBLC9601; MTBLC9770; MTBLC9969; MTBLC2697; MTBLC2722; MTBLC6080; MTBLC8822; MTBLC52070; MTBLC9912; MTBLC8247; MTBLC32003; MTBLC10329; MTBLC135757; MTBLC42; MTBLC6066; MTBLC7458; MTBLC9519; MTBLC4856; MTBLC9120; MTBLC79434; MTBLC16684; MTBLC6140; MTBLC58164; MTBLC6506; MTBLC31789; MTBLC6778; MTBLC79600; MTBLC137783; MTBLC51211; MTBLC135016; MTBLC6535; MTBLC5990; MTBLC3094; MTBLC16112; MTBLC16065; MTBLC16952; MTBLC74725; MTBLC16475; MTBLC28155; MTBLC4732; MTBLC79423; MTBLC79564; MTBLC9291; MTBLC62431; MTBLC2365; MTBLC22152; MTBLC2620; MTBLC2851; MTBLC2870; MTBLC2982; MTBLC3574; MTBLC3888; MTBLC5095; MTBLC5281; MTBLC5536; MTBLC5727; MTBLC5867; MTBLC6560; MTBLC6921; MTBLC8115; MTBLC8267; MTBLC8268; MTBLC8856; MTBLC9013; MTBLC9956; MTBLC10024; MTBLC79890; MTBLC6863; MTBLC29612; MTBLC93369; MTBLC30805; MTBLC140088; MTBLC74966; MTBLC43966; MTBLC85252; MTBLC63924; MTBLC4973; MTBLC6419; MTBLC16725; MTBLC27769; MTBLC86068; MTBLC2404; MTBLC133419; MTBLC10070; MTBLC93847; MTBLC28708; MTBLC29458; MTBLC15830; MTBLC134834; MTBLC34769; MTBLC139312; MTBLC3061; MTBLC10099; MTBLC6738; MTBLC3005; MTBLC135349; MTBLC92338; MTBLC7789; MTBLC7640; MTBLC8597; MTBLC93626; MTBLC28865; MTBLC38258; MTBLC5859; MTBLC8021; MTBLC636; MTBLC67547; MTBLC137192; MTBLC88935; MTBLC86119; MTBLC86121; MTBLC89734; MTBLC86117; MTBLC78022; MTBLC89691; MTBLC84831; MTBLC74670; MTBLC89599; MTBLC89597; MTBLC89548; MTBLC89438; MTBLC89078; MTBLC89127; MTBLC89177; MTBLC88712; MTBLC21484; MTBLC15874; MTBLC17976; MTBLC5093; MTBLC63630; MTBLC2294; MTBLC2425; MTBLC16363; MTBLC2629; MTBLC69335; MTBLC28356; MTBLC4441; MTBLC135002; MTBLC10058; MTBLC10076; MTBLC10103; MTBLC28714; MTBLC43415; MTBLC5855; MTBLC28325; MTBLC74405; MTBLC3300; MTBLC9515; MTBLC41509; MTBLC2156; MTBLC2368; MTBLC9439; MTBLC74274; MTBLC8386; MTBLC18278; MTBLC27993; MTBLC82684; MTBLC9997; MTBLC80033; MTBLC29527; MTBLC29536; MTBLC135701; MTBLC16778; MTBLC18330; MTBLC4783; MTBLC27514; MTBLC5304; MTBLC31967; MTBLC16954; MTBLC8028; MTBLC133473; MTBLC29043; MTBLC38266; MTBLC80494; MTBLC72609; MTBLC62881; MTBLC135932; MTBLC9943; MTBLC58552; MTBLC42797; MTBLC31871; MTBLC82763; MTBLC31922; MTBLC135703; MTBLC64210; MTBLC135483; MTBLC32181; MTBLC474014; MTBLC3825; MTBLC34668; MTBLC7736; MTBLC17713; MTBLC10037; MTBLC8922; MTBLC7471; MTBLC31563; MTBLC3740; MTBLC4320; MTBLC24293; MTBLC80538; MTBLC79465; MTBLC4773; MTBLC5527; MTBLC9959; MTBLC131852; MTBLC9665; MTBLC473990; MTBLC17433; MTBLC80393; MTBLC3162; MTBLC5970; MTBLC44492; MTBLC79394; MTBLC15430; MTBLC57306; MTBLC2341; MTBLC34163; MTBLC31561; MTBLC135525; MTBLC8039; MTBLC79655; MTBLC79502; MTBLC34461; MTBLC79892; MTBLC34353; MTBLC34355; MTBLC79657; MTBLC17457; MTBLC4453; MTBLC9261; MTBLC79432; MTBLC79620; MTBLC29510; MTBLC52075; MTBLC15416; MTBLC31578; MTBLC52484; MTBLC29611; MTBLC52482; MTBLC29654; MTBLC81594; MTBLC30038; MTBLC31896; MTBLC9108; MTBLC9946; MTBLC847; MTBLC9205; MTBLC15735; MTBLC3745; MTBLC82461; MTBLC27796; MTBLC34580; MTBLC6147; MTBLC135451; MTBLC2565; MTBLC4038; MTBLC28833; MTBLC29592; MTBLC29594; MTBLC29602; MTBLC5606; MTBLC6962; MTBLC8330; MTBLC9042; MTBLC9290; MTBLC2534; MTBLC799; MTBLC34139; MTBLC79668; MTBLC79797; MTBLC136980; MTBLC1189; MTBLC136972; MTBLC79907; MTBLC63641; MTBLC79715; MTBLC2495; MTBLC79887; MTBLC9460; MTBLC17078; MTBLC141472; MTBLC28192; MTBLC135231; MTBLC79496; MTBLC79601; MTBLC5887; MTBLC59788; MTBLC31086; MTBLC2626; MTBLC8402; MTBLC32185; MTBLC4417; MTBLC31298; MTBLC31497; MTBLC8713; MTBLC31459; MTBLC113542; MTBLC40070; MTBLC27510; MTBLC17148; MTBLC716; MTBLC2327; MTBLC2544; MTBLC3614; MTBLC89837; MTBLC89829; MTBLC89824; MTBLC90028; MTBLC90034; MTBLC90021; MTBLC77677; MTBLC88798; MTBLC88446; MTBLC41847; MTBLC89028; MTBLC90068; MTBLC64793; MTBLC84266; MTBLC5674; MTBLC142272; MTBLC2939; MTBLC6798; MTBLC1749; MTBLC8602; MTBLC17467; MTBLC34605; MTBLC9425; MTBLC2725; MTBLC9923; MTBLC73; MTBLC30725; MTBLC34968; MTBLC31753; MTBLC2934; MTBLC7948; MTBLC86251; MTBLC30248; MTBLC34227; MTBLC142243; MTBLC136795; MTBLC2504; MTBLC3081; MTBLC16188; MTBLC16011; MTBLC85158; MTBLC79925; MTBLC79522; MTBLC34175; MTBLC79455; MTBLC80656; MTBLC79735; MTBLC135981; MTBLC6085; MTBLC49191; MTBLC9419; MTBLC89642; MTBLC16374; MTBLC10136; MTBLC4778; MTBLC8196; MTBLC28794; MTBLC90355; MTBLC79553; MTBLC28090; MTBLC2197; MTBLC3163; MTBLC28436; MTBLC5837; MTBLC6006; MTBLC75092; MTBLC16243; MTBLC8876; MTBLC507499; MTBLC204; MTBLC214; MTBLC241; MTBLC242; MTBLC78668; MTBLC138752; MTBLC17130; MTBLC34301; MTBLC37157; MTBLC78853; MTBLC61024; MTBLC8607; MTBLC4389; MTBLC5528; MTBLC89343; MTBLC89314; MTBLC89088; MTBLC89075; MTBLC89076; MTBLC89371; MTBLC89333; MTBLC89334; MTBLC89311; MTBLC89316; MTBLC138499; MTBLC18227; MTBLC94661; MTBLC36108; MTBLC80383; MTBLC8273; MTBLC8773; MTBLC31049; MTBLC18393; MTBLC137750; MTBLC17224; MTBLC5679; MTBLC18127; MTBLC17166; MTBLC28091; MTBLC36466; MTBLC36106; MTBLC4366; MTBLC28869; MTBLC28925; MTBLC9185; MTBLC9188; MTBLC86162; MTBLC88930; MTBLC88929; MTBLC89739; MTBLC89576; MTBLC89557; MTBLC89559; MTBLC89441; MTBLC86161; MTBLC89419; MTBLC88925; MTBLC88841; MTBLC88430; MTBLC88654; MTBLC10219; MTBLC86344; MTBLC84549; MTBLC84837; MTBLC78268; MTBLC7492; MTBLC91712; MTBLC4974; MTBLC4572; MTBLC6414; MTBLC81785; MTBLC135138; MTBLC60656; MTBLC16312; MTBLC16390; MTBLC138401; MTBLC88108; MTBLC2812; MTBLC79833; MTBLC47818; MTBLC79918; MTBLC34838; MTBLC31523; MTBLC138422; MTBLC47214; MTBLC28818; MTBLC32176; MTBLC15578; MTBLC89324; MTBLC89079; MTBLC19290; MTBLC79996; MTBLC28477; MTBLC81013; MTBLC17823; MTBLC86378; MTBLC7931; MTBLC28933; MTBLC9595; MTBLC34667; MTBLC31648; MTBLC4819; MTBLC32645; MTBLC8764; MTBLC4921; MTBLC9165; MTBLC31857; MTBLC31174; MTBLC34831; MTBLC31894; MTBLC9316; MTBLC27617; MTBLC80461; MTBLC80167; MTBLC1107; MTBLC82949; MTBLC88480; MTBLC88479; MTBLC88547; MTBLC89218; MTBLC89203; MTBLC89202; MTBLC89162; MTBLC89160; MTBLC89238; MTBLC89237; MTBLC88966; MTBLC89040; MTBLC89780; MTBLC89784; MTBLC89799; MTBLC89797; MTBLC89684; MTBLC89669; MTBLC89670; MTBLC89671; MTBLC89433; MTBLC89322; MTBLC89337; MTBLC136371; MTBLC64396; MTBLC88779; MTBLC28517; MTBLC18171; MTBLC32086; MTBLC5206; MTBLC15575; MTBLC2513; MTBLC50749; MTBLC31893; MTBLC9463; MTBLC15574; MTBLC90980; MTBLC47812; MTBLC80533; MTBLC3863; MTBLC5633; MTBLC8913; MTBLC6145; MTBLC64668; MTBLC7800; MTBLC9039; MTBLC8621; MTBLC80017; MTBLC34042; MTBLC7752; MTBLC28285; MTBLC18010; MTBLC3719; MTBLC5718; MTBLC6674; MTBLC59979; MTBLC34499; MTBLC34503; MTBLC34506; MTBLC91217; MTBLC138082; MTBLC15658; MTBLC15655; MTBLC15657; MTBLC64008; MTBLC138786; MTBLC88461; MTBLC34148; MTBLC91272; MTBLC34485; MTBLC34498; MTBLC34500; MTBLC88440; MTBLC34504; MTBLC143972; MTBLC88465; MTBLC89257; MTBLC3403; MTBLC3898; MTBLC79904; MTBLC34352; MTBLC1689; MTBLC89328; MTBLC79870; MTBLC9481; MTBLC93; MTBLC1941; MTBLC8603; MTBLC134767; MTBLC74562; MTBLC61725; MTBLC142079; MTBLC16310; MTBLC42471; MTBLC7567; MTBLC16147; MTBLC85232; MTBLC90230; MTBLC133979; MTBLC137172; MTBLC85166; MTBLC133325; MTBLC135350; MTBLC545687; MTBLC7496; MTBLC34322; MTBLC79177; MTBLC84854; MTBLC34295; MTBLC29479; MTBLC17903; MTBLC4045; MTBLC10445; MTBLC6706; MTBLC79519; MTBLC34293; MTBLC34294; MTBLC135489; MTBLC9238; MTBLC137712; MTBLC19143; MTBLC18446; MTBLC8648; MTBLC19144; MTBLC49265; MTBLC15654; MTBLC88462; MTBLC80442; MTBLC84441; MTBLC72641; MTBLC136531; MTBLC72815; MTBLC80463; MTBLC76234; MTBLC34491; MTBLC88441; MTBLC80447; MTBLC88438; MTBLC72843; MTBLC72842; MTBLC88460; MTBLC60956; MTBLC133329; MTBLC80413; MTBLC63067; MTBLC18230; MTBLC65247; MTBLC3705; MTBLC31352; MTBLC76334; MTBLC9510; MTBLC3128; MTBLC61726; MTBLC89365; MTBLC89339; MTBLC89342; MTBLC89318; MTBLC89313; MTBLC60273; MTBLC65211; MTBLC138212; MTBLC78700; MTBLC55523; MTBLC27706; MTBLC38299; MTBLC137495; MTBLC34154; MTBLC72639; MTBLC133357; MTBLC34494; MTBLC78730; MTBLC34496; MTBLC72651; MTBLC131659; MTBLC5833; MTBLC73074; MTBLC2366; MTBLC1019; MTBLC88696; MTBLC52897; MTBLC79575; MTBLC135210; MTBLC132495; MTBLC73751; MTBLC34828; MTBLC88667; MTBLC9778; MTBLC28919; MTBLC10088; MTBLC69081; MTBLC75542; MTBLC95216; MTBLC134424; MTBLC134423; MTBLC29627; MTBLC10120; MTBLC34034; MTBLC34443; MTBLC40131; MTBLC4918; MTBLC14469; MTBLC2492; MTBLC5166; MTBLC88808; MTBLC88807; MTBLC88782; MTBLC89214; MTBLC89189; MTBLC89149; MTBLC1418; MTBLC27867; MTBLC80419; MTBLC3375; MTBLC5087; MTBLC27448; MTBLC80177; MTBLC19793; MTBLC28485; MTBLC88765; MTBLC28810; MTBLC32157; MTBLC31279; MTBLC7720; MTBLC73728; MTBLC133875; MTBLC34920; MTBLC6088; MTBLC137139; MTBLC138782; MTBLC34652; MTBLC34680; MTBLC33913; MTBLC75219; MTBLC133456; MTBLC88698; MTBLC88697; MTBLC79838; MTBLC50106; MTBLC34229; MTBLC138081; MTBLC38833; MTBLC22469; MTBLC28093; MTBLC15405; MTBLC17580; MTBLC36503; MTBLC15393; MTBLC36492; MTBLC98; MTBLC31; MTBLC60; MTBLC61; MTBLC149; MTBLC150; MTBLC152; MTBLC153; MTBLC50232; MTBLC158; MTBLC50233; MTBLC50235; MTBLC300; MTBLC299; MTBLC368; MTBLC27961; MTBLC61727; MTBLC47856; MTBLC17447; MTBLC29452; MTBLC28071; MTBLC692; MTBLC35002; MTBLC9602; MTBLC137135; MTBLC34537; MTBLC79794; MTBLC79879; MTBLC28125; MTBLC79767; MTBLC79635; MTBLC34476; MTBLC79801; MTBLC135402; MTBLC32095; MTBLC79581; MTBLC76937; MTBLC39567; MTBLC36206; MTBLC36214; MTBLC85510; MTBLC36211; MTBLC7989; MTBLC79096; MTBLC75103; MTBLC32411; MTBLC138778; MTBLC36412; MTBLC86135; MTBLC142250; MTBLC86506; MTBLC32409; MTBLC32389; MTBLC37810; MTBLC2905; MTBLC135532; MTBLC79179; MTBLC84855; MTBLC80050; MTBLC48635; MTBLC5644; MTBLC63916; MTBLC79523; MTBLC79689; MTBLC80001; MTBLC52421; MTBLC448; MTBLC72665; MTBLC138258; MTBLC138255; MTBLC72663; MTBLC133381; MTBLC133086; MTBLC131762; MTBLC73882; MTBLC84067; MTBLC86403; MTBLC31850; MTBLC132479; MTBLC92833; MTBLC34370; MTBLC135041; MTBLC134981; MTBLC31547; MTBLC79883; MTBLC79939; MTBLC6645; MTBLC57905; MTBLC84094; MTBLC116278; MTBLC9232; MTBLC28661; MTBLC10275; MTBLC27432; MTBLC44602; MTBLC79716; MTBLC86136; MTBLC86148; MTBLC38384; MTBLC16423; MTBLC61676; MTBLC8638; MTBLC88809; MTBLC75465; MTBLC88786; MTBLC84394; MTBLC88471; MTBLC88536; MTBLC88367; MTBLC75446; MTBLC138077; MTBLC28627; MTBLC80415; MTBLC88796; MTBLC88725; MTBLC82927; MTBLC88501; MTBLC88500; MTBLC88364; MTBLC89229; MTBLC89211; MTBLC88942; MTBLC89034; MTBLC89029; MTBLC50585; MTBLC138489; MTBLC31571; MTBLC45571; MTBLC31725; MTBLC144339; MTBLC9194; MTBLC89605; MTBLC15843; MTBLC79754; MTBLC79694; MTBLC1182; MTBLC79480; MTBLC79869; MTBLC82835; MTBLC2451; MTBLC36033; MTBLC31825; MTBLC135293; MTBLC34834; MTBLC30041; MTBLC10419; MTBLC3425; MTBLC8996; MTBLC6991; MTBLC32345; MTBLC137651; MTBLC641; MTBLC1784; MTBLC4640; MTBLC72800; MTBLC20096; MTBLC72758; MTBLC73889; MTBLC3456; MTBLC9242; MTBLC44526; MTBLC83063; MTBLC38394; MTBLC142447; MTBLC24993; MTBLC138083; MTBLC38362; MTBLC82749; MTBLC32798; MTBLC88464; MTBLC86141; MTBLC27939; MTBLC75108; MTBLC6673; MTBLC28801; MTBLC84299; MTBLC4650; MTBLC58303; MTBLC46979; MTBLC136623; MTBLC46859; MTBLC83058; MTBLC9189; MTBLC86570; MTBLC31542; MTBLC89519; MTBLC85028; MTBLC74971; MTBLC4021; MTBLC48923; MTBLC64483; MTBLC131738; MTBLC64489; MTBLC78103; MTBLC63959; MTBLC31000; MTBLC75454; MTBLC75536; MTBLC31831; MTBLC75565; MTBLC137215; MTBLC135498; MTBLC3961; MTBLC71025; MTBLC73792; MTBLC137845; MTBLC9011; MTBLC33276; MTBLC80541; MTBLC137134; MTBLC47805; MTBLC79517; MTBLC4629; MTBLC31826; MTBLC10086; MTBLC64124; MTBLC46961; MTBLC15913; MTBLC18129; MTBLC79182; MTBLC143095; MTBLC85208; MTBLC136406; MTBLC50578; MTBLC136819; MTBLC136638; MTBLC74789; MTBLC79951; MTBLC5382; MTBLC69833; MTBLC80540; MTBLC3450; MTBLC37779; MTBLC37537; MTBLC49254; MTBLC28724; MTBLC136767; MTBLC85633; MTBLC34004; MTBLC85639; MTBLC45478; MTBLC79312; MTBLC30820; MTBLC50576; MTBLC138260; MTBLC82464; MTBLC28592; MTBLC84874; MTBLC70850; MTBLC85057; MTBLC32365; MTBLC90027; MTBLC3433; MTBLC9184; MTBLC74330; MTBLC62834; MTBLC77492; MTBLC73741; MTBLC79501; MTBLC34464; MTBLC11152; MTBLC29644; MTBLC84519; MTBLC34726; MTBLC133741; MTBLC46703; MTBLC73829; MTBLC34402; MTBLC137126; MTBLC81246; MTBLC67061; MTBLC73851; MTBLC84752; MTBLC79723; MTBLC33216; MTBLC6689; MTBLC7443; MTBLC79824; MTBLC135488; MTBLC88790; MTBLC77096; MTBLC88474; MTBLC88495; MTBLC88490; MTBLC88520; MTBLC88371; MTBLC88395; MTBLC89225; MTBLC75475; MTBLC77127; MTBLC89169; MTBLC89168; MTBLC89260; MTBLC75578; MTBLC88989; MTBLC89046; MTBLC89795; MTBLC89682; MTBLC89665; MTBLC89811; MTBLC80207; MTBLC131692; MTBLC17862; MTBLC71464; MTBLC16393; MTBLC28727; MTBLC28194; MTBLC27997; MTBLC16196; MTBLC82617; MTBLC50575; MTBLC32375; MTBLC50464; MTBLC29735; MTBLC30829; MTBLC28193; MTBLC50572; MTBLC36023; MTBLC35517; MTBLC79612; MTBLC18054; MTBLC3430; MTBLC6965; MTBLC82985; MTBLC10087; MTBLC9916; MTBLC35464; MTBLC142241; MTBLC28716; MTBLC35465; MTBLC76244; MTBLC37252; MTBLC76090; MTBLC9199; MTBLC9951; MTBLC77148; MTBLC58206; MTBLC31872; MTBLC3944; MTBLC5933; MTBLC72828; MTBLC72952; MTBLC27620; MTBLC91006; MTBLC67309; MTBLC3940; MTBLC7909; MTBLC79407; MTBLC79791; MTBLC79792; MTBLC66666; MTBLC135355; MTBLC88112; MTBLC135566; MTBLC79513; MTBLC73092; MTBLC31501; MTBLC88109; MTBLC31297; MTBLC28941; MTBLC84901; MTBLC28733; MTBLC6144; MTBLC75612; MTBLC52392; MTBLC3427; MTBLC137833; MTBLC16566; MTBLC84896; MTBLC28842; MTBLC88686; MTBLC29702; MTBLC34478; MTBLC137844; MTBLC53154; MTBLC72736; MTBLC133144; MTBLC75036; MTBLC131924; MTBLC8416; MTBLC9190; MTBLC18318; MTBLC86422; MTBLC89413; MTBLC89431; MTBLC89391; MTBLC89140; MTBLC89196; MTBLC89294; MTBLC88904; MTBLC88905; MTBLC88760; MTBLC88761; MTBLC88731; MTBLC88729; MTBLC88871; MTBLC88869; MTBLC88587; MTBLC89500; MTBLC89501; MTBLC34542; MTBLC61473; MTBLC3249; MTBLC4746; MTBLC80169; MTBLC34121; MTBLC52971; MTBLC93175; MTBLC137734; MTBLC73854; MTBLC90040; MTBLC89382; MTBLC89352; MTBLC89368; MTBLC89366; MTBLC89340; MTBLC89317; MTBLC137279; MTBLC137293; MTBLC134075; MTBLC90459; MTBLC134076; MTBLC134077; MTBLC134078; MTBLC39934; MTBLC134227; MTBLC134228; MTBLC16038; MTBLC9970; MTBLC4592; MTBLC79643; MTBLC34554; MTBLC2927; MTBLC27722; MTBLC28277; MTBLC80014; MTBLC77258; MTBLC4915; MTBLC5746; MTBLC28468; MTBLC64563; MTBLC76078; MTBLC72998; MTBLC78101; MTBLC73721; MTBLC73134; MTBLC73004; MTBLC62837; MTBLC78270; MTBLC36476; MTBLC79536; MTBLC73894; MTBLC31676; MTBLC50782; MTBLC31650; MTBLC6574; MTBLC31940; MTBLC44247; MTBLC79899; MTBLC27965; MTBLC79098; MTBLC75038; MTBLC133623; MTBLC84577; MTBLC84234; MTBLC64032; MTBLC53486; MTBLC53460; MTBLC79878; MTBLC79900; MTBLC525464; MTBLC79409; MTBLC79578; MTBLC82832; MTBLC71589; MTBLC32023; MTBLC34349; MTBLC32068; MTBLC31020; MTBLC2502; MTBLC28593; MTBLC15854; MTBLC309594; MTBLC84116; MTBLC3560; MTBLC79190; MTBLC76992; MTBLC52347; MTBLC18164; MTBLC32027; MTBLC135857; MTBLC88780; MTBLC88468; MTBLC75342; MTBLC744; MTBLC34115; MTBLC84911; MTBLC32154; MTBLC131508; MTBLC32906; MTBLC29596; MTBLC28211; MTBLC6927; MTBLC7603; MTBLC80537; MTBLC10137; MTBLC80732; MTBLC79113; MTBLC90041; MTBLC133599; MTBLC133617; MTBLC84845; MTBLC84844; MTBLC74986; MTBLC143985; MTBLC80203; MTBLC143980; MTBLC57409; MTBLC134453; MTBLC34126; MTBLC34130; MTBLC79851; MTBLC72606; MTBLC19138; MTBLC137345; MTBLC34157; MTBLC88823; MTBLC78837; MTBLC64017; MTBLC34162; MTBLC79557; MTBLC79656; MTBLC63995; MTBLC79561; MTBLC63579; MTBLC34185; MTBLC34306; MTBLC79485; MTBLC34450; MTBLC60943; MTBLC137344; MTBLC34490; MTBLC72643; MTBLC72786; MTBLC36275; MTBLC86031; MTBLC73733; MTBLC89091; MTBLC75646; MTBLC89387; MTBLC89392; MTBLC89395; MTBLC89394; MTBLC53081; MTBLC76284; MTBLC137704; MTBLC34438; MTBLC32319; MTBLC32325; MTBLC34711; MTBLC4676; MTBLC34136; MTBLC39449; MTBLC39451; MTBLC39453; MTBLC39454; MTBLC31406; MTBLC10580; MTBLC39448; MTBLC4722; MTBLC19287; MTBLC31164; MTBLC27655; MTBLC5715; MTBLC6567; MTBLC6586; MTBLC34883; MTBLC88902; MTBLC8034; MTBLC10045; MTBLC10089; MTBLC80194; MTBLC79956; MTBLC79588; MTBLC81561; MTBLC2296; MTBLC3321; MTBLC65585; MTBLC134353; MTBLC143960; MTBLC30088; MTBLC29589; MTBLC29601; MTBLC6696; MTBLC133423; MTBLC134511; MTBLC140267; MTBLC8390; MTBLC5783; MTBLC80531; MTBLC16688; MTBLC28135; MTBLC137137; MTBLC139534; MTBLC31731; MTBLC73923; MTBLC31801; MTBLC35459; MTBLC135729; MTBLC135684; MTBLC86197; MTBLC86196; MTBLC86189; MTBLC86190; MTBLC86188; MTBLC80532; MTBLC18531; MTBLC18532; MTBLC46739; MTBLC79839; MTBLC28033; MTBLC17168; MTBLC16608; MTBLC17762; MTBLC16074; MTBLC16113; MTBLC143982; MTBLC28610; MTBLC86255; MTBLC76071; MTBLC143713; MTBLC72589; MTBLC131658; MTBLC31025; MTBLC17390; MTBLC27808; MTBLC5191; MTBLC31123; MTBLC82648; MTBLC135276; MTBLC4670; MTBLC143989; MTBLC9669; MTBLC52672; MTBLC37945; MTBLC34899; MTBLC37923; MTBLC8710; MTBLC31550; MTBLC3156; MTBLC48742; MTBLC135719; MTBLC8036; MTBLC7352; MTBLC90970; MTBLC47834; MTBLC63911; MTBLC137141; MTBLC47799; MTBLC72727; MTBLC80530; MTBLC5363; MTBLC52348; MTBLC17314; MTBLC76980; MTBLC76304; MTBLC6113; MTBLC143987; MTBLC143990; MTBLC9911; MTBLC135737; MTBLC28700; MTBLC79923; MTBLC73794; MTBLC62736; MTBLC62737; MTBLC84958; MTBLC86418; MTBLC89703; MTBLC89592; MTBLC89589; MTBLC89384; MTBLC89098; MTBLC89143; MTBLC89070; MTBLC88726; MTBLC88872; MTBLC88588; MTBLC89498; MTBLC89502; MTBLC143981; MTBLC143983; MTBLC71466; MTBLC9453; MTBLC31264; MTBLC131689; MTBLC74340; MTBLC131668; MTBLC131687; MTBLC131688; MTBLC52639; MTBLC85403; MTBLC29613; MTBLC79453; MTBLC28047; MTBLC132620; MTBLC31257; MTBLC29677; MTBLC31222; MTBLC5197; MTBLC135094; MTBLC32277; MTBLC15929; MTBLC25242; MTBLC28258; MTBLC134924; MTBLC86975; MTBLC88529; MTBLC89026; MTBLC137784; MTBLC32002; MTBLC125; MTBLC46734; MTBLC141283; MTBLC16774; MTBLC35966; MTBLC16619; MTBLC10217; MTBLC10278; MTBLC10417; MTBLC3431; MTBLC4001; MTBLC5552; MTBLC5719; MTBLC6401; MTBLC7524; MTBLC7940; MTBLC64792; MTBLC137092; MTBLC144025; MTBLC10274; MTBLC3087; MTBLC37659; MTBLC135741; MTBLC9908; MTBLC18067; MTBLC89279; MTBLC89380; MTBLC89383; MTBLC89360; MTBLC89359; MTBLC89370; MTBLC84566; MTBLC137216; MTBLC85680; MTBLC18168; MTBLC52350; MTBLC73731; MTBLC78706; MTBLC31572; MTBLC36036; MTBLC9053; MTBLC89090; MTBLC89089; MTBLC89074; MTBLC89390; MTBLC89357; MTBLC89374; MTBLC89373; MTBLC90454; MTBLC75376; MTBLC17058; MTBLC28688; MTBLC34184; MTBLC3941; MTBLC53424; MTBLC1309; MTBLC1310; MTBLC79897; MTBLC63065; MTBLC143013; MTBLC4813; MTBLC134507; MTBLC84759; MTBLC34835; MTBLC84877; MTBLC39248; MTBLC34122; MTBLC84386; MTBLC88781; MTBLC88757; MTBLC88469; MTBLC75550; MTBLC83055; MTBLC27423; MTBLC37998; MTBLC2944; MTBLC132949; MTBLC137858; MTBLC137136; MTBLC79992; MTBLC9948; MTBLC135723; MTBLC90233; MTBLC137178; MTBLC73736; MTBLC39826; MTBLC50158; MTBLC17177; MTBLC16697; MTBLC52052; MTBLC16101; MTBLC28488; MTBLC28063; MTBLC27417; MTBLC84341; MTBLC88756; MTBLC3663; MTBLC59912; MTBLC80083; MTBLC94686; MTBLC137229; MTBLC82836; MTBLC77525; MTBLC34743; MTBLC133914; MTBLC89451; MTBLC135440; MTBLC72844; MTBLC79787; MTBLC79494; MTBLC88359; MTBLC140473; MTBLC137304; MTBLC63836; MTBLC73135; MTBLC48131; MTBLC79444; MTBLC2696; MTBLC46750; MTBLC7952; MTBLC8186; MTBLC32249; MTBLC15884; MTBLC41872; MTBLC33275; MTBLC33277</t>
   </si>
   <si>
     <t>MTBLS9794</t>
@@ -533,42 +569,6 @@
   </si>
   <si>
     <t>MTBLC22652; MTBLC15551; MTBLC72663; MTBLC15843; MTBLC53487; MTBLC61204; MTBLC53486; MTBLC36005; MTBLC65136; MTBLC16359; MTBLC30781; MTBLC27997; MTBLC24309; MTBLC166934; MTBLC228727; MTBLC194379; MTBLC64568; MTBLC30797; MTBLC15741; MTBLC72606; MTBLC37011; MTBLC180275; MTBLC64563; MTBLC183255; MTBLC16010; MTBLC72639; MTBLC15908; MTBLC22660; MTBLC190591; MTBLC17242; MTBLC156126; MTBLC16755; MTBLC64549; MTBLC136218; MTBLC190189; MTBLC35374; MTBLC24266; MTBLC86542; MTBLC30829; MTBLC17858; MTBLC506227; MTBLC91312; MTBLC75097; MTBLC21547; MTBLC7125; MTBLC64566; MTBLC88108; MTBLC74349; MTBLC90456; MTBLC139132; MTBLC87625; MTBLC64560; MTBLC67168; MTBLC43355; MTBLC30794; MTBLC17050; MTBLC25998; MTBLC183258; MTBLC20067; MTBLC5390; MTBLC30769; MTBLC190566; MTBLC91286; MTBLC228770; MTBLC73853; MTBLC166932; MTBLC17351; MTBLC138555; MTBLC183648; MTBLC17376; MTBLC88459; MTBLC87818; MTBLC190570; MTBLC16300; MTBLC59270; MTBLC183650; MTBLC72737; MTBLC75117; MTBLC60647; MTBLC6784; MTBLC166933; MTBLC6499; MTBLC166931; MTBLC28875; MTBLC183932; MTBLC183249; MTBLC18012; MTBLC183350; MTBLC27570; MTBLC183661; MTBLC72665; MTBLC141435; MTBLC177850; MTBLC62084; MTBLC15555; MTBLC17069; MTBLC64575; MTBLC17553; MTBLC138794; MTBLC17680; MTBLC165324; MTBLC15628; MTBLC16325; MTBLC44897; MTBLC183253; MTBLC28364; MTBLC178165; MTBLC18066; MTBLC18186; MTBLC28044; MTBLC230582; MTBLC2877; MTBLC138556; MTBLC64153; MTBLC190576; MTBLC72657; MTBLC73723; MTBLC40992; MTBLC17361; MTBLC193578; MTBLC15545; MTBLC16440; MTBLC228787; MTBLC15721; MTBLC183243; MTBLC18211; MTBLC81559; MTBLC183701; MTBLC62837; MTBLC136066; MTBLC190590; MTBLC16551; MTBLC70979; MTBLC27562; MTBLC190567; MTBLC90452; MTBLC9008; MTBLC172431; MTBLC9300; MTBLC4676; MTBLC183327; MTBLC141511; MTBLC17385; MTBLC74791; MTBLC169990; MTBLC36259; MTBLC28822; MTBLC27814; MTBLC72802; MTBLC183349; MTBLC84444; MTBLC64481; MTBLC15824; MTBLC183244; MTBLC15646; MTBLC183250; MTBLC183259; MTBLC229814; MTBLC18135; MTBLC68503; MTBLC183254; MTBLC183643; MTBLC136485; MTBLC30832; MTBLC73510; MTBLC228768; MTBLC545687; MTBLC28680; MTBLC74099; MTBLC17409; MTBLC183760; MTBLC741548; MTBLC39246; MTBLC228751; MTBLC50202; MTBLC184291; MTBLC73830; MTBLC132958; MTBLC15846; MTBLC73907; MTBLC21626; MTBLC172574; MTBLC17515; MTBLC141514; MTBLC64559; MTBLC27849; MTBLC27386; MTBLC73018; MTBLC64483; MTBLC183252; MTBLC35697; MTBLC67056; MTBLC167715; MTBLC138084; MTBLC30838; MTBLC55481; MTBLC34133; MTBLC6810; MTBLC27584; MTBLC228754; MTBLC183722; MTBLC16914; MTBLC88522; MTBLC183257; MTBLC28997; MTBLC31883; MTBLC183646; MTBLC30805; MTBLC17521; MTBLC16753; MTBLC27891; MTBLC18280; MTBLC156113; MTBLC183247; MTBLC141512; MTBLC16043; MTBLC170073; MTBLC91296; MTBLC55328; MTBLC194259; MTBLC183332; MTBLC183245; MTBLC183705; MTBLC136113; MTBLC183370; MTBLC75757; MTBLC138537; MTBLC78682; MTBLC132983; MTBLC14336; MTBLC29750; MTBLC228698; MTBLC190545; MTBLC28832; MTBLC134510; MTBLC17884; MTBLC53678; MTBLC27407; MTBLC190548; MTBLC60175; MTBLC228401; MTBLC75648; MTBLC75095; MTBLC16734; MTBLC190534; MTBLC132244; MTBLC17189; MTBLC145255; MTBLC183248; MTBLC228745; MTBLC17474; MTBLC16988; MTBLC190527; MTBLC26711; MTBLC63986; MTBLC67057; MTBLC28077; MTBLC113543; MTBLC9299; MTBLC72999; MTBLC228712; MTBLC15414; MTBLC192587; MTBLC73017; MTBLC28941; MTBLC17172; MTBLC15550; MTBLC28683; MTBLC165343; MTBLC74750; MTBLC190537; MTBLC37998; MTBLC27485; MTBLC183372; MTBLC189055; MTBLC39567; MTBLC190741; MTBLC165310; MTBLC34494; MTBLC28324; MTBLC228717; MTBLC18332; MTBLC60989; MTBLC183700; MTBLC72390; MTBLC183496; MTBLC18283; MTBLC28587; MTBLC15756; MTBLC16196; MTBLC15891; MTBLC170124; MTBLC16704; MTBLC195266; MTBLC28728; MTBLC16581; MTBLC24848; MTBLC16813; MTBLC48131; MTBLC28667; MTBLC136141; MTBLC73912; MTBLC64567; MTBLC73024; MTBLC72734; MTBLC12777; MTBLC72384; MTBLC174217; MTBLC131993; MTBLC28834; MTBLC17712; MTBLC70984; MTBLC72735; MTBLC16856; MTBLC17775; MTBLC16032; MTBLC228541; MTBLC15676; MTBLC18107; MTBLC138532; MTBLC28716; MTBLC16556; MTBLC72844; MTBLC17748; MTBLC17405; MTBLC73688; MTBLC73994; MTBLC15765; MTBLC72386; MTBLC64576; MTBLC31445; MTBLC36751; MTBLC15373; MTBLC183236; MTBLC82846; MTBLC42504; MTBLC132559; MTBLC72392; MTBLC16908; MTBLC228529; MTBLC28842; MTBLC82969; MTBLC76308; MTBLC72381; MTBLC28918; MTBLC143045; MTBLC72998; MTBLC64561; MTBLC72736; MTBLC15956; MTBLC34130; MTBLC142219; MTBLC72795; MTBLC42539; MTBLC116314; MTBLC74475; MTBLC34900; MTBLC75342; MTBLC15354; MTBLC17154; MTBLC16919; MTBLC57589; MTBLC132244; MTBLC17750; MTBLC16643; MTBLC26271; MTBLC17568; MTBLC17126; MTBLC73067; MTBLC27266; MTBLC78646; MTBLC69081; MTBLC16811; MTBLC29016; MTBLC28037; MTBLC16040; MTBLC41117; MTBLC25094; MTBLC17964; MTBLC90727; MTBLC37024; MTBLC71466; MTBLC16349; MTBLC46968; MTBLC170064; MTBLC178624; MTBLC26986; MTBLC17562; MTBLC28867; MTBLC17858; MTBLC35720; MTBLC17597; MTBLC68830; MTBLC25682; MTBLC15971; MTBLC28671; MTBLC16610; MTBLC70749; MTBLC143245; MTBLC35581; MTBLC140761; MTBLC15940; MTBLC70958; MTBLC18095; MTBLC68616; MTBLC16436; MTBLC67818; MTBLC27632; MTBLC15846; MTBLC73261; MTBLC193587; MTBLC16422; MTBLC49033; MTBLC16171; MTBLC18257; MTBLC17515; MTBLC16411; MTBLC18295; MTBLC71464; MTBLC16092; MTBLC73830; MTBLC27468; MTBLC17311; MTBLC17821; MTBLC73393; MTBLC48981; MTBLC184023; MTBLC167742; MTBLC16962; MTBLC228605; MTBLC17295; MTBLC17026; MTBLC17368; MTBLC16015; MTBLC27897; MTBLC17596; MTBLC17895; MTBLC18183; MTBLC18089; MTBLC27480; MTBLC16235; MTBLC17061; MTBLC36006; MTBLC7916; MTBLC17053; MTBLC17687; MTBLC28865; MTBLC17509; MTBLC17015; MTBLC143163; MTBLC16543; MTBLC17786; MTBLC137830; MTBLC23316; MTBLC18347; MTBLC183451; MTBLC18176; MTBLC69187; MTBLC176697; MTBLC18132; MTBLC138785; MTBLC183493; MTBLC190618; MTBLC137125; MTBLC64564; MTBLC1606; MTBLC183699; MTBLC91038; MTBLC28201; MTBLC183779; MTBLC183379; MTBLC190600; MTBLC176723; MTBLC70101; MTBLC29019; MTBLC176730; MTBLC156149; MTBLC183755; MTBLC48093; MTBLC181232; MTBLC177499; MTBLC168877; MTBLC171809; MTBLC190661; MTBLC194256; MTBLC16737; MTBLC34800; MTBLC34162; MTBLC42255; MTBLC27452; MTBLC16668; MTBLC73580; MTBLC183436; MTBLC183696; MTBLC190647; MTBLC182459; MTBLC17033; MTBLC190604; MTBLC136218; MTBLC180593; MTBLC16576; MTBLC16562; MTBLC16856; MTBLC183468; MTBLC73707; MTBLC143265; MTBLC194258; MTBLC89242; MTBLC183477; MTBLC70744; MTBLC183428; MTBLC31747; MTBLC39867; MTBLC28801; MTBLC194286; MTBLC194252; MTBLC24741; MTBLC167825; MTBLC190551; MTBLC17553; MTBLC138364; MTBLC7027; MTBLC89310; MTBLC64566; MTBLC90355; MTBLC89469; MTBLC72842; MTBLC183449; MTBLC28054; MTBLC91272; MTBLC17306; MTBLC182253; MTBLC7125; MTBLC16634; MTBLC165632; MTBLC27647; MTBLC183424; MTBLC25013; MTBLC75539; MTBLC1457; MTBLC228637; MTBLC230582; MTBLC136086; MTBLC16393; MTBLC16283; MTBLC3291; MTBLC74860; MTBLC84883; MTBLC183650; MTBLC1015; MTBLC89929; MTBLC94459; MTBLC190627; MTBLC183259; MTBLC17362; MTBLC21547; MTBLC165271; MTBLC81689; MTBLC22198; MTBLC190535; MTBLC9171; MTBLC65408; MTBLC31459; MTBLC190634; MTBLC2003; MTBLC28792; MTBLC16680; MTBLC165794; MTBLC17252; MTBLC52392; MTBLC40131; MTBLC190555; MTBLC183438; MTBLC190585; MTBLC64294; MTBLC17859; MTBLC183726; MTBLC183679; MTBLC17115; MTBLC190588; MTBLC17490; MTBLC176732; MTBLC170065; MTBLC74767; MTBLC34450; MTBLC136085; MTBLC16335; MTBLC228611; MTBLC61694; MTBLC73527; MTBLC228718; MTBLC183748; MTBLC5812; MTBLC190569; MTBLC61646; MTBLC190648; MTBLC1301; MTBLC5070; MTBLC72605; MTBLC192673; MTBLC201644; MTBLC74838; MTBLC190638; MTBLC28821; MTBLC87625; MTBLC178528; MTBLC183729; MTBLC228459; MTBLC183677; MTBLC16831; MTBLC190622; MTBLC16344; MTBLC15746; MTBLC190643; MTBLC28918; MTBLC183666; MTBLC72843; MTBLC28940; MTBLC18385; MTBLC88714; MTBLC170016; MTBLC27961; MTBLC3086; MTBLC176815; MTBLC183382; MTBLC4743; MTBLC183416; MTBLC4828; MTBLC176703; MTBLC18040; MTBLC16600; MTBLC4629; MTBLC6052; MTBLC29009; MTBLC78033; MTBLC62434; MTBLC194266; MTBLC68499; MTBLC15414; MTBLC183716; MTBLC176817; MTBLC157747; MTBLC70700; MTBLC169985; MTBLC190579; MTBLC165524; MTBLC170048; MTBLC183757; MTBLC46932; MTBLC183329; MTBLC30860; MTBLC89640; MTBLC190593; MTBLC195592; MTBLC183718; MTBLC31575; MTBLC21363; MTBLC183453; MTBLC17482; MTBLC181895; MTBLC183762; MTBLC48153; MTBLC4874; MTBLC165591; MTBLC192630; MTBLC17621; MTBLC192664; MTBLC17622; MTBLC167001; MTBLC32065; MTBLC21803; MTBLC170038; MTBLC183427; MTBLC174991; MTBLC32805; MTBLC190641; MTBLC183480; MTBLC190581; MTBLC228791; MTBLC183450; MTBLC141472; MTBLC192649; MTBLC42534; MTBLC90031; MTBLC183706; MTBLC66729; MTBLC63795; MTBLC192628; MTBLC17345; MTBLC6775; MTBLC17561; MTBLC228831; MTBLC183474; MTBLC136995; MTBLC228686; MTBLC170032; MTBLC170023; MTBLC228673; MTBLC228559; MTBLC1189; MTBLC81771; MTBLC16998; MTBLC183322; MTBLC228654; MTBLC183353; MTBLC192567; MTBLC17263; MTBLC32365; MTBLC167561; MTBLC183406; MTBLC136100; MTBLC741548; MTBLC176838; MTBLC183673; MTBLC24536; MTBLC183684; MTBLC182331; MTBLC192631; MTBLC132121; MTBLC28140; MTBLC183459; MTBLC31111; MTBLC183418; MTBLC183681; MTBLC183767; MTBLC183793; MTBLC2295; MTBLC16347; MTBLC180410; MTBLC85299; MTBLC172483; MTBLC19702; MTBLC20794; MTBLC144783; MTBLC170045; MTBLC190542; MTBLC17310; MTBLC167860; MTBLC21557; MTBLC183784; MTBLC38572; MTBLC135338; MTBLC190559; MTBLC165293; MTBLC228725; MTBLC4047; MTBLC28195; MTBLC192590; MTBLC27551; MTBLC228797; MTBLC90324; MTBLC190642; MTBLC36575; MTBLC183687; MTBLC28689; MTBLC172139; MTBLC192584; MTBLC163396; MTBLC19289; MTBLC228761; MTBLC164107; MTBLC16828; MTBLC44811; MTBLC143747; MTBLC190633; MTBLC16946; MTBLC68234; MTBLC190659; MTBLC9172; MTBLC15919; MTBLC27436; MTBLC228794; MTBLC156288; MTBLC89315; MTBLC16020; MTBLC41033; MTBLC183417; MTBLC23965; MTBLC69686; MTBLC2696; MTBLC68451; MTBLC181512; MTBLC7563; MTBLC170055; MTBLC35018; MTBLC18145; MTBLC37574; MTBLC17215; MTBLC7466; MTBLC16978; MTBLC228643; MTBLC134592; MTBLC16709; MTBLC228532; MTBLC68433; MTBLC17898; MTBLC125255; MTBLC183776; MTBLC192735; MTBLC17347; MTBLC190603; MTBLC136071; MTBLC1387; MTBLC15964; MTBLC228451; MTBLC182644; MTBLC190601; MTBLC9629; MTBLC48526; MTBLC90027; MTBLC192635; MTBLC133246; MTBLC16908; MTBLC6754; MTBLC73688; MTBLC89649; MTBLC28171; MTBLC190578; MTBLC1582; MTBLC192611; MTBLC192650; MTBLC228696; MTBLC6067; MTBLC4591; MTBLC15714; MTBLC89741; MTBLC181492; MTBLC228554; MTBLC194278; MTBLC190595; MTBLC168507; MTBLC228692; MTBLC194288; MTBLC21626; MTBLC228418; MTBLC86612; MTBLC183758; MTBLC37455; MTBLC6257; MTBLC190621; MTBLC177757; MTBLC181115; MTBLC183732; MTBLC228561; MTBLC64983; MTBLC15374; MTBLC211931; MTBLC170034; MTBLC135554; MTBLC32692; MTBLC190538; MTBLC18406; MTBLC183401; MTBLC183490; MTBLC3359; MTBLC191070; MTBLC190547; MTBLC5262; MTBLC190611; MTBLC173349; MTBLC190592; MTBLC228439; MTBLC27974; MTBLC137590; MTBLC18332; MTBLC47417; MTBLC17489; MTBLC7602; MTBLC192661; MTBLC89187; MTBLC192607; MTBLC228433; MTBLC75095; MTBLC174296; MTBLC31345; MTBLC72723; MTBLC16797; MTBLC9449; MTBLC183769; MTBLC228471; MTBLC166929; MTBLC94686; MTBLC21563; MTBLC9400; MTBLC34135; MTBLC84940; MTBLC194260; MTBLC52446; MTBLC190612; MTBLC183482; MTBLC183484; MTBLC176699; MTBLC183778; MTBLC93879; MTBLC191093; MTBLC190646; MTBLC173050; MTBLC182811; MTBLC15760; MTBLC192660; MTBLC183780; MTBLC228526; MTBLC181585; MTBLC174417; MTBLC168762; MTBLC48400; MTBLC183788; MTBLC16231; MTBLC40799; MTBLC28388; MTBLC190582; MTBLC7478; MTBLC33216; MTBLC167729; MTBLC194178; MTBLC82679; MTBLC16750; MTBLC29073; MTBLC64569; MTBLC183825; MTBLC64575; MTBLC72387; MTBLC75913; MTBLC64032; MTBLC17443; MTBLC85252; MTBLC27747; MTBLC17012; MTBLC22653; MTBLC52075; MTBLC15811; MTBLC30915; MTBLC48928; MTBLC91296; MTBLC12962; MTBLC64565; MTBLC17287; MTBLC183683; MTBLC78697; MTBLC27823; MTBLC67055; MTBLC82965; MTBLC39236; MTBLC40410; MTBLC18240; MTBLC73805; MTBLC72391; MTBLC9481; MTBLC45996; MTBLC16027; MTBLC16708; MTBLC84441; MTBLC72385; MTBLC28670; MTBLC73713; MTBLC73517; MTBLC16345; MTBLC15727; MTBLC16927; MTBLC61058; MTBLC17381; MTBLC73828; MTBLC16990; MTBLC192679; MTBLC15560; MTBLC55484; MTBLC183317; MTBLC53210; MTBLC17460; MTBLC15694; MTBLC194267; MTBLC73770; MTBLC104011; MTBLC132403; MTBLC58527; MTBLC27373; MTBLC18323; MTBLC19062; MTBLC70989; MTBLC138533; MTBLC70976; MTBLC189117; MTBLC73026</t>
-  </si>
-  <si>
-    <t>MTBLS804</t>
-  </si>
-  <si>
-    <t>Rapid UHPLC-MS metabolite profiling and phenotypic assays reveal genotypic impacts of nitrogen supplementation in oats</t>
-  </si>
-  <si>
-    <t>&lt;div&gt;&lt;b&gt;INTRODUCTION:&lt;/b&gt; Oats (Avena sativa L.) are a whole grain cereal recognised for their health benefits and which are cultivated largely in temperate regions providing both a source of food for humans and animals, as well as being used in cosmetics and as a potential treatment for a number of diseases. Oats are known as being a cereal source high in dietary fibre (e.g. beta-glucans), as well as being high in antioxidants, minerals and vitamins. Recently, oats have been gaining increased global attention due to their large number of beneficial health effects. Consumption of oats has been proven to lower blood LDL cholesterol levels and blood pressure, thus reducing the risk of heart disease, as well as reducing blood-sugar and insulin levels.&lt;/div&gt;&lt;div&gt;&lt;b&gt;OBJECTIVES:&lt;/b&gt; Oats are seen as a low input cereal. Current agricultural guidelines on nitrogen application are believed to be suboptimal and only consider the effect of nitrogen on grain yield. It is important to understand the role of both variety and of crop management in determining nutritional quality of oats. In this study the response of yield, grain quality and grain metabolites to increasing nitrogen application to levels greater than current guidelines were investigated.&lt;/div&gt;&lt;div&gt;&lt;b&gt;METHODS:&lt;/b&gt; Four winter oat varieties (Mascani, Tardis, Balado and Gerald) were grown in a replicated nitrogen response trial consisting of a no added nitrogen control and four added nitrogen treatments between 50 and 200&amp;nbsp;kg&amp;nbsp;N&amp;nbsp;ha-1 in a randomised split-plot design. Grain yield, milling quality traits, beta-glucan, total protein and oil content were assessed. The de-hulled oats (groats) were also subjected to a rapid Ultra High Performance Liquid Chromatography-Mass Spectrometry (UHPLC-MS) metabolomic screening approach.&lt;/div&gt;&lt;div&gt;&lt;b&gt;RESULTS:&lt;/b&gt; Application of nitrogen had a significant effect on grain yield but there was no significant difference between the response of the four varieties. Grain quality traits however displayed significant differences both between varieties and nitrogen application level. beta-glucan content significantly increased with nitrogen application. The UHPLC-MS approach has provided a rapid, sub 15&amp;nbsp;min per sample, metabolite profiling method that is repeatable and appropriate for the screening of large numbers of cereal samples. The method captured a wide range of compounds, inclusive of primary metabolites such as the amino acids, organic acids, vitamins and lipids, as well as a number of key secondary metabolites, including the avenanthramides, caffeic acid, and sinapic acid and its derivatives and was able to identify distinct metabolic phenotypes for the varieties studied. Amino acid metabolism was massively upregulated by nitrogen supplementation as were total protein levels, whilst the levels of organic acids were decreased, likely due to them acting as a carbon skeleton source. Several TCA cycle intermediates were also impacted, potentially indicating increased TCA cycle turn over, thus providing the plant with a source of energy and reductant power to aid elevated nitrogen assimilation. Elevated nitrogen availability was also directed towards the increased production of nitrogen containing phospholipids. A number of both positive and negative impacts on the metabolism of phenolic compounds that have influence upon the health beneficial value of oats and their products were also observed.&lt;/div&gt;&lt;div&gt;&lt;b&gt;CONCLUSIONS:&lt;/b&gt; Although the developed method has broad applicability as a rapid screening method or a rapid metabolite profiling method and in this study has provided valuable metabolic insights, it still must be considered that much greater confidence in metabolite identification, as well as quantitative precision, will be gained by the application of higher resolution chromatography methods, although at a large expense to sample throughput. Follow up studies will apply higher resolution GC (gas chromatography) and LC (reversed phase and HILIC) approaches, oats will be also analysed from across multiple growth locations and growth seasons, effectively providing a cross validation for the results obtained within this preliminary study. It will also be fascinating to perform more controlled experiments with sampling of green tissues, as well as oat grains, throughout the plants and grains development, to reveal greater insight of carbon and nitrogen metabolism balance, as well as resource partitioning into lipid and secondary metabolism.&lt;/div&gt;</t>
-  </si>
-  <si>
-    <t>ultra-performance liquid chromatography-mass spectrometry; nitrogen molecular entity; bio-variety; grain quality trait; beta-D-glucan; amino acid; Lipidomics; Avenanthramides</t>
-  </si>
-  <si>
-    <t>Rapid UHPLC-MS metabolite profiling and phenotypic assays reveal genotypic impacts of nitrogen supplementation in oats. 10.1007/s11306-019-1501-x. PMID:30868357</t>
-  </si>
-  <si>
-    <t>The trial was conducted at Lydbury North, Shropshire, UK (latitude 52.45, longitude 2.94, medium soil type) in a split plot design with 3 replicates using 5 levels of nitrogen application (main plot treatment) and 4 commercially available winter oat varieties (sub-plot treatment) from the Aberystwyth University winter oat breeding programme. These included 2 of the most widely grown winter oat varieties in the UK over the last 20 years, Gerald and Mascani (AHDB 2015). 3 varieties were of conventional height (Mascani, Gerald and Tardis) and the fourth was a dwarf variety (Balado). Plots (1.8 x 6 m) were sown on the 9th October 2013 at a sowing rate of 300 seeds/m^2 and harvested on the 7th August 2014 using a small plot combine. Fungicides and weed control followed standard practise for winter oats including the use of a plant growth regulator (Cycocel 5C). Soils were sampled to a depth of 90 cm in early spring and residual soil nitrogen was determined to be 58 kg N/ha. Nitrogen (ammonium nitrate) doses were split between 3 different developmental stages in early to late spring as indicated in Table S1 in the paper associated with this study, to provide 5 final doses: Control, no applied nitrogen; level 1, 50 kg N/ha applied; level 2, 100 kg N/ha applied; level 3, 150 kg N/ha applied; level 4, 200 kg N/ha applied. The 17th April application date corresponded to growth stage 31 (early stem elongation, Zadoks et al. 1974). Prior to harvest the number of fertile shoots (panicles) per m2 were counted and plant heights from soil surface to panicle tip measured.&lt;/br&gt;&lt;/br&gt;Ref:&lt;/br&gt;[1] Zadoks JC, Chang TT, Konzak CF. Decimal code for growth stages of cereals. Weed Research. 1974;14:415421. doi:10.1111/j.1365-3180.1974.tb01084.x&lt;/br&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;The dehulled oat samples were first homogenised using a Retsch Cyclone Mill-Twister with the following settings: speed 12,000 rpm/min; 62 ms peripheral rotor speed; 1 mm sieve; 1 min cycle. 100 mg  2 mg FW of oats were weighed into 2 ml safe-lock Eppendorf microcentrifuge tubes, 1.5 ml of extraction buffer (10 uM reserpine and 10 M morin in 75% methanol 24.9% water 0.1% formic acid) was added, the sample was vortexed for 15 s, ultrasonicated for 15 min with an Elma S40 ultrasonicator, vortexed for 15 s, agitated on an IKA VXR basic vibrax fitted with the VX2E.n Eppendorf tube adapter set on speed 8 for 30 min, and centrifuged for 10 min at 3 C and 18,407 x g with an Eppendorf 5424R (rotor FA-45-24-11). The extract supernatants were next filtered with 0.45um PTFE filter vials (Thomson single step) and transferred to 2 ml HPLC vials with pre-slit caps (Thermo-Fisher, Chromacol 2SVW and 9-SCK(B)-ST1 X, respectively). A quality assurance (QA) sample was prepared by mixing equal quantities of each sample extract, thus providing a QA sample representative of the average of the entire sample set. A number of representative samples were also extracted and analysed in triplicate (denoted as a, b, and c, within the sample number) to serve as reference samples to define extraction and analytical repeatability. The samples were stored in the HPLC autosampler at 10 C and analysed within 72 h of extraction in positive and negative electrospray ionisation (ESI) modes. The ESI source spray cone and ion tube were cleaned between running the sample set in each ionisation mode.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>UHPLC separations were performed with a Thermo Accela 600 HPLC system coupled with an Accela PDA detector (Thermo-Fisher Ltd. U.K). The HPLC was operated at a flow rate of 400 l/min, the column and guard column (Thermo Hypersil Gold C18 50 x 2.1 mm, 1.9 m particle size; Hypersil Gold C18 Guard 10 x 2.1 mm, 3 m particle size; Thermo Universal Uniguard guard holder 2.1/3 mm) were maintained at a temperature of 40 C. The solvent A, HPLC grade water, and solvent B, HPLC grade acetonitrile, were acidified with 0.1% [v/v] MS grade formic acid. Prior to sample analysis a new UHPLC column and guard column were conditioned with solvents A and B for a minimum of 40 min at a flow rate of 400 l/min. A sample injection volume of 5 l was employed in full-loop mode. The gradient programme was as follows: hold 5% B 01 min, 5100% B 18 min, hold 100% B 811 min, 1005% B 1111.1 min, hold 5% B 11.115 min. Autosampler syringe and line washes were performed with 80% HPLC grade acetonitrile 20% HPLC grade water. The UHPLC column eluent was first monitored by the Accela PDA detector where spectra were collected in wavelength/absorbance mode from 200 to 600 nm with a filter bandwidth and wavelength step of 1 nm, the filter rise time was 1 s, the sample rate was 10 Hz. Additionally three channel set points were employed, Channel A 280 nm, Channel B 365 nm, Channel C 520 nm, with a bandwidth of 9 nm and a sample rate of 10 Hz.</t>
-  </si>
-  <si>
-    <t>The PDA detector eluent was next transfered to a Thermo LTQ-Orbitrap XL mass spectrometry system operated under Xcalibur software (Thermo-Fisher Ltd. UK). Mass spectra were primarilly collected in full scan mode (m/z 1001200) at a mass resolution of 30,000 (FWHM defined at m/z 400) within the FT detector for all samples. An additional method was applied to obtain ion trees by performing data-dependent analysis (DDA) MS2 on the top 3 most intense ions for the mixed QA sample[1]. The DDA method applied a primary full scan event within the FT, followed by a secondary scan event within the LTQ-IT to collect MS2 CID fragmentation spectra for the top 3 most intense ions as defined within the preliminary full MS scan. Helium was applied as a collision gas for CID at a normalised collision energy of 45%, a trapping window width of 2 ( 1) m/z was applied, an activation time of 30 ms and activation Q of 0.25 were applied, only singly charged ions were selected for DDA, isotopic ions were also excluded. The preliminary full scan event within the FT generated profile mode data, whereas the LTQ-IT MS2 data were collected in 'centroid' mode.&lt;/br&gt;&lt;/br&gt;A scan speed of 0.1 s and 0.4 s were applied in the LTQ-IT and FT-MS respectively. The Automatic Gain Control was set to 1 x 10^5 and 1 x 10^6 for the LTQ-IT and FT-MS respectively. Prior to the analytical run the LTQ-IT and FT-MS were tuned to optimise conditions for the detection of ions in the mid detection range of m/z 1001200, as well as being calibrated with the manufacturers recommended calibration mixture and procedures. The ESI conditions were optimised to allow efficient ionisation and ion transmission whilst limiting insource fragmentation. The following settings were applied to ESI: Spray voltage 3.5 kV (ESI) and +4.5 kV (ESI+); Sheath gas 60; Auxiliary gas 30; Capillary voltage 35 V (ESI)+35 V (ESI+); Tube lens voltage 100 V (ESI) and +100 V (ESI+); Capillary temperature 280 C; ESI probe temperature 100 C.&lt;/br&gt;&lt;/br&gt;The samples were analysed in a completely randomised order as 2 independent analytical blocks, each of approximately 100 injections, respective of ESI positive and ESI negative polarities. For each analytical block, initially 8 injections of QA sample were performed for LC-MS system conditioning, after which 3 further injections of QA sample were performed, followed by 6 injections of experimental samples and a further QA injection. This was repeated until all samples were analysed, finally the analytical block was concluded with a further 3 QA injections. A control blank sample was analysed at the start and end of the analytical block, thus providing a measure of the sample background and also a measure of compound carry over resulting from dirtying of the ESI source. Each analytical block was finally concluded by collection of the DDA MS2 profiles for the QA sample.&lt;/br&gt;&lt;/br&gt;Ref:&lt;/br&gt;[1] Mullard G, Allwood JW, Webber RJM, Brown M, Begley P, Hollywood KA, Jones M, Unwin RD, Bishop PN, Cooper GJS, Dunn WB. A new strategy for MS/MS data acquisition applying multiple data dependent experiments on Orbitrap mass spectrometers in non-targeted metabolomics applications. Metabolomics. 2015;11(5):10681080. doi:10.1007/s11306-014-0763-6.&lt;/br&gt;</t>
-  </si>
-  <si>
-    <t>The UHPLC-PDA-MS raw data profiles were first converted into an MZML centroid format within the Proteowizard (http://proteowizard.sourceforge.net/) MSConvert software package. Each MZML based three-dimensional data matrix (intensityxm/zxtime1 per sample) was converted (or deconvolved) into a vector of peak responses, where a peak response is defined as the sum of intensities over a window of specified mass and time range (e.g. m/z = 102.1  0.01 and time = 130  10 s). In this experiment the deconvolution was performed using the freely available XCMS online package (https://xcmsonline.scripps.edu/). XCMS online was operated with the following parameter set points: Feature detection; methodCentWave; mass error 5 ppm, minimum and maximum peak width 5 and 30 s respectively, mzdiff 0.01, S/N threshold 10, integration method 1, prefilter peaks 3, prefilter intensity 40,000, noise filter 100,000: RT correction; method  Obiwarp, profstep 1: Alignment; minfrac 0.5, mz width 0.015, bw 5, min samp 1, max samp 100: Annotation; Search for isotopes + adducts, mz absolute error 0.015, ppm error 5.&lt;/br&gt;&lt;/br&gt;The XCMS deconvolution results in the production of a Microsoft Excel based XY matrix containing the paired RT and m/z of each feature, along with the peak area in each profiled sample, and where provided, adduct and isotope annotations for each m/z. The XY matrix was trimmed of peaks that eluted within the first 0.3 min and final 4 min of chromatography (the void and equilibration periods), as well as removal of peaks that were dominant within blank sample extracts (more than 2 more intense than the peaks highest intensity within a biological sample)[1]. &lt;/br&gt;&lt;/br&gt;Ref:&lt;/br&gt;[1] Di Guida R, Engel J, Allwood JW, Weber RJ, Jones MR, Sommer U, Viant MR, Dunn WB. Non-targeted UHPLC-MS metabolomic data processing methods: a comparative investigation of normalisation, missing value imputation, transformation and scaling. Metabolomics. 2016;12:93. Epub 2016 Apr 15. doi:10.1007/s11306-016-1030-9. PMID:27123000&lt;/br&gt;</t>
-  </si>
-  <si>
-    <t>Applying a set of workflows known as PutMedID which are operated within the Taverna Workbench 1.7.2 software package[1]-[3], peak to peak Pearson correlations were first calculated within a 5 s moving RT window, peaks that show a high level of Pearson correlation (greater than 0.8) within the same RT window were grouped as m/z features that were likely associated with the same compound (i.e. an m/z group). As a second step, accurate mass differences between m/z within each peak group were calculated to allow the annotation of the parent m/z from isotopic and adduct ions. Consensus was drawn between the two methods of peak annotation performed within XCMS online and PutMedID. Once the parent ion, adducts and isotopes are annotated within each peak group, the neutral accurate mass is calculated for each ion (5 ppm mass error) and in turn matched to possible molecular formula(s), which are then matched to metabolite name(s). Molecular formula and metabolite matching were based upon a library of known plant metabolites obtained from the Plant Metabolic Network PlantCyc database (http://www.plantcyc.org) in addition to the Manchester Metabolomics Database (MMD: http://dbkgroup.org/MMD/), thus in most cases providing an MSI level 2 or 3 identification[4]. Where multiple putative molecular formula or metabolite identifications were obtained by the peak annotation approach, the identifications were also manually checked for having been previously reported as an oat metabolite (FooDB: http://foodb.ca/), thus increasing confidence in the assigned putative identification(s). In the case of lipids where multiple isomeric species could be assigned to a given accurate mass, the lipids fatty acid chain lengths and numbers of unsaturated bonds were summed in order to condense the high numbers of isomeric identifications.&lt;/br&gt;&lt;/br&gt;Ref:&lt;/br&gt;[1] Brown M, Dunn WB, Dobson P, Patel Y, Winder CL, Francis-McIntyre S, Begley P, Carroll K, Broadhurst D, Tseng A, Swainston N, Spasic I, Goodacre R, Kell DB. Mass spectrometry tools and metabolite-specific databases for molecular identification in metabolomics. Analyst. 2009 Jul;134(7):1322-32. doi:10.1039/b901179j. PMID:19562197&lt;/br&gt;[2] Brown M, Wedge DC, Goodacre R, Kell DB, Baker PN, Kenny LC, Mamas MA, Neyses L, Dunn WB. Automated workflows for accurate mass-based putative metabolite identification in LC/MS-derived metabolomic datasets. Bioinformatics. 2011 Apr 15;27(8):1108-12. doi: 0.1093/bioinformatics/btr079. PMID:21325300&lt;/br&gt;[3] Allwood JW, Weber RJ, Zhou J, He S, Viant MR, Dunn WB. CASMI-The Small Molecule Identification Process from a Birmingham Perspective. Metabolites. 2013 May 21;3(2):397-411. doi:10.3390/metabo3020397. PMID:24957998&gt;/br&gt;[4] Sumner LW, Amberg A, Barrett D, Beale MH, Beger R, Daykin CA, Fan TW et al. Proposed minimum reporting standards for chemical analysis Chemical Analysis Working Group (CAWG) Metabolomics Standards Initiative (MSI). Metabolomics. 2007 Sep;3(3):211-221. doi:10.1007/s11306-007-0082-2. PMID:24039616&lt;/br&gt;</t>
-  </si>
-  <si>
-    <t>MTBLC34262; MTBLC27951; MTBLC27797; MTBLC16713; MTBLC34454; MTBLC47220; MTBLC28967; MTBLC37144; MTBLC28960; MTBLC28905; MTBLC15368; MTBLC1217; MTBLC44692; MTBLC45285; MTBLC1467; MTBLC72700; MTBLC16119; MTBLC16199; MTBLC16607; MTBLC16610; MTBLC4614; MTBLC19092; MTBLC28638; MTBLC30322; MTBLC17203; MTBLC1439; MTBLC37600; MTBLC27371; MTBLC16070; MTBLC74863; MTBLC27411; MTBLC15866; MTBLC28847; MTBLC28140; MTBLC18287; MTBLC42606; MTBLC27907; MTBLC27442; MTBLC27586; MTBLC137774; MTBLC63150; MTBLC17617; MTBLC16935; MTBLC62345; MTBLC17897; MTBLC27708; MTBLC9652; MTBLC17059; MTBLC16357; MTBLC15971; MTBLC17064; MTBLC30818; MTBLC89640; MTBLC27248; MTBLC31042; MTBLC16572; MTBLC1580; MTBLC1879; MTBLC26797; MTBLC17578; MTBLC34213; MTBLC27869; MTBLC15767; MTBLC16089; MTBLC2319; MTBLC5966; MTBLC16380; MTBLC17143; MTBLC31173; MTBLC31278; MTBLC64977; MTBLC5320; MTBLC71166; MTBLC27480; MTBLC16355; MTBLC2600; MTBLC133351; MTBLC17881; MTBLC28928; MTBLC27616; MTBLC16100; MTBLC17641; MTBLC90886; MTBLC1139; MTBLC1387; MTBLC17095; MTBLC76163; MTBLC114204; MTBLC34252; MTBLC34256; MTBLC79445; MTBLC34876; MTBLC34877; MTBLC3007; MTBLC8986; MTBLC31054; MTBLC2932; MTBLC31435; MTBLC6945; MTBLC8616; MTBLC9183; MTBLC5959; MTBLC5708; MTBLC7468; MTBLC88104; MTBLC139134; MTBLC73926; MTBLC139133; MTBLC82679; MTBLC137760; MTBLC82678; MTBLC79877; MTBLC17747; MTBLC34710; MTBLC34679; MTBLC34097; MTBLC16323; MTBLC18385; MTBLC43997; MTBLC80424; MTBLC134287; MTBLC16929; MTBLC508; MTBLC60872; MTBLC70824; MTBLC68451; MTBLC16852; MTBLC134850; MTBLC9008; MTBLC16181; MTBLC28393; MTBLC28328; MTBLC47977; MTBLC62324; MTBLC24103; MTBLC31747; MTBLC28945; MTBLC31997; MTBLC19332; MTBLC16467; MTBLC10454; MTBLC5121; MTBLC5139; MTBLC5356; MTBLC5358; MTBLC69039; MTBLC93403; MTBLC63112; MTBLC16870; MTBLC17874; MTBLC28057; MTBLC28586; MTBLC62976; MTBLC62006; MTBLC17321; MTBLC3017; MTBLC51805; MTBLC2302; MTBLC2304; MTBLC17913; MTBLC3766; MTBLC79576; MTBLC38159; MTBLC25426; MTBLC16060; MTBLC3703; MTBLC27509; MTBLC4740; MTBLC6931; MTBLC7906; MTBLC5578; MTBLC59560; MTBLC15372; MTBLC80385; MTBLC952; MTBLC1141; MTBLC27852; MTBLC41941; MTBLC86553; MTBLC30816; MTBLC16388; MTBLC20415; MTBLC1881; MTBLC89830; MTBLC44747; MTBLC32807; MTBLC17151; MTBLC18403; MTBLC15963; MTBLC16207; MTBLC17597; MTBLC30746; MTBLC16008; MTBLC79966; MTBLC46807; MTBLC133314; MTBLC19891; MTBLC16138; MTBLC57653; MTBLC33917; MTBLC22357; MTBLC37690; MTBLC28061; MTBLC17925; MTBLC28729; MTBLC10295; MTBLC28645; MTBLC27667; MTBLC15903; MTBLC28994; MTBLC28563; MTBLC17393; MTBLC28385; MTBLC15824; MTBLC16824; MTBLC4139; MTBLC4167; MTBLC27611; MTBLC18004; MTBLC4194; MTBLC28014; MTBLC16024; MTBLC27605; MTBLC17317; MTBLC16443; MTBLC28458; MTBLC48095; MTBLC17234; MTBLC24978; MTBLC17357; MTBLC27987; MTBLC17268; MTBLC10642; MTBLC27922; MTBLC25858; MTBLC28946; MTBLC28177; MTBLC17605; MTBLC18280; MTBLC8240; MTBLC28354; MTBLC27806; MTBLC27816; MTBLC28816; MTBLC40274; MTBLC30156; MTBLC44842; MTBLC17807; MTBLC20106; MTBLC68329; MTBLC16899; MTBLC17924; MTBLC17505; MTBLC18202; MTBLC28789; MTBLC29864; MTBLC6259; MTBLC17656; MTBLC32800; MTBLC18414; MTBLC28478; MTBLC19868; MTBLC27978; MTBLC17445; MTBLC1581; MTBLC18346; MTBLC85239; MTBLC20414; MTBLC35164; MTBLC18101; MTBLC40813; MTBLC20450; MTBLC17637; MTBLC31835; MTBLC31832; MTBLC8075; MTBLC29672; MTBLC17702; MTBLC28889; MTBLC17631; MTBLC64835; MTBLC27603; MTBLC1683; MTBLC62974; MTBLC28087; MTBLC28460; MTBLC17164; MTBLC15354; MTBLC16182; MTBLC16638; MTBLC16133; MTBLC16472; MTBLC87755; MTBLC84069; MTBLC16019; MTBLC46941; MTBLC53608; MTBLC79569; MTBLC17243; MTBLC134341; MTBLC88427; MTBLC34687; MTBLC79053; MTBLC4316; MTBLC10607; MTBLC88526; MTBLC32337; MTBLC10525; MTBLC27801; MTBLC29732; MTBLC2959; MTBLC52859; MTBLC80420; MTBLC2818; MTBLC17929; MTBLC25682; MTBLC81297; MTBLC17417; MTBLC144066; MTBLC142578; MTBLC18037; MTBLC3210; MTBLC3474; MTBLC8613; MTBLC2247; MTBLC17311; MTBLC35619; MTBLC138425; MTBLC27971; MTBLC27389; MTBLC16865; MTBLC33094; MTBLC28797; MTBLC37081; MTBLC5588; MTBLC17724; MTBLC15620; MTBLC138669; MTBLC17519; MTBLC37581; MTBLC17217; MTBLC16413; MTBLC23500; MTBLC16583; MTBLC36253; MTBLC46916; MTBLC478164; MTBLC17765; MTBLC15754; MTBLC24168; MTBLC4728; MTBLC134255; MTBLC77131; MTBLC15643; MTBLC33098; MTBLC39931; MTBLC86390; MTBLC30753; MTBLC35227; MTBLC30754; MTBLC42682; MTBLC134761; MTBLC18123; MTBLC32114; MTBLC47564; MTBLC139; MTBLC16703; MTBLC531; MTBLC27380; MTBLC16885; MTBLC17332; MTBLC64833; MTBLC28782; MTBLC28793; MTBLC3528; MTBLC31005; MTBLC27680; MTBLC27649; MTBLC6364; MTBLC27931; MTBLC6731; MTBLC7912; MTBLC18154; MTBLC16634; MTBLC9859; MTBLC32059; MTBLC83804; MTBLC16546; MTBLC18428; MTBLC28102; MTBLC37165; MTBLC28808; MTBLC90185; MTBLC141517; MTBLC50663; MTBLC4954; MTBLC135681; MTBLC73275; MTBLC140748; MTBLC7982; MTBLC31576; MTBLC135209; MTBLC137782; MTBLC23875; MTBLC73892; MTBLC33020; MTBLC1230; MTBLC16551; MTBLC39244; MTBLC28676; MTBLC18260; MTBLC27554; MTBLC77436; MTBLC18167; MTBLC36217; MTBLC71422; MTBLC36218; MTBLC18147; MTBLC17057; MTBLC4125; MTBLC21010; MTBLC17306; MTBLC4808; MTBLC133330; MTBLC28066; MTBLC16751; MTBLC28189; MTBLC17716; MTBLC6359; MTBLC18411; MTBLC6435; MTBLC25164; MTBLC28053; MTBLC7570; MTBLC18394; MTBLC17992; MTBLC5105; MTBLC143968; MTBLC17705; MTBLC16708; MTBLC16347; MTBLC73707; MTBLC89341; MTBLC16817; MTBLC6907; MTBLC80354; MTBLC31085; MTBLC2089; MTBLC4055; MTBLC48294; MTBLC35090; MTBLC6415; MTBLC75627; MTBLC16246; MTBLC16772; MTBLC20582; MTBLC111; MTBLC18427; MTBLC28310; MTBLC18266; MTBLC15975; MTBLC28762; MTBLC28548; MTBLC43943; MTBLC17540; MTBLC320055; MTBLC27732; MTBLC126237; MTBLC36090; MTBLC137825; MTBLC36633; MTBLC28323; MTBLC28873; MTBLC23401; MTBLC32815; MTBLC30851; MTBLC18125; MTBLC32374; MTBLC18697; MTBLC882; MTBLC15980; MTBLC1416; MTBLC27778; MTBLC59052; MTBLC25351; MTBLC6933; MTBLC15607; MTBLC52222; MTBLC36458; MTBLC30835; MTBLC25311; MTBLC30314; MTBLC5958; MTBLC29717; MTBLC27645; MTBLC30906; MTBLC30940; MTBLC29722; MTBLC28176; MTBLC29724; MTBLC15798; MTBLC18128; MTBLC16590; MTBLC3693; MTBLC17989; MTBLC4853; MTBLC139533; MTBLC17618; MTBLC4117; MTBLC82348; MTBLC5673; MTBLC64305; MTBLC3337; MTBLC138529; MTBLC15567; MTBLC17275; MTBLC4607; MTBLC87897; MTBLC37331; MTBLC16939; MTBLC44303; MTBLC82573; MTBLC134821; MTBLC16795; MTBLC17895; MTBLC89461; MTBLC134820; MTBLC34019; MTBLC74516; MTBLC2628; MTBLC3244; MTBLC28709; MTBLC5989; MTBLC7502; MTBLC3546; MTBLC137728; MTBLC27468; MTBLC27578; MTBLC28474; MTBLC16364; MTBLC17681; MTBLC29053; MTBLC28630; MTBLC36751; MTBLC52143; MTBLC62768; MTBLC62770; MTBLC27747; MTBLC28229; MTBLC139383; MTBLC17115; MTBLC29480; MTBLC17960; MTBLC32816; MTBLC6604; MTBLC34867; MTBLC2196; MTBLC39564; MTBLC94764; MTBLC139388; MTBLC74076; MTBLC73580; MTBLC6257; MTBLC28346; MTBLC6792; MTBLC6839; MTBLC18106; MTBLC17286; MTBLC87407; MTBLC4683; MTBLC7797; MTBLC10044; MTBLC3697; MTBLC6765; MTBLC31030; MTBLC28462; MTBLC5792; MTBLC5979; MTBLC31827; MTBLC109895; MTBLC1927; MTBLC46295; MTBLC16009; MTBLC16335; MTBLC17172; MTBLC24088; MTBLC10110; MTBLC8674; MTBLC90721; MTBLC32; MTBLC134766; MTBLC135744; MTBLC63616; MTBLC5384; MTBLC79587; MTBLC44616; MTBLC34731; MTBLC2376; MTBLC64020; MTBLC4071; MTBLC3748; MTBLC23359; MTBLC50540; MTBLC16512; MTBLC6739; MTBLC137234; MTBLC27441; MTBLC28309; MTBLC19065; MTBLC70971; MTBLC16299; MTBLC490877; MTBLC37754; MTBLC27748; MTBLC6520; MTBLC107635; MTBLC84500; MTBLC15781; MTBLC81545; MTBLC81546; MTBLC27478; MTBLC29012; MTBLC9200; MTBLC8245; MTBLC9173; MTBLC32322; MTBLC31311; MTBLC171741; MTBLC92675; MTBLC138493; MTBLC74112; MTBLC61138; MTBLC37079; MTBLC33033; MTBLC16530; MTBLC27401; MTBLC39153; MTBLC45630; MTBLC38531; MTBLC8882; MTBLC6521; MTBLC50973; MTBLC8774; MTBLC137248; MTBLC2819; MTBLC27713; MTBLC19450; MTBLC17645; MTBLC58183; MTBLC17027; MTBLC70979; MTBLC17917; MTBLC724125; MTBLC89963; MTBLC28998; MTBLC1142; MTBLC18395; MTBLC16370; MTBLC15847; MTBLC71429; MTBLC88455; MTBLC42654; MTBLC17596; MTBLC17901; MTBLC87248; MTBLC9447; MTBLC28715; MTBLC21412; MTBLC143078; MTBLC8665; MTBLC55344; MTBLC37755; MTBLC15887; MTBLC17750; MTBLC58441; MTBLC18314; MTBLC16414; MTBLC138668; MTBLC77042; MTBLC134261; MTBLC41139; MTBLC2540; MTBLC10226; MTBLC10364; MTBLC3900; MTBLC4817; MTBLC5177; MTBLC5379; MTBLC5981; MTBLC6070; MTBLC8216; MTBLC73719; MTBLC50178; MTBLC135187; MTBLC17144; MTBLC6407; MTBLC73880; MTBLC79449; MTBLC7575; MTBLC11946; MTBLC3926; MTBLC35280; MTBLC29565; MTBLC15565; MTBLC16856; MTBLC32153; MTBLC6413; MTBLC8426; MTBLC80592; MTBLC51032; MTBLC28598; MTBLC17799; MTBLC57630; MTBLC28718; MTBLC15699; MTBLC16857; MTBLC16256; MTBLC30831; MTBLC137232; MTBLC15344; MTBLC51850; MTBLC16265; MTBLC28867; MTBLC18261; MTBLC17201; MTBLC17196; MTBLC15737; MTBLC29045; MTBLC16770; MTBLC17374; MTBLC28376; MTBLC2165; MTBLC29637; MTBLC39501; MTBLC32069; MTBLC6874; MTBLC5044; MTBLC37628; MTBLC64366; MTBLC17053; MTBLC29990; MTBLC5159; MTBLC18012; MTBLC18300; MTBLC17257; MTBLC135747; MTBLC31785; MTBLC10556; MTBLC5511; MTBLC5534; MTBLC2532; MTBLC2821; MTBLC3287; MTBLC6511; MTBLC1670; MTBLC73757; MTBLC21305; MTBLC18050; MTBLC16352; MTBLC37011; MTBLC16010; MTBLC94613; MTBLC6151; MTBLC139123; MTBLC1241; MTBLC28791; MTBLC62637; MTBLC16015; MTBLC16439; MTBLC45441; MTBLC31882; MTBLC17981; MTBLC36461; MTBLC17415; MTBLC17626; MTBLC17204; MTBLC2424; MTBLC15670; MTBLC30838; MTBLC16600; MTBLC51330; MTBLC75984; MTBLC3734; MTBLC7856; MTBLC9196; MTBLC7959; MTBLC16643; MTBLC50868; MTBLC9384; MTBLC15604; MTBLC89185; MTBLC57826; MTBLC28825; MTBLC18347; MTBLC17191; MTBLC15603; MTBLC64348; MTBLC17878; MTBLC17611; MTBLC17915; MTBLC85235; MTBLC38355; MTBLC49283; MTBLC143856; MTBLC61206; MTBLC79634; MTBLC79456; MTBLC79768; MTBLC79876; MTBLC34930; MTBLC6536; MTBLC17472; MTBLC73740; MTBLC7034; MTBLC5158; MTBLC30845; MTBLC30846; MTBLC74104; MTBLC19274; MTBLC85162; MTBLC23757; MTBLC5826; MTBLC62069; MTBLC223316; MTBLC44934; MTBLC10018; MTBLC135072; MTBLC34405; MTBLC34788; MTBLC31268; MTBLC34756; MTBLC3391; MTBLC53490; MTBLC5847; MTBLC5597; MTBLC79439; MTBLC34619; MTBLC135714; MTBLC7807; MTBLC78549; MTBLC1957; MTBLC20013; MTBLC40521; MTBLC31111; MTBLC34522; MTBLC16079; MTBLC37287; MTBLC37291; MTBLC29064; MTBLC2128; MTBLC9212; MTBLC53763; MTBLC86455; MTBLC45652; MTBLC30449; MTBLC34291; MTBLC17397; MTBLC24814; MTBLC74018; MTBLC52172; MTBLC28682; MTBLC66876; MTBLC9741; MTBLC5515; MTBLC47899; MTBLC8397; MTBLC695; MTBLC9403; MTBLC34307; MTBLC3767; MTBLC68428; MTBLC27527; MTBLC27588; MTBLC29573; MTBLC7599; MTBLC61645; MTBLC79626; MTBLC79729; MTBLC134923; MTBLC16043; MTBLC5457; MTBLC34048; MTBLC48541; MTBLC137772; MTBLC16547; MTBLC9957; MTBLC10366; MTBLC10423; MTBLC15582; MTBLC15583; MTBLC49076; MTBLC18104; MTBLC18078; MTBLC17023; MTBLC27861; MTBLC27550; MTBLC15591; MTBLC16831; MTBLC89205; MTBLC138367; MTBLC28381; MTBLC59051; MTBLC30997; MTBLC6452; MTBLC17937; MTBLC62112; MTBLC3207; MTBLC66913; MTBLC50131; MTBLC31989; MTBLC8097; MTBLC2705; MTBLC137310; MTBLC28502; MTBLC16765; MTBLC31993; MTBLC3085; MTBLC59020; MTBLC28948; MTBLC28136; MTBLC132335; MTBLC31584; MTBLC31952; MTBLC3112; MTBLC15676; MTBLC21860; MTBLC79347; MTBLC68606; MTBLC610092; MTBLC139380; MTBLC34598; MTBLC80544; MTBLC23812; MTBLC87166; MTBLC37245; MTBLC35460; MTBLC16093; MTBLC16558; MTBLC28568; MTBLC218; MTBLC18297; MTBLC2559; MTBLC17973; MTBLC27818; MTBLC17665; MTBLC12350; MTBLC16084; MTBLC27973; MTBLC78736; MTBLC78697; MTBLC37480; MTBLC12937; MTBLC16077; MTBLC14314; MTBLC16588; MTBLC35374; MTBLC17369; MTBLC17837; MTBLC78737; MTBLC24588; MTBLC25448; MTBLC80181; MTBLC28173; MTBLC18365; MTBLC28992; MTBLC1369; MTBLC67375; MTBLC2373; MTBLC17488; MTBLC59353; MTBLC43468; MTBLC35128; MTBLC28652; MTBLC28635; MTBLC30850; MTBLC8809; MTBLC69440; MTBLC4910; MTBLC27429; MTBLC32506; MTBLC79659; MTBLC45980; MTBLC6375; MTBLC3534; MTBLC4997; MTBLC73873; MTBLC9735; MTBLC16927; MTBLC31657; MTBLC135111; MTBLC136292; MTBLC6758; MTBLC16734; MTBLC102524; MTBLC134922; MTBLC17409; MTBLC133172; MTBLC132983; MTBLC78951; MTBLC16445; MTBLC151; MTBLC160; MTBLC15622; MTBLC35453; MTBLC18281; MTBLC17305; MTBLC41893; MTBLC42819; MTBLC30769; MTBLC30887; MTBLC30915; MTBLC17803; MTBLC6885; MTBLC4488; MTBLC27837; MTBLC86556; MTBLC84058; MTBLC3805; MTBLC4520; MTBLC73026; MTBLC73025; MTBLC34923; MTBLC64; MTBLC4628; MTBLC31585; MTBLC76160; MTBLC31981; MTBLC17802; MTBLC16704; MTBLC73715; MTBLC70353; MTBLC34698; MTBLC70453; MTBLC134913; MTBLC90038; MTBLC86004; MTBLC9274; MTBLC9275; MTBLC89730; MTBLC11222; MTBLC34447; MTBLC31402; MTBLC4895; MTBLC6347; MTBLC35796; MTBLC137768; MTBLC3158; MTBLC29513; MTBLC58556; MTBLC17533; MTBLC36554; MTBLC28249; MTBLC1162; MTBLC1243; MTBLC87507; MTBLC48061; MTBLC30918; MTBLC17902; MTBLC17568; MTBLC28942; MTBLC22099; MTBLC13497; MTBLC32275; MTBLC135817; MTBLC49026; MTBLC17012; MTBLC28879; MTBLC91807; MTBLC15809; MTBLC6381; MTBLC9605; MTBLC79471; MTBLC79566; MTBLC6851; MTBLC38546; MTBLC10561; MTBLC3146; MTBLC49260; MTBLC144027; MTBLC27574; MTBLC49004; MTBLC9308; MTBLC27407; MTBLC40304; MTBLC3927; MTBLC16750; MTBLC27427; MTBLC17643; MTBLC31552; MTBLC43755; MTBLC3088; MTBLC50271; MTBLC69499; MTBLC4994; MTBLC6008; MTBLC7161; MTBLC94381; MTBLC116; MTBLC4962; MTBLC29474; MTBLC17693; MTBLC16409; MTBLC17405; MTBLC2085; MTBLC34334; MTBLC20367; MTBLC28719; MTBLC137246; MTBLC29069; MTBLC29009; MTBLC74321; MTBLC2685; MTBLC3082; MTBLC135310; MTBLC116735; MTBLC17295; MTBLC46209; MTBLC28438; MTBLC28170; MTBLC28353; MTBLC16151; MTBLC35697; MTBLC4888; MTBLC134865; MTBLC5862; MTBLC16828; MTBLC79441; MTBLC9935; MTBLC9962; MTBLC135165; MTBLC3845; MTBLC135386; MTBLC15637; MTBLC63606; MTBLC45981; MTBLC8772; MTBLC4708; MTBLC9259; MTBLC51141; MTBLC17509; MTBLC53727; MTBLC32162; MTBLC102516; MTBLC32164; MTBLC9593; MTBLC7209; MTBLC24479; MTBLC4822; MTBLC6617; MTBLC4724; MTBLC10026; MTBLC35028; MTBLC10022; MTBLC69088; MTBLC17501; MTBLC28523; MTBLC89486; MTBLC2108; MTBLC2336; MTBLC4774; MTBLC34712; MTBLC60069; MTBLC6891; MTBLC16389; MTBLC8418; MTBLC8419; MTBLC18082; MTBLC28334; MTBLC88677; MTBLC15490; MTBLC34041; MTBLC60076; MTBLC16305; MTBLC31682; MTBLC73970; MTBLC3695; MTBLC132058; MTBLC74533; MTBLC137196; MTBLC2978; MTBLC80227; MTBLC34087; MTBLC89521; MTBLC86095; MTBLC88906; MTBLC89602; MTBLC89539; MTBLC89536; MTBLC73739; MTBLC75145; MTBLC64356; MTBLC86544; MTBLC29564; MTBLC31447; MTBLC4512; MTBLC6001; MTBLC32771; MTBLC37108; MTBLC29019; MTBLC86618; MTBLC82864; MTBLC135383; MTBLC4682; MTBLC76258; MTBLC135151; MTBLC36665; MTBLC18094; MTBLC4718; MTBLC9239; MTBLC25357; MTBLC27504; MTBLC2699; MTBLC8837; MTBLC9198; MTBLC9524; MTBLC9601; MTBLC9770; MTBLC9969; MTBLC2697; MTBLC2722; MTBLC6080; MTBLC8822; MTBLC52070; MTBLC9912; MTBLC8247; MTBLC32003; MTBLC10329; MTBLC135757; MTBLC42; MTBLC6066; MTBLC7458; MTBLC9519; MTBLC4856; MTBLC9120; MTBLC79434; MTBLC16684; MTBLC6140; MTBLC58164; MTBLC6506; MTBLC31789; MTBLC6778; MTBLC79600; MTBLC137783; MTBLC51211; MTBLC135016; MTBLC6535; MTBLC5990; MTBLC3094; MTBLC16112; MTBLC16065; MTBLC16952; MTBLC74725; MTBLC16475; MTBLC28155; MTBLC4732; MTBLC79423; MTBLC79564; MTBLC9291; MTBLC62431; MTBLC2365; MTBLC22152; MTBLC2620; MTBLC2851; MTBLC2870; MTBLC2982; MTBLC3574; MTBLC3888; MTBLC5095; MTBLC5281; MTBLC5536; MTBLC5727; MTBLC5867; MTBLC6560; MTBLC6921; MTBLC8115; MTBLC8267; MTBLC8268; MTBLC8856; MTBLC9013; MTBLC9956; MTBLC10024; MTBLC79890; MTBLC6863; MTBLC29612; MTBLC93369; MTBLC30805; MTBLC140088; MTBLC74966; MTBLC43966; MTBLC85252; MTBLC63924; MTBLC4973; MTBLC6419; MTBLC16725; MTBLC27769; MTBLC86068; MTBLC2404; MTBLC133419; MTBLC10070; MTBLC93847; MTBLC28708; MTBLC29458; MTBLC15830; MTBLC134834; MTBLC34769; MTBLC139312; MTBLC3061; MTBLC10099; MTBLC6738; MTBLC3005; MTBLC135349; MTBLC92338; MTBLC7789; MTBLC7640; MTBLC8597; MTBLC93626; MTBLC28865; MTBLC38258; MTBLC5859; MTBLC8021; MTBLC636; MTBLC67547; MTBLC137192; MTBLC88935; MTBLC86119; MTBLC86121; MTBLC89734; MTBLC86117; MTBLC78022; MTBLC89691; MTBLC84831; MTBLC74670; MTBLC89599; MTBLC89597; MTBLC89548; MTBLC89438; MTBLC89078; MTBLC89127; MTBLC89177; MTBLC88712; MTBLC21484; MTBLC15874; MTBLC17976; MTBLC5093; MTBLC63630; MTBLC2294; MTBLC2425; MTBLC16363; MTBLC2629; MTBLC69335; MTBLC28356; MTBLC4441; MTBLC135002; MTBLC10058; MTBLC10076; MTBLC10103; MTBLC28714; MTBLC43415; MTBLC5855; MTBLC28325; MTBLC74405; MTBLC3300; MTBLC9515; MTBLC41509; MTBLC2156; MTBLC2368; MTBLC9439; MTBLC74274; MTBLC8386; MTBLC18278; MTBLC27993; MTBLC82684; MTBLC9997; MTBLC80033; MTBLC29527; MTBLC29536; MTBLC135701; MTBLC16778; MTBLC18330; MTBLC4783; MTBLC27514; MTBLC5304; MTBLC31967; MTBLC16954; MTBLC8028; MTBLC133473; MTBLC29043; MTBLC38266; MTBLC80494; MTBLC72609; MTBLC62881; MTBLC135932; MTBLC9943; MTBLC58552; MTBLC42797; MTBLC31871; MTBLC82763; MTBLC31922; MTBLC135703; MTBLC64210; MTBLC135483; MTBLC32181; MTBLC474014; MTBLC3825; MTBLC34668; MTBLC7736; MTBLC17713; MTBLC10037; MTBLC8922; MTBLC7471; MTBLC31563; MTBLC3740; MTBLC4320; MTBLC24293; MTBLC80538; MTBLC79465; MTBLC4773; MTBLC5527; MTBLC9959; MTBLC131852; MTBLC9665; MTBLC473990; MTBLC17433; MTBLC80393; MTBLC3162; MTBLC5970; MTBLC44492; MTBLC79394; MTBLC15430; MTBLC2341; MTBLC34163; MTBLC31561; MTBLC135525; MTBLC8039; MTBLC79655; MTBLC79502; MTBLC34461; MTBLC79892; MTBLC34353; MTBLC34355; MTBLC79657; MTBLC17457; MTBLC4453; MTBLC9261; MTBLC79432; MTBLC79620; MTBLC29510; MTBLC52075; MTBLC15416; MTBLC31578; MTBLC52484; MTBLC29611; MTBLC52482; MTBLC29654; MTBLC81594; MTBLC30038; MTBLC31896; MTBLC9108; MTBLC9946; MTBLC847; MTBLC9205; MTBLC15735; MTBLC3745; MTBLC82461; MTBLC27796; MTBLC34580; MTBLC6147; MTBLC135451; MTBLC2565; MTBLC4038; MTBLC28833; MTBLC29592; MTBLC29594; MTBLC29602; MTBLC5606; MTBLC6962; MTBLC8330; MTBLC9042; MTBLC9290; MTBLC2534; MTBLC799; MTBLC34139; MTBLC79668; MTBLC79797; MTBLC136980; MTBLC1189; MTBLC136972; MTBLC79907; MTBLC63641; MTBLC79715; MTBLC2495; MTBLC79887; MTBLC9460; MTBLC17078; MTBLC141472; MTBLC28192; MTBLC135231; MTBLC79496; MTBLC79601; MTBLC5887; MTBLC59788; MTBLC31086; MTBLC2626; MTBLC8402; MTBLC32185; MTBLC4417; MTBLC31298; MTBLC31497; MTBLC8713; MTBLC31459; MTBLC113542; MTBLC40070; MTBLC27510; MTBLC17148; MTBLC716; MTBLC2327; MTBLC2544; MTBLC3614; MTBLC89837; MTBLC89829; MTBLC89824; MTBLC90028; MTBLC90034; MTBLC90021; MTBLC77677; MTBLC88798; MTBLC88446; MTBLC41847; MTBLC89028; MTBLC90068; MTBLC64793; MTBLC84266; MTBLC5674; MTBLC142272; MTBLC2939; MTBLC6798; MTBLC1749; MTBLC8602; MTBLC17467; MTBLC34605; MTBLC9425; MTBLC2725; MTBLC9923; MTBLC73; MTBLC30725; MTBLC34968; MTBLC31753; MTBLC2934; MTBLC7948; MTBLC86251; MTBLC30248; MTBLC34227; MTBLC142243; MTBLC136795; MTBLC2504; MTBLC3081; MTBLC16188; MTBLC16011; MTBLC85158; MTBLC79925; MTBLC79522; MTBLC34175; MTBLC79455; MTBLC80656; MTBLC79735; MTBLC135981; MTBLC6085; MTBLC49191; MTBLC9419; MTBLC89642; MTBLC16374; MTBLC10136; MTBLC4778; MTBLC8196; MTBLC28794; MTBLC90355; MTBLC79553; MTBLC28090; MTBLC2197; MTBLC3163; MTBLC28436; MTBLC5837; MTBLC6006; MTBLC75092; MTBLC16243; MTBLC8876; MTBLC507499; MTBLC204; MTBLC214; MTBLC241; MTBLC242; MTBLC78668; MTBLC138752; MTBLC17130; MTBLC34301; MTBLC37157; MTBLC78853; MTBLC61024; MTBLC8607; MTBLC4389; MTBLC5528; MTBLC89343; MTBLC89314; MTBLC89088; MTBLC89075; MTBLC89076; MTBLC89371; MTBLC89333; MTBLC89334; MTBLC89311; MTBLC89316; MTBLC138499; MTBLC18227; MTBLC94661; MTBLC36108; MTBLC80383; MTBLC8273; MTBLC8773; MTBLC31049; MTBLC18393; MTBLC137750; MTBLC17224; MTBLC5679; MTBLC18127; MTBLC17166; MTBLC28091; MTBLC36466; MTBLC36106; MTBLC4366; MTBLC28869; MTBLC28925; MTBLC9185; MTBLC9188; MTBLC86162; MTBLC88930; MTBLC88929; MTBLC89739; MTBLC89576; MTBLC89557; MTBLC89559; MTBLC89441; MTBLC86161; MTBLC89419; MTBLC88925; MTBLC88841; MTBLC88430; MTBLC88654; MTBLC10219; MTBLC86344; MTBLC84549; MTBLC84837; MTBLC78268; MTBLC7492; MTBLC91712; MTBLC4974; MTBLC4572; MTBLC6414; MTBLC81785; MTBLC135138; MTBLC60656; MTBLC16312; MTBLC16390; MTBLC138401; MTBLC88108; MTBLC2812; MTBLC79833; MTBLC47818; MTBLC79918; MTBLC34838; MTBLC31523; MTBLC138422; MTBLC47214; MTBLC28818; MTBLC32176; MTBLC15578; MTBLC89324; MTBLC89079; MTBLC19290; MTBLC79996; MTBLC28477; MTBLC81013; MTBLC17823; MTBLC86378; MTBLC7931; MTBLC28933; MTBLC9595; MTBLC34667; MTBLC31648; MTBLC4819; MTBLC32645; MTBLC8764; MTBLC4921; MTBLC9165; MTBLC31857; MTBLC31174; MTBLC34831; MTBLC31894; MTBLC9316; MTBLC27617; MTBLC80461; MTBLC80167; MTBLC1107; MTBLC82949; MTBLC88480; MTBLC88479; MTBLC88547; MTBLC89218; MTBLC89203; MTBLC89202; MTBLC89162; MTBLC89160; MTBLC89238; MTBLC89237; MTBLC88966; MTBLC89040; MTBLC89780; MTBLC89784; MTBLC89799; MTBLC89797; MTBLC89684; MTBLC89669; MTBLC89670; MTBLC89671; MTBLC89433; MTBLC89322; MTBLC89337; MTBLC136371; MTBLC64396; MTBLC88779; MTBLC28517; MTBLC18171; MTBLC32086; MTBLC5206; MTBLC15575; MTBLC2513; MTBLC50749; MTBLC31893; MTBLC9463; MTBLC15574; MTBLC90980; MTBLC47812; MTBLC80533; MTBLC3863; MTBLC5633; MTBLC8913; MTBLC6145; MTBLC64668; MTBLC7800; MTBLC9039; MTBLC8621; MTBLC80017; MTBLC34042; MTBLC7752; MTBLC28285; MTBLC18010; MTBLC3719; MTBLC5718; MTBLC6674; MTBLC59979; MTBLC34499; MTBLC34503; MTBLC34506; MTBLC91217; MTBLC138082; MTBLC15658; MTBLC15655; MTBLC15657; MTBLC64008; MTBLC138786; MTBLC88461; MTBLC34148; MTBLC91272; MTBLC34485; MTBLC34498; MTBLC34500; MTBLC88440; MTBLC34504; MTBLC143972; MTBLC88465; MTBLC89257; MTBLC3403; MTBLC3898; MTBLC79904; MTBLC34352; MTBLC1689; MTBLC89328; MTBLC79870; MTBLC9481; MTBLC93; MTBLC1941; MTBLC8603; MTBLC134767; MTBLC74562; MTBLC61725; MTBLC142079; MTBLC16310; MTBLC42471; MTBLC7567; MTBLC16147; MTBLC85232; MTBLC90230; MTBLC133979; MTBLC137172; MTBLC85166; MTBLC133325; MTBLC135350; MTBLC545687; MTBLC7496; MTBLC34322; MTBLC79177; MTBLC84854; MTBLC34295; MTBLC29479; MTBLC17903; MTBLC4045; MTBLC10445; MTBLC6706; MTBLC79519; MTBLC34293; MTBLC34294; MTBLC135489; MTBLC9238; MTBLC137712; MTBLC19143; MTBLC18446; MTBLC8648; MTBLC19144; MTBLC49265; MTBLC15654; MTBLC88462; MTBLC80442; MTBLC84441; MTBLC72641; MTBLC136531; MTBLC72815; MTBLC80463; MTBLC76234; MTBLC34491; MTBLC88441; MTBLC80447; MTBLC88438; MTBLC72843; MTBLC72842; MTBLC88460; MTBLC60956; MTBLC133329; MTBLC80413; MTBLC63067; MTBLC18230; MTBLC65247; MTBLC3705; MTBLC31352; MTBLC76334; MTBLC9510; MTBLC3128; MTBLC61726; MTBLC89365; MTBLC89339; MTBLC89342; MTBLC89318; MTBLC89313; MTBLC60273; MTBLC65211; MTBLC138212; MTBLC78700; MTBLC55523; MTBLC27706; MTBLC38299; MTBLC137495; MTBLC34154; MTBLC72639; MTBLC133357; MTBLC34494; MTBLC78730; MTBLC34496; MTBLC72651; MTBLC131659; MTBLC5833; MTBLC73074; MTBLC2366; MTBLC1019; MTBLC88696; MTBLC52897; MTBLC79575; MTBLC135210; MTBLC132495; MTBLC73751; MTBLC34828; MTBLC88667; MTBLC9778; MTBLC28919; MTBLC10088; MTBLC69081; MTBLC75542; MTBLC95216; MTBLC134424; MTBLC134423; MTBLC29627; MTBLC10120; MTBLC34034; MTBLC34443; MTBLC40131; MTBLC4918; MTBLC14469; MTBLC2492; MTBLC5166; MTBLC88808; MTBLC88807; MTBLC88782; MTBLC89214; MTBLC89189; MTBLC89149; MTBLC1418; MTBLC27867; MTBLC80419; MTBLC3375; MTBLC5087; MTBLC27448; MTBLC80177; MTBLC19793; MTBLC28485; MTBLC88765; MTBLC28810; MTBLC32157; MTBLC31279; MTBLC7720; MTBLC73728; MTBLC133875; MTBLC34920; MTBLC6088; MTBLC137139; MTBLC138782; MTBLC34652; MTBLC34680; MTBLC33913; MTBLC75219; MTBLC133456; MTBLC88698; MTBLC88697; MTBLC79838; MTBLC50106; MTBLC34229; MTBLC138081; MTBLC38833; MTBLC22469; MTBLC28093; MTBLC15405; MTBLC17580; MTBLC36503; MTBLC15393; MTBLC36492; MTBLC98; MTBLC31; MTBLC60; MTBLC61; MTBLC149; MTBLC150; MTBLC152; MTBLC153; MTBLC50232; MTBLC158; MTBLC50233; MTBLC50235; MTBLC300; MTBLC299; MTBLC368; MTBLC27961; MTBLC61727; MTBLC47856; MTBLC17447; MTBLC29452; MTBLC28071; MTBLC692; MTBLC35002; MTBLC9602; MTBLC137135; MTBLC34537; MTBLC79794; MTBLC79879; MTBLC28125; MTBLC79767; MTBLC79635; MTBLC34476; MTBLC79801; MTBLC135402; MTBLC32095; MTBLC79581; MTBLC76937; MTBLC39567; MTBLC36206; MTBLC36214; MTBLC85510; MTBLC36211; MTBLC7989; MTBLC79096; MTBLC75103; MTBLC32411; MTBLC138778; MTBLC36412; MTBLC86135; MTBLC142250; MTBLC86506; MTBLC32409; MTBLC32389; MTBLC37810; MTBLC2905; MTBLC135532; MTBLC79179; MTBLC84855; MTBLC80050; MTBLC48635; MTBLC5644; MTBLC63916; MTBLC79523; MTBLC79689; MTBLC80001; MTBLC52421; MTBLC448; MTBLC72665; MTBLC138258; MTBLC138255; MTBLC72663; MTBLC133381; MTBLC133086; MTBLC131762; MTBLC73882; MTBLC84067; MTBLC86403; MTBLC31850; MTBLC132479; MTBLC92833; MTBLC34370; MTBLC135041; MTBLC134981; MTBLC31547; MTBLC79883; MTBLC79939; MTBLC6645; MTBLC84094; MTBLC116278; MTBLC9232; MTBLC28661; MTBLC10275; MTBLC27432; MTBLC44602; MTBLC79716; MTBLC86136; MTBLC86148; MTBLC38384; MTBLC16423; MTBLC61676; MTBLC8638; MTBLC88809; MTBLC75465; MTBLC88786; MTBLC84394; MTBLC88471; MTBLC88536; MTBLC88367; MTBLC75446; MTBLC138077; MTBLC28627; MTBLC80415; MTBLC88796; MTBLC88725; MTBLC82927; MTBLC88501; MTBLC88500; MTBLC88364; MTBLC89229; MTBLC89211; MTBLC88942; MTBLC89034; MTBLC89029; MTBLC50585; MTBLC138489; MTBLC31571; MTBLC45571; MTBLC31725; MTBLC144339; MTBLC9194; MTBLC89605; MTBLC15843; MTBLC79754; MTBLC79694; MTBLC1182; MTBLC79480; MTBLC79869; MTBLC82835; MTBLC2451; MTBLC36033; MTBLC31825; MTBLC135293; MTBLC34834; MTBLC30041; MTBLC10419; MTBLC3425; MTBLC8996; MTBLC6991; MTBLC32345; MTBLC137651; MTBLC641; MTBLC1784; MTBLC4640; MTBLC72800; MTBLC20096; MTBLC72758; MTBLC73889; MTBLC3456; MTBLC9242; MTBLC44526; MTBLC83063; MTBLC38394; MTBLC142447; MTBLC24993; MTBLC138083; MTBLC38362; MTBLC82749; MTBLC32798; MTBLC88464; MTBLC86141; MTBLC27939; MTBLC75108; MTBLC6673; MTBLC28801; MTBLC84299; MTBLC4650; MTBLC46979; MTBLC136623; MTBLC46859; MTBLC83058; MTBLC9189; MTBLC86570; MTBLC31542; MTBLC89519; MTBLC85028; MTBLC74971; MTBLC4021; MTBLC48923; MTBLC64483; MTBLC131738; MTBLC64489; MTBLC78103; MTBLC63959; MTBLC31000; MTBLC75454; MTBLC75536; MTBLC31831; MTBLC75565; MTBLC137215; MTBLC135498; MTBLC3961; MTBLC71025; MTBLC73792; MTBLC137845; MTBLC9011; MTBLC33276; MTBLC80541; MTBLC137134; MTBLC47805; MTBLC79517; MTBLC4629; MTBLC31826; MTBLC10086; MTBLC64124; MTBLC46961; MTBLC15913; MTBLC18129; MTBLC79182; MTBLC143095; MTBLC85208; MTBLC136406; MTBLC50578; MTBLC136819; MTBLC136638; MTBLC74789; MTBLC79951; MTBLC5382; MTBLC69833; MTBLC80540; MTBLC3450; MTBLC37779; MTBLC37537; MTBLC49254; MTBLC28724; MTBLC136767; MTBLC85633; MTBLC34004; MTBLC85639; MTBLC45478; MTBLC79312; MTBLC30820; MTBLC50576; MTBLC138260; MTBLC82464; MTBLC28592; MTBLC84874; MTBLC70850; MTBLC85057; MTBLC32365; MTBLC90027; MTBLC3433; MTBLC9184; MTBLC74330; MTBLC62834; MTBLC73741; MTBLC79501; MTBLC34464; MTBLC11152; MTBLC29644; MTBLC84519; MTBLC34726; MTBLC133741; MTBLC46703; MTBLC73829; MTBLC34402; MTBLC137126; MTBLC81246; MTBLC67061; MTBLC73851; MTBLC84752; MTBLC79723; MTBLC33216; MTBLC6689; MTBLC7443; MTBLC79824; MTBLC135488; MTBLC88790; MTBLC77096; MTBLC88474; MTBLC88495; MTBLC88490; MTBLC88520; MTBLC88371; MTBLC88395; MTBLC89225; MTBLC75475; MTBLC77127; MTBLC89169; MTBLC89168; MTBLC89260; MTBLC75578; MTBLC88989; MTBLC89046; MTBLC89795; MTBLC89682; MTBLC89665; MTBLC89811; MTBLC80207; MTBLC131692; MTBLC17862; MTBLC71464; MTBLC16393; MTBLC28727; MTBLC28194; MTBLC27997; MTBLC16196; MTBLC82617; MTBLC50575; MTBLC32375; MTBLC50464; MTBLC29735; MTBLC30829; MTBLC28193; MTBLC50572; MTBLC36023; MTBLC35517; MTBLC79612; MTBLC18054; MTBLC3430; MTBLC6965; MTBLC82985; MTBLC10087; MTBLC9916; MTBLC35464; MTBLC142241; MTBLC28716; MTBLC35465; MTBLC76244; MTBLC37252; MTBLC76090; MTBLC9199; MTBLC9951; MTBLC77148; MTBLC31872; MTBLC3944; MTBLC5933; MTBLC72828; MTBLC72952; MTBLC27620; MTBLC91006; MTBLC67309; MTBLC3940; MTBLC7909; MTBLC79407; MTBLC79791; MTBLC79792; MTBLC66666; MTBLC135355; MTBLC88112; MTBLC135566; MTBLC79513; MTBLC73092; MTBLC31501; MTBLC88109; MTBLC31297; MTBLC28941; MTBLC84901; MTBLC28733; MTBLC6144; MTBLC75612; MTBLC52392; MTBLC3427; MTBLC137833; MTBLC16566; MTBLC84896; MTBLC28842; MTBLC88686; MTBLC29702; MTBLC34478; MTBLC137844; MTBLC53154; MTBLC72736; MTBLC133144; MTBLC75036; MTBLC131924; MTBLC8416; MTBLC9190; MTBLC18318; MTBLC86422; MTBLC89413; MTBLC89431; MTBLC89391; MTBLC89140; MTBLC89196; MTBLC89294; MTBLC88904; MTBLC88905; MTBLC88760; MTBLC88761; MTBLC88731; MTBLC88729; MTBLC88871; MTBLC88869; MTBLC88587; MTBLC89500; MTBLC89501; MTBLC34542; MTBLC61473; MTBLC3249; MTBLC4746; MTBLC80169; MTBLC34121; MTBLC52971; MTBLC93175; MTBLC137734; MTBLC73854; MTBLC90040; MTBLC89382; MTBLC89352; MTBLC89368; MTBLC89366; MTBLC89340; MTBLC89317; MTBLC137279; MTBLC137293; MTBLC134075; MTBLC90459; MTBLC134076; MTBLC134077; MTBLC134078; MTBLC39934; MTBLC134227; MTBLC134228; MTBLC16038; MTBLC9970; MTBLC4592; MTBLC79643; MTBLC34554; MTBLC2927; MTBLC27722; MTBLC28277; MTBLC80014; MTBLC77258; MTBLC4915; MTBLC5746; MTBLC28468; MTBLC64563; MTBLC76078; MTBLC72998; MTBLC78101; MTBLC73721; MTBLC73134; MTBLC73004; MTBLC62837; MTBLC78270; MTBLC79536; MTBLC73894; MTBLC31676; MTBLC50782; MTBLC31650; MTBLC6574; MTBLC31940; MTBLC44247; MTBLC79899; MTBLC27965; MTBLC79098; MTBLC75038; MTBLC133623; MTBLC84577; MTBLC84234; MTBLC64032; MTBLC53486; MTBLC53460; MTBLC79878; MTBLC79900; MTBLC525464; MTBLC79409; MTBLC79578; MTBLC82832; MTBLC71589; MTBLC32023; MTBLC34349; MTBLC32068; MTBLC31020; MTBLC2502; MTBLC28593; MTBLC15854; MTBLC309594; MTBLC84116; MTBLC3560; MTBLC79190; MTBLC76992; MTBLC52347; MTBLC18164; MTBLC32027; MTBLC135857; MTBLC88780; MTBLC88468; MTBLC75342; MTBLC744; MTBLC34115; MTBLC84911; MTBLC32154; MTBLC131508; MTBLC32906; MTBLC29596; MTBLC28211; MTBLC6927; MTBLC7603; MTBLC80537; MTBLC10137; MTBLC80732; MTBLC79113; MTBLC90041; MTBLC133599; MTBLC133617; MTBLC84845; MTBLC84844; MTBLC74986; MTBLC143985; MTBLC80203; MTBLC143980; MTBLC134453; MTBLC34126; MTBLC34130; MTBLC79851; MTBLC72606; MTBLC19138; MTBLC137345; MTBLC34157; MTBLC88823; MTBLC78837; MTBLC64017; MTBLC34162; MTBLC79557; MTBLC79656; MTBLC63995; MTBLC79561; MTBLC63579; MTBLC34185; MTBLC34306; MTBLC79485; MTBLC34450; MTBLC60943; MTBLC137344; MTBLC34490; MTBLC72643; MTBLC72786; MTBLC36275; MTBLC86031; MTBLC73733; MTBLC89091; MTBLC75646; MTBLC89387; MTBLC89392; MTBLC89395; MTBLC89394; MTBLC53081; MTBLC76284; MTBLC137704; MTBLC34438; MTBLC32319; MTBLC32325; MTBLC34711; MTBLC4676; MTBLC34136; MTBLC39449; MTBLC39451; MTBLC39453; MTBLC39454; MTBLC31406; MTBLC10580; MTBLC39448; MTBLC4722; MTBLC19287; MTBLC31164; MTBLC27655; MTBLC5715; MTBLC6567; MTBLC6586; MTBLC34883; MTBLC88902; MTBLC8034; MTBLC10045; MTBLC10089; MTBLC80194; MTBLC79956; MTBLC79588; MTBLC81561; MTBLC2296; MTBLC3321; MTBLC65585; MTBLC134353; MTBLC143960; MTBLC30088; MTBLC29589; MTBLC29601; MTBLC6696; MTBLC134511; MTBLC140267; MTBLC8390; MTBLC5783; MTBLC80531; MTBLC16688; MTBLC28135; MTBLC137137; MTBLC139534; MTBLC31731; MTBLC73923; MTBLC31801; MTBLC35459; MTBLC135729; MTBLC135684; MTBLC86197; MTBLC86196; MTBLC86189; MTBLC86190; MTBLC86188; MTBLC80532; MTBLC18531; MTBLC18532; MTBLC46739; MTBLC79839; MTBLC28033; MTBLC17168; MTBLC16608; MTBLC17762; MTBLC16074; MTBLC16113; MTBLC143982; MTBLC28610; MTBLC86255; MTBLC76071; MTBLC143713; MTBLC72589; MTBLC131658; MTBLC31025; MTBLC17390; MTBLC27808; MTBLC5191; MTBLC31123; MTBLC82648; MTBLC135276; MTBLC4670; MTBLC143989; MTBLC9669; MTBLC52672; MTBLC37945; MTBLC34899; MTBLC37923; MTBLC8710; MTBLC31550; MTBLC3156; MTBLC48742; MTBLC135719; MTBLC8036; MTBLC7352; MTBLC90970; MTBLC47834; MTBLC63911; MTBLC137141; MTBLC47799; MTBLC72727; MTBLC80530; MTBLC5363; MTBLC52348; MTBLC17314; MTBLC76980; MTBLC76304; MTBLC6113; MTBLC143987; MTBLC143990; MTBLC9911; MTBLC135737; MTBLC28700; MTBLC79923; MTBLC73794; MTBLC62736; MTBLC62737; MTBLC84958; MTBLC86418; MTBLC89703; MTBLC89592; MTBLC89589; MTBLC89384; MTBLC89098; MTBLC89143; MTBLC89070; MTBLC88726; MTBLC88872; MTBLC88588; MTBLC89498; MTBLC89502; MTBLC143981; MTBLC143983; MTBLC71466; MTBLC9453; MTBLC31264; MTBLC131689; MTBLC74340; MTBLC131668; MTBLC131687; MTBLC131688; MTBLC52639; MTBLC85403; MTBLC29613; MTBLC79453; MTBLC28047; MTBLC132620; MTBLC31257; MTBLC29677; MTBLC31222; MTBLC5197; MTBLC135094; MTBLC32277; MTBLC15929; MTBLC25242; MTBLC28258; MTBLC134924; MTBLC86975; MTBLC88529; MTBLC89026; MTBLC137784; MTBLC32002; MTBLC125; MTBLC46734; MTBLC141283; MTBLC16774; MTBLC35966; MTBLC16619; MTBLC10217; MTBLC10278; MTBLC10417; MTBLC3431; MTBLC4001; MTBLC5552; MTBLC5719; MTBLC6401; MTBLC7524; MTBLC7940; MTBLC64792; MTBLC137092; MTBLC144025; MTBLC10274; MTBLC3087; MTBLC37659; MTBLC135741; MTBLC9908; MTBLC18067; MTBLC89279; MTBLC89380; MTBLC89383; MTBLC89360; MTBLC89359; MTBLC89370; MTBLC84566; MTBLC137216; MTBLC85680; MTBLC18168; MTBLC52350; MTBLC73731; MTBLC78706; MTBLC31572; MTBLC36036; MTBLC9053; MTBLC89090; MTBLC89089; MTBLC89074; MTBLC89390; MTBLC89357; MTBLC89374; MTBLC89373; MTBLC90454; MTBLC75376; MTBLC17058; MTBLC28688; MTBLC34184; MTBLC3941; MTBLC53424; MTBLC1309; MTBLC1310; MTBLC79897; MTBLC63065; MTBLC143013; MTBLC4813; MTBLC134507; MTBLC84759; MTBLC34835; MTBLC84877; MTBLC39248; MTBLC34122; MTBLC84386; MTBLC88781; MTBLC88757; MTBLC88469; MTBLC75550; MTBLC83055; MTBLC27423; MTBLC37998; MTBLC2944; MTBLC132949; MTBLC137858; MTBLC137136; MTBLC79992; MTBLC9948; MTBLC135723; MTBLC90233; MTBLC137178; MTBLC73736; MTBLC39826; MTBLC50158; MTBLC17177; MTBLC16697; MTBLC52052; MTBLC16101; MTBLC28488; MTBLC28063; MTBLC27417; MTBLC84341; MTBLC88756; MTBLC3663; MTBLC59912; MTBLC80083; MTBLC94686; MTBLC137229; MTBLC82836; MTBLC77525; MTBLC34743; MTBLC133914; MTBLC89451; MTBLC135440; MTBLC72844; MTBLC79787; MTBLC79494; MTBLC88359; MTBLC140473; MTBLC137304; MTBLC63836; MTBLC73135; MTBLC48131; MTBLC79444; MTBLC2696; MTBLC46750; MTBLC7952; MTBLC8186; MTBLC32249; MTBLC15884; MTBLC41872; MTBLC33275; MTBLC33277; MTBLC135704; MTBLC4429; MTBLC15414; MTBLC88735; MTBLC17685; MTBLC4391; MTBLC8038; MTBLC17858; MTBLC2669; MTBLC5762; MTBLC9122; MTBLC79874; MTBLC34141; MTBLC73773; MTBLC79786; MTBLC79448; MTBLC5120; MTBLC16264; MTBLC16650; MTBLC16287; MTBLC3421; MTBLC7500; MTBLC135923; MTBLC40957; MTBLC41938; MTBLC79970; MTBLC4289; MTBLC59276; MTBLC16654; MTBLC86537; MTBLC982; MTBLC17094; MTBLC28710; MTBLC37032; MTBLC27530; MTBLC30832; MTBLC68566; MTBLC17646; MTBLC86396; MTBLC89760; MTBLC137770; MTBLC32350; MTBLC17400; MTBLC28870; MTBLC3354; MTBLC2310; MTBLC31759; MTBLC45951; MTBLC28657; MTBLC27520; MTBLC42976; MTBLC16802; MTBLC3014; MTBLC2155; MTBLC2185; MTBLC2321; MTBLC135989; MTBLC6709; MTBLC6888; MTBLC79546; MTBLC79481; MTBLC81712; MTBLC6995; MTBLC6960; MTBLC35040; MTBLC3533; MTBLC35421; MTBLC33509; MTBLC48093; MTBLC33510; MTBLC33511; MTBLC34237; MTBLC80471; MTBLC43996; MTBLC18226; MTBLC17532; MTBLC30734; MTBLC134814; MTBLC37753; MTBLC27469; MTBLC16142; MTBLC17426; MTBLC28860; MTBLC20937; MTBLC47962; MTBLC4178; MTBLC16224; MTBLC21099; MTBLC24113; MTBLC33830; MTBLC24769; MTBLC28378; MTBLC85187; MTBLC17077; MTBLC46644; MTBLC33198; MTBLC24149; MTBLC24266; MTBLC24462; MTBLC18246; MTBLC681850; MTBLC32709; MTBLC31677; MTBLC8871; MTBLC27513; MTBLC613; MTBLC1945; MTBLC15937; MTBLC9513; MTBLC63624; MTBLC17748; MTBLC17293; MTBLC2555; MTBLC7785; MTBLC8256; MTBLC7821; MTBLC135842; MTBLC66773; MTBLC2913; MTBLC6076; MTBLC15532; MTBLC6791; MTBLC87625; MTBLC6859; MTBLC30860; MTBLC15741; MTBLC30347; MTBLC77780; MTBLC89639; MTBLC254496; MTBLC35034; MTBLC4364; MTBLC17506; MTBLC18321; MTBLC15934; MTBLC6819; MTBLC30527; MTBLC2653; MTBLC39462; MTBLC79807; MTBLC3897; MTBLC8380; MTBLC15362; MTBLC8478; MTBLC48058; MTBLC27444; MTBLC41607; MTBLC705; MTBLC5954; MTBLC50885; MTBLC135324; MTBLC836; MTBLC3276; MTBLC89060; MTBLC89499; MTBLC6650; MTBLC32242; MTBLC2431; MTBLC34801; MTBLC63622; MTBLC79719; MTBLC34321; MTBLC5810; MTBLC17871; MTBLC30966; MTBLC27957; MTBLC18419; MTBLC30768; MTBLC137814; MTBLC86348; MTBLC86391; MTBLC36532; MTBLC27904; MTBLC16023; MTBLC27378; MTBLC28587; MTBLC3641; MTBLC9653; MTBLC135517; MTBLC3918; MTBLC79692; MTBLC79988; MTBLC9961; MTBLC6838; MTBLC1547; MTBLC2076; MTBLC63581; MTBLC141154; MTBLC8049; MTBLC16992; MTBLC30841; MTBLC30794; MTBLC135928; MTBLC6628; MTBLC8341; MTBLC73758; MTBLC15436; MTBLC27630; MTBLC32398; MTBLC15366; MTBLC17071; MTBLC15586; MTBLC29003; MTBLC17647; MTBLC17084; MTBLC58511; MTBLC15584; MTBLC16292; MTBLC27736; MTBLC16392; MTBLC15867; MTBLC6177; MTBLC37434; MTBLC47518; MTBLC31441; MTBLC75988; MTBLC80438; MTBLC3978; MTBLC80441; MTBLC133224; MTBLC31743; MTBLC80528; MTBLC6553; MTBLC133244; MTBLC28527; MTBLC135754; MTBLC27994; MTBLC66905; MTBLC3439; MTBLC27475; MTBLC28426; MTBLC80434; MTBLC5065; MTBLC17965; MTBLC31742; MTBLC30200; MTBLC75790; MTBLC7781; MTBLC17558; MTBLC43136; MTBLC17456; MTBLC18320; MTBLC31784; MTBLC101278; MTBLC31901; MTBLC34474; MTBLC34511; MTBLC79863; MTBLC57681; MTBLC16211; MTBLC16773; MTBLC16898; MTBLC44932; MTBLC53770; MTBLC79369; MTBLC13714; MTBLC63609; MTBLC79929; MTBLC10285; MTBLC2883; MTBLC135745; MTBLC34574; MTBLC31359; MTBLC31849; MTBLC7814; MTBLC33138; MTBLC18043; MTBLC28459; MTBLC17798; MTBLC10072; MTBLC35014; MTBLC73688; MTBLC135289; MTBLC2506; MTBLC2769; MTBLC9045; MTBLC141; MTBLC89487; MTBLC30821; MTBLC79630; MTBLC1734; MTBLC12257; MTBLC133809; MTBLC135613; MTBLC50742; MTBLC15623; MTBLC15624; MTBLC16715; MTBLC27583; MTBLC16278; MTBLC17782; MTBLC22652; MTBLC17039; MTBLC18268; MTBLC73681; MTBLC17801; MTBLC45969; MTBLC21241; MTBLC30923; MTBLC4083; MTBLC28411; MTBLC36622; MTBLC58468; MTBLC18383; MTBLC135643; MTBLC34170; MTBLC87820; MTBLC79702; MTBLC31215; MTBLC4919; MTBLC8880; MTBLC1656; MTBLC49003; MTBLC17032; MTBLC16609; MTBLC27972; MTBLC16622; MTBLC27453; MTBLC17011; MTBLC16222; MTBLC15895; MTBLC15945; MTBLC16165; MTBLC16217; MTBLC28991; MTBLC24150; MTBLC5571; MTBLC5711; MTBLC48657; MTBLC8355; MTBLC29484; MTBLC17413; MTBLC16444; MTBLC17281; MTBLC17667; MTBLC17655; MTBLC111517; MTBLC741548; MTBLC17859; MTBLC91315; MTBLC75146; MTBLC76138; MTBLC80222; MTBLC30751; MTBLC28624; MTBLC135926; MTBLC57303; MTBLC15426; MTBLC6049; MTBLC7851; MTBLC3364; MTBLC7564; MTBLC16719; MTBLC31046; MTBLC34288; MTBLC86365; MTBLC17308; MTBLC35932; MTBLC28422; MTBLC48430; MTBLC15888; MTBLC17075; MTBLC29024; MTBLC4893; MTBLC15825; MTBLC16486; MTBLC89540; MTBLC89917; MTBLC9603; MTBLC2801; MTBLC92373; MTBLC2724; MTBLC90086; MTBLC16820; MTBLC7986; MTBLC82603; MTBLC3746; MTBLC8955; MTBLC34596; MTBLC34597; MTBLC50729; MTBLC28463; MTBLC135497; MTBLC34379; MTBLC5138; MTBLC81321; MTBLC5321; MTBLC58778; MTBLC8982; MTBLC9783; MTBLC31113; MTBLC8393; MTBLC44185; MTBLC79670; MTBLC7577; MTBLC79483; MTBLC135464; MTBLC27683; MTBLC15999; MTBLC16433; MTBLC15365; MTBLC17395; MTBLC89749; MTBLC137819; MTBLC88868; MTBLC70851; MTBLC15566; MTBLC68502; MTBLC68503; MTBLC7773; MTBLC17990; MTBLC15711; MTBLC18412; MTBLC94706; MTBLC7470; MTBLC31592; MTBLC16252; MTBLC27949; MTBLC9725; MTBLC40947; MTBLC32019; MTBLC3154; MTBLC8682; MTBLC6737; MTBLC8205; MTBLC16279; MTBLC15645; MTBLC2735; MTBLC17340; MTBLC3868; MTBLC6563; MTBLC8339; MTBLC59583; MTBLC45257; MTBLC10003; MTBLC3451; MTBLC141529; MTBLC137236; MTBLC18026; MTBLC17189; MTBLC68465; MTBLC36062; MTBLC17253; MTBLC16509; MTBLC133083; MTBLC86542; MTBLC131434; MTBLC17869; MTBLC59783; MTBLC55534; MTBLC28707; MTBLC27909; MTBLC134808; MTBLC64390; MTBLC136818; MTBLC136917; MTBLC17786; MTBLC9367; MTBLC138495; MTBLC43533; MTBLC17945; MTBLC37419; MTBLC75; MTBLC2702; MTBLC27920; MTBLC5557; MTBLC2527; MTBLC67461; MTBLC17727; MTBLC34921; MTBLC15932; MTBLC7513; MTBLC9047; MTBLC31433; MTBLC80391; MTBLC3384; MTBLC6003; MTBLC79609; MTBLC135445; MTBLC7628; MTBLC133152; MTBLC80000; MTBLC7421; MTBLC71498; MTBLC17335; MTBLC3103; MTBLC62251; MTBLC17531; MTBLC2469; MTBLC34550; MTBLC2515; MTBLC79698; MTBLC8173; MTBLC18328; MTBLC2672; MTBLC6369; MTBLC7659; MTBLC9468; MTBLC82542; MTBLC63628; MTBLC6109; MTBLC7609; MTBLC28064; MTBLC16726; MTBLC28596; MTBLC17379; MTBLC31788; MTBLC7910; MTBLC134007; MTBLC7951; MTBLC133365; MTBLC75439; MTBLC69814; MTBLC16631; MTBLC79936; MTBLC34236; MTBLC51016; MTBLC3419; MTBLC136949; MTBLC135542; MTBLC135408; MTBLC17249; MTBLC614; MTBLC3293; MTBLC34715; MTBLC9300; MTBLC39618; MTBLC663; MTBLC20092; MTBLC35057; MTBLC36152; MTBLC35067; MTBLC3245; MTBLC38363; MTBLC4892; MTBLC4352; MTBLC80493; MTBLC28766; MTBLC15437; MTBLC6090; MTBLC8198; MTBLC8333; MTBLC49005; MTBLC3251; MTBLC32061; MTBLC75529; MTBLC79637; MTBLC3302; MTBLC4409; MTBLC4748; MTBLC32288; MTBLC5178; MTBLC79484; MTBLC59781; MTBLC567361; MTBLC31184; MTBLC3002; MTBLC5944; MTBLC135161; MTBLC2538; MTBLC5980; MTBLC38545; MTBLC59297; MTBLC136009; MTBLC15641; MTBLC3190; MTBLC5988; MTBLC7889; MTBLC3205; MTBLC32047; MTBLC3189; MTBLC22584; MTBLC38209; MTBLC89227; MTBLC89226; MTBLC89265; MTBLC89264; MTBLC89386; MTBLC89404; MTBLC89349; MTBLC89348; MTBLC89329; MTBLC89346; MTBLC7751; MTBLC18144; MTBLC89312; MTBLC89182; MTBLC4575; MTBLC4909; MTBLC42944; MTBLC6777; MTBLC8872; MTBLC32309; MTBLC31969; MTBLC8878; MTBLC71003; MTBLC16874; MTBLC71981; MTBLC4877; MTBLC73713; MTBLC135149; MTBLC30764; MTBLC30763; MTBLC28508; MTBLC50205; MTBLC16914; MTBLC9126; MTBLC73752; MTBLC78774; MTBLC79112; MTBLC141205; MTBLC89206; MTBLC89891; MTBLC17998; MTBLC28857; MTBLC18099; MTBLC89215; MTBLC88528; MTBLC82344; MTBLC9878; MTBLC28276; MTBLC131951; MTBLC27540; MTBLC748; MTBLC34311; MTBLC2429; MTBLC5831; MTBLC29491; MTBLC3299; MTBLC3329; MTBLC8891; MTBLC31070; MTBLC138195; MTBLC137853; MTBLC34697; MTBLC41865; MTBLC73112; MTBLC143910; MTBLC142593; MTBLC3570; MTBLC10575; MTBLC16111; MTBLC3555; MTBLC6372; MTBLC35038; MTBLC63610; MTBLC79675; MTBLC79848; MTBLC34114; MTBLC64496; MTBLC143715; MTBLC135277; MTBLC5541; MTBLC135317; MTBLC6565; MTBLC29544; MTBLC138814; MTBLC79429; MTBLC34866; MTBLC78661; MTBLC80148; MTBLC79962; MTBLC137230; MTBLC83030; MTBLC10225; MTBLC75097; MTBLC75094; MTBLC78448; MTBLC80550; MTBLC29736; MTBLC32110; MTBLC60723; MTBLC77122; MTBLC80188; MTBLC6357; MTBLC28838; MTBLC138919; MTBLC80411; MTBLC27325; MTBLC27547; MTBLC29526; MTBLC29535; MTBLC70549; MTBLC3953; MTBLC16587; MTBLC80534; MTBLC2528; MTBLC27495; MTBLC8629; MTBLC27471; MTBLC36274; MTBLC89929; MTBLC7190; MTBLC79995; MTBLC6426; MTBLC39251; MTBLC39250; MTBLC42504; MTBLC79074; MTBLC247956; MTBLC72715; MTBLC73072; MTBLC9250; MTBLC27752; MTBLC31116; MTBLC94461; MTBLC37550; MTBLC34120; MTBLC4648; MTBLC5016; MTBLC51963; MTBLC81262; MTBLC81252; MTBLC81249; MTBLC81245; MTBLC89219; MTBLC136724; MTBLC81299; MTBLC81298; MTBLC36240; MTBLC81308; MTBLC16359; MTBLC138876; MTBLC81261; MTBLC88105; MTBLC137810; MTBLC22868; MTBLC81244; MTBLC134216; MTBLC81240; MTBLC137147; MTBLC87823; MTBLC3216; MTBLC75029; MTBLC34086; MTBLC75106; MTBLC136790; MTBLC73121; MTBLC73008; MTBLC78810; MTBLC76151; MTBLC15889; MTBLC136361; MTBLC64153; MTBLC52979; MTBLC582124; MTBLC84883; MTBLC53488; MTBLC79914; MTBLC79922; MTBLC61204; MTBLC30042; MTBLC2740; MTBLC17034; MTBLC73504; MTBLC79961; MTBLC137717; MTBLC135699; MTBLC89608; MTBLC137921; MTBLC20538; MTBLC64023; MTBLC2625; MTBLC135865; MTBLC37658; MTBLC80134; MTBLC62481; MTBLC10223; MTBLC27793; MTBLC10362; MTBLC6602; MTBLC7037; MTBLC8907; MTBLC65244; MTBLC27776; MTBLC52649; MTBLC31602; MTBLC80020; MTBLC4787; MTBLC75062; MTBLC86088; MTBLC75304; MTBLC138215; MTBLC136139; MTBLC3902; MTBLC29532; MTBLC29541; MTBLC65657; MTBLC9612; MTBLC732; MTBLC27783; MTBLC1684; MTBLC9901; MTBLC135424; MTBLC28371; MTBLC4384; MTBLC4747; MTBLC5540; MTBLC66682; MTBLC28373; MTBLC3115; MTBLC27799; MTBLC9455; MTBLC9644; MTBLC81242; MTBLC28834; MTBLC88098; MTBLC88102; MTBLC72724; MTBLC81258; MTBLC81276; MTBLC16755; MTBLC52023; MTBLC81256; MTBLC43419; MTBLC9907; MTBLC2364; MTBLC83267; MTBLC67554; MTBLC80214; MTBLC80215; MTBLC4851; MTBLC28753; MTBLC16835; MTBLC89266; MTBLC89273; MTBLC89275; MTBLC84525; MTBLC89410; MTBLC75385; MTBLC89353; MTBLC18197; MTBLC53042; MTBLC84372; MTBLC72797; MTBLC138421; MTBLC8484; MTBLC62739; MTBLC84875; MTBLC85058; MTBLC133136; MTBLC144310; MTBLC84262; MTBLC39246; MTBLC51340; MTBLC68565; MTBLC29582; MTBLC80164; MTBLC80133; MTBLC62505; MTBLC35331; MTBLC5760; MTBLC89656; MTBLC137056; MTBLC2440; MTBLC3948; MTBLC70548; MTBLC53041; MTBLC137855; MTBLC73858; MTBLC64561; MTBLC76076; MTBLC44811; MTBLC18081; MTBLC17495; MTBLC76325; MTBLC76986; MTBLC76218; MTBLC136990; MTBLC136991; MTBLC136988; MTBLC136989; MTBLC4356; MTBLC132492; MTBLC132493; MTBLC80086; MTBLC137161; MTBLC50108; MTBLC135810; MTBLC32065; MTBLC28292; MTBLC73060; MTBLC80206; MTBLC2987; MTBLC43602; MTBLC79548; MTBLC77254; MTBLC73262; MTBLC3946; MTBLC4668; MTBLC4669; MTBLC7522; MTBLC134518; MTBLC136105; MTBLC136110; MTBLC80082; MTBLC80079; MTBLC77996; MTBLC34979; MTBLC8711; MTBLC79875; MTBLC53487; MTBLC88685; MTBLC34031; MTBLC28805; MTBLC29027; MTBLC15577; MTBLC16286; MTBLC87046; MTBLC87289; MTBLC78242; MTBLC84863; MTBLC73215; MTBLC84945; MTBLC72714; MTBLC52717; MTBLC34894; MTBLC84392; MTBLC88784; MTBLC88783; MTBLC84417; MTBLC88368; MTBLC89231; MTBLC89212; MTBLC3441; MTBLC18430; MTBLC70069; MTBLC7868; MTBLC583; MTBLC2888; MTBLC3887; MTBLC4804; MTBLC39; MTBLC29457; MTBLC28364; MTBLC79531; MTBLC79820; MTBLC79590; MTBLC79957; MTBLC79761; MTBLC79913; MTBLC79540; MTBLC79701; MTBLC79417; MTBLC34183; MTBLC79526; MTBLC79705; MTBLC79558; MTBLC132927; MTBLC28987; MTBLC15417; MTBLC6039; MTBLC29615; MTBLC135283; MTBLC27436; MTBLC34849; MTBLC29653; MTBLC135282; MTBLC78258; MTBLC31946; MTBLC29660; MTBLC16179; MTBLC34980; MTBLC139131; MTBLC73676; MTBLC81253; MTBLC16325; MTBLC63598; MTBLC7731; MTBLC135233; MTBLC36461; MTBLC17415; MTBLC17626; MTBLC17204; MTBLC2424; MTBLC15670; MTBLC30838; MTBLC16600; MTBLC135704; MTBLC4429; MTBLC15414; MTBLC88735; MTBLC51805; MTBLC17685; MTBLC4391; MTBLC8038; MTBLC17858; MTBLC2669; MTBLC17631; MTBLC64835; MTBLC27603; MTBLC1683; MTBLC62974; MTBLC28087; MTBLC28460; MTBLC17164; MTBLC8809; MTBLC5762; MTBLC18261; MTBLC17201; MTBLC17196; MTBLC15737; MTBLC29045; MTBLC134287; MTBLC16929; MTBLC17143; MTBLC31173; MTBLC31278; MTBLC64977; MTBLC5320; MTBLC71166; MTBLC27480; MTBLC30449; MTBLC34291; MTBLC17397; MTBLC24814; MTBLC15604; MTBLC89185; MTBLC57826; MTBLC28825; MTBLC18347; MTBLC17191; MTBLC15603; MTBLC64348; MTBLC9122; MTBLC79874; MTBLC34141; MTBLC73773; MTBLC79786; MTBLC79448; MTBLC5120; MTBLC16899; MTBLC17924; MTBLC17505; MTBLC18202; MTBLC28789; MTBLC29864; MTBLC17702; MTBLC17151; MTBLC18403; MTBLC15963; MTBLC16138; MTBLC57653; MTBLC33917; MTBLC22357; MTBLC37690; MTBLC28061; MTBLC17925; MTBLC28729; MTBLC10295; MTBLC28645; MTBLC27667; MTBLC15903; MTBLC28994; MTBLC28563; MTBLC17393; MTBLC28385; MTBLC15824; MTBLC16824; MTBLC4139; MTBLC4167; MTBLC27611; MTBLC18004; MTBLC4194; MTBLC28014; MTBLC16024; MTBLC27605; MTBLC17317; MTBLC16443; MTBLC28458; MTBLC48095; MTBLC17234; MTBLC24978; MTBLC17357; MTBLC27987; MTBLC17268; MTBLC10642; MTBLC27922; MTBLC28354; MTBLC11424; MTBLC27806; MTBLC27816; MTBLC28816; MTBLC17053; MTBLC29990; MTBLC5159; MTBLC18012; MTBLC18300; MTBLC1241; MTBLC28791; MTBLC62637; MTBLC16015; MTBLC58724; MTBLC16439; MTBLC45441; MTBLC31882; MTBLC17981; MTBLC16264; MTBLC16650; MTBLC16287; MTBLC3421; MTBLC7500; MTBLC32059; MTBLC135923; MTBLC40957; MTBLC41938; MTBLC79970; MTBLC4289; MTBLC59276; MTBLC133622; MTBLC16654; MTBLC86537; MTBLC982; MTBLC17094; MTBLC28710; MTBLC37032; MTBLC27530; MTBLC30832; MTBLC68566; MTBLC17646; MTBLC86396; MTBLC89760; MTBLC79634; MTBLC79456; MTBLC79768; MTBLC79876; MTBLC34930; MTBLC137770; MTBLC32350; MTBLC33020; MTBLC1230; MTBLC16551; MTBLC39244; MTBLC28676; MTBLC18260; MTBLC27554; MTBLC77436; MTBLC18167; MTBLC36217; MTBLC71422; MTBLC36218; MTBLC18147; MTBLC17057; MTBLC4125; MTBLC21010; MTBLC17306; MTBLC4808; MTBLC133330; MTBLC28066; MTBLC16751; MTBLC28189; MTBLC17716; MTBLC6359; MTBLC18411; MTBLC6435; MTBLC25164; MTBLC28053; MTBLC7570; MTBLC18394; MTBLC17992; MTBLC17400; MTBLC28870; MTBLC3354; MTBLC5158; MTBLC2310; MTBLC89730; MTBLC11222; MTBLC53490; MTBLC5847; MTBLC31759; MTBLC5597; MTBLC79439; MTBLC45951; MTBLC34619; MTBLC28657; MTBLC27520; MTBLC42976; MTBLC16802; MTBLC3014; MTBLC2155; MTBLC2185; MTBLC2321; MTBLC135989; MTBLC6709; MTBLC6888; MTBLC79546; MTBLC79481; MTBLC81712; MTBLC6995; MTBLC6960; MTBLC35040; MTBLC3533; MTBLC35421; MTBLC33509; MTBLC48093; MTBLC33510; MTBLC33511; MTBLC34237; MTBLC15847; MTBLC57541; MTBLC71429; MTBLC102524; MTBLC134923; MTBLC134922; MTBLC80471; MTBLC43996; MTBLC18226; MTBLC17532; MTBLC30734; MTBLC134814; MTBLC37753; MTBLC27469; MTBLC16142; MTBLC17426; MTBLC28860; MTBLC20937; MTBLC47962; MTBLC4178; MTBLC16224; MTBLC21099; MTBLC24113; MTBLC33830; MTBLC24769; MTBLC28378; MTBLC85187; MTBLC15676; MTBLC29474; MTBLC17693; MTBLC16409; MTBLC17405; MTBLC2085; MTBLC34334; MTBLC20367; MTBLC28719; MTBLC137246; MTBLC29069; MTBLC30801; MTBLC29009; MTBLC17077; MTBLC46644; MTBLC33198; MTBLC24149; MTBLC24266; MTBLC24462; MTBLC18246; MTBLC681850; MTBLC9669; MTBLC52672; MTBLC32709; MTBLC31677; MTBLC8871; MTBLC27513; MTBLC77872; MTBLC60076; MTBLC613; MTBLC1945; MTBLC15937; MTBLC9513; MTBLC63624; MTBLC17748; MTBLC17293; MTBLC2555; MTBLC137768; MTBLC3158; MTBLC7785; MTBLC8256; MTBLC7821; MTBLC135842; MTBLC66773; MTBLC139; MTBLC16703; MTBLC531; MTBLC27380; MTBLC16885; MTBLC17332; MTBLC64833; MTBLC28782; MTBLC28793; MTBLC3528; MTBLC31005; MTBLC27680; MTBLC27649; MTBLC6364; MTBLC27931; MTBLC6731; MTBLC7912; MTBLC18154; MTBLC16634; MTBLC9859; MTBLC2913; MTBLC6076; MTBLC135714; MTBLC15532; MTBLC57385; MTBLC16043; MTBLC5457; MTBLC134255; MTBLC77131; MTBLC6791; MTBLC34048; MTBLC48541; MTBLC137772; MTBLC16547; MTBLC9957; MTBLC10366; MTBLC10423; MTBLC87625; MTBLC6859; MTBLC30860; MTBLC15741; MTBLC30347; MTBLC77780; MTBLC89639; MTBLC9735; MTBLC135111; MTBLC136292; MTBLC254496; MTBLC35034; MTBLC4364; MTBLC17506; MTBLC57874; MTBLC58330; MTBLC18321; MTBLC15934; MTBLC6819; MTBLC30527; MTBLC2653; MTBLC39462; MTBLC79807; MTBLC3897; MTBLC8380; MTBLC57831; MTBLC15362; MTBLC8478; MTBLC37079; MTBLC33033; MTBLC16530; MTBLC27401; MTBLC39153; MTBLC45630; MTBLC48058; MTBLC27444; MTBLC41607; MTBLC705; MTBLC5954; MTBLC50885; MTBLC135324; MTBLC78158; MTBLC836; MTBLC3276; MTBLC3614; MTBLC89060; MTBLC89499; MTBLC799; MTBLC34139; MTBLC79668; MTBLC79797; MTBLC136980; MTBLC1189; MTBLC136972; MTBLC79907; MTBLC63641; MTBLC79715; MTBLC2495; MTBLC79887; MTBLC9460; MTBLC57958; MTBLC6650; MTBLC32242; MTBLC2431; MTBLC34801; MTBLC63622; MTBLC79719; MTBLC34321; MTBLC5810; MTBLC17871; MTBLC30966; MTBLC27957; MTBLC18419; MTBLC30768; MTBLC137814; MTBLC86348; MTBLC86391; MTBLC36532; MTBLC27904; MTBLC16023; MTBLC27378; MTBLC28587; MTBLC3641; MTBLC9653; MTBLC135517; MTBLC3918; MTBLC79692; MTBLC79988; MTBLC9961; MTBLC16546; MTBLC18428; MTBLC28102; MTBLC37165; MTBLC28808; MTBLC90185; MTBLC6838; MTBLC1547; MTBLC2076; MTBLC63581; MTBLC141154; MTBLC8049; MTBLC16992; MTBLC30841; MTBLC30794; MTBLC135928; MTBLC6628; MTBLC57905; MTBLC84094; MTBLC8341; MTBLC79347; MTBLC68606; MTBLC610092; MTBLC139380; MTBLC73758; MTBLC15436; MTBLC27630; MTBLC32398; MTBLC15366; MTBLC17071; MTBLC15586; MTBLC29003; MTBLC16699; MTBLC17647; MTBLC35173; MTBLC17084; MTBLC58511; MTBLC15584; MTBLC16292; MTBLC27736; MTBLC16392; MTBLC15867; MTBLC6177; MTBLC37434; MTBLC47518; MTBLC31441; MTBLC75988; MTBLC80438; MTBLC3978; MTBLC80441; MTBLC133224; MTBLC31743; MTBLC80528; MTBLC6553; MTBLC133244; MTBLC28527; MTBLC135754; MTBLC27994; MTBLC66905; MTBLC3439; MTBLC27475; MTBLC28426; MTBLC80434; MTBLC5065; MTBLC17965; MTBLC31742; MTBLC30200; MTBLC75790; MTBLC7781; MTBLC17558; MTBLC43136; MTBLC17456; MTBLC18320; MTBLC31784; MTBLC2905; MTBLC101278; MTBLC31901; MTBLC34474; MTBLC34511; MTBLC79863; MTBLC57681; MTBLC16211; MTBLC16773; MTBLC16898; MTBLC3697; MTBLC44932; MTBLC53770; MTBLC31682; MTBLC79369; MTBLC13714; MTBLC63609; MTBLC16856; MTBLC32153; MTBLC6413; MTBLC80592; MTBLC51032; MTBLC79929; MTBLC10285; MTBLC2883; MTBLC135745; MTBLC34574; MTBLC31359; MTBLC31849; MTBLC4708; MTBLC5384; MTBLC151; MTBLC160; MTBLC15622; MTBLC35453; MTBLC18281; MTBLC17305; MTBLC41893; MTBLC42819; MTBLC57992; MTBLC30769; MTBLC30887; MTBLC7814; MTBLC1670; MTBLC73757; MTBLC21305; MTBLC18050; MTBLC33138; MTBLC15607; MTBLC52222; MTBLC36458; MTBLC30835; MTBLC36455; MTBLC25311; MTBLC30314; MTBLC18043; MTBLC16352; MTBLC37011; MTBLC16010; MTBLC94613; MTBLC6151; MTBLC139123; MTBLC30845; MTBLC30846; MTBLC28459; MTBLC58560; MTBLC17798; MTBLC10072; MTBLC29513; MTBLC58556; MTBLC17533; MTBLC52859; MTBLC17802; MTBLC16704; MTBLC86004; MTBLC9274; MTBLC9275; MTBLC35014; MTBLC73688; MTBLC135289; MTBLC2506; MTBLC2769; MTBLC9045; MTBLC141; MTBLC89487; MTBLC30821; MTBLC79630; MTBLC1734; MTBLC12257; MTBLC133809; MTBLC135613; MTBLC50742; MTBLC131508; MTBLC34262; MTBLC27951; MTBLC15623; MTBLC15624; MTBLC16715; MTBLC27583; MTBLC16278; MTBLC17782; MTBLC22652; MTBLC17039; MTBLC18268; MTBLC73681; MTBLC17801; MTBLC45969; MTBLC21241; MTBLC27797; MTBLC30923; MTBLC4083; MTBLC28411; MTBLC36622; MTBLC58468; MTBLC18383; MTBLC135643; MTBLC34170; MTBLC87820; MTBLC79702; MTBLC31215; MTBLC4919; MTBLC8880; MTBLC1656; MTBLC49003; MTBLC17032; MTBLC16609; MTBLC27972; MTBLC16622; MTBLC27453; MTBLC16669; MTBLC17011; MTBLC16222; MTBLC15895; MTBLC15945; MTBLC16165; MTBLC16217; MTBLC28991; MTBLC24150; MTBLC5571; MTBLC5711; MTBLC48657; MTBLC8355; MTBLC29484; MTBLC17413; MTBLC16444; MTBLC17281; MTBLC17667; MTBLC17655; MTBLC111517; MTBLC741548; MTBLC17859; MTBLC91315; MTBLC75146; MTBLC76138; MTBLC15582; MTBLC15583; MTBLC57424; MTBLC49076; MTBLC18104; MTBLC18078; MTBLC17023; MTBLC27861; MTBLC27550; MTBLC15591; MTBLC16831; MTBLC89205; MTBLC138367; MTBLC28381; MTBLC59051; MTBLC30997; MTBLC6452; MTBLC17937; MTBLC3088; MTBLC50271; MTBLC69499; MTBLC4994; MTBLC6008; MTBLC7161; MTBLC80222; MTBLC473990; MTBLC17433; MTBLC30751; MTBLC28624; MTBLC135926; MTBLC143968; MTBLC17705; MTBLC57303; MTBLC15426; MTBLC6049; MTBLC7851; MTBLC3364; MTBLC4888; MTBLC134865; MTBLC5862; MTBLC16828; MTBLC79441; MTBLC9935; MTBLC7564; MTBLC16719; MTBLC31046; MTBLC34288; MTBLC86365; MTBLC17308; MTBLC35932; MTBLC28422; MTBLC48430; MTBLC15888; MTBLC17075; MTBLC18322; MTBLC29024; MTBLC4893; MTBLC15825; MTBLC16486; MTBLC89540; MTBLC15637; MTBLC63606; MTBLC45981; MTBLC8772; MTBLC4071; MTBLC3748; MTBLC51141; MTBLC89917; MTBLC9603; MTBLC2801; MTBLC92373; MTBLC2724; MTBLC90086; MTBLC16820; MTBLC7986; MTBLC82603; MTBLC3746; MTBLC8955; MTBLC37923; MTBLC10026; MTBLC35028; MTBLC10022; MTBLC34712; MTBLC60069; MTBLC6891; MTBLC16389; MTBLC43468; MTBLC35128; MTBLC28652; MTBLC35121; MTBLC28635; MTBLC30850; MTBLC4822; MTBLC6617; MTBLC34596; MTBLC34597; MTBLC50729; MTBLC28463; MTBLC135497; MTBLC34379; MTBLC25357; MTBLC27504; MTBLC5138; MTBLC81321; MTBLC5321; MTBLC58778; MTBLC8982; MTBLC9783; MTBLC31113; MTBLC8393; MTBLC44185; MTBLC79670; MTBLC7577; MTBLC79483; MTBLC60078; MTBLC135464; MTBLC82864; MTBLC135383; MTBLC4682; MTBLC76258; MTBLC135151; MTBLC27683; MTBLC15999; MTBLC16433; MTBLC15365; MTBLC58129; MTBLC17395; MTBLC89749; MTBLC58642; MTBLC137819; MTBLC88868; MTBLC70851; MTBLC15566; MTBLC68502; MTBLC68503; MTBLC36165; MTBLC17878; MTBLC17611; MTBLC17915; MTBLC85235; MTBLC38355; MTBLC49283; MTBLC143856; MTBLC61206; MTBLC7773; MTBLC17990; MTBLC15711; MTBLC18412; MTBLC94706; MTBLC40521; MTBLC7470; MTBLC31592; MTBLC16252; MTBLC57621; MTBLC27949; MTBLC9725; MTBLC40947; MTBLC32019; MTBLC3154; MTBLC8682; MTBLC6737; MTBLC8205; MTBLC16279; MTBLC2697; MTBLC2722; MTBLC6080; MTBLC8822; MTBLC52070; MTBLC9912; MTBLC8247; MTBLC32003; MTBLC15645; MTBLC2735; MTBLC17340; MTBLC3868; MTBLC6563; MTBLC8339; MTBLC59583; MTBLC45257; MTBLC3451; MTBLC141529; MTBLC137236; MTBLC18026; MTBLC17189; MTBLC68465; MTBLC36062; MTBLC17253; MTBLC16509; MTBLC133083; MTBLC86542; MTBLC131434; MTBLC17869; MTBLC59783; MTBLC55534; MTBLC28707; MTBLC27909; MTBLC16182; MTBLC16638; MTBLC16133; MTBLC16472; MTBLC87755; MTBLC84069; MTBLC16019; MTBLC46941; MTBLC134808; MTBLC64390; MTBLC136818; MTBLC136917; MTBLC17786; MTBLC9367; MTBLC138495; MTBLC43533; MTBLC17945; MTBLC37419; MTBLC85162; MTBLC23757; MTBLC5826; MTBLC62069; MTBLC223316; MTBLC135072; MTBLC75; MTBLC2702; MTBLC27920; MTBLC5557; MTBLC34405; MTBLC34788; MTBLC2527; MTBLC67461; MTBLC17727; MTBLC34921; MTBLC15932; MTBLC7513; MTBLC9047; MTBLC31433; MTBLC80391; MTBLC3384; MTBLC2156; MTBLC2368; MTBLC6003; MTBLC2532; MTBLC2821; MTBLC3287; MTBLC6511; MTBLC79609; MTBLC135445; MTBLC7628; MTBLC133152; MTBLC80000; MTBLC7421; MTBLC71498; MTBLC17335; MTBLC3103; MTBLC62251; MTBLC17531; MTBLC29458; MTBLC15830; MTBLC134834; MTBLC34769; MTBLC46750; MTBLC7952; MTBLC8186; MTBLC32249; MTBLC15884; MTBLC28865; MTBLC21484; MTBLC15874; MTBLC2469; MTBLC5093; MTBLC63630; MTBLC2294; MTBLC2425; MTBLC16363; MTBLC2629; MTBLC69335; MTBLC28356; MTBLC4441; MTBLC135002; MTBLC10058; MTBLC10076; MTBLC10103; MTBLC28714; MTBLC34550; MTBLC2515; MTBLC79698; MTBLC8173; MTBLC18328; MTBLC2672; MTBLC6369; MTBLC7659; MTBLC9468; MTBLC82542; MTBLC63628; MTBLC6109; MTBLC7609; MTBLC28064; MTBLC16726; MTBLC28596; MTBLC17379; MTBLC31788; MTBLC7910; MTBLC134007; MTBLC7951; MTBLC133365; MTBLC75439; MTBLC69814; MTBLC16631; MTBLC135701; MTBLC16778; MTBLC18330; MTBLC4783; MTBLC27514; MTBLC5304; MTBLC31967; MTBLC16954; MTBLC3740; MTBLC4320; MTBLC24293; MTBLC79936; MTBLC34236; MTBLC51016; MTBLC3419; MTBLC136949; MTBLC135542; MTBLC135408; MTBLC17249; MTBLC614; MTBLC3293; MTBLC34715; MTBLC9300; MTBLC39618; MTBLC663; MTBLC20092; MTBLC35057; MTBLC36152; MTBLC35067; MTBLC3245; MTBLC27804; MTBLC38363; MTBLC4892; MTBLC4352; MTBLC34580; MTBLC27993; MTBLC82684; MTBLC135703; MTBLC80493; MTBLC87947; MTBLC28766; MTBLC15437; MTBLC6090; MTBLC8198; MTBLC8333; MTBLC49005; MTBLC3251; MTBLC32061; MTBLC75529; MTBLC79637; MTBLC3302; MTBLC4409; MTBLC4748; MTBLC32288; MTBLC5178; MTBLC79484; MTBLC17713; MTBLC10037; MTBLC8922; MTBLC7471; MTBLC59781; MTBLC31563; MTBLC6863; MTBLC567361; MTBLC31184; MTBLC3002; MTBLC5944; MTBLC135161; MTBLC2538; MTBLC5980; MTBLC38545; MTBLC59297; MTBLC136009; MTBLC15641; MTBLC3190; MTBLC5988; MTBLC7889; MTBLC3205; MTBLC32047; MTBLC3189; MTBLC22584; MTBLC38209; MTBLC89227; MTBLC89226; MTBLC89265; MTBLC89264; MTBLC89386; MTBLC89404; MTBLC89349; MTBLC89348; MTBLC89329; MTBLC89346; MTBLC7751; MTBLC18144; MTBLC89312; MTBLC89182; MTBLC78700; MTBLC55523; MTBLC31896; MTBLC9108; MTBLC9946; MTBLC847; MTBLC9205; MTBLC4575; MTBLC4909; MTBLC42944; MTBLC6777; MTBLC8872; MTBLC32309; MTBLC31969; MTBLC8878; MTBLC79612; MTBLC18054; MTBLC3430; MTBLC6965; MTBLC71003; MTBLC16874; MTBLC71981; MTBLC4877; MTBLC73713; MTBLC4417; MTBLC31298; MTBLC8713; MTBLC79465; MTBLC4773; MTBLC5527; MTBLC9959; MTBLC31086; MTBLC2626; MTBLC8402; MTBLC32185; MTBLC48131; MTBLC86544; MTBLC29564; MTBLC31447; MTBLC73; MTBLC30725; MTBLC34968; MTBLC135149; MTBLC6798; MTBLC91807; MTBLC2939; MTBLC30764; MTBLC30763; MTBLC28508; MTBLC50205; MTBLC16914; MTBLC9126; MTBLC73752; MTBLC78774; MTBLC79112; MTBLC141205; MTBLC89206; MTBLC89891; MTBLC17998; MTBLC28857; MTBLC18099; MTBLC89215; MTBLC88528; MTBLC82344; MTBLC9878; MTBLC28276; MTBLC1749; MTBLC8602; MTBLC17467; MTBLC34605; MTBLC9425; MTBLC34252; MTBLC34256; MTBLC79445; MTBLC131951; MTBLC27540; MTBLC31049; MTBLC748; MTBLC34311; MTBLC2429; MTBLC5831; MTBLC29491; MTBLC3299; MTBLC3329; MTBLC8891; MTBLC18227; MTBLC94661; MTBLC31070; MTBLC138195; MTBLC137853; MTBLC142272; MTBLC34697; MTBLC41865; MTBLC73112; MTBLC143910; MTBLC142593; MTBLC3570; MTBLC10575; MTBLC16111; MTBLC138422; MTBLC3555; MTBLC6372; MTBLC3284; MTBLC15809; MTBLC135723; MTBLC90233; MTBLC137178; MTBLC82985; MTBLC35038; MTBLC79471; MTBLC79566; MTBLC63610; MTBLC79675; MTBLC79848; MTBLC34114; MTBLC64496; MTBLC143715; MTBLC135277; MTBLC4819; MTBLC5541; MTBLC18171; MTBLC32086; MTBLC5206; MTBLC135317; MTBLC6565; MTBLC8621; MTBLC89382; MTBLC89352; MTBLC89368; MTBLC89366; MTBLC89340; MTBLC89317; MTBLC29544; MTBLC138814; MTBLC136905; MTBLC133325; MTBLC135350; MTBLC79177; MTBLC84854; MTBLC34295; MTBLC29479; MTBLC17903; MTBLC4045; MTBLC10445; MTBLC6706; MTBLC79429; MTBLC34866; MTBLC34499; MTBLC34503; MTBLC34506; MTBLC91217; MTBLC138082; MTBLC79519; MTBLC34293; MTBLC34294; MTBLC78661; MTBLC73794; MTBLC80148; MTBLC34229; MTBLC138081; MTBLC79962; MTBLC137230; MTBLC83030; MTBLC10225; MTBLC448; MTBLC72665; MTBLC138258; MTBLC138255; MTBLC72663; MTBLC133381; MTBLC133086; MTBLC75097; MTBLC75094; MTBLC78448; MTBLC80550; MTBLC29736; MTBLC15658; MTBLC15655; MTBLC15657; MTBLC64008; MTBLC138786; MTBLC88461; MTBLC34148; MTBLC91272; MTBLC34485; MTBLC34498; MTBLC34500; MTBLC88440; MTBLC34504; MTBLC143972; MTBLC88465; MTBLC32110; MTBLC16089; MTBLC60723; MTBLC77122; MTBLC80188; MTBLC6357; MTBLC28838; MTBLC138919; MTBLC80411; MTBLC27325; MTBLC27547; MTBLC82763; MTBLC29526; MTBLC29535; MTBLC70549; MTBLC131659; MTBLC15575; MTBLC2513; MTBLC2492; MTBLC5166; MTBLC3953; MTBLC16587; MTBLC80534; MTBLC2528; MTBLC27495; MTBLC8629; MTBLC63916; MTBLC27471; MTBLC36274; MTBLC89929; MTBLC34920; MTBLC6088; MTBLC7190; MTBLC79995; MTBLC6426; MTBLC692; MTBLC39251; MTBLC39250; MTBLC42504; MTBLC75219; MTBLC30805; MTBLC140088; MTBLC74966; MTBLC34163; MTBLC31561; MTBLC135525; MTBLC8039; MTBLC17457; MTBLC4453; MTBLC9261; MTBLC48742; MTBLC52421; MTBLC79074; MTBLC474014; MTBLC247956; MTBLC83058; MTBLC2366; MTBLC72715; MTBLC73072; MTBLC64483; MTBLC131738; MTBLC64489; MTBLC78103; MTBLC58206; MTBLC9250; MTBLC1418; MTBLC27752; MTBLC31116; MTBLC84299; MTBLC58303; MTBLC46979; MTBLC136623; MTBLC94461; MTBLC37550; MTBLC64124; MTBLC46961; MTBLC65247; MTBLC32345; MTBLC4746; MTBLC80169; MTBLC34120; MTBLC85403; MTBLC74971; MTBLC4648; MTBLC5016; MTBLC51963; MTBLC71025; MTBLC73792; MTBLC137845; MTBLC81262; MTBLC81252; MTBLC81249; MTBLC81245; MTBLC89219; MTBLC136724; MTBLC81299; MTBLC81298; MTBLC36240; MTBLC81308; MTBLC16359; MTBLC138876; MTBLC81261; MTBLC88105; MTBLC137810; MTBLC22868; MTBLC81244; MTBLC134216; MTBLC81240; MTBLC28468; MTBLC64563; MTBLC76078; MTBLC72998; MTBLC78101; MTBLC134424; MTBLC134423; MTBLC133456; MTBLC88698; MTBLC88697; MTBLC137147; MTBLC87823; MTBLC3216; MTBLC76334; MTBLC73135; MTBLC34097; MTBLC75029; MTBLC34086; MTBLC75106; MTBLC136790; MTBLC73121; MTBLC73008; MTBLC78810; MTBLC49265; MTBLC15654; MTBLC88462; MTBLC80442; MTBLC84441; MTBLC72641; MTBLC136531; MTBLC72815; MTBLC80463; MTBLC76234; MTBLC34491; MTBLC88441; MTBLC80447; MTBLC88438; MTBLC72843; MTBLC72842; MTBLC88460; MTBLC60956; MTBLC133329; MTBLC76151; MTBLC15889; MTBLC136361; MTBLC64153; MTBLC1309; MTBLC1310; MTBLC52979; MTBLC49254; MTBLC28724; MTBLC136767; MTBLC85633; MTBLC84874; MTBLC70850; MTBLC85057; MTBLC32365; MTBLC90027; MTBLC582124; MTBLC84883; MTBLC53488; MTBLC79914; MTBLC79922; MTBLC61204; MTBLC30042; MTBLC79179; MTBLC84855; MTBLC2740; MTBLC17034; MTBLC73504; MTBLC131692; MTBLC74330; MTBLC62834; MTBLC77492; MTBLC73741; MTBLC10087; MTBLC73851; MTBLC84752; MTBLC27706; MTBLC38299; MTBLC137495; MTBLC34154; MTBLC72639; MTBLC133357; MTBLC34494; MTBLC78730; MTBLC34496; MTBLC72651; MTBLC79961; MTBLC79513; MTBLC137717; MTBLC135699; MTBLC75612; MTBLC52392; MTBLC89608; MTBLC67309; MTBLC3940; MTBLC137921; MTBLC7909; MTBLC20538; MTBLC73092; MTBLC31501; MTBLC88109; MTBLC31297; MTBLC64023; MTBLC2625; MTBLC135865; MTBLC37658; MTBLC80134; MTBLC62481; MTBLC10223; MTBLC27793; MTBLC10362; MTBLC6602; MTBLC7037; MTBLC8907; MTBLC65244; MTBLC27776; MTBLC90454; MTBLC75376; MTBLC32157; MTBLC31279; MTBLC17058; MTBLC28688; MTBLC7720; MTBLC34835; MTBLC76090; MTBLC37998; MTBLC9951; MTBLC52649; MTBLC31602; MTBLC80020; MTBLC72828; MTBLC72952; MTBLC72736; MTBLC133144; MTBLC75036; MTBLC131924; MTBLC4787; MTBLC75062; MTBLC86088; MTBLC75304; MTBLC138215; MTBLC136139; MTBLC89521; MTBLC86095; MTBLC88906; MTBLC89602; MTBLC89539; MTBLC89536; MTBLC3902; MTBLC29532; MTBLC29541; MTBLC65657; MTBLC9612; MTBLC90040; MTBLC732; MTBLC27783; MTBLC1684; MTBLC9901; MTBLC135424; MTBLC89091; MTBLC75646; MTBLC89387; MTBLC89392; MTBLC89395; MTBLC89394; MTBLC134075; MTBLC90459; MTBLC134076; MTBLC134077; MTBLC134078; MTBLC39934; MTBLC134227; MTBLC134228; MTBLC16038; MTBLC137279; MTBLC137293; MTBLC28733; MTBLC28371; MTBLC4384; MTBLC28610; MTBLC86255; MTBLC76071; MTBLC143713; MTBLC72589; MTBLC131658; MTBLC4747; MTBLC5540; MTBLC66682; MTBLC28373; MTBLC3115; MTBLC27799; MTBLC73134; MTBLC73004; MTBLC62837; MTBLC78270; MTBLC36476; MTBLC79536; MTBLC73894; MTBLC9455; MTBLC9644; MTBLC1107; MTBLC31676; MTBLC50782; MTBLC31650; MTBLC6574; MTBLC31940; MTBLC81242; MTBLC28834; MTBLC88098; MTBLC88102; MTBLC72724; MTBLC58876; MTBLC81258; MTBLC81276; MTBLC16755; MTBLC52023; MTBLC81256; MTBLC43419; MTBLC9907; MTBLC27965; MTBLC744; MTBLC2364; MTBLC83267; MTBLC67554; MTBLC80214; MTBLC80215; MTBLC4851; MTBLC28753; MTBLC16835; MTBLC84519; MTBLC89266; MTBLC89273; MTBLC89275; MTBLC84525; MTBLC89410; MTBLC75385; MTBLC89353; MTBLC75038; MTBLC133623; MTBLC84577; MTBLC84234; MTBLC143985; MTBLC18197; MTBLC53042; MTBLC143980; MTBLC84372; MTBLC72797; MTBLC138421; MTBLC34004; MTBLC85639; MTBLC45478; MTBLC79312; MTBLC30820; MTBLC50576; MTBLC138260; MTBLC82464; MTBLC28592; MTBLC8484; MTBLC62739; MTBLC3427; MTBLC86197; MTBLC86196; MTBLC86189; MTBLC86190; MTBLC86188; MTBLC29613; MTBLC79453; MTBLC28047; MTBLC132620; MTBLC5783; MTBLC80531; MTBLC16688; MTBLC28135; MTBLC137137; MTBLC139534; MTBLC31731; MTBLC73923; MTBLC31801; MTBLC35459; MTBLC144339; MTBLC9194; MTBLC84875; MTBLC85058; MTBLC133136; MTBLC144310; MTBLC84262; MTBLC39246; MTBLC51340; MTBLC68565; MTBLC29582; MTBLC80164; MTBLC80133; MTBLC62505; MTBLC35331; MTBLC5760; MTBLC89656; MTBLC137056; MTBLC86418; MTBLC89703; MTBLC89592; MTBLC89589; MTBLC89384; MTBLC89098; MTBLC89143; MTBLC89070; MTBLC88726; MTBLC88872; MTBLC88588; MTBLC89498; MTBLC89502; MTBLC143982; MTBLC34041; MTBLC2440; MTBLC3948; MTBLC70548; MTBLC53041; MTBLC143989; MTBLC143981; MTBLC143983; MTBLC143987; MTBLC143990; MTBLC137855; MTBLC73858; MTBLC64561; MTBLC76076; MTBLC44811; MTBLC18081; MTBLC17495; MTBLC76325; MTBLC76986; MTBLC76218; MTBLC84566; MTBLC137216; MTBLC85680; MTBLC136990; MTBLC136991; MTBLC136988; MTBLC136989; MTBLC4356; MTBLC84877; MTBLC39248; MTBLC132492; MTBLC132493; MTBLC131689; MTBLC74340; MTBLC131668; MTBLC131687; MTBLC131688; MTBLC83055; MTBLC80086; MTBLC137161; MTBLC11152; MTBLC50108; MTBLC135810; MTBLC32065; MTBLC28292; MTBLC31550; MTBLC73060; MTBLC6991; MTBLC64032; MTBLC73736; MTBLC80206; MTBLC3300; MTBLC9515; MTBLC2987; MTBLC43602; MTBLC3249; MTBLC52897; MTBLC79548; MTBLC77254; MTBLC73262; MTBLC3944; MTBLC3946; MTBLC4668; MTBLC4669; MTBLC7522; MTBLC5933; MTBLC73854; MTBLC134518; MTBLC136105; MTBLC136110; MTBLC80082; MTBLC80079; MTBLC77996; MTBLC8774; MTBLC137248; MTBLC34979; MTBLC8711; MTBLC79875; MTBLC53487; MTBLC135165; MTBLC3845; MTBLC31831; MTBLC75565; MTBLC137215; MTBLC135498; MTBLC88685; MTBLC34031; MTBLC28805; MTBLC29027; MTBLC15577; MTBLC16286; MTBLC87046; MTBLC87289; MTBLC78242; MTBLC84863; MTBLC72837; MTBLC73215; MTBLC69081; MTBLC75542; MTBLC74274; MTBLC84945; MTBLC72714; MTBLC52717; MTBLC34894; MTBLC84392; MTBLC88784; MTBLC88783; MTBLC84417; MTBLC88368; MTBLC89231; MTBLC89212; MTBLC3441; MTBLC18430; MTBLC70069; MTBLC34322; MTBLC7868; MTBLC583; MTBLC2888; MTBLC3887; MTBLC4804; MTBLC39; MTBLC60025; MTBLC29457; MTBLC28364; MTBLC79531; MTBLC79820; MTBLC79590; MTBLC79957; MTBLC79761; MTBLC79913; MTBLC79540; MTBLC79701; MTBLC79417; MTBLC34183; MTBLC79526; MTBLC79705; MTBLC79558; MTBLC132927; MTBLC28987; MTBLC61330; MTBLC15417; MTBLC6039; MTBLC29615; MTBLC135283; MTBLC27436; MTBLC34849; MTBLC29653; MTBLC135282; MTBLC78258; MTBLC31946; MTBLC29660; MTBLC16179; MTBLC34980; MTBLC75342; MTBLC139131; MTBLC29744; MTBLC73676; MTBLC81253; MTBLC16325; MTBLC44526; MTBLC83063; MTBLC38394; MTBLC142447; MTBLC24993; MTBLC138083; MTBLC38362; MTBLC82749; MTBLC32798; MTBLC88464; MTBLC86141; MTBLC27939; MTBLC75108; MTBLC6673; MTBLC28801; MTBLC52639; MTBLC86455; MTBLC63598; MTBLC7731; MTBLC15843; MTBLC79754; MTBLC79694; MTBLC1182; MTBLC79480; MTBLC79869; MTBLC82835; MTBLC2451; MTBLC36033; MTBLC31825; MTBLC135293; MTBLC34834; MTBLC34838; MTBLC30041; MTBLC135233; MTBLC9738; MTBLC6389; MTBLC7454; MTBLC79582; MTBLC34530; MTBLC70708; MTBLC9234; MTBLC4724; MTBLC8411; MTBLC62439; MTBLC73358; MTBLC5613; MTBLC6414; MTBLC63607; MTBLC84701; MTBLC28727; MTBLC28194; MTBLC27997; MTBLC16196; MTBLC82617; MTBLC50575; MTBLC32375; MTBLC50464; MTBLC29735; MTBLC30829; MTBLC28193; MTBLC50572; MTBLC36023; MTBLC80539; MTBLC7954; MTBLC53486; MTBLC53460; MTBLC79878; MTBLC79900; MTBLC525464; MTBLC79409; MTBLC79578; MTBLC82832; MTBLC71589; MTBLC32023; MTBLC134218; MTBLC73000; MTBLC140861; MTBLC75026; MTBLC134231; MTBLC134232; MTBLC137779; MTBLC134229; MTBLC88935; MTBLC86119; MTBLC86121; MTBLC89734; MTBLC86117; MTBLC78022; MTBLC89691; MTBLC84831; MTBLC74670; MTBLC89599; MTBLC89597; MTBLC89548; MTBLC89438; MTBLC89078; MTBLC89127; MTBLC89177; MTBLC88712; MTBLC9916; MTBLC75092; MTBLC34262; MTBLC27951; MTBLC27797; MTBLC16713; MTBLC57999; MTBLC34454; MTBLC47220; MTBLC28967; MTBLC37144; MTBLC28960; MTBLC28905; MTBLC15368; MTBLC57841; MTBLC1217; MTBLC44692; MTBLC45285; MTBLC1467; MTBLC17214; MTBLC72700; MTBLC16119; MTBLC16199; MTBLC16607; MTBLC16610; MTBLC4614; MTBLC19092; MTBLC28638; MTBLC30322; MTBLC17203; MTBLC1439; MTBLC37600; MTBLC27371; MTBLC16070; MTBLC74863; MTBLC27411; MTBLC15866; MTBLC28847; MTBLC28140; MTBLC18287; MTBLC42606; MTBLC27907; MTBLC27442; MTBLC27586; MTBLC137774; MTBLC63150; MTBLC17617; MTBLC16935; MTBLC62345; MTBLC17897; MTBLC27708; MTBLC9652; MTBLC17059; MTBLC58286; MTBLC16357; MTBLC15971; MTBLC17064; MTBLC30818; MTBLC89640; MTBLC27248; MTBLC31042; MTBLC16572; MTBLC1580; MTBLC1879; MTBLC26797; MTBLC17578; MTBLC34213; MTBLC27869; MTBLC15767; MTBLC16089; MTBLC2319; MTBLC5966; MTBLC16380; MTBLC17143; MTBLC31173; MTBLC31278; MTBLC64977; MTBLC5320; MTBLC71166; MTBLC27480; MTBLC16355; MTBLC2600; MTBLC133351; MTBLC17881; MTBLC28928; MTBLC27616; MTBLC16100; MTBLC17641; MTBLC90886; MTBLC1139; MTBLC1387; MTBLC17095; MTBLC76163; MTBLC114204; MTBLC34252; MTBLC34256; MTBLC79445; MTBLC34876; MTBLC34877; MTBLC3007; MTBLC8986; MTBLC31054; MTBLC2932; MTBLC60078; MTBLC31435; MTBLC6945; MTBLC8616; MTBLC9183; MTBLC5959; MTBLC5708; MTBLC7468; MTBLC88104; MTBLC139134; MTBLC73926; MTBLC139133; MTBLC82679; MTBLC137760; MTBLC82678; MTBLC79877; MTBLC17747; MTBLC34710; MTBLC34679; MTBLC34097; MTBLC16323; MTBLC18385; MTBLC43997; MTBLC80424; MTBLC134287; MTBLC16929; MTBLC508; MTBLC60872; MTBLC70824; MTBLC68451; MTBLC16852; MTBLC134850; MTBLC9008; MTBLC16181; MTBLC28393; MTBLC28328; MTBLC47977; MTBLC62324; MTBLC24103; MTBLC31747; MTBLC28945; MTBLC31997; MTBLC19332; MTBLC16467; MTBLC10454; MTBLC5121; MTBLC5139; MTBLC5356; MTBLC5358; MTBLC69039; MTBLC93403; MTBLC63112; MTBLC16870; MTBLC17874; MTBLC28057; MTBLC28586; MTBLC62976; MTBLC62006; MTBLC17321; MTBLC3017; MTBLC51805; MTBLC2302; MTBLC2304; MTBLC136582; MTBLC17913; MTBLC3766; MTBLC79576; MTBLC38159; MTBLC25426; MTBLC16060; MTBLC3703; MTBLC27509; MTBLC4740; MTBLC6931; MTBLC7906; MTBLC5578; MTBLC59560; MTBLC15372; MTBLC80385; MTBLC952; MTBLC1141; MTBLC27852; MTBLC41941; MTBLC86553; MTBLC30816; MTBLC16388; MTBLC20415; MTBLC1881; MTBLC89830; MTBLC44747; MTBLC32807; MTBLC17151; MTBLC18403; MTBLC15963; MTBLC16207; MTBLC17597; MTBLC30746; MTBLC16008; MTBLC79966; MTBLC46807; MTBLC133314; MTBLC19891; MTBLC16138; MTBLC57653; MTBLC33917; MTBLC22357; MTBLC37690; MTBLC28061; MTBLC17925; MTBLC28729; MTBLC10295; MTBLC28645; MTBLC27667; MTBLC15903; MTBLC28994; MTBLC28563; MTBLC17393; MTBLC28385; MTBLC15824; MTBLC16824; MTBLC4139; MTBLC4167; MTBLC27611; MTBLC18004; MTBLC4194; MTBLC28014; MTBLC16024; MTBLC27605; MTBLC17317; MTBLC16443; MTBLC28458; MTBLC48095; MTBLC17234; MTBLC24978; MTBLC17357; MTBLC27987; MTBLC17268; MTBLC10642; MTBLC27922; MTBLC25858; MTBLC28946; MTBLC28177; MTBLC17605; MTBLC18280; MTBLC8240; MTBLC28354; MTBLC11424; MTBLC27806; MTBLC27816; MTBLC28816; MTBLC40274; MTBLC30156; MTBLC44842; MTBLC17807; MTBLC20106; MTBLC68329; MTBLC16899; MTBLC17924; MTBLC17505; MTBLC18202; MTBLC28789; MTBLC29864; MTBLC6259; MTBLC17656; MTBLC32800; MTBLC18414; MTBLC28478; MTBLC19868; MTBLC27978; MTBLC17445; MTBLC1581; MTBLC18346; MTBLC85239; MTBLC20414; MTBLC35164; MTBLC18101; MTBLC40813; MTBLC20450; MTBLC17637; MTBLC31835; MTBLC31832; MTBLC8075; MTBLC29672; MTBLC17702; MTBLC28889; MTBLC17631; MTBLC64835; MTBLC27603; MTBLC1683; MTBLC62974; MTBLC28087; MTBLC28460; MTBLC17164; MTBLC15354; MTBLC16182; MTBLC16638; MTBLC16133; MTBLC16472; MTBLC87755; MTBLC84069; MTBLC16019; MTBLC46941; MTBLC53608; MTBLC79569; MTBLC17243; MTBLC134341; MTBLC88427; MTBLC34687; MTBLC79053; MTBLC4316; MTBLC10607; MTBLC88526; MTBLC32337; MTBLC10525; MTBLC27801; MTBLC29732; MTBLC2959; MTBLC52859; MTBLC80420; MTBLC2818; MTBLC17929; MTBLC25682; MTBLC81297; MTBLC17417; MTBLC144066; MTBLC142578; MTBLC18037; MTBLC3210; MTBLC3474; MTBLC8613; MTBLC2247; MTBLC17311; MTBLC35619; MTBLC138425; MTBLC27971; MTBLC27389; MTBLC16865; MTBLC33094; MTBLC28797; MTBLC37081; MTBLC5588; MTBLC17724; MTBLC15620; MTBLC138669; MTBLC17519; MTBLC37581; MTBLC17217; MTBLC16413; MTBLC23500; MTBLC16583; MTBLC36253; MTBLC46916; MTBLC478164; MTBLC17765; MTBLC15754; MTBLC24168; MTBLC4728; MTBLC134255; MTBLC77131; MTBLC15643; MTBLC33098; MTBLC39931; MTBLC86390; MTBLC30753; MTBLC35227; MTBLC30754; MTBLC42682; MTBLC134761; MTBLC18123; MTBLC32114; MTBLC47564; MTBLC139; MTBLC16703; MTBLC531; MTBLC27380; MTBLC16885; MTBLC17332; MTBLC64833; MTBLC28782; MTBLC28793; MTBLC3528; MTBLC31005; MTBLC27680; MTBLC27649; MTBLC6364; MTBLC27931; MTBLC6731; MTBLC7912; MTBLC18154; MTBLC16634; MTBLC9859; MTBLC32059; MTBLC83804; MTBLC16546; MTBLC18428; MTBLC28102; MTBLC37165; MTBLC28808; MTBLC90185; MTBLC141517; MTBLC50663; MTBLC4954; MTBLC135681; MTBLC73275; MTBLC140748; MTBLC7982; MTBLC31576; MTBLC135209; MTBLC137782; MTBLC23875; MTBLC73892; MTBLC33020; MTBLC1230; MTBLC16551; MTBLC39244; MTBLC28676; MTBLC18260; MTBLC27554; MTBLC77436; MTBLC18167; MTBLC36217; MTBLC71422; MTBLC36218; MTBLC18147; MTBLC17057; MTBLC4125; MTBLC21010; MTBLC17306; MTBLC4808; MTBLC133330; MTBLC28066; MTBLC16751; MTBLC28189; MTBLC17716; MTBLC6359; MTBLC18411; MTBLC6435; MTBLC25164; MTBLC28053; MTBLC7570; MTBLC18394; MTBLC17992; MTBLC5105; MTBLC143968; MTBLC17705; MTBLC16708; MTBLC16347; MTBLC73707; MTBLC89341; MTBLC16817; MTBLC6907; MTBLC80354; MTBLC31085; MTBLC2089; MTBLC4055; MTBLC48294; MTBLC35090; MTBLC6415; MTBLC75627; MTBLC16246; MTBLC16772; MTBLC20582; MTBLC111; MTBLC18427; MTBLC28310; MTBLC18266; MTBLC15975; MTBLC28762; MTBLC28548; MTBLC43943; MTBLC17540; MTBLC320055; MTBLC27732; MTBLC126237; MTBLC36090; MTBLC137825; MTBLC36633; MTBLC28323; MTBLC28873; MTBLC58152; MTBLC23401; MTBLC32815; MTBLC30851; MTBLC18125; MTBLC47928; MTBLC32374; MTBLC18697; MTBLC882; MTBLC15980; MTBLC1416; MTBLC27778; MTBLC59052; MTBLC25351; MTBLC6933; MTBLC15607; MTBLC52222; MTBLC36458; MTBLC30835; MTBLC36455; MTBLC25311; MTBLC30314; MTBLC5958; MTBLC29717; MTBLC27645; MTBLC30906; MTBLC30940; MTBLC29722; MTBLC28176; MTBLC29724; MTBLC15798; MTBLC77671; MTBLC18128; MTBLC16590; MTBLC3693; MTBLC17989; MTBLC4853; MTBLC139533; MTBLC17618; MTBLC4117; MTBLC82348; MTBLC5673; MTBLC64305; MTBLC3337; MTBLC138529; MTBLC15567; MTBLC17275; MTBLC4607; MTBLC87897; MTBLC37331; MTBLC16939; MTBLC44303; MTBLC82573; MTBLC134821; MTBLC16795; MTBLC17895; MTBLC89461; MTBLC134820; MTBLC34019; MTBLC74516; MTBLC2628; MTBLC3244; MTBLC28709; MTBLC5989; MTBLC7502; MTBLC3546; MTBLC137728; MTBLC27468; MTBLC27578; MTBLC28474; MTBLC16364; MTBLC17681; MTBLC29053; MTBLC28630; MTBLC36751; MTBLC52143; MTBLC62768; MTBLC62770; MTBLC27747; MTBLC28229; MTBLC139383; MTBLC17115; MTBLC29480; MTBLC17960; MTBLC32816; MTBLC6604; MTBLC34867; MTBLC2196; MTBLC39564; MTBLC94764; MTBLC139388; MTBLC74076; MTBLC73580; MTBLC6257; MTBLC28346; MTBLC6792; MTBLC6839; MTBLC18106; MTBLC17286; MTBLC87407; MTBLC4683; MTBLC7797; MTBLC10044; MTBLC3697; MTBLC6765; MTBLC31030; MTBLC28462; MTBLC5792; MTBLC5979; MTBLC31827; MTBLC109895; MTBLC1927; MTBLC46295; MTBLC16009; MTBLC16335; MTBLC17172; MTBLC24088; MTBLC10110; MTBLC8674; MTBLC90721; MTBLC32; MTBLC134766; MTBLC135744; MTBLC63616; MTBLC5384; MTBLC79587; MTBLC44616; MTBLC34731; MTBLC2376; MTBLC64020; MTBLC4071; MTBLC3748; MTBLC23359; MTBLC50540; MTBLC16512; MTBLC6739; MTBLC137234; MTBLC27441; MTBLC28309; MTBLC19065; MTBLC70971; MTBLC16299; MTBLC490877; MTBLC37754; MTBLC27748; MTBLC6520; MTBLC107635; MTBLC84500; MTBLC15781; MTBLC81545; MTBLC81546; MTBLC27478; MTBLC29012; MTBLC9200; MTBLC8245; MTBLC9173; MTBLC32322; MTBLC31311; MTBLC171741; MTBLC92675; MTBLC138493; MTBLC74112; MTBLC61138; MTBLC37079; MTBLC33033; MTBLC16530; MTBLC27401; MTBLC39153; MTBLC45630; MTBLC38531; MTBLC8882; MTBLC6521; MTBLC50973; MTBLC8774; MTBLC137248; MTBLC2819; MTBLC27713; MTBLC19450; MTBLC17645; MTBLC58183; MTBLC17027; MTBLC70979; MTBLC17917; MTBLC724125; MTBLC89963; MTBLC28998; MTBLC1142; MTBLC18395; MTBLC16370; MTBLC15847; MTBLC57541; MTBLC71429; MTBLC88455; MTBLC42654; MTBLC17596; MTBLC17901; MTBLC87248; MTBLC9447; MTBLC28715; MTBLC21412; MTBLC143078; MTBLC8665; MTBLC55344; MTBLC37755; MTBLC15887; MTBLC17750; MTBLC58441; MTBLC18314; MTBLC16414; MTBLC138668; MTBLC77042; MTBLC134261; MTBLC41139; MTBLC2540; MTBLC10226; MTBLC10364; MTBLC3900; MTBLC4817; MTBLC5177; MTBLC5379; MTBLC5981; MTBLC6070; MTBLC8216; MTBLC73719; MTBLC50178; MTBLC135187; MTBLC17144; MTBLC6407; MTBLC73880; MTBLC79449; MTBLC7575; MTBLC11946; MTBLC3926; MTBLC35280; MTBLC29565; MTBLC15565; MTBLC16856; MTBLC32153; MTBLC6413; MTBLC8426; MTBLC80592; MTBLC51032; MTBLC28598; MTBLC17799; MTBLC57630; MTBLC28718; MTBLC15699; MTBLC16857; MTBLC62413; MTBLC16256; MTBLC30831; MTBLC137232; MTBLC15344; MTBLC51850; MTBLC16265; MTBLC28867; MTBLC18261; MTBLC17201; MTBLC17196; MTBLC15737; MTBLC29045; MTBLC16770; MTBLC17374; MTBLC28376; MTBLC2165; MTBLC29637; MTBLC61511; MTBLC39501; MTBLC32069; MTBLC6874; MTBLC5044; MTBLC37628; MTBLC64366; MTBLC17053; MTBLC29990; MTBLC5159; MTBLC18012; MTBLC18300; MTBLC17257; MTBLC135747; MTBLC31785; MTBLC10556; MTBLC5511; MTBLC5534; MTBLC2532; MTBLC2821; MTBLC3287; MTBLC6511; MTBLC1670; MTBLC73757; MTBLC21305; MTBLC18050; MTBLC16352; MTBLC37011; MTBLC16010; MTBLC94613; MTBLC6151; MTBLC139123; MTBLC1241; MTBLC28791; MTBLC62637; MTBLC16015; MTBLC58724; MTBLC16439; MTBLC45441; MTBLC31882; MTBLC17981; MTBLC36461; MTBLC17415; MTBLC17626; MTBLC17204; MTBLC2424; MTBLC15670; MTBLC30838; MTBLC16600; MTBLC51330; MTBLC75984; MTBLC3734; MTBLC7856; MTBLC9196; MTBLC7959; MTBLC16643; MTBLC50868; MTBLC9384; MTBLC15604; MTBLC89185; MTBLC57826; MTBLC28825; MTBLC18347; MTBLC17191; MTBLC15603; MTBLC64348; MTBLC17878; MTBLC17611; MTBLC17915; MTBLC85235; MTBLC38355; MTBLC49283; MTBLC143856; MTBLC61206; MTBLC79634; MTBLC79456; MTBLC79768; MTBLC79876; MTBLC34930; MTBLC6536; MTBLC17472; MTBLC73740; MTBLC7034; MTBLC5158; MTBLC30845; MTBLC30846; MTBLC74104; MTBLC19274; MTBLC85162; MTBLC23757; MTBLC5826; MTBLC62069; MTBLC223316; MTBLC44934; MTBLC10018; MTBLC135072; MTBLC34405; MTBLC34788; MTBLC31268; MTBLC34756; MTBLC3391; MTBLC53490; MTBLC5847; MTBLC5597; MTBLC79439; MTBLC34619; MTBLC135714; MTBLC7807; MTBLC78549; MTBLC1957; MTBLC20013; MTBLC40521; MTBLC31111; MTBLC34522; MTBLC16079; MTBLC37287; MTBLC37291; MTBLC29064; MTBLC2128; MTBLC9212; MTBLC53763; MTBLC86455; MTBLC45652; MTBLC30449; MTBLC34291; MTBLC17397; MTBLC24814; MTBLC74018; MTBLC52172; MTBLC28682; MTBLC66876; MTBLC9741; MTBLC5515; MTBLC47899; MTBLC8397; MTBLC695; MTBLC9403; MTBLC34307; MTBLC3767; MTBLC68428; MTBLC27527; MTBLC27588; MTBLC29573; MTBLC7599; MTBLC61645; MTBLC79626; MTBLC79729; MTBLC134923; MTBLC16043; MTBLC5457; MTBLC34048; MTBLC48541; MTBLC137772; MTBLC16547; MTBLC9957; MTBLC10366; MTBLC10423; MTBLC15582; MTBLC15583; MTBLC57424; MTBLC49076; MTBLC18104; MTBLC18078; MTBLC17023; MTBLC27861; MTBLC27550; MTBLC15591; MTBLC16831; MTBLC89205; MTBLC138367; MTBLC28381; MTBLC59051; MTBLC30997; MTBLC6452; MTBLC17937; MTBLC62112; MTBLC3207; MTBLC66913; MTBLC50131; MTBLC31989; MTBLC8097; MTBLC2705; MTBLC137310; MTBLC28502; MTBLC16765; MTBLC31993; MTBLC3085; MTBLC59020; MTBLC28948; MTBLC28136; MTBLC132335; MTBLC31584; MTBLC31952; MTBLC3112; MTBLC15676; MTBLC21860; MTBLC79347; MTBLC68606; MTBLC610092; MTBLC139380; MTBLC34598; MTBLC80544; MTBLC23812; MTBLC58056; MTBLC87166; MTBLC37245; MTBLC35460; MTBLC16093; MTBLC16558; MTBLC28568; MTBLC218; MTBLC18297; MTBLC2559; MTBLC17973; MTBLC27818; MTBLC17665; MTBLC57734; MTBLC12350; MTBLC16084; MTBLC57684; MTBLC58247; MTBLC58328; MTBLC27973; MTBLC78736; MTBLC78697; MTBLC37480; MTBLC12937; MTBLC16077; MTBLC14314; MTBLC57828; MTBLC16588; MTBLC35374; MTBLC17369; MTBLC138150; MTBLC17837; MTBLC78737; MTBLC24588; MTBLC25448; MTBLC80181; MTBLC84141; MTBLC137409; MTBLC28173; MTBLC18365; MTBLC28992; MTBLC1369; MTBLC67375; MTBLC2373; MTBLC17488; MTBLC59353; MTBLC43468; MTBLC35128; MTBLC28652; MTBLC35121; MTBLC28635; MTBLC30850; MTBLC8809; MTBLC69440; MTBLC4910; MTBLC27429; MTBLC32506; MTBLC79659; MTBLC45980; MTBLC6375; MTBLC3534; MTBLC4997; MTBLC73873; MTBLC9735; MTBLC16927; MTBLC31657; MTBLC135111; MTBLC136292; MTBLC6758; MTBLC16734; MTBLC102524; MTBLC134922; MTBLC17409; MTBLC133172; MTBLC132983; MTBLC78951; MTBLC16445; MTBLC151; MTBLC160; MTBLC15622; MTBLC35453; MTBLC18281; MTBLC17305; MTBLC41893; MTBLC42819; MTBLC57992; MTBLC30769; MTBLC30887; MTBLC30915; MTBLC17803; MTBLC6885; MTBLC57927; MTBLC4488; MTBLC27837; MTBLC86556; MTBLC84058; MTBLC3805; MTBLC4520; MTBLC73026; MTBLC73025; MTBLC34923; MTBLC64; MTBLC4628; MTBLC31585; MTBLC76160; MTBLC31981; MTBLC17802; MTBLC16704; MTBLC73715; MTBLC70353; MTBLC34698; MTBLC70453; MTBLC134913; MTBLC90038; MTBLC86004; MTBLC9274; MTBLC9275; MTBLC89730; MTBLC11222; MTBLC34447; MTBLC31402; MTBLC4895; MTBLC6347; MTBLC35796; MTBLC137768; MTBLC3158; MTBLC29513; MTBLC58556; MTBLC17533; MTBLC36554; MTBLC28249; MTBLC1162; MTBLC1243; MTBLC87507; MTBLC48061; MTBLC30918; MTBLC16630; MTBLC17902; MTBLC17568; MTBLC28942; MTBLC22099; MTBLC13497; MTBLC32275; MTBLC135817; MTBLC49026; MTBLC17012; MTBLC28879; MTBLC91807; MTBLC15809; MTBLC6381; MTBLC9605; MTBLC79471; MTBLC79566; MTBLC6851; MTBLC38546; MTBLC10561; MTBLC58800; MTBLC3146; MTBLC49260; MTBLC144027; MTBLC27574; MTBLC58767; MTBLC49004; MTBLC9308; MTBLC27407; MTBLC40304; MTBLC3927; MTBLC16750; MTBLC27427; MTBLC17643; MTBLC31552; MTBLC43755; MTBLC3088; MTBLC50271; MTBLC69499; MTBLC4994; MTBLC6008; MTBLC7161; MTBLC94381; MTBLC116; MTBLC4962; MTBLC29474; MTBLC17693; MTBLC16409; MTBLC17405; MTBLC2085; MTBLC34334; MTBLC20367; MTBLC28719; MTBLC137246; MTBLC29069; MTBLC30801; MTBLC29009; MTBLC74321; MTBLC2685; MTBLC3082; MTBLC135310; MTBLC116735; MTBLC17295; MTBLC46209; MTBLC28438; MTBLC28170; MTBLC28353; MTBLC16151; MTBLC35697; MTBLC4888; MTBLC134865; MTBLC5862; MTBLC16828; MTBLC79441; MTBLC9935; MTBLC9962; MTBLC135165; MTBLC3845; MTBLC135386; MTBLC15637; MTBLC63606; MTBLC45981; MTBLC8772; MTBLC4708; MTBLC9259; MTBLC51141; MTBLC17509; MTBLC53727; MTBLC32162; MTBLC102516; MTBLC32164; MTBLC9593; MTBLC7209; MTBLC24479; MTBLC4822; MTBLC6617; MTBLC4724; MTBLC10026; MTBLC35028; MTBLC10022; MTBLC69088; MTBLC17501; MTBLC28523; MTBLC89486; MTBLC2108; MTBLC2336; MTBLC4774; MTBLC34712; MTBLC60069; MTBLC6891; MTBLC16389; MTBLC8418; MTBLC8419; MTBLC18082; MTBLC28334; MTBLC88677; MTBLC15490; MTBLC34041; MTBLC60076; MTBLC16305; MTBLC31682; MTBLC73970; MTBLC3695; MTBLC132058; MTBLC74533; MTBLC137196; MTBLC2978; MTBLC80227; MTBLC34087; MTBLC89521; MTBLC86095; MTBLC88906; MTBLC89602; MTBLC89539; MTBLC89536; MTBLC73739; MTBLC75145; MTBLC64356; MTBLC86544; MTBLC29564; MTBLC31447; MTBLC4512; MTBLC6001; MTBLC32771; MTBLC37108; MTBLC29019; MTBLC86618; MTBLC82864; MTBLC135383; MTBLC4682; MTBLC76258; MTBLC135151; MTBLC36665; MTBLC18094; MTBLC4718; MTBLC9239; MTBLC25357; MTBLC27504; MTBLC2699; MTBLC8837; MTBLC9198; MTBLC9524; MTBLC9601; MTBLC9770; MTBLC9969; MTBLC2697; MTBLC2722; MTBLC6080; MTBLC8822; MTBLC52070; MTBLC9912; MTBLC8247; MTBLC32003; MTBLC10329; MTBLC135757; MTBLC42; MTBLC6066; MTBLC7458; MTBLC9519; MTBLC4856; MTBLC9120; MTBLC79434; MTBLC16684; MTBLC6140; MTBLC58164; MTBLC6506; MTBLC31789; MTBLC6778; MTBLC79600; MTBLC137783; MTBLC51211; MTBLC135016; MTBLC6535; MTBLC5990; MTBLC3094; MTBLC16112; MTBLC16065; MTBLC16952; MTBLC74725; MTBLC16475; MTBLC28155; MTBLC4732; MTBLC79423; MTBLC79564; MTBLC9291; MTBLC62431; MTBLC2365; MTBLC22152; MTBLC2620; MTBLC2851; MTBLC2870; MTBLC2982; MTBLC3574; MTBLC3888; MTBLC5095; MTBLC5281; MTBLC5536; MTBLC5727; MTBLC5867; MTBLC6560; MTBLC6921; MTBLC8115; MTBLC8267; MTBLC8268; MTBLC8856; MTBLC9013; MTBLC9956; MTBLC10024; MTBLC79890; MTBLC6863; MTBLC29612; MTBLC93369; MTBLC30805; MTBLC140088; MTBLC74966; MTBLC43966; MTBLC85252; MTBLC63924; MTBLC4973; MTBLC6419; MTBLC16725; MTBLC27769; MTBLC86068; MTBLC2404; MTBLC133419; MTBLC10070; MTBLC93847; MTBLC28708; MTBLC29458; MTBLC15830; MTBLC134834; MTBLC34769; MTBLC139312; MTBLC3061; MTBLC10099; MTBLC6738; MTBLC3005; MTBLC135349; MTBLC92338; MTBLC7789; MTBLC7640; MTBLC8597; MTBLC93626; MTBLC28865; MTBLC38258; MTBLC5859; MTBLC8021; MTBLC636; MTBLC67547; MTBLC137192; MTBLC88935; MTBLC86119; MTBLC86121; MTBLC89734; MTBLC86117; MTBLC78022; MTBLC89691; MTBLC84831; MTBLC74670; MTBLC89599; MTBLC89597; MTBLC89548; MTBLC89438; MTBLC89078; MTBLC89127; MTBLC89177; MTBLC88712; MTBLC21484; MTBLC15874; MTBLC17976; MTBLC5093; MTBLC63630; MTBLC2294; MTBLC2425; MTBLC16363; MTBLC2629; MTBLC69335; MTBLC28356; MTBLC4441; MTBLC135002; MTBLC10058; MTBLC10076; MTBLC10103; MTBLC28714; MTBLC43415; MTBLC5855; MTBLC28325; MTBLC74405; MTBLC3300; MTBLC9515; MTBLC41509; MTBLC2156; MTBLC2368; MTBLC9439; MTBLC74274; MTBLC8386; MTBLC18278; MTBLC27993; MTBLC82684; MTBLC9997; MTBLC80033; MTBLC29527; MTBLC29536; MTBLC135701; MTBLC16778; MTBLC18330; MTBLC4783; MTBLC27514; MTBLC5304; MTBLC31967; MTBLC16954; MTBLC8028; MTBLC133473; MTBLC29043; MTBLC38266; MTBLC80494; MTBLC72609; MTBLC62881; MTBLC135932; MTBLC9943; MTBLC58552; MTBLC42797; MTBLC31871; MTBLC82763; MTBLC31922; MTBLC135703; MTBLC64210; MTBLC135483; MTBLC32181; MTBLC474014; MTBLC3825; MTBLC34668; MTBLC7736; MTBLC17713; MTBLC10037; MTBLC8922; MTBLC7471; MTBLC31563; MTBLC3740; MTBLC4320; MTBLC24293; MTBLC80538; MTBLC79465; MTBLC4773; MTBLC5527; MTBLC9959; MTBLC131852; MTBLC9665; MTBLC473990; MTBLC17433; MTBLC80393; MTBLC3162; MTBLC5970; MTBLC44492; MTBLC79394; MTBLC15430; MTBLC57306; MTBLC2341; MTBLC34163; MTBLC31561; MTBLC135525; MTBLC8039; MTBLC79655; MTBLC79502; MTBLC34461; MTBLC79892; MTBLC34353; MTBLC34355; MTBLC79657; MTBLC17457; MTBLC4453; MTBLC9261; MTBLC79432; MTBLC79620; MTBLC29510; MTBLC52075; MTBLC15416; MTBLC31578; MTBLC52484; MTBLC29611; MTBLC52482; MTBLC29654; MTBLC81594; MTBLC30038; MTBLC31896; MTBLC9108; MTBLC9946; MTBLC847; MTBLC9205; MTBLC15735; MTBLC3745; MTBLC82461; MTBLC27796; MTBLC34580; MTBLC6147; MTBLC135451; MTBLC2565; MTBLC4038; MTBLC28833; MTBLC29592; MTBLC29594; MTBLC29602; MTBLC5606; MTBLC6962; MTBLC8330; MTBLC9042; MTBLC9290; MTBLC2534; MTBLC799; MTBLC34139; MTBLC79668; MTBLC79797; MTBLC136980; MTBLC1189; MTBLC136972; MTBLC79907; MTBLC63641; MTBLC79715; MTBLC2495; MTBLC79887; MTBLC9460; MTBLC17078; MTBLC141472; MTBLC28192; MTBLC135231; MTBLC79496; MTBLC79601; MTBLC5887; MTBLC59788; MTBLC31086; MTBLC2626; MTBLC8402; MTBLC32185; MTBLC4417; MTBLC31298; MTBLC31497; MTBLC8713; MTBLC31459; MTBLC113542; MTBLC40070; MTBLC27510; MTBLC17148; MTBLC716; MTBLC2327; MTBLC2544; MTBLC3614; MTBLC89837; MTBLC89829; MTBLC89824; MTBLC90028; MTBLC90034; MTBLC90021; MTBLC77677; MTBLC88798; MTBLC88446; MTBLC41847; MTBLC89028; MTBLC90068; MTBLC64793; MTBLC84266; MTBLC5674; MTBLC142272; MTBLC2939; MTBLC6798; MTBLC1749; MTBLC8602; MTBLC17467; MTBLC34605; MTBLC9425; MTBLC2725; MTBLC9923; MTBLC73; MTBLC30725; MTBLC34968; MTBLC31753; MTBLC2934; MTBLC7948; MTBLC86251; MTBLC30248; MTBLC34227; MTBLC142243; MTBLC136795; MTBLC2504; MTBLC3081; MTBLC16188; MTBLC16011; MTBLC85158; MTBLC79925; MTBLC79522; MTBLC34175; MTBLC79455; MTBLC80656; MTBLC79735; MTBLC135981; MTBLC6085; MTBLC49191; MTBLC9419; MTBLC89642; MTBLC16374; MTBLC10136; MTBLC4778; MTBLC8196; MTBLC28794; MTBLC90355; MTBLC79553; MTBLC28090; MTBLC2197; MTBLC3163; MTBLC28436; MTBLC5837; MTBLC6006; MTBLC75092; MTBLC16243; MTBLC8876; MTBLC507499; MTBLC204; MTBLC214; MTBLC241; MTBLC242; MTBLC78668; MTBLC138752; MTBLC17130; MTBLC34301; MTBLC37157; MTBLC78853; MTBLC61024; MTBLC8607; MTBLC4389; MTBLC5528; MTBLC89343; MTBLC89314; MTBLC89088; MTBLC89075; MTBLC89076; MTBLC89371; MTBLC89333; MTBLC89334; MTBLC89311; MTBLC89316; MTBLC138499; MTBLC18227; MTBLC94661; MTBLC36108; MTBLC80383; MTBLC8273; MTBLC8773; MTBLC31049; MTBLC18393; MTBLC137750; MTBLC17224; MTBLC5679; MTBLC18127; MTBLC17166; MTBLC28091; MTBLC36466; MTBLC36106; MTBLC4366; MTBLC28869; MTBLC28925; MTBLC9185; MTBLC9188; MTBLC86162; MTBLC88930; MTBLC88929; MTBLC89739; MTBLC89576; MTBLC89557; MTBLC89559; MTBLC89441; MTBLC86161; MTBLC89419; MTBLC88925; MTBLC88841; MTBLC88430; MTBLC88654; MTBLC10219; MTBLC86344; MTBLC84549; MTBLC84837; MTBLC78268; MTBLC7492; MTBLC91712; MTBLC4974; MTBLC4572; MTBLC6414; MTBLC81785; MTBLC135138; MTBLC60656; MTBLC16312; MTBLC16390; MTBLC138401; MTBLC88108; MTBLC2812; MTBLC79833; MTBLC47818; MTBLC79918; MTBLC34838; MTBLC31523; MTBLC138422; MTBLC47214; MTBLC28818; MTBLC32176; MTBLC15578; MTBLC89324; MTBLC89079; MTBLC19290; MTBLC79996; MTBLC28477; MTBLC81013; MTBLC17823; MTBLC86378; MTBLC7931; MTBLC28933; MTBLC9595; MTBLC34667; MTBLC31648; MTBLC4819; MTBLC32645; MTBLC8764; MTBLC4921; MTBLC9165; MTBLC31857; MTBLC31174; MTBLC34831; MTBLC31894; MTBLC9316; MTBLC27617; MTBLC80461; MTBLC80167; MTBLC1107; MTBLC82949; MTBLC88480; MTBLC88479; MTBLC88547; MTBLC89218; MTBLC89203; MTBLC89202; MTBLC89162; MTBLC89160; MTBLC89238; MTBLC89237; MTBLC88966; MTBLC89040; MTBLC89780; MTBLC89784; MTBLC89799; MTBLC89797; MTBLC89684; MTBLC89669; MTBLC89670; MTBLC89671; MTBLC89433; MTBLC89322; MTBLC89337; MTBLC136371; MTBLC64396; MTBLC88779; MTBLC28517; MTBLC18171; MTBLC32086; MTBLC5206; MTBLC15575; MTBLC2513; MTBLC50749; MTBLC31893; MTBLC9463; MTBLC15574; MTBLC90980; MTBLC47812; MTBLC80533; MTBLC3863; MTBLC5633; MTBLC8913; MTBLC6145; MTBLC64668; MTBLC7800; MTBLC9039; MTBLC8621; MTBLC80017; MTBLC34042; MTBLC7752; MTBLC28285; MTBLC18010; MTBLC3719; MTBLC5718; MTBLC6674; MTBLC59979; MTBLC34499; MTBLC34503; MTBLC34506; MTBLC91217; MTBLC138082; MTBLC15658; MTBLC15655; MTBLC15657; MTBLC64008; MTBLC138786; MTBLC88461; MTBLC34148; MTBLC91272; MTBLC34485; MTBLC34498; MTBLC34500; MTBLC88440; MTBLC34504; MTBLC143972; MTBLC88465; MTBLC89257; MTBLC3403; MTBLC3898; MTBLC79904; MTBLC34352; MTBLC1689; MTBLC89328; MTBLC79870; MTBLC9481; MTBLC93; MTBLC1941; MTBLC8603; MTBLC134767; MTBLC74562; MTBLC61725; MTBLC142079; MTBLC16310; MTBLC42471; MTBLC7567; MTBLC16147; MTBLC85232; MTBLC90230; MTBLC133979; MTBLC137172; MTBLC85166; MTBLC133325; MTBLC135350; MTBLC545687; MTBLC7496; MTBLC34322; MTBLC79177; MTBLC84854; MTBLC34295; MTBLC29479; MTBLC17903; MTBLC4045; MTBLC10445; MTBLC6706; MTBLC79519; MTBLC34293; MTBLC34294; MTBLC135489; MTBLC9238; MTBLC137712; MTBLC19143; MTBLC18446; MTBLC8648; MTBLC19144; MTBLC49265; MTBLC15654; MTBLC88462; MTBLC80442; MTBLC84441; MTBLC72641; MTBLC136531; MTBLC72815; MTBLC80463; MTBLC76234; MTBLC34491; MTBLC88441; MTBLC80447; MTBLC88438; MTBLC72843; MTBLC72842; MTBLC88460; MTBLC60956; MTBLC133329; MTBLC80413; MTBLC63067; MTBLC18230; MTBLC65247; MTBLC3705; MTBLC31352; MTBLC76334; MTBLC9510; MTBLC3128; MTBLC61726; MTBLC89365; MTBLC89339; MTBLC89342; MTBLC89318; MTBLC89313; MTBLC60273; MTBLC65211; MTBLC138212; MTBLC78700; MTBLC55523; MTBLC27706; MTBLC38299; MTBLC137495; MTBLC34154; MTBLC72639; MTBLC133357; MTBLC34494; MTBLC78730; MTBLC34496; MTBLC72651; MTBLC131659; MTBLC5833; MTBLC73074; MTBLC2366; MTBLC1019; MTBLC88696; MTBLC52897; MTBLC79575; MTBLC135210; MTBLC132495; MTBLC73751; MTBLC34828; MTBLC88667; MTBLC9778; MTBLC28919; MTBLC10088; MTBLC69081; MTBLC75542; MTBLC95216; MTBLC134424; MTBLC134423; MTBLC29627; MTBLC10120; MTBLC34034; MTBLC34443; MTBLC40131; MTBLC4918; MTBLC14469; MTBLC2492; MTBLC5166; MTBLC88808; MTBLC88807; MTBLC88782; MTBLC89214; MTBLC89189; MTBLC89149; MTBLC1418; MTBLC27867; MTBLC80419; MTBLC3375; MTBLC5087; MTBLC27448; MTBLC80177; MTBLC19793; MTBLC28485; MTBLC88765; MTBLC28810; MTBLC32157; MTBLC31279; MTBLC7720; MTBLC73728; MTBLC133875; MTBLC34920; MTBLC6088; MTBLC137139; MTBLC138782; MTBLC34652; MTBLC34680; MTBLC33913; MTBLC75219; MTBLC133456; MTBLC88698; MTBLC88697; MTBLC79838; MTBLC50106; MTBLC34229; MTBLC138081; MTBLC38833; MTBLC22469; MTBLC28093; MTBLC15405; MTBLC17580; MTBLC36503; MTBLC15393; MTBLC36492; MTBLC98; MTBLC31; MTBLC60; MTBLC61; MTBLC149; MTBLC150; MTBLC152; MTBLC153; MTBLC50232; MTBLC158; MTBLC50233; MTBLC50235; MTBLC300; MTBLC299; MTBLC368; MTBLC27961; MTBLC61727; MTBLC47856; MTBLC17447; MTBLC29452; MTBLC28071; MTBLC692; MTBLC35002; MTBLC9602; MTBLC137135; MTBLC34537; MTBLC79794; MTBLC79879; MTBLC28125; MTBLC79767; MTBLC79635; MTBLC34476; MTBLC79801; MTBLC135402; MTBLC32095; MTBLC79581; MTBLC76937; MTBLC39567; MTBLC36206; MTBLC36214; MTBLC85510; MTBLC36211; MTBLC7989; MTBLC79096; MTBLC75103; MTBLC32411; MTBLC138778; MTBLC36412; MTBLC86135; MTBLC142250; MTBLC86506; MTBLC32409; MTBLC32389; MTBLC37810; MTBLC2905; MTBLC135532; MTBLC79179; MTBLC84855; MTBLC80050; MTBLC48635; MTBLC5644; MTBLC63916; MTBLC79523; MTBLC79689; MTBLC80001; MTBLC52421; MTBLC448; MTBLC72665; MTBLC138258; MTBLC138255; MTBLC72663; MTBLC133381; MTBLC133086; MTBLC131762; MTBLC73882; MTBLC84067; MTBLC86403; MTBLC31850; MTBLC132479; MTBLC92833; MTBLC34370; MTBLC135041; MTBLC134981; MTBLC31547; MTBLC79883; MTBLC79939; MTBLC6645; MTBLC57905; MTBLC84094; MTBLC116278; MTBLC9232; MTBLC28661; MTBLC10275; MTBLC27432; MTBLC44602; MTBLC79716; MTBLC86136; MTBLC86148; MTBLC38384; MTBLC16423; MTBLC61676; MTBLC8638; MTBLC88809; MTBLC75465; MTBLC88786; MTBLC84394; MTBLC88471; MTBLC88536; MTBLC88367; MTBLC75446; MTBLC138077; MTBLC28627; MTBLC80415; MTBLC88796; MTBLC88725; MTBLC82927; MTBLC88501; MTBLC88500; MTBLC88364; MTBLC89229; MTBLC89211; MTBLC88942; MTBLC89034; MTBLC89029; MTBLC50585; MTBLC138489; MTBLC31571; MTBLC45571; MTBLC31725; MTBLC144339; MTBLC9194; MTBLC89605; MTBLC15843; MTBLC79754; MTBLC79694; MTBLC1182; MTBLC79480; MTBLC79869; MTBLC82835; MTBLC2451; MTBLC36033; MTBLC31825; MTBLC135293; MTBLC34834; MTBLC30041; MTBLC10419; MTBLC3425; MTBLC8996; MTBLC6991; MTBLC32345; MTBLC137651; MTBLC641; MTBLC1784; MTBLC4640; MTBLC72800; MTBLC20096; MTBLC72758; MTBLC73889; MTBLC3456; MTBLC9242; MTBLC44526; MTBLC83063; MTBLC38394; MTBLC142447; MTBLC24993; MTBLC138083; MTBLC38362; MTBLC82749; MTBLC32798; MTBLC88464; MTBLC86141; MTBLC27939; MTBLC75108; MTBLC6673; MTBLC28801; MTBLC84299; MTBLC4650; MTBLC58303; MTBLC46979; MTBLC136623; MTBLC46859; MTBLC83058; MTBLC9189; MTBLC86570; MTBLC31542; MTBLC89519; MTBLC85028; MTBLC74971; MTBLC4021; MTBLC48923; MTBLC64483; MTBLC131738; MTBLC64489; MTBLC78103; MTBLC63959; MTBLC31000; MTBLC75454; MTBLC75536; MTBLC31831; MTBLC75565; MTBLC137215; MTBLC135498; MTBLC3961; MTBLC71025; MTBLC73792; MTBLC137845; MTBLC9011; MTBLC33276; MTBLC80541; MTBLC137134; MTBLC47805; MTBLC79517; MTBLC4629; MTBLC31826; MTBLC10086; MTBLC64124; MTBLC46961; MTBLC15913; MTBLC18129; MTBLC79182; MTBLC143095; MTBLC85208; MTBLC136406; MTBLC50578; MTBLC136819; MTBLC136638; MTBLC74789; MTBLC79951; MTBLC5382; MTBLC69833; MTBLC80540; MTBLC3450; MTBLC37779; MTBLC37537; MTBLC49254; MTBLC28724; MTBLC136767; MTBLC85633; MTBLC34004; MTBLC85639; MTBLC45478; MTBLC79312; MTBLC30820; MTBLC50576; MTBLC138260; MTBLC82464; MTBLC28592; MTBLC84874; MTBLC70850; MTBLC85057; MTBLC32365; MTBLC90027; MTBLC3433; MTBLC9184; MTBLC74330; MTBLC62834; MTBLC77492; MTBLC73741; MTBLC79501; MTBLC34464; MTBLC11152; MTBLC29644; MTBLC84519; MTBLC34726; MTBLC133741; MTBLC46703; MTBLC73829; MTBLC34402; MTBLC137126; MTBLC81246; MTBLC67061; MTBLC73851; MTBLC84752; MTBLC79723; MTBLC33216; MTBLC6689; MTBLC7443; MTBLC79824; MTBLC135488; MTBLC88790; MTBLC77096; MTBLC88474; MTBLC88495; MTBLC88490; MTBLC88520; MTBLC88371; MTBLC88395; MTBLC89225; MTBLC75475; MTBLC77127; MTBLC89169; MTBLC89168; MTBLC89260; MTBLC75578; MTBLC88989; MTBLC89046; MTBLC89795; MTBLC89682; MTBLC89665; MTBLC89811; MTBLC80207; MTBLC131692; MTBLC17862; MTBLC71464; MTBLC16393; MTBLC28727; MTBLC28194; MTBLC27997; MTBLC16196; MTBLC82617; MTBLC50575; MTBLC32375; MTBLC50464; MTBLC29735; MTBLC30829; MTBLC28193; MTBLC50572; MTBLC36023; MTBLC35517; MTBLC79612; MTBLC18054; MTBLC3430; MTBLC6965; MTBLC82985; MTBLC10087; MTBLC9916; MTBLC35464; MTBLC142241; MTBLC28716; MTBLC35465; MTBLC76244; MTBLC37252; MTBLC76090; MTBLC9199; MTBLC9951; MTBLC77148; MTBLC58206; MTBLC31872; MTBLC3944; MTBLC5933; MTBLC72828; MTBLC72952; MTBLC27620; MTBLC91006; MTBLC67309; MTBLC3940; MTBLC7909; MTBLC79407; MTBLC79791; MTBLC79792; MTBLC66666; MTBLC135355; MTBLC88112; MTBLC135566; MTBLC79513; MTBLC73092; MTBLC31501; MTBLC88109; MTBLC31297; MTBLC28941; MTBLC84901; MTBLC28733; MTBLC6144; MTBLC75612; MTBLC52392; MTBLC3427; MTBLC137833; MTBLC16566; MTBLC84896; MTBLC28842; MTBLC88686; MTBLC29702; MTBLC34478; MTBLC137844; MTBLC53154; MTBLC72736; MTBLC133144; MTBLC75036; MTBLC131924; MTBLC8416; MTBLC9190; MTBLC18318; MTBLC86422; MTBLC89413; MTBLC89431; MTBLC89391; MTBLC89140; MTBLC89196; MTBLC89294; MTBLC88904; MTBLC88905; MTBLC88760; MTBLC88761; MTBLC88731; MTBLC88729; MTBLC88871; MTBLC88869; MTBLC88587; MTBLC89500; MTBLC89501; MTBLC34542; MTBLC61473; MTBLC3249; MTBLC4746; MTBLC80169; MTBLC34121; MTBLC52971; MTBLC93175; MTBLC137734; MTBLC73854; MTBLC90040; MTBLC89382; MTBLC89352; MTBLC89368; MTBLC89366; MTBLC89340; MTBLC89317; MTBLC137279; MTBLC137293; MTBLC134075; MTBLC90459; MTBLC134076; MTBLC134077; MTBLC134078; MTBLC39934; MTBLC134227; MTBLC134228; MTBLC16038; MTBLC9970; MTBLC4592; MTBLC79643; MTBLC34554; MTBLC2927; MTBLC27722; MTBLC28277; MTBLC80014; MTBLC77258; MTBLC4915; MTBLC5746; MTBLC28468; MTBLC64563; MTBLC76078; MTBLC72998; MTBLC78101; MTBLC73721; MTBLC73134; MTBLC73004; MTBLC62837; MTBLC78270; MTBLC36476; MTBLC79536; MTBLC73894; MTBLC31676; MTBLC50782; MTBLC31650; MTBLC6574; MTBLC31940; MTBLC44247; MTBLC79899; MTBLC27965; MTBLC79098; MTBLC75038; MTBLC133623; MTBLC84577; MTBLC84234; MTBLC64032; MTBLC53486; MTBLC53460; MTBLC79878; MTBLC79900; MTBLC525464; MTBLC79409; MTBLC79578; MTBLC82832; MTBLC71589; MTBLC32023; MTBLC34349; MTBLC32068; MTBLC31020; MTBLC2502; MTBLC28593; MTBLC15854; MTBLC309594; MTBLC84116; MTBLC3560; MTBLC79190; MTBLC76992; MTBLC52347; MTBLC18164; MTBLC32027; MTBLC135857; MTBLC88780; MTBLC88468; MTBLC75342; MTBLC744; MTBLC34115; MTBLC84911; MTBLC32154; MTBLC131508; MTBLC32906; MTBLC29596; MTBLC28211; MTBLC6927; MTBLC7603; MTBLC80537; MTBLC10137; MTBLC80732; MTBLC79113; MTBLC90041; MTBLC133599; MTBLC133617; MTBLC84845; MTBLC84844; MTBLC74986; MTBLC143985; MTBLC80203; MTBLC143980; MTBLC57409; MTBLC134453; MTBLC34126; MTBLC34130; MTBLC79851; MTBLC72606; MTBLC19138; MTBLC137345; MTBLC34157; MTBLC88823; MTBLC78837; MTBLC64017; MTBLC34162; MTBLC79557; MTBLC79656; MTBLC63995; MTBLC79561; MTBLC63579; MTBLC34185; MTBLC34306; MTBLC79485; MTBLC34450; MTBLC60943; MTBLC137344; MTBLC34490; MTBLC72643; MTBLC72786; MTBLC36275; MTBLC86031; MTBLC73733; MTBLC89091; MTBLC75646; MTBLC89387; MTBLC89392; MTBLC89395; MTBLC89394; MTBLC53081; MTBLC76284; MTBLC137704; MTBLC34438; MTBLC32319; MTBLC32325; MTBLC34711; MTBLC4676; MTBLC34136; MTBLC39449; MTBLC39451; MTBLC39453; MTBLC39454; MTBLC31406; MTBLC10580; MTBLC39448; MTBLC4722; MTBLC19287; MTBLC31164; MTBLC27655; MTBLC5715; MTBLC6567; MTBLC6586; MTBLC34883; MTBLC88902; MTBLC8034; MTBLC10045; MTBLC10089; MTBLC80194; MTBLC79956; MTBLC79588; MTBLC81561; MTBLC2296; MTBLC3321; MTBLC65585; MTBLC134353; MTBLC143960; MTBLC30088; MTBLC29589; MTBLC29601; MTBLC6696; MTBLC133423; MTBLC134511; MTBLC140267; MTBLC8390; MTBLC5783; MTBLC80531; MTBLC16688; MTBLC28135; MTBLC137137; MTBLC139534; MTBLC31731; MTBLC73923; MTBLC31801; MTBLC35459; MTBLC135729; MTBLC135684; MTBLC86197; MTBLC86196; MTBLC86189; MTBLC86190; MTBLC86188; MTBLC80532; MTBLC18531; MTBLC18532; MTBLC46739; MTBLC79839; MTBLC28033; MTBLC17168; MTBLC16608; MTBLC17762; MTBLC16074; MTBLC16113; MTBLC143982; MTBLC28610; MTBLC86255; MTBLC76071; MTBLC143713; MTBLC72589; MTBLC131658; MTBLC31025; MTBLC17390; MTBLC27808; MTBLC5191; MTBLC31123; MTBLC82648; MTBLC135276; MTBLC4670; MTBLC143989; MTBLC9669; MTBLC52672; MTBLC37945; MTBLC34899; MTBLC37923; MTBLC8710; MTBLC31550; MTBLC3156; MTBLC48742; MTBLC135719; MTBLC8036; MTBLC7352; MTBLC90970; MTBLC47834; MTBLC63911; MTBLC137141; MTBLC47799; MTBLC72727; MTBLC80530; MTBLC5363; MTBLC52348; MTBLC17314; MTBLC76980; MTBLC76304; MTBLC6113; MTBLC143987; MTBLC143990; MTBLC9911; MTBLC135737; MTBLC28700; MTBLC79923; MTBLC73794; MTBLC62736; MTBLC62737; MTBLC84958; MTBLC86418; MTBLC89703; MTBLC89592; MTBLC89589; MTBLC89384; MTBLC89098; MTBLC89143; MTBLC89070; MTBLC88726; MTBLC88872; MTBLC88588; MTBLC89498; MTBLC89502; MTBLC143981; MTBLC143983; MTBLC71466; MTBLC9453; MTBLC31264; MTBLC131689; MTBLC74340; MTBLC131668; MTBLC131687; MTBLC131688; MTBLC52639; MTBLC85403; MTBLC29613; MTBLC79453; MTBLC28047; MTBLC132620; MTBLC31257; MTBLC29677; MTBLC31222; MTBLC5197; MTBLC135094; MTBLC32277; MTBLC15929; MTBLC25242; MTBLC28258; MTBLC134924; MTBLC86975; MTBLC88529; MTBLC89026; MTBLC137784; MTBLC32002; MTBLC125; MTBLC46734; MTBLC141283; MTBLC16774; MTBLC35966; MTBLC16619; MTBLC10217; MTBLC10278; MTBLC10417; MTBLC3431; MTBLC4001; MTBLC5552; MTBLC5719; MTBLC6401; MTBLC7524; MTBLC7940; MTBLC64792; MTBLC137092; MTBLC144025; MTBLC10274; MTBLC3087; MTBLC37659; MTBLC135741; MTBLC9908; MTBLC18067; MTBLC89279; MTBLC89380; MTBLC89383; MTBLC89360; MTBLC89359; MTBLC89370; MTBLC84566; MTBLC137216; MTBLC85680; MTBLC18168; MTBLC52350; MTBLC73731; MTBLC78706; MTBLC31572; MTBLC36036; MTBLC9053; MTBLC89090; MTBLC89089; MTBLC89074; MTBLC89390; MTBLC89357; MTBLC89374; MTBLC89373; MTBLC90454; MTBLC75376; MTBLC17058; MTBLC28688; MTBLC34184; MTBLC3941; MTBLC53424; MTBLC1309; MTBLC1310; MTBLC79897; MTBLC63065; MTBLC143013; MTBLC4813; MTBLC134507; MTBLC84759; MTBLC34835; MTBLC84877; MTBLC39248; MTBLC34122; MTBLC84386; MTBLC88781; MTBLC88757; MTBLC88469; MTBLC75550; MTBLC83055; MTBLC27423; MTBLC37998; MTBLC2944; MTBLC132949; MTBLC137858; MTBLC137136; MTBLC79992; MTBLC9948; MTBLC135723; MTBLC90233; MTBLC137178; MTBLC73736; MTBLC39826; MTBLC50158; MTBLC17177; MTBLC16697; MTBLC52052; MTBLC16101; MTBLC28488; MTBLC28063; MTBLC27417; MTBLC84341; MTBLC88756; MTBLC3663; MTBLC59912; MTBLC80083; MTBLC94686; MTBLC137229; MTBLC82836; MTBLC77525; MTBLC34743; MTBLC133914; MTBLC89451; MTBLC135440; MTBLC72844; MTBLC79787; MTBLC79494; MTBLC88359; MTBLC140473; MTBLC137304; MTBLC63836; MTBLC73135; MTBLC48131; MTBLC79444; MTBLC2696; MTBLC46750; MTBLC7952; MTBLC8186; MTBLC32249; MTBLC15884; MTBLC41872; MTBLC33275; MTBLC33277</t>
   </si>
 </sst>
 </file>
@@ -1182,22 +1182,22 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="F13" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="G13" t="s">
         <v>0</v>
@@ -1206,45 +1206,45 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="J13" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="K13" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="L13" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="M13" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="N13" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="O13" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="C14" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="D14" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="E14" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="F14" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="G14" t="s">
         <v>0</v>
@@ -1253,25 +1253,25 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="J14" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="K14" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="L14" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="M14" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="N14" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="O14" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15">
@@ -1379,13 +1379,13 @@
         <v>173</v>
       </c>
       <c r="D17" t="s">
-        <v>138</v>
+        <v>174</v>
       </c>
       <c r="E17" t="s">
-        <v>138</v>
+        <v>174</v>
       </c>
       <c r="F17" t="s">
-        <v>139</v>
+        <v>175</v>
       </c>
       <c r="G17" t="s">
         <v>0</v>
@@ -1394,45 +1394,45 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>140</v>
+        <v>176</v>
       </c>
       <c r="J17" t="s">
-        <v>141</v>
+        <v>177</v>
       </c>
       <c r="K17" t="s">
-        <v>142</v>
+        <v>178</v>
       </c>
       <c r="L17" t="s">
-        <v>143</v>
+        <v>179</v>
       </c>
       <c r="M17" t="s">
-        <v>144</v>
+        <v>180</v>
       </c>
       <c r="N17" t="s">
-        <v>145</v>
+        <v>181</v>
       </c>
       <c r="O17" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="B18" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="C18" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="D18" t="s">
-        <v>178</v>
+        <v>138</v>
       </c>
       <c r="E18" t="s">
-        <v>178</v>
+        <v>138</v>
       </c>
       <c r="F18" t="s">
-        <v>179</v>
+        <v>139</v>
       </c>
       <c r="G18" t="s">
         <v>0</v>
@@ -1441,22 +1441,22 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="J18" t="s">
-        <v>181</v>
+        <v>141</v>
       </c>
       <c r="K18" t="s">
-        <v>182</v>
+        <v>142</v>
       </c>
       <c r="L18" t="s">
-        <v>183</v>
+        <v>143</v>
       </c>
       <c r="M18" t="s">
-        <v>184</v>
+        <v>144</v>
       </c>
       <c r="N18" t="s">
-        <v>185</v>
+        <v>145</v>
       </c>
       <c r="O18" t="s">
         <v>186</v>

</xml_diff>